<commit_message>
add RKI data downloaded 2020-12-31--13-35-01
</commit_message>
<xml_diff>
--- a/rki-data/RKI-Altersverteilung.xlsx
+++ b/rki-data/RKI-Altersverteilung.xlsx
@@ -1,28 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20368"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Wissdaten\RKI_nCoV-Lage\3.Kommunikation\3.7.Lageberichte\2020-12-22\Webmaster\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD1B2BD-6910-486B-BB29-8D4E396A7CF1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20367"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE7BB3E-9FFE-47CF-AB11-0420EEE0E5B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6525" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Erläuterungen" sheetId="3" r:id="rId1"/>
-    <sheet name="Fallzahlen" sheetId="1" r:id="rId2"/>
-    <sheet name="inzidenz_tabelle" sheetId="2" r:id="rId3"/>
+    <sheet name="Fallzahlen" sheetId="2" r:id="rId2"/>
+    <sheet name="Inzidenzen" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
   <si>
     <t>Altersgruppe</t>
   </si>
@@ -81,20 +76,14 @@
     <t>0 - 4</t>
   </si>
   <si>
-    <t>5 - 9</t>
-  </si>
-  <si>
-    <t>10 - 14</t>
-  </si>
-  <si>
-    <t>Für die Berechnung von Inzidenzen wurde die Bevölkerungsstatistik
-mit Stand 31.12.2019 herangezogen.</t>
+    <t xml:space="preserve">Zur besseren Übersicht werden mit Berichtswoche 46 die altersspezifischen Anteile als 7-Tage-Inzidenz pro 100.000 Einwohner nach Meldewoche dargestellt. </t>
   </si>
   <si>
     <t xml:space="preserve">Auf den folgenden Tabellenblättern finden sich die altersspezifischen Fallzahlen sowie die altersspezifischen 7-Tage-Inzidenzen. </t>
   </si>
   <si>
-    <t xml:space="preserve">Zur besseren Übersicht werden mit Berichtswoche 46 die altersspezifischen Anteile als 7-Tage-Inzidenz pro 100.000 Einwohner nach Meldewoche dargestellt. </t>
+    <t>Für die Berechnung von Inzidenzen wurde die Bevölkerungsstatistik
+mit Stand 31.12.2019 herangezogen.</t>
   </si>
 </sst>
 </file>
@@ -578,9 +567,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -938,52 +928,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7365347A-3546-4959-9669-FB1805DC4E35}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E2FB09-40BA-467A-9A47-7CEA9C443D24}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.140625" customWidth="1"/>
+    <col min="1" max="1" width="48.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>23</v>
+    <row r="1" spans="1:1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>22</v>
+    <row r="2" spans="1:1" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+      <c r="A3" s="3"/>
     </row>
     <row r="4" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AQ21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AR21"/>
   <sheetViews>
-    <sheetView topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1113,49 +1102,52 @@
       <c r="AQ1">
         <v>51</v>
       </c>
+      <c r="AR1">
+        <v>52</v>
+      </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="C2">
         <v>6433</v>
       </c>
       <c r="D2">
-        <v>22430</v>
+        <v>22431</v>
       </c>
       <c r="E2">
-        <v>34027</v>
+        <v>34028</v>
       </c>
       <c r="F2">
-        <v>36092</v>
+        <v>36094</v>
       </c>
       <c r="G2">
-        <v>27185</v>
+        <v>27188</v>
       </c>
       <c r="H2">
-        <v>17361</v>
+        <v>17363</v>
       </c>
       <c r="I2">
         <v>12381</v>
       </c>
       <c r="J2">
-        <v>7443</v>
+        <v>7442</v>
       </c>
       <c r="K2">
         <v>6229</v>
       </c>
       <c r="L2">
-        <v>4736</v>
+        <v>4735</v>
       </c>
       <c r="M2">
-        <v>3618</v>
+        <v>3617</v>
       </c>
       <c r="N2">
-        <v>3209</v>
+        <v>3211</v>
       </c>
       <c r="O2">
         <v>2360</v>
@@ -1164,10 +1156,10 @@
         <v>2345</v>
       </c>
       <c r="Q2">
-        <v>4094</v>
+        <v>4095</v>
       </c>
       <c r="R2">
-        <v>3206</v>
+        <v>3207</v>
       </c>
       <c r="S2">
         <v>2694</v>
@@ -1179,73 +1171,76 @@
         <v>3024</v>
       </c>
       <c r="V2">
-        <v>3936</v>
+        <v>3938</v>
       </c>
       <c r="W2">
-        <v>4822</v>
+        <v>4824</v>
       </c>
       <c r="X2">
-        <v>6062</v>
+        <v>6063</v>
       </c>
       <c r="Y2">
-        <v>7953</v>
+        <v>7956</v>
       </c>
       <c r="Z2">
-        <v>9592</v>
+        <v>9587</v>
       </c>
       <c r="AA2">
-        <v>8816</v>
+        <v>8819</v>
       </c>
       <c r="AB2">
-        <v>8614</v>
+        <v>8616</v>
       </c>
       <c r="AC2">
-        <v>9767</v>
+        <v>9766</v>
       </c>
       <c r="AD2">
-        <v>12271</v>
+        <v>12278</v>
       </c>
       <c r="AE2">
-        <v>13057</v>
+        <v>13058</v>
       </c>
       <c r="AF2">
-        <v>15913</v>
+        <v>15914</v>
       </c>
       <c r="AG2">
-        <v>26154</v>
+        <v>26158</v>
       </c>
       <c r="AH2">
-        <v>42059</v>
+        <v>42068</v>
       </c>
       <c r="AI2">
-        <v>74802</v>
+        <v>74826</v>
       </c>
       <c r="AJ2">
-        <v>111168</v>
+        <v>111161</v>
       </c>
       <c r="AK2">
-        <v>125751</v>
+        <v>125775</v>
       </c>
       <c r="AL2">
-        <v>127786</v>
+        <v>127842</v>
       </c>
       <c r="AM2">
-        <v>128491</v>
+        <v>128532</v>
       </c>
       <c r="AN2">
-        <v>123367</v>
+        <v>123357</v>
       </c>
       <c r="AO2">
-        <v>128270</v>
+        <v>128304</v>
       </c>
       <c r="AP2">
-        <v>155803</v>
+        <v>155956</v>
       </c>
       <c r="AQ2">
-        <v>171262</v>
+        <v>173481</v>
+      </c>
+      <c r="AR2">
+        <v>135974</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1280,7 +1275,7 @@
         <v>208</v>
       </c>
       <c r="L3">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M3">
         <v>103</v>
@@ -1325,7 +1320,7 @@
         <v>18</v>
       </c>
       <c r="AA3">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB3">
         <v>24</v>
@@ -1334,7 +1329,7 @@
         <v>44</v>
       </c>
       <c r="AD3">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AE3">
         <v>94</v>
@@ -1346,37 +1341,40 @@
         <v>186</v>
       </c>
       <c r="AH3">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="AI3">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="AJ3">
         <v>1464</v>
       </c>
       <c r="AK3">
-        <v>1714</v>
+        <v>1716</v>
       </c>
       <c r="AL3">
-        <v>2310</v>
+        <v>2311</v>
       </c>
       <c r="AM3">
-        <v>3061</v>
+        <v>3064</v>
       </c>
       <c r="AN3">
         <v>3504</v>
       </c>
       <c r="AO3">
-        <v>4147</v>
+        <v>4141</v>
       </c>
       <c r="AP3">
-        <v>5382</v>
+        <v>5393</v>
       </c>
       <c r="AQ3">
-        <v>5744</v>
+        <v>5842</v>
+      </c>
+      <c r="AR3">
+        <v>5100</v>
       </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1450,7 +1448,7 @@
         <v>40</v>
       </c>
       <c r="Y4">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Z4">
         <v>23</v>
@@ -1477,37 +1475,40 @@
         <v>305</v>
       </c>
       <c r="AH4">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="AI4">
-        <v>1133</v>
+        <v>1136</v>
       </c>
       <c r="AJ4">
         <v>1780</v>
       </c>
       <c r="AK4">
-        <v>2280</v>
+        <v>2282</v>
       </c>
       <c r="AL4">
-        <v>2822</v>
+        <v>2827</v>
       </c>
       <c r="AM4">
-        <v>3358</v>
+        <v>3366</v>
       </c>
       <c r="AN4">
-        <v>4084</v>
+        <v>4090</v>
       </c>
       <c r="AO4">
-        <v>4582</v>
+        <v>4581</v>
       </c>
       <c r="AP4">
-        <v>5894</v>
+        <v>5900</v>
       </c>
       <c r="AQ4">
-        <v>6731</v>
+        <v>6831</v>
+      </c>
+      <c r="AR4">
+        <v>5674</v>
       </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1515,7 +1516,7 @@
         <v>11</v>
       </c>
       <c r="C5">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D5">
         <v>468</v>
@@ -1527,7 +1528,7 @@
         <v>1966</v>
       </c>
       <c r="G5">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="H5">
         <v>1183</v>
@@ -1536,13 +1537,13 @@
         <v>823</v>
       </c>
       <c r="J5">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="K5">
         <v>299</v>
       </c>
       <c r="L5">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="M5">
         <v>152</v>
@@ -1575,7 +1576,7 @@
         <v>50</v>
       </c>
       <c r="W5">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="X5">
         <v>69</v>
@@ -1593,7 +1594,7 @@
         <v>61</v>
       </c>
       <c r="AC5">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AD5">
         <v>195</v>
@@ -1617,28 +1618,31 @@
         <v>2843</v>
       </c>
       <c r="AK5">
-        <v>3430</v>
+        <v>3432</v>
       </c>
       <c r="AL5">
-        <v>3794</v>
+        <v>3796</v>
       </c>
       <c r="AM5">
-        <v>4351</v>
+        <v>4357</v>
       </c>
       <c r="AN5">
-        <v>4786</v>
+        <v>4787</v>
       </c>
       <c r="AO5">
-        <v>5432</v>
+        <v>5425</v>
       </c>
       <c r="AP5">
-        <v>7023</v>
+        <v>7029</v>
       </c>
       <c r="AQ5">
-        <v>8017</v>
+        <v>8164</v>
+      </c>
+      <c r="AR5">
+        <v>7221</v>
       </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1655,7 +1659,7 @@
         <v>1408</v>
       </c>
       <c r="F6">
-        <v>1785</v>
+        <v>1786</v>
       </c>
       <c r="G6">
         <v>1313</v>
@@ -1664,7 +1668,7 @@
         <v>853</v>
       </c>
       <c r="I6">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="J6">
         <v>351</v>
@@ -1703,7 +1707,7 @@
         <v>44</v>
       </c>
       <c r="V6">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="W6">
         <v>71</v>
@@ -1712,7 +1716,7 @@
         <v>56</v>
       </c>
       <c r="Y6">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Z6">
         <v>67</v>
@@ -1748,28 +1752,31 @@
         <v>2646</v>
       </c>
       <c r="AK6">
-        <v>3048</v>
+        <v>3047</v>
       </c>
       <c r="AL6">
         <v>3286</v>
       </c>
       <c r="AM6">
-        <v>3382</v>
+        <v>3386</v>
       </c>
       <c r="AN6">
         <v>3492</v>
       </c>
       <c r="AO6">
-        <v>3959</v>
+        <v>3955</v>
       </c>
       <c r="AP6">
-        <v>4964</v>
+        <v>4971</v>
       </c>
       <c r="AQ6">
-        <v>5820</v>
+        <v>5903</v>
+      </c>
+      <c r="AR6">
+        <v>4940</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1864,43 +1871,46 @@
         <v>266</v>
       </c>
       <c r="AF7">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="AG7">
         <v>591</v>
       </c>
       <c r="AH7">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="AI7">
         <v>1793</v>
       </c>
       <c r="AJ7">
-        <v>2881</v>
+        <v>2882</v>
       </c>
       <c r="AK7">
-        <v>3170</v>
+        <v>3173</v>
       </c>
       <c r="AL7">
-        <v>3289</v>
+        <v>3288</v>
       </c>
       <c r="AM7">
-        <v>3352</v>
+        <v>3354</v>
       </c>
       <c r="AN7">
-        <v>3201</v>
+        <v>3196</v>
       </c>
       <c r="AO7">
-        <v>3464</v>
+        <v>3473</v>
       </c>
       <c r="AP7">
-        <v>4362</v>
+        <v>4366</v>
       </c>
       <c r="AQ7">
-        <v>5045</v>
+        <v>5141</v>
+      </c>
+      <c r="AR7">
+        <v>4318</v>
       </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1917,19 +1927,19 @@
         <v>1650</v>
       </c>
       <c r="F8">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="G8">
         <v>1116</v>
       </c>
       <c r="H8">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="I8">
         <v>506</v>
       </c>
       <c r="J8">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="K8">
         <v>208</v>
@@ -2001,37 +2011,40 @@
         <v>686</v>
       </c>
       <c r="AH8">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="AI8">
-        <v>2267</v>
+        <v>2268</v>
       </c>
       <c r="AJ8">
-        <v>3547</v>
+        <v>3549</v>
       </c>
       <c r="AK8">
-        <v>4237</v>
+        <v>4239</v>
       </c>
       <c r="AL8">
-        <v>4013</v>
+        <v>4014</v>
       </c>
       <c r="AM8">
-        <v>4143</v>
+        <v>4147</v>
       </c>
       <c r="AN8">
-        <v>4128</v>
+        <v>4124</v>
       </c>
       <c r="AO8">
-        <v>4129</v>
+        <v>4127</v>
       </c>
       <c r="AP8">
-        <v>5125</v>
+        <v>5141</v>
       </c>
       <c r="AQ8">
-        <v>6171</v>
+        <v>6257</v>
+      </c>
+      <c r="AR8">
+        <v>5433</v>
       </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2054,7 +2067,7 @@
         <v>1799</v>
       </c>
       <c r="H9">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="I9">
         <v>674</v>
@@ -2114,19 +2127,19 @@
         <v>243</v>
       </c>
       <c r="AB9">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AC9">
         <v>338</v>
       </c>
       <c r="AD9">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="AE9">
         <v>539</v>
       </c>
       <c r="AF9">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="AG9">
         <v>1270</v>
@@ -2141,28 +2154,31 @@
         <v>5984</v>
       </c>
       <c r="AK9">
-        <v>6838</v>
+        <v>6845</v>
       </c>
       <c r="AL9">
-        <v>6891</v>
+        <v>6895</v>
       </c>
       <c r="AM9">
-        <v>7299</v>
+        <v>7304</v>
       </c>
       <c r="AN9">
-        <v>6984</v>
+        <v>6982</v>
       </c>
       <c r="AO9">
-        <v>7644</v>
+        <v>7645</v>
       </c>
       <c r="AP9">
-        <v>9373</v>
+        <v>9386</v>
       </c>
       <c r="AQ9">
-        <v>10715</v>
+        <v>10902</v>
+      </c>
+      <c r="AR9">
+        <v>8887</v>
       </c>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2227,7 +2243,7 @@
         <v>177</v>
       </c>
       <c r="V10">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="W10">
         <v>286</v>
@@ -2260,40 +2276,43 @@
         <v>1106</v>
       </c>
       <c r="AG10">
-        <v>1864</v>
+        <v>1865</v>
       </c>
       <c r="AH10">
         <v>2998</v>
       </c>
       <c r="AI10">
-        <v>5750</v>
+        <v>5756</v>
       </c>
       <c r="AJ10">
-        <v>8953</v>
+        <v>8950</v>
       </c>
       <c r="AK10">
         <v>10148</v>
       </c>
       <c r="AL10">
-        <v>10293</v>
+        <v>10296</v>
       </c>
       <c r="AM10">
-        <v>10238</v>
+        <v>10239</v>
       </c>
       <c r="AN10">
-        <v>9844</v>
+        <v>9842</v>
       </c>
       <c r="AO10">
-        <v>10324</v>
+        <v>10330</v>
       </c>
       <c r="AP10">
-        <v>12955</v>
+        <v>12977</v>
       </c>
       <c r="AQ10">
-        <v>14667</v>
+        <v>14840</v>
+      </c>
+      <c r="AR10">
+        <v>11985</v>
       </c>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2319,7 +2338,7 @@
         <v>1557</v>
       </c>
       <c r="I11">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="J11">
         <v>603</v>
@@ -2328,7 +2347,7 @@
         <v>520</v>
       </c>
       <c r="L11">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="M11">
         <v>250</v>
@@ -2346,7 +2365,7 @@
         <v>314</v>
       </c>
       <c r="R11">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="S11">
         <v>186</v>
@@ -2376,13 +2395,13 @@
         <v>539</v>
       </c>
       <c r="AB11">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="AC11">
         <v>669</v>
       </c>
       <c r="AD11">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="AE11">
         <v>995</v>
@@ -2391,13 +2410,13 @@
         <v>1203</v>
       </c>
       <c r="AG11">
-        <v>2264</v>
+        <v>2265</v>
       </c>
       <c r="AH11">
-        <v>3569</v>
+        <v>3571</v>
       </c>
       <c r="AI11">
-        <v>6407</v>
+        <v>6409</v>
       </c>
       <c r="AJ11">
         <v>9764</v>
@@ -2406,36 +2425,39 @@
         <v>10941</v>
       </c>
       <c r="AL11">
-        <v>10976</v>
+        <v>10985</v>
       </c>
       <c r="AM11">
-        <v>10822</v>
+        <v>10823</v>
       </c>
       <c r="AN11">
-        <v>10313</v>
+        <v>10321</v>
       </c>
       <c r="AO11">
-        <v>10528</v>
+        <v>10533</v>
       </c>
       <c r="AP11">
-        <v>13181</v>
+        <v>13190</v>
       </c>
       <c r="AQ11">
-        <v>14618</v>
+        <v>14801</v>
+      </c>
+      <c r="AR11">
+        <v>11660</v>
       </c>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C12">
         <v>745</v>
       </c>
       <c r="D12">
-        <v>2095</v>
+        <v>2096</v>
       </c>
       <c r="E12">
         <v>2923</v>
@@ -2516,7 +2538,7 @@
         <v>875</v>
       </c>
       <c r="AE12">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="AF12">
         <v>1197</v>
@@ -2525,37 +2547,40 @@
         <v>2036</v>
       </c>
       <c r="AH12">
-        <v>3118</v>
+        <v>3120</v>
       </c>
       <c r="AI12">
-        <v>5804</v>
+        <v>5805</v>
       </c>
       <c r="AJ12">
-        <v>8379</v>
+        <v>8378</v>
       </c>
       <c r="AK12">
-        <v>9467</v>
+        <v>9466</v>
       </c>
       <c r="AL12">
-        <v>9271</v>
+        <v>9276</v>
       </c>
       <c r="AM12">
-        <v>9651</v>
+        <v>9657</v>
       </c>
       <c r="AN12">
         <v>9036</v>
       </c>
       <c r="AO12">
-        <v>9208</v>
+        <v>9215</v>
       </c>
       <c r="AP12">
-        <v>11044</v>
+        <v>11048</v>
       </c>
       <c r="AQ12">
-        <v>12168</v>
+        <v>12317</v>
+      </c>
+      <c r="AR12">
+        <v>9460</v>
       </c>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2569,13 +2594,13 @@
         <v>1803</v>
       </c>
       <c r="E13">
-        <v>2329</v>
+        <v>2330</v>
       </c>
       <c r="F13">
         <v>2309</v>
       </c>
       <c r="G13">
-        <v>1673</v>
+        <v>1674</v>
       </c>
       <c r="H13">
         <v>1023</v>
@@ -2584,7 +2609,7 @@
         <v>699</v>
       </c>
       <c r="J13">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="K13">
         <v>405</v>
@@ -2629,7 +2654,7 @@
         <v>488</v>
       </c>
       <c r="Y13">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="Z13">
         <v>716</v>
@@ -2650,43 +2675,46 @@
         <v>860</v>
       </c>
       <c r="AF13">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="AG13">
-        <v>1868</v>
+        <v>1869</v>
       </c>
       <c r="AH13">
-        <v>2907</v>
+        <v>2908</v>
       </c>
       <c r="AI13">
-        <v>5298</v>
+        <v>5299</v>
       </c>
       <c r="AJ13">
-        <v>7861</v>
+        <v>7858</v>
       </c>
       <c r="AK13">
-        <v>8850</v>
+        <v>8853</v>
       </c>
       <c r="AL13">
-        <v>8969</v>
+        <v>8968</v>
       </c>
       <c r="AM13">
-        <v>9228</v>
+        <v>9234</v>
       </c>
       <c r="AN13">
-        <v>8785</v>
+        <v>8776</v>
       </c>
       <c r="AO13">
-        <v>8804</v>
+        <v>8811</v>
       </c>
       <c r="AP13">
-        <v>10827</v>
+        <v>10840</v>
       </c>
       <c r="AQ13">
-        <v>11715</v>
+        <v>11873</v>
+      </c>
+      <c r="AR13">
+        <v>9275</v>
       </c>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -2697,7 +2725,7 @@
         <v>546</v>
       </c>
       <c r="D14">
-        <v>1754</v>
+        <v>1755</v>
       </c>
       <c r="E14">
         <v>2387</v>
@@ -2724,10 +2752,10 @@
         <v>351</v>
       </c>
       <c r="M14">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="N14">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="O14">
         <v>156</v>
@@ -2763,7 +2791,7 @@
         <v>645</v>
       </c>
       <c r="Z14">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="AA14">
         <v>715</v>
@@ -2775,7 +2803,7 @@
         <v>696</v>
       </c>
       <c r="AD14">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="AE14">
         <v>1004</v>
@@ -2784,40 +2812,43 @@
         <v>1148</v>
       </c>
       <c r="AG14">
-        <v>1827</v>
+        <v>1826</v>
       </c>
       <c r="AH14">
         <v>3107</v>
       </c>
       <c r="AI14">
-        <v>5385</v>
+        <v>5387</v>
       </c>
       <c r="AJ14">
-        <v>8080</v>
+        <v>8079</v>
       </c>
       <c r="AK14">
         <v>8950</v>
       </c>
       <c r="AL14">
-        <v>9169</v>
+        <v>9175</v>
       </c>
       <c r="AM14">
-        <v>9188</v>
+        <v>9189</v>
       </c>
       <c r="AN14">
-        <v>8709</v>
+        <v>8708</v>
       </c>
       <c r="AO14">
-        <v>9110</v>
+        <v>9118</v>
       </c>
       <c r="AP14">
-        <v>10922</v>
+        <v>10932</v>
       </c>
       <c r="AQ14">
-        <v>11944</v>
+        <v>12099</v>
+      </c>
+      <c r="AR14">
+        <v>9275</v>
       </c>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -2837,7 +2868,7 @@
         <v>2419</v>
       </c>
       <c r="G15">
-        <v>1750</v>
+        <v>1751</v>
       </c>
       <c r="H15">
         <v>1202</v>
@@ -2852,7 +2883,7 @@
         <v>489</v>
       </c>
       <c r="L15">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="M15">
         <v>323</v>
@@ -2891,13 +2922,13 @@
         <v>515</v>
       </c>
       <c r="Y15">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="Z15">
         <v>946</v>
       </c>
       <c r="AA15">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="AB15">
         <v>938</v>
@@ -2915,40 +2946,43 @@
         <v>1523</v>
       </c>
       <c r="AG15">
-        <v>2363</v>
+        <v>2364</v>
       </c>
       <c r="AH15">
-        <v>3863</v>
+        <v>3861</v>
       </c>
       <c r="AI15">
-        <v>6705</v>
+        <v>6706</v>
       </c>
       <c r="AJ15">
         <v>9570</v>
       </c>
       <c r="AK15">
-        <v>10462</v>
+        <v>10468</v>
       </c>
       <c r="AL15">
-        <v>10462</v>
+        <v>10468</v>
       </c>
       <c r="AM15">
-        <v>10094</v>
+        <v>10099</v>
       </c>
       <c r="AN15">
-        <v>9348</v>
+        <v>9349</v>
       </c>
       <c r="AO15">
-        <v>9437</v>
+        <v>9440</v>
       </c>
       <c r="AP15">
-        <v>11464</v>
+        <v>11473</v>
       </c>
       <c r="AQ15">
-        <v>12738</v>
+        <v>12896</v>
+      </c>
+      <c r="AR15">
+        <v>9847</v>
       </c>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -2959,13 +2993,13 @@
         <v>548</v>
       </c>
       <c r="D16">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="E16">
         <v>2694</v>
       </c>
       <c r="F16">
-        <v>2484</v>
+        <v>2485</v>
       </c>
       <c r="G16">
         <v>1935</v>
@@ -2998,7 +3032,7 @@
         <v>243</v>
       </c>
       <c r="Q16">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="R16">
         <v>325</v>
@@ -3028,7 +3062,7 @@
         <v>1192</v>
       </c>
       <c r="AA16">
-        <v>1220</v>
+        <v>1222</v>
       </c>
       <c r="AB16">
         <v>1157</v>
@@ -3049,10 +3083,10 @@
         <v>2690</v>
       </c>
       <c r="AH16">
-        <v>4477</v>
+        <v>4476</v>
       </c>
       <c r="AI16">
-        <v>7308</v>
+        <v>7309</v>
       </c>
       <c r="AJ16">
         <v>10325</v>
@@ -3061,25 +3095,28 @@
         <v>11142</v>
       </c>
       <c r="AL16">
-        <v>10678</v>
+        <v>10685</v>
       </c>
       <c r="AM16">
-        <v>9932</v>
+        <v>9931</v>
       </c>
       <c r="AN16">
         <v>8974</v>
       </c>
       <c r="AO16">
-        <v>9110</v>
+        <v>9112</v>
       </c>
       <c r="AP16">
-        <v>10743</v>
+        <v>10754</v>
       </c>
       <c r="AQ16">
-        <v>11897</v>
+        <v>12036</v>
+      </c>
+      <c r="AR16">
+        <v>9261</v>
       </c>
     </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -3090,13 +3127,13 @@
         <v>323</v>
       </c>
       <c r="D17">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="E17">
         <v>2274</v>
       </c>
       <c r="F17">
-        <v>2244</v>
+        <v>2245</v>
       </c>
       <c r="G17">
         <v>1732</v>
@@ -3147,28 +3184,28 @@
         <v>377</v>
       </c>
       <c r="W17">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="X17">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="Y17">
         <v>1168</v>
       </c>
       <c r="Z17">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="AA17">
         <v>1327</v>
       </c>
       <c r="AB17">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="AC17">
         <v>1289</v>
       </c>
       <c r="AD17">
-        <v>1515</v>
+        <v>1516</v>
       </c>
       <c r="AE17">
         <v>1583</v>
@@ -3183,34 +3220,37 @@
         <v>4374</v>
       </c>
       <c r="AI17">
-        <v>7547</v>
+        <v>7546</v>
       </c>
       <c r="AJ17">
-        <v>10434</v>
+        <v>10429</v>
       </c>
       <c r="AK17">
-        <v>11740</v>
+        <v>11744</v>
       </c>
       <c r="AL17">
-        <v>11030</v>
+        <v>11033</v>
       </c>
       <c r="AM17">
         <v>10222</v>
       </c>
       <c r="AN17">
-        <v>8944</v>
+        <v>8940</v>
       </c>
       <c r="AO17">
-        <v>9174</v>
+        <v>9180</v>
       </c>
       <c r="AP17">
-        <v>10742</v>
+        <v>10755</v>
       </c>
       <c r="AQ17">
-        <v>11887</v>
+        <v>12032</v>
+      </c>
+      <c r="AR17">
+        <v>8902</v>
       </c>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -3218,7 +3258,7 @@
         <v>42</v>
       </c>
       <c r="C18">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D18">
         <v>541</v>
@@ -3230,7 +3270,7 @@
         <v>1080</v>
       </c>
       <c r="G18">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="H18">
         <v>571</v>
@@ -3251,7 +3291,7 @@
         <v>154</v>
       </c>
       <c r="N18">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="O18">
         <v>162</v>
@@ -3299,51 +3339,54 @@
         <v>831</v>
       </c>
       <c r="AD18">
-        <v>1032</v>
+        <v>1034</v>
       </c>
       <c r="AE18">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="AF18">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="AG18">
-        <v>2072</v>
+        <v>2073</v>
       </c>
       <c r="AH18">
-        <v>2962</v>
+        <v>2964</v>
       </c>
       <c r="AI18">
-        <v>4851</v>
+        <v>4850</v>
       </c>
       <c r="AJ18">
-        <v>7189</v>
+        <v>7186</v>
       </c>
       <c r="AK18">
         <v>8399</v>
       </c>
       <c r="AL18">
-        <v>8681</v>
+        <v>8687</v>
       </c>
       <c r="AM18">
-        <v>8188</v>
+        <v>8192</v>
       </c>
       <c r="AN18">
-        <v>7447</v>
+        <v>7451</v>
       </c>
       <c r="AO18">
-        <v>7703</v>
+        <v>7710</v>
       </c>
       <c r="AP18">
-        <v>8797</v>
+        <v>8806</v>
       </c>
       <c r="AQ18">
-        <v>8324</v>
+        <v>8416</v>
+      </c>
+      <c r="AR18">
+        <v>5706</v>
       </c>
     </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>20</v>
+    <row r="19" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>41913</v>
       </c>
       <c r="B19">
         <v>21</v>
@@ -3400,7 +3443,7 @@
         <v>104</v>
       </c>
       <c r="T19">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="U19">
         <v>150</v>
@@ -3418,13 +3461,13 @@
         <v>545</v>
       </c>
       <c r="Z19">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="AA19">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="AB19">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="AC19">
         <v>498</v>
@@ -3445,36 +3488,39 @@
         <v>1652</v>
       </c>
       <c r="AI19">
-        <v>2740</v>
+        <v>2741</v>
       </c>
       <c r="AJ19">
-        <v>4082</v>
+        <v>4085</v>
       </c>
       <c r="AK19">
         <v>4768</v>
       </c>
       <c r="AL19">
-        <v>5341</v>
+        <v>5342</v>
       </c>
       <c r="AM19">
-        <v>5294</v>
+        <v>5293</v>
       </c>
       <c r="AN19">
-        <v>5168</v>
+        <v>5167</v>
       </c>
       <c r="AO19">
-        <v>5140</v>
+        <v>5141</v>
       </c>
       <c r="AP19">
-        <v>5631</v>
+        <v>5644</v>
       </c>
       <c r="AQ19">
-        <v>5133</v>
+        <v>5217</v>
+      </c>
+      <c r="AR19">
+        <v>3300</v>
       </c>
     </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>19</v>
+    <row r="20" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>44079</v>
       </c>
       <c r="B20">
         <v>10</v>
@@ -3531,7 +3577,7 @@
         <v>124</v>
       </c>
       <c r="T20">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="U20">
         <v>138</v>
@@ -3549,7 +3595,7 @@
         <v>407</v>
       </c>
       <c r="Z20">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="AA20">
         <v>352</v>
@@ -3564,7 +3610,7 @@
         <v>354</v>
       </c>
       <c r="AE20">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AF20">
         <v>429</v>
@@ -3573,37 +3619,40 @@
         <v>625</v>
       </c>
       <c r="AH20">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="AI20">
-        <v>1830</v>
+        <v>1834</v>
       </c>
       <c r="AJ20">
-        <v>2790</v>
+        <v>2792</v>
       </c>
       <c r="AK20">
-        <v>3355</v>
+        <v>3358</v>
       </c>
       <c r="AL20">
-        <v>3619</v>
+        <v>3620</v>
       </c>
       <c r="AM20">
-        <v>3905</v>
+        <v>3906</v>
       </c>
       <c r="AN20">
-        <v>3800</v>
+        <v>3805</v>
       </c>
       <c r="AO20">
-        <v>3662</v>
+        <v>3666</v>
       </c>
       <c r="AP20">
-        <v>4231</v>
+        <v>4234</v>
       </c>
       <c r="AQ20">
-        <v>4207</v>
+        <v>4266</v>
+      </c>
+      <c r="AR20">
+        <v>2961</v>
       </c>
     </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -3623,7 +3672,7 @@
         <v>274</v>
       </c>
       <c r="G21">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="H21">
         <v>161</v>
@@ -3680,7 +3729,7 @@
         <v>276</v>
       </c>
       <c r="Z21">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="AA21">
         <v>223</v>
@@ -3704,52 +3753,56 @@
         <v>524</v>
       </c>
       <c r="AH21">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="AI21">
-        <v>1462</v>
+        <v>1464</v>
       </c>
       <c r="AJ21">
-        <v>2246</v>
+        <v>2247</v>
       </c>
       <c r="AK21">
-        <v>2431</v>
+        <v>2427</v>
       </c>
       <c r="AL21">
         <v>2428</v>
       </c>
       <c r="AM21">
-        <v>2388</v>
+        <v>2386</v>
       </c>
       <c r="AN21">
-        <v>2343</v>
+        <v>2340</v>
       </c>
       <c r="AO21">
-        <v>2324</v>
+        <v>2321</v>
       </c>
       <c r="AP21">
-        <v>2695</v>
+        <v>2694</v>
       </c>
       <c r="AQ21">
-        <v>3111</v>
+        <v>3126</v>
+      </c>
+      <c r="AR21">
+        <v>2138</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AQ21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AR21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3879,8 +3932,11 @@
       <c r="AQ1">
         <v>51</v>
       </c>
+      <c r="AR1">
+        <v>52</v>
+      </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -3894,7 +3950,7 @@
         <v>26.97</v>
       </c>
       <c r="E2">
-        <v>40.909999999999997</v>
+        <v>40.92</v>
       </c>
       <c r="F2">
         <v>43.4</v>
@@ -3903,7 +3959,7 @@
         <v>32.69</v>
       </c>
       <c r="H2">
-        <v>20.87</v>
+        <v>20.88</v>
       </c>
       <c r="I2">
         <v>14.89</v>
@@ -3933,7 +3989,7 @@
         <v>4.92</v>
       </c>
       <c r="R2">
-        <v>3.85</v>
+        <v>3.86</v>
       </c>
       <c r="S2">
         <v>3.24</v>
@@ -3945,7 +4001,7 @@
         <v>3.64</v>
       </c>
       <c r="V2">
-        <v>4.7300000000000004</v>
+        <v>4.74</v>
       </c>
       <c r="W2">
         <v>5.8</v>
@@ -3954,7 +4010,7 @@
         <v>7.29</v>
       </c>
       <c r="Y2">
-        <v>9.56</v>
+        <v>9.57</v>
       </c>
       <c r="Z2">
         <v>11.53</v>
@@ -3969,49 +4025,52 @@
         <v>11.74</v>
       </c>
       <c r="AD2">
-        <v>14.75</v>
+        <v>14.76</v>
       </c>
       <c r="AE2">
         <v>15.7</v>
       </c>
       <c r="AF2">
-        <v>19.13</v>
+        <v>19.14</v>
       </c>
       <c r="AG2">
         <v>31.45</v>
       </c>
       <c r="AH2">
-        <v>50.57</v>
+        <v>50.58</v>
       </c>
       <c r="AI2">
-        <v>89.94</v>
+        <v>89.97</v>
       </c>
       <c r="AJ2">
-        <v>133.66999999999999</v>
+        <v>133.66</v>
       </c>
       <c r="AK2">
-        <v>151.19999999999999</v>
+        <v>151.22999999999999</v>
       </c>
       <c r="AL2">
-        <v>153.65</v>
+        <v>153.72</v>
       </c>
       <c r="AM2">
-        <v>154.5</v>
+        <v>154.55000000000001</v>
       </c>
       <c r="AN2">
-        <v>148.34</v>
+        <v>148.32</v>
       </c>
       <c r="AO2">
-        <v>154.22999999999999</v>
+        <v>154.27000000000001</v>
       </c>
       <c r="AP2">
-        <v>187.34</v>
+        <v>187.52</v>
       </c>
       <c r="AQ2">
-        <v>205.93</v>
+        <v>208.59</v>
+      </c>
+      <c r="AR2">
+        <v>163.5</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -4046,7 +4105,7 @@
         <v>25.27</v>
       </c>
       <c r="L3">
-        <v>17.25</v>
+        <v>17.13</v>
       </c>
       <c r="M3">
         <v>12.51</v>
@@ -4091,7 +4150,7 @@
         <v>2.19</v>
       </c>
       <c r="AA3">
-        <v>3.52</v>
+        <v>3.64</v>
       </c>
       <c r="AB3">
         <v>2.92</v>
@@ -4100,7 +4159,7 @@
         <v>5.35</v>
       </c>
       <c r="AD3">
-        <v>8.8699999999999992</v>
+        <v>8.99</v>
       </c>
       <c r="AE3">
         <v>11.42</v>
@@ -4112,37 +4171,40 @@
         <v>22.6</v>
       </c>
       <c r="AH3">
-        <v>52.12</v>
+        <v>52.37</v>
       </c>
       <c r="AI3">
-        <v>107.41</v>
+        <v>107.53</v>
       </c>
       <c r="AJ3">
         <v>177.88</v>
       </c>
       <c r="AK3">
-        <v>208.25</v>
+        <v>208.49</v>
       </c>
       <c r="AL3">
-        <v>280.66000000000003</v>
+        <v>280.79000000000002</v>
       </c>
       <c r="AM3">
-        <v>371.91</v>
+        <v>372.28</v>
       </c>
       <c r="AN3">
         <v>425.74</v>
       </c>
       <c r="AO3">
-        <v>503.86</v>
+        <v>503.13</v>
       </c>
       <c r="AP3">
-        <v>653.91</v>
+        <v>655.25</v>
       </c>
       <c r="AQ3">
-        <v>697.89</v>
+        <v>709.8</v>
+      </c>
+      <c r="AR3">
+        <v>619.65</v>
       </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -4216,7 +4278,7 @@
         <v>2.56</v>
       </c>
       <c r="Y4">
-        <v>3.52</v>
+        <v>3.58</v>
       </c>
       <c r="Z4">
         <v>1.47</v>
@@ -4243,37 +4305,40 @@
         <v>19.5</v>
       </c>
       <c r="AH4">
-        <v>36.19</v>
+        <v>36.32</v>
       </c>
       <c r="AI4">
-        <v>72.45</v>
+        <v>72.64</v>
       </c>
       <c r="AJ4">
         <v>113.82</v>
       </c>
       <c r="AK4">
-        <v>145.80000000000001</v>
+        <v>145.93</v>
       </c>
       <c r="AL4">
-        <v>180.46</v>
+        <v>180.78</v>
       </c>
       <c r="AM4">
-        <v>214.73</v>
+        <v>215.24</v>
       </c>
       <c r="AN4">
-        <v>261.16000000000003</v>
+        <v>261.54000000000002</v>
       </c>
       <c r="AO4">
-        <v>293</v>
+        <v>292.94</v>
       </c>
       <c r="AP4">
-        <v>376.9</v>
+        <v>377.28</v>
       </c>
       <c r="AQ4">
-        <v>430.42</v>
+        <v>436.82</v>
+      </c>
+      <c r="AR4">
+        <v>362.83</v>
       </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -4281,7 +4346,7 @@
         <v>0.33</v>
       </c>
       <c r="C5">
-        <v>2.46</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="D5">
         <v>14.21</v>
@@ -4293,7 +4358,7 @@
         <v>59.68</v>
       </c>
       <c r="G5">
-        <v>52.24</v>
+        <v>52.21</v>
       </c>
       <c r="H5">
         <v>35.909999999999997</v>
@@ -4302,13 +4367,13 @@
         <v>24.98</v>
       </c>
       <c r="J5">
-        <v>13.69</v>
+        <v>13.66</v>
       </c>
       <c r="K5">
         <v>9.08</v>
       </c>
       <c r="L5">
-        <v>7.5</v>
+        <v>7.47</v>
       </c>
       <c r="M5">
         <v>4.6100000000000003</v>
@@ -4341,7 +4406,7 @@
         <v>1.52</v>
       </c>
       <c r="W5">
-        <v>2.67</v>
+        <v>2.7</v>
       </c>
       <c r="X5">
         <v>2.09</v>
@@ -4359,7 +4424,7 @@
         <v>1.85</v>
       </c>
       <c r="AC5">
-        <v>4.01</v>
+        <v>3.98</v>
       </c>
       <c r="AD5">
         <v>5.92</v>
@@ -4383,28 +4448,31 @@
         <v>86.3</v>
       </c>
       <c r="AK5">
-        <v>104.12</v>
+        <v>104.18</v>
       </c>
       <c r="AL5">
-        <v>115.17</v>
+        <v>115.23</v>
       </c>
       <c r="AM5">
-        <v>132.08000000000001</v>
+        <v>132.26</v>
       </c>
       <c r="AN5">
-        <v>145.28</v>
+        <v>145.31</v>
       </c>
       <c r="AO5">
-        <v>164.89</v>
+        <v>164.68</v>
       </c>
       <c r="AP5">
-        <v>213.19</v>
+        <v>213.37</v>
       </c>
       <c r="AQ5">
-        <v>243.36</v>
+        <v>247.82</v>
+      </c>
+      <c r="AR5">
+        <v>219.2</v>
       </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -4421,7 +4489,7 @@
         <v>36.32</v>
       </c>
       <c r="F6">
-        <v>46.05</v>
+        <v>46.07</v>
       </c>
       <c r="G6">
         <v>33.869999999999997</v>
@@ -4430,7 +4498,7 @@
         <v>22</v>
       </c>
       <c r="I6">
-        <v>15.14</v>
+        <v>15.17</v>
       </c>
       <c r="J6">
         <v>9.0500000000000007</v>
@@ -4469,7 +4537,7 @@
         <v>1.1399999999999999</v>
       </c>
       <c r="V6">
-        <v>1.44</v>
+        <v>1.47</v>
       </c>
       <c r="W6">
         <v>1.83</v>
@@ -4478,7 +4546,7 @@
         <v>1.44</v>
       </c>
       <c r="Y6">
-        <v>1.86</v>
+        <v>1.83</v>
       </c>
       <c r="Z6">
         <v>1.73</v>
@@ -4514,28 +4582,31 @@
         <v>68.260000000000005</v>
       </c>
       <c r="AK6">
-        <v>78.63</v>
+        <v>78.599999999999994</v>
       </c>
       <c r="AL6">
         <v>84.77</v>
       </c>
       <c r="AM6">
-        <v>87.25</v>
+        <v>87.35</v>
       </c>
       <c r="AN6">
         <v>90.08</v>
       </c>
       <c r="AO6">
-        <v>102.13</v>
+        <v>102.03</v>
       </c>
       <c r="AP6">
-        <v>128.06</v>
+        <v>128.24</v>
       </c>
       <c r="AQ6">
-        <v>150.13999999999999</v>
+        <v>152.28</v>
+      </c>
+      <c r="AR6">
+        <v>127.44</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -4630,43 +4701,46 @@
         <v>7.24</v>
       </c>
       <c r="AF7">
-        <v>9.5</v>
+        <v>9.5299999999999994</v>
       </c>
       <c r="AG7">
         <v>16.09</v>
       </c>
       <c r="AH7">
-        <v>25.34</v>
+        <v>25.37</v>
       </c>
       <c r="AI7">
         <v>48.8</v>
       </c>
       <c r="AJ7">
-        <v>78.41</v>
+        <v>78.44</v>
       </c>
       <c r="AK7">
-        <v>86.28</v>
+        <v>86.36</v>
       </c>
       <c r="AL7">
-        <v>89.52</v>
+        <v>89.49</v>
       </c>
       <c r="AM7">
-        <v>91.23</v>
+        <v>91.29</v>
       </c>
       <c r="AN7">
-        <v>87.12</v>
+        <v>86.99</v>
       </c>
       <c r="AO7">
-        <v>94.28</v>
+        <v>94.53</v>
       </c>
       <c r="AP7">
-        <v>118.72</v>
+        <v>118.83</v>
       </c>
       <c r="AQ7">
-        <v>137.31</v>
+        <v>139.93</v>
+      </c>
+      <c r="AR7">
+        <v>117.53</v>
       </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -4683,19 +4757,19 @@
         <v>33.96</v>
       </c>
       <c r="F8">
-        <v>34.840000000000003</v>
+        <v>34.82</v>
       </c>
       <c r="G8">
         <v>22.97</v>
       </c>
       <c r="H8">
-        <v>13.6</v>
+        <v>13.62</v>
       </c>
       <c r="I8">
         <v>10.41</v>
       </c>
       <c r="J8">
-        <v>5.45</v>
+        <v>5.47</v>
       </c>
       <c r="K8">
         <v>4.28</v>
@@ -4767,37 +4841,40 @@
         <v>14.12</v>
       </c>
       <c r="AH8">
-        <v>26.47</v>
+        <v>26.45</v>
       </c>
       <c r="AI8">
-        <v>46.66</v>
+        <v>46.68</v>
       </c>
       <c r="AJ8">
-        <v>73</v>
+        <v>73.040000000000006</v>
       </c>
       <c r="AK8">
-        <v>87.2</v>
+        <v>87.24</v>
       </c>
       <c r="AL8">
-        <v>82.59</v>
+        <v>82.61</v>
       </c>
       <c r="AM8">
-        <v>85.26</v>
+        <v>85.35</v>
       </c>
       <c r="AN8">
-        <v>84.96</v>
+        <v>84.87</v>
       </c>
       <c r="AO8">
-        <v>84.98</v>
+        <v>84.93</v>
       </c>
       <c r="AP8">
-        <v>105.47</v>
+        <v>105.8</v>
       </c>
       <c r="AQ8">
-        <v>127</v>
+        <v>128.77000000000001</v>
+      </c>
+      <c r="AR8">
+        <v>111.81</v>
       </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -4820,7 +4897,7 @@
         <v>31.85</v>
       </c>
       <c r="H9">
-        <v>19.21</v>
+        <v>19.23</v>
       </c>
       <c r="I9">
         <v>11.93</v>
@@ -4880,19 +4957,19 @@
         <v>4.3</v>
       </c>
       <c r="AB9">
-        <v>4.34</v>
+        <v>4.3600000000000003</v>
       </c>
       <c r="AC9">
         <v>5.98</v>
       </c>
       <c r="AD9">
-        <v>8.7100000000000009</v>
+        <v>8.73</v>
       </c>
       <c r="AE9">
         <v>9.5399999999999991</v>
       </c>
       <c r="AF9">
-        <v>12.06</v>
+        <v>12.02</v>
       </c>
       <c r="AG9">
         <v>22.49</v>
@@ -4907,28 +4984,31 @@
         <v>105.95</v>
       </c>
       <c r="AK9">
-        <v>121.07</v>
+        <v>121.2</v>
       </c>
       <c r="AL9">
-        <v>122.01</v>
+        <v>122.08</v>
       </c>
       <c r="AM9">
-        <v>129.24</v>
+        <v>129.33000000000001</v>
       </c>
       <c r="AN9">
-        <v>123.66</v>
+        <v>123.62</v>
       </c>
       <c r="AO9">
-        <v>135.35</v>
+        <v>135.36000000000001</v>
       </c>
       <c r="AP9">
-        <v>165.96</v>
+        <v>166.19</v>
       </c>
       <c r="AQ9">
-        <v>189.72</v>
+        <v>193.03</v>
+      </c>
+      <c r="AR9">
+        <v>157.35</v>
       </c>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -4993,7 +5073,7 @@
         <v>2.63</v>
       </c>
       <c r="V10">
-        <v>3.58</v>
+        <v>3.59</v>
       </c>
       <c r="W10">
         <v>4.25</v>
@@ -5026,40 +5106,43 @@
         <v>16.420000000000002</v>
       </c>
       <c r="AG10">
-        <v>27.67</v>
+        <v>27.68</v>
       </c>
       <c r="AH10">
         <v>44.5</v>
       </c>
       <c r="AI10">
-        <v>85.35</v>
+        <v>85.43</v>
       </c>
       <c r="AJ10">
-        <v>132.88999999999999</v>
+        <v>132.84</v>
       </c>
       <c r="AK10">
         <v>150.62</v>
       </c>
       <c r="AL10">
-        <v>152.78</v>
+        <v>152.82</v>
       </c>
       <c r="AM10">
-        <v>151.96</v>
+        <v>151.97</v>
       </c>
       <c r="AN10">
-        <v>146.11000000000001</v>
+        <v>146.08000000000001</v>
       </c>
       <c r="AO10">
-        <v>153.24</v>
+        <v>153.33000000000001</v>
       </c>
       <c r="AP10">
-        <v>192.29</v>
+        <v>192.61</v>
       </c>
       <c r="AQ10">
-        <v>217.7</v>
+        <v>220.27</v>
+      </c>
+      <c r="AR10">
+        <v>177.89</v>
       </c>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -5085,7 +5168,7 @@
         <v>23.2</v>
       </c>
       <c r="I11">
-        <v>14.77</v>
+        <v>14.75</v>
       </c>
       <c r="J11">
         <v>8.99</v>
@@ -5094,7 +5177,7 @@
         <v>7.75</v>
       </c>
       <c r="L11">
-        <v>5.54</v>
+        <v>5.53</v>
       </c>
       <c r="M11">
         <v>3.73</v>
@@ -5112,7 +5195,7 @@
         <v>4.68</v>
       </c>
       <c r="R11">
-        <v>3.95</v>
+        <v>3.96</v>
       </c>
       <c r="S11">
         <v>2.77</v>
@@ -5142,13 +5225,13 @@
         <v>8.0299999999999994</v>
       </c>
       <c r="AB11">
-        <v>8.26</v>
+        <v>8.27</v>
       </c>
       <c r="AC11">
         <v>9.9700000000000006</v>
       </c>
       <c r="AD11">
-        <v>13.35</v>
+        <v>13.37</v>
       </c>
       <c r="AE11">
         <v>14.83</v>
@@ -5157,13 +5240,13 @@
         <v>17.93</v>
       </c>
       <c r="AG11">
-        <v>33.74</v>
+        <v>33.75</v>
       </c>
       <c r="AH11">
-        <v>53.19</v>
+        <v>53.22</v>
       </c>
       <c r="AI11">
-        <v>95.48</v>
+        <v>95.51</v>
       </c>
       <c r="AJ11">
         <v>145.51</v>
@@ -5172,36 +5255,39 @@
         <v>163.05000000000001</v>
       </c>
       <c r="AL11">
-        <v>163.57</v>
+        <v>163.71</v>
       </c>
       <c r="AM11">
-        <v>161.28</v>
+        <v>161.29</v>
       </c>
       <c r="AN11">
-        <v>153.69</v>
+        <v>153.81</v>
       </c>
       <c r="AO11">
-        <v>156.88999999999999</v>
+        <v>156.97</v>
       </c>
       <c r="AP11">
-        <v>196.43</v>
+        <v>196.57</v>
       </c>
       <c r="AQ11">
-        <v>217.85</v>
+        <v>220.57</v>
+      </c>
+      <c r="AR11">
+        <v>173.76</v>
       </c>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>1.9</v>
+        <v>1.92</v>
       </c>
       <c r="C12">
         <v>14.13</v>
       </c>
       <c r="D12">
-        <v>39.729999999999997</v>
+        <v>39.75</v>
       </c>
       <c r="E12">
         <v>55.43</v>
@@ -5282,7 +5368,7 @@
         <v>16.59</v>
       </c>
       <c r="AE12">
-        <v>17.010000000000002</v>
+        <v>17.03</v>
       </c>
       <c r="AF12">
         <v>22.7</v>
@@ -5291,37 +5377,40 @@
         <v>38.61</v>
       </c>
       <c r="AH12">
-        <v>59.13</v>
+        <v>59.17</v>
       </c>
       <c r="AI12">
-        <v>110.06</v>
+        <v>110.08</v>
       </c>
       <c r="AJ12">
-        <v>158.88999999999999</v>
+        <v>158.87</v>
       </c>
       <c r="AK12">
-        <v>179.53</v>
+        <v>179.51</v>
       </c>
       <c r="AL12">
-        <v>175.81</v>
+        <v>175.9</v>
       </c>
       <c r="AM12">
-        <v>183.01</v>
+        <v>183.13</v>
       </c>
       <c r="AN12">
         <v>171.35</v>
       </c>
       <c r="AO12">
-        <v>174.61</v>
+        <v>174.75</v>
       </c>
       <c r="AP12">
-        <v>209.43</v>
+        <v>209.51</v>
       </c>
       <c r="AQ12">
-        <v>230.74</v>
+        <v>233.57</v>
+      </c>
+      <c r="AR12">
+        <v>179.39</v>
       </c>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -5335,13 +5424,13 @@
         <v>36.729999999999997</v>
       </c>
       <c r="E13">
-        <v>47.44</v>
+        <v>47.46</v>
       </c>
       <c r="F13">
         <v>47.04</v>
       </c>
       <c r="G13">
-        <v>34.08</v>
+        <v>34.1</v>
       </c>
       <c r="H13">
         <v>20.84</v>
@@ -5350,7 +5439,7 @@
         <v>14.24</v>
       </c>
       <c r="J13">
-        <v>9.2899999999999991</v>
+        <v>9.27</v>
       </c>
       <c r="K13">
         <v>8.25</v>
@@ -5395,7 +5484,7 @@
         <v>9.94</v>
       </c>
       <c r="Y13">
-        <v>13</v>
+        <v>13.04</v>
       </c>
       <c r="Z13">
         <v>14.59</v>
@@ -5416,43 +5505,46 @@
         <v>17.52</v>
       </c>
       <c r="AF13">
-        <v>21.23</v>
+        <v>21.25</v>
       </c>
       <c r="AG13">
-        <v>38.049999999999997</v>
+        <v>38.07</v>
       </c>
       <c r="AH13">
-        <v>59.22</v>
+        <v>59.24</v>
       </c>
       <c r="AI13">
-        <v>107.92</v>
+        <v>107.94</v>
       </c>
       <c r="AJ13">
-        <v>160.13</v>
+        <v>160.07</v>
       </c>
       <c r="AK13">
-        <v>180.28</v>
+        <v>180.34</v>
       </c>
       <c r="AL13">
-        <v>182.7</v>
+        <v>182.68</v>
       </c>
       <c r="AM13">
-        <v>187.98</v>
+        <v>188.1</v>
       </c>
       <c r="AN13">
-        <v>178.96</v>
+        <v>178.77</v>
       </c>
       <c r="AO13">
-        <v>179.34</v>
+        <v>179.49</v>
       </c>
       <c r="AP13">
-        <v>220.55</v>
+        <v>220.82</v>
       </c>
       <c r="AQ13">
-        <v>238.64</v>
+        <v>241.86</v>
+      </c>
+      <c r="AR13">
+        <v>188.94</v>
       </c>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -5463,7 +5555,7 @@
         <v>10.32</v>
       </c>
       <c r="D14">
-        <v>33.159999999999997</v>
+        <v>33.18</v>
       </c>
       <c r="E14">
         <v>45.13</v>
@@ -5490,10 +5582,10 @@
         <v>6.64</v>
       </c>
       <c r="M14">
-        <v>5.24</v>
+        <v>5.22</v>
       </c>
       <c r="N14">
-        <v>4.54</v>
+        <v>4.5599999999999996</v>
       </c>
       <c r="O14">
         <v>2.95</v>
@@ -5529,7 +5621,7 @@
         <v>12.19</v>
       </c>
       <c r="Z14">
-        <v>14.43</v>
+        <v>14.39</v>
       </c>
       <c r="AA14">
         <v>13.52</v>
@@ -5541,7 +5633,7 @@
         <v>13.16</v>
       </c>
       <c r="AD14">
-        <v>17</v>
+        <v>17.02</v>
       </c>
       <c r="AE14">
         <v>18.98</v>
@@ -5550,40 +5642,43 @@
         <v>21.7</v>
       </c>
       <c r="AG14">
-        <v>34.54</v>
+        <v>34.520000000000003</v>
       </c>
       <c r="AH14">
         <v>58.74</v>
       </c>
       <c r="AI14">
-        <v>101.81</v>
+        <v>101.85</v>
       </c>
       <c r="AJ14">
-        <v>152.76</v>
+        <v>152.74</v>
       </c>
       <c r="AK14">
         <v>169.21</v>
       </c>
       <c r="AL14">
-        <v>173.35</v>
+        <v>173.47</v>
       </c>
       <c r="AM14">
-        <v>173.71</v>
+        <v>173.73</v>
       </c>
       <c r="AN14">
-        <v>164.66</v>
+        <v>164.64</v>
       </c>
       <c r="AO14">
-        <v>172.24</v>
+        <v>172.39</v>
       </c>
       <c r="AP14">
-        <v>206.5</v>
+        <v>206.68</v>
       </c>
       <c r="AQ14">
-        <v>225.82</v>
+        <v>228.75</v>
+      </c>
+      <c r="AR14">
+        <v>175.36</v>
       </c>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -5603,7 +5698,7 @@
         <v>44.02</v>
       </c>
       <c r="G15">
-        <v>31.84</v>
+        <v>31.86</v>
       </c>
       <c r="H15">
         <v>21.87</v>
@@ -5618,7 +5713,7 @@
         <v>8.9</v>
       </c>
       <c r="L15">
-        <v>7.13</v>
+        <v>7.17</v>
       </c>
       <c r="M15">
         <v>5.88</v>
@@ -5657,13 +5752,13 @@
         <v>9.3699999999999992</v>
       </c>
       <c r="Y15">
-        <v>12.72</v>
+        <v>12.74</v>
       </c>
       <c r="Z15">
         <v>17.21</v>
       </c>
       <c r="AA15">
-        <v>15.54</v>
+        <v>15.52</v>
       </c>
       <c r="AB15">
         <v>17.07</v>
@@ -5681,40 +5776,43 @@
         <v>27.71</v>
       </c>
       <c r="AG15">
-        <v>43</v>
+        <v>43.02</v>
       </c>
       <c r="AH15">
-        <v>70.290000000000006</v>
+        <v>70.25</v>
       </c>
       <c r="AI15">
-        <v>122</v>
+        <v>122.02</v>
       </c>
       <c r="AJ15">
         <v>174.14</v>
       </c>
       <c r="AK15">
-        <v>190.37</v>
+        <v>190.48</v>
       </c>
       <c r="AL15">
-        <v>190.37</v>
+        <v>190.48</v>
       </c>
       <c r="AM15">
-        <v>183.67</v>
+        <v>183.76</v>
       </c>
       <c r="AN15">
-        <v>170.1</v>
+        <v>170.11</v>
       </c>
       <c r="AO15">
-        <v>171.72</v>
+        <v>171.77</v>
       </c>
       <c r="AP15">
-        <v>208.6</v>
+        <v>208.76</v>
       </c>
       <c r="AQ15">
-        <v>231.78</v>
+        <v>234.66</v>
+      </c>
+      <c r="AR15">
+        <v>179.18</v>
       </c>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -5725,13 +5823,13 @@
         <v>10.8</v>
       </c>
       <c r="D16">
-        <v>39.49</v>
+        <v>39.47</v>
       </c>
       <c r="E16">
         <v>53.09</v>
       </c>
       <c r="F16">
-        <v>48.95</v>
+        <v>48.97</v>
       </c>
       <c r="G16">
         <v>38.130000000000003</v>
@@ -5764,7 +5862,7 @@
         <v>4.79</v>
       </c>
       <c r="Q16">
-        <v>7.71</v>
+        <v>7.72</v>
       </c>
       <c r="R16">
         <v>6.4</v>
@@ -5794,7 +5892,7 @@
         <v>23.49</v>
       </c>
       <c r="AA16">
-        <v>24.04</v>
+        <v>24.08</v>
       </c>
       <c r="AB16">
         <v>22.8</v>
@@ -5815,10 +5913,10 @@
         <v>53.01</v>
       </c>
       <c r="AH16">
-        <v>88.23</v>
+        <v>88.21</v>
       </c>
       <c r="AI16">
-        <v>144.02000000000001</v>
+        <v>144.03</v>
       </c>
       <c r="AJ16">
         <v>203.47</v>
@@ -5827,25 +5925,28 @@
         <v>219.57</v>
       </c>
       <c r="AL16">
-        <v>210.43</v>
+        <v>210.56</v>
       </c>
       <c r="AM16">
-        <v>195.72</v>
+        <v>195.71</v>
       </c>
       <c r="AN16">
         <v>176.85</v>
       </c>
       <c r="AO16">
-        <v>179.53</v>
+        <v>179.57</v>
       </c>
       <c r="AP16">
-        <v>211.71</v>
+        <v>211.92</v>
       </c>
       <c r="AQ16">
-        <v>234.45</v>
+        <v>237.19</v>
+      </c>
+      <c r="AR16">
+        <v>182.5</v>
       </c>
     </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -5856,13 +5957,13 @@
         <v>7.01</v>
       </c>
       <c r="D17">
-        <v>31.38</v>
+        <v>31.4</v>
       </c>
       <c r="E17">
         <v>49.34</v>
       </c>
       <c r="F17">
-        <v>48.69</v>
+        <v>48.72</v>
       </c>
       <c r="G17">
         <v>37.58</v>
@@ -5913,28 +6014,28 @@
         <v>8.18</v>
       </c>
       <c r="W17">
-        <v>11.28</v>
+        <v>11.31</v>
       </c>
       <c r="X17">
-        <v>16.170000000000002</v>
+        <v>16.190000000000001</v>
       </c>
       <c r="Y17">
         <v>25.34</v>
       </c>
       <c r="Z17">
-        <v>33.549999999999997</v>
+        <v>33.57</v>
       </c>
       <c r="AA17">
         <v>28.8</v>
       </c>
       <c r="AB17">
-        <v>27.06</v>
+        <v>27.08</v>
       </c>
       <c r="AC17">
         <v>27.97</v>
       </c>
       <c r="AD17">
-        <v>32.869999999999997</v>
+        <v>32.9</v>
       </c>
       <c r="AE17">
         <v>34.35</v>
@@ -5949,34 +6050,37 @@
         <v>94.91</v>
       </c>
       <c r="AI17">
-        <v>163.77000000000001</v>
+        <v>163.74</v>
       </c>
       <c r="AJ17">
-        <v>226.41</v>
+        <v>226.3</v>
       </c>
       <c r="AK17">
-        <v>254.75</v>
+        <v>254.84</v>
       </c>
       <c r="AL17">
-        <v>239.34</v>
+        <v>239.41</v>
       </c>
       <c r="AM17">
         <v>221.81</v>
       </c>
       <c r="AN17">
-        <v>194.08</v>
+        <v>193.99</v>
       </c>
       <c r="AO17">
-        <v>199.07</v>
+        <v>199.2</v>
       </c>
       <c r="AP17">
-        <v>233.09</v>
+        <v>233.38</v>
       </c>
       <c r="AQ17">
-        <v>257.94</v>
+        <v>261.08999999999997</v>
+      </c>
+      <c r="AR17">
+        <v>193.17</v>
       </c>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -5984,7 +6088,7 @@
         <v>1.07</v>
       </c>
       <c r="C18">
-        <v>4.62</v>
+        <v>4.59</v>
       </c>
       <c r="D18">
         <v>13.73</v>
@@ -5996,7 +6100,7 @@
         <v>27.42</v>
       </c>
       <c r="G18">
-        <v>21.76</v>
+        <v>21.78</v>
       </c>
       <c r="H18">
         <v>14.5</v>
@@ -6017,7 +6121,7 @@
         <v>3.91</v>
       </c>
       <c r="N18">
-        <v>4.09</v>
+        <v>4.1100000000000003</v>
       </c>
       <c r="O18">
         <v>4.1100000000000003</v>
@@ -6065,51 +6169,54 @@
         <v>21.1</v>
       </c>
       <c r="AD18">
-        <v>26.2</v>
+        <v>26.25</v>
       </c>
       <c r="AE18">
-        <v>26.5</v>
+        <v>26.53</v>
       </c>
       <c r="AF18">
-        <v>33.64</v>
+        <v>33.659999999999997</v>
       </c>
       <c r="AG18">
-        <v>52.6</v>
+        <v>52.62</v>
       </c>
       <c r="AH18">
-        <v>75.19</v>
+        <v>75.239999999999995</v>
       </c>
       <c r="AI18">
-        <v>123.15</v>
+        <v>123.12</v>
       </c>
       <c r="AJ18">
-        <v>182.5</v>
+        <v>182.42</v>
       </c>
       <c r="AK18">
         <v>213.21</v>
       </c>
       <c r="AL18">
-        <v>220.37</v>
+        <v>220.52</v>
       </c>
       <c r="AM18">
-        <v>207.86</v>
+        <v>207.96</v>
       </c>
       <c r="AN18">
-        <v>189.05</v>
+        <v>189.15</v>
       </c>
       <c r="AO18">
-        <v>195.55</v>
+        <v>195.72</v>
       </c>
       <c r="AP18">
-        <v>223.32</v>
+        <v>223.55</v>
       </c>
       <c r="AQ18">
-        <v>211.31</v>
+        <v>213.65</v>
+      </c>
+      <c r="AR18">
+        <v>144.85</v>
       </c>
     </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>20</v>
+    <row r="19" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>41913</v>
       </c>
       <c r="B19">
         <v>0.56999999999999995</v>
@@ -6166,7 +6273,7 @@
         <v>2.81</v>
       </c>
       <c r="T19">
-        <v>2.81</v>
+        <v>2.78</v>
       </c>
       <c r="U19">
         <v>4.05</v>
@@ -6184,13 +6291,13 @@
         <v>14.72</v>
       </c>
       <c r="Z19">
-        <v>15.58</v>
+        <v>15.53</v>
       </c>
       <c r="AA19">
-        <v>13.02</v>
+        <v>13.04</v>
       </c>
       <c r="AB19">
-        <v>11.64</v>
+        <v>11.61</v>
       </c>
       <c r="AC19">
         <v>13.45</v>
@@ -6211,36 +6318,39 @@
         <v>44.61</v>
       </c>
       <c r="AI19">
-        <v>74</v>
+        <v>74.02</v>
       </c>
       <c r="AJ19">
-        <v>110.24</v>
+        <v>110.32</v>
       </c>
       <c r="AK19">
         <v>128.76</v>
       </c>
       <c r="AL19">
-        <v>144.24</v>
+        <v>144.26</v>
       </c>
       <c r="AM19">
-        <v>142.97</v>
+        <v>142.94</v>
       </c>
       <c r="AN19">
-        <v>139.57</v>
+        <v>139.54</v>
       </c>
       <c r="AO19">
-        <v>138.81</v>
+        <v>138.84</v>
       </c>
       <c r="AP19">
-        <v>152.07</v>
+        <v>152.41999999999999</v>
       </c>
       <c r="AQ19">
-        <v>138.62</v>
+        <v>140.88999999999999</v>
+      </c>
+      <c r="AR19">
+        <v>89.12</v>
       </c>
     </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>19</v>
+    <row r="20" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>44079</v>
       </c>
       <c r="B20">
         <v>0.27</v>
@@ -6297,7 +6407,7 @@
         <v>3.33</v>
       </c>
       <c r="T20">
-        <v>3.06</v>
+        <v>3.09</v>
       </c>
       <c r="U20">
         <v>3.7</v>
@@ -6315,7 +6425,7 @@
         <v>10.92</v>
       </c>
       <c r="Z20">
-        <v>10.220000000000001</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="AA20">
         <v>9.44</v>
@@ -6330,7 +6440,7 @@
         <v>9.5</v>
       </c>
       <c r="AE20">
-        <v>10.38</v>
+        <v>10.36</v>
       </c>
       <c r="AF20">
         <v>11.51</v>
@@ -6339,37 +6449,40 @@
         <v>16.77</v>
       </c>
       <c r="AH20">
-        <v>26.03</v>
+        <v>26.05</v>
       </c>
       <c r="AI20">
-        <v>49.1</v>
+        <v>49.21</v>
       </c>
       <c r="AJ20">
-        <v>74.86</v>
+        <v>74.91</v>
       </c>
       <c r="AK20">
-        <v>90.02</v>
+        <v>90.1</v>
       </c>
       <c r="AL20">
-        <v>97.1</v>
+        <v>97.13</v>
       </c>
       <c r="AM20">
-        <v>104.78</v>
+        <v>104.8</v>
       </c>
       <c r="AN20">
-        <v>101.96</v>
+        <v>102.09</v>
       </c>
       <c r="AO20">
-        <v>98.26</v>
+        <v>98.36</v>
       </c>
       <c r="AP20">
-        <v>113.52</v>
+        <v>113.6</v>
       </c>
       <c r="AQ20">
-        <v>112.88</v>
+        <v>114.46</v>
+      </c>
+      <c r="AR20">
+        <v>79.45</v>
       </c>
     </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -6389,7 +6502,7 @@
         <v>6.92</v>
       </c>
       <c r="G21">
-        <v>5.91</v>
+        <v>5.93</v>
       </c>
       <c r="H21">
         <v>4.0599999999999996</v>
@@ -6446,7 +6559,7 @@
         <v>6.97</v>
       </c>
       <c r="Z21">
-        <v>7.19</v>
+        <v>7.17</v>
       </c>
       <c r="AA21">
         <v>5.63</v>
@@ -6470,37 +6583,41 @@
         <v>13.23</v>
       </c>
       <c r="AH21">
-        <v>22.39</v>
+        <v>22.37</v>
       </c>
       <c r="AI21">
-        <v>36.909999999999997</v>
+        <v>36.96</v>
       </c>
       <c r="AJ21">
-        <v>56.7</v>
+        <v>56.72</v>
       </c>
       <c r="AK21">
-        <v>61.37</v>
+        <v>61.27</v>
       </c>
       <c r="AL21">
         <v>61.29</v>
       </c>
       <c r="AM21">
-        <v>60.28</v>
+        <v>60.23</v>
       </c>
       <c r="AN21">
-        <v>59.15</v>
+        <v>59.07</v>
       </c>
       <c r="AO21">
-        <v>58.67</v>
+        <v>58.59</v>
       </c>
       <c r="AP21">
-        <v>68.03</v>
+        <v>68.010000000000005</v>
       </c>
       <c r="AQ21">
-        <v>78.53</v>
+        <v>78.91</v>
+      </c>
+      <c r="AR21">
+        <v>53.97</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add RKI data downloaded 2021-01-11--13-35-01
</commit_message>
<xml_diff>
--- a/rki-data/RKI-Altersverteilung.xlsx
+++ b/rki-data/RKI-Altersverteilung.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20367"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE7BB3E-9FFE-47CF-AB11-0420EEE0E5B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20368"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Wissdaten\RKI_nCoV-Lage\3.Kommunikation\3.7.Lageberichte\2021-01-05\Dienstagstabellen für Webmaster\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1EB18B60-5CBF-44F6-BAA1-0D44F128DCEC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Erläuterungen" sheetId="3" r:id="rId1"/>
-    <sheet name="Fallzahlen" sheetId="2" r:id="rId2"/>
+    <sheet name="Fallzahlen" sheetId="4" r:id="rId2"/>
     <sheet name="Inzidenzen" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -17,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
   <si>
     <t>Altersgruppe</t>
   </si>
@@ -84,6 +89,12 @@
   <si>
     <t>Für die Berechnung von Inzidenzen wurde die Bevölkerungsstatistik
 mit Stand 31.12.2019 herangezogen.</t>
+  </si>
+  <si>
+    <t>10 - 14</t>
+  </si>
+  <si>
+    <t>5 - 9</t>
   </si>
 </sst>
 </file>
@@ -567,13 +578,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -958,21 +970,20 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AR21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B293DFE1-BAFB-40E8-B6D1-BB4B9F25B3FF}">
+  <dimension ref="A1:AS21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1105,46 +1116,49 @@
       <c r="AR1">
         <v>52</v>
       </c>
+      <c r="AS1">
+        <v>53</v>
+      </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="C2">
-        <v>6433</v>
+        <v>6434</v>
       </c>
       <c r="D2">
         <v>22431</v>
       </c>
       <c r="E2">
-        <v>34028</v>
+        <v>34029</v>
       </c>
       <c r="F2">
         <v>36094</v>
       </c>
       <c r="G2">
-        <v>27188</v>
+        <v>27185</v>
       </c>
       <c r="H2">
-        <v>17363</v>
+        <v>17362</v>
       </c>
       <c r="I2">
-        <v>12381</v>
+        <v>12382</v>
       </c>
       <c r="J2">
-        <v>7442</v>
+        <v>7443</v>
       </c>
       <c r="K2">
         <v>6229</v>
       </c>
       <c r="L2">
-        <v>4735</v>
+        <v>4734</v>
       </c>
       <c r="M2">
-        <v>3617</v>
+        <v>3618</v>
       </c>
       <c r="N2">
         <v>3211</v>
@@ -1156,22 +1170,22 @@
         <v>2345</v>
       </c>
       <c r="Q2">
-        <v>4095</v>
+        <v>4096</v>
       </c>
       <c r="R2">
         <v>3207</v>
       </c>
       <c r="S2">
-        <v>2694</v>
+        <v>2695</v>
       </c>
       <c r="T2">
-        <v>2425</v>
+        <v>2426</v>
       </c>
       <c r="U2">
         <v>3024</v>
       </c>
       <c r="V2">
-        <v>3938</v>
+        <v>3942</v>
       </c>
       <c r="W2">
         <v>4824</v>
@@ -1180,67 +1194,70 @@
         <v>6063</v>
       </c>
       <c r="Y2">
-        <v>7956</v>
+        <v>7955</v>
       </c>
       <c r="Z2">
-        <v>9587</v>
+        <v>9603</v>
       </c>
       <c r="AA2">
-        <v>8819</v>
+        <v>8821</v>
       </c>
       <c r="AB2">
-        <v>8616</v>
+        <v>8619</v>
       </c>
       <c r="AC2">
-        <v>9766</v>
+        <v>9767</v>
       </c>
       <c r="AD2">
-        <v>12278</v>
+        <v>12279</v>
       </c>
       <c r="AE2">
-        <v>13058</v>
+        <v>13070</v>
       </c>
       <c r="AF2">
-        <v>15914</v>
+        <v>15920</v>
       </c>
       <c r="AG2">
-        <v>26158</v>
+        <v>26164</v>
       </c>
       <c r="AH2">
-        <v>42068</v>
+        <v>42069</v>
       </c>
       <c r="AI2">
-        <v>74826</v>
+        <v>74835</v>
       </c>
       <c r="AJ2">
-        <v>111161</v>
+        <v>111149</v>
       </c>
       <c r="AK2">
-        <v>125775</v>
+        <v>125794</v>
       </c>
       <c r="AL2">
-        <v>127842</v>
+        <v>127875</v>
       </c>
       <c r="AM2">
-        <v>128532</v>
+        <v>128528</v>
       </c>
       <c r="AN2">
-        <v>123357</v>
+        <v>123370</v>
       </c>
       <c r="AO2">
-        <v>128304</v>
+        <v>128337</v>
       </c>
       <c r="AP2">
-        <v>155956</v>
+        <v>156115</v>
       </c>
       <c r="AQ2">
-        <v>173481</v>
+        <v>174066</v>
       </c>
       <c r="AR2">
-        <v>135974</v>
+        <v>138246</v>
+      </c>
+      <c r="AS2">
+        <v>120472</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1260,7 +1277,7 @@
         <v>1172</v>
       </c>
       <c r="G3">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="H3">
         <v>847</v>
@@ -1305,7 +1322,7 @@
         <v>27</v>
       </c>
       <c r="V3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="W3">
         <v>39</v>
@@ -1344,37 +1361,40 @@
         <v>431</v>
       </c>
       <c r="AI3">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="AJ3">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="AK3">
-        <v>1716</v>
+        <v>1717</v>
       </c>
       <c r="AL3">
-        <v>2311</v>
+        <v>2316</v>
       </c>
       <c r="AM3">
         <v>3064</v>
       </c>
       <c r="AN3">
-        <v>3504</v>
+        <v>3513</v>
       </c>
       <c r="AO3">
-        <v>4141</v>
+        <v>4140</v>
       </c>
       <c r="AP3">
-        <v>5393</v>
+        <v>5407</v>
       </c>
       <c r="AQ3">
-        <v>5842</v>
+        <v>5916</v>
       </c>
       <c r="AR3">
-        <v>5100</v>
+        <v>5213</v>
+      </c>
+      <c r="AS3">
+        <v>4832</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1394,7 +1414,7 @@
         <v>1445</v>
       </c>
       <c r="G4">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="H4">
         <v>926</v>
@@ -1403,7 +1423,7 @@
         <v>684</v>
       </c>
       <c r="J4">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="K4">
         <v>263</v>
@@ -1478,37 +1498,40 @@
         <v>568</v>
       </c>
       <c r="AI4">
-        <v>1136</v>
+        <v>1138</v>
       </c>
       <c r="AJ4">
-        <v>1780</v>
+        <v>1779</v>
       </c>
       <c r="AK4">
-        <v>2282</v>
+        <v>2287</v>
       </c>
       <c r="AL4">
-        <v>2827</v>
+        <v>2829</v>
       </c>
       <c r="AM4">
-        <v>3366</v>
+        <v>3368</v>
       </c>
       <c r="AN4">
-        <v>4090</v>
+        <v>4092</v>
       </c>
       <c r="AO4">
-        <v>4581</v>
+        <v>4579</v>
       </c>
       <c r="AP4">
-        <v>5900</v>
+        <v>5910</v>
       </c>
       <c r="AQ4">
-        <v>6831</v>
+        <v>6887</v>
       </c>
       <c r="AR4">
-        <v>5674</v>
+        <v>5820</v>
+      </c>
+      <c r="AS4">
+        <v>5430</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1516,7 +1539,7 @@
         <v>11</v>
       </c>
       <c r="C5">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D5">
         <v>468</v>
@@ -1531,7 +1554,7 @@
         <v>1720</v>
       </c>
       <c r="H5">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="I5">
         <v>823</v>
@@ -1546,7 +1569,7 @@
         <v>246</v>
       </c>
       <c r="M5">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="N5">
         <v>113</v>
@@ -1573,7 +1596,7 @@
         <v>39</v>
       </c>
       <c r="V5">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="W5">
         <v>89</v>
@@ -1600,7 +1623,7 @@
         <v>195</v>
       </c>
       <c r="AE5">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AF5">
         <v>316</v>
@@ -1612,37 +1635,40 @@
         <v>855</v>
       </c>
       <c r="AI5">
-        <v>1834</v>
+        <v>1836</v>
       </c>
       <c r="AJ5">
-        <v>2843</v>
+        <v>2842</v>
       </c>
       <c r="AK5">
-        <v>3432</v>
+        <v>3431</v>
       </c>
       <c r="AL5">
-        <v>3796</v>
+        <v>3797</v>
       </c>
       <c r="AM5">
-        <v>4357</v>
+        <v>4356</v>
       </c>
       <c r="AN5">
-        <v>4787</v>
+        <v>4786</v>
       </c>
       <c r="AO5">
-        <v>5425</v>
+        <v>5424</v>
       </c>
       <c r="AP5">
-        <v>7029</v>
+        <v>7044</v>
       </c>
       <c r="AQ5">
-        <v>8164</v>
+        <v>8223</v>
       </c>
       <c r="AR5">
-        <v>7221</v>
+        <v>7391</v>
+      </c>
+      <c r="AS5">
+        <v>6678</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1662,7 +1688,7 @@
         <v>1786</v>
       </c>
       <c r="G6">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="H6">
         <v>853</v>
@@ -1740,43 +1766,46 @@
         <v>306</v>
       </c>
       <c r="AG6">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="AH6">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="AI6">
-        <v>1624</v>
+        <v>1625</v>
       </c>
       <c r="AJ6">
-        <v>2646</v>
+        <v>2645</v>
       </c>
       <c r="AK6">
         <v>3047</v>
       </c>
       <c r="AL6">
-        <v>3286</v>
+        <v>3288</v>
       </c>
       <c r="AM6">
-        <v>3386</v>
+        <v>3388</v>
       </c>
       <c r="AN6">
-        <v>3492</v>
+        <v>3490</v>
       </c>
       <c r="AO6">
-        <v>3955</v>
+        <v>3956</v>
       </c>
       <c r="AP6">
-        <v>4971</v>
+        <v>4974</v>
       </c>
       <c r="AQ6">
-        <v>5903</v>
+        <v>5935</v>
       </c>
       <c r="AR6">
-        <v>4940</v>
+        <v>5050</v>
+      </c>
+      <c r="AS6">
+        <v>4522</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1784,7 +1813,7 @@
         <v>11</v>
       </c>
       <c r="C7">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D7">
         <v>622</v>
@@ -1799,13 +1828,13 @@
         <v>1051</v>
       </c>
       <c r="H7">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="I7">
         <v>424</v>
       </c>
       <c r="J7">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K7">
         <v>207</v>
@@ -1859,7 +1888,7 @@
         <v>93</v>
       </c>
       <c r="AB7">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AC7">
         <v>152</v>
@@ -1868,7 +1897,7 @@
         <v>259</v>
       </c>
       <c r="AE7">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AF7">
         <v>350</v>
@@ -1877,40 +1906,43 @@
         <v>591</v>
       </c>
       <c r="AH7">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="AI7">
-        <v>1793</v>
+        <v>1792</v>
       </c>
       <c r="AJ7">
-        <v>2882</v>
+        <v>2880</v>
       </c>
       <c r="AK7">
         <v>3173</v>
       </c>
       <c r="AL7">
-        <v>3288</v>
+        <v>3292</v>
       </c>
       <c r="AM7">
-        <v>3354</v>
+        <v>3355</v>
       </c>
       <c r="AN7">
-        <v>3196</v>
+        <v>3192</v>
       </c>
       <c r="AO7">
         <v>3473</v>
       </c>
       <c r="AP7">
-        <v>4366</v>
+        <v>4374</v>
       </c>
       <c r="AQ7">
-        <v>5141</v>
+        <v>5154</v>
       </c>
       <c r="AR7">
-        <v>4318</v>
+        <v>4408</v>
+      </c>
+      <c r="AS7">
+        <v>4043</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1921,7 +1953,7 @@
         <v>237</v>
       </c>
       <c r="D8">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="E8">
         <v>1650</v>
@@ -1930,7 +1962,7 @@
         <v>1692</v>
       </c>
       <c r="G8">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="H8">
         <v>662</v>
@@ -2002,13 +2034,13 @@
         <v>289</v>
       </c>
       <c r="AE8">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="AF8">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="AG8">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="AH8">
         <v>1285</v>
@@ -2017,34 +2049,37 @@
         <v>2268</v>
       </c>
       <c r="AJ8">
-        <v>3549</v>
+        <v>3550</v>
       </c>
       <c r="AK8">
-        <v>4239</v>
+        <v>4238</v>
       </c>
       <c r="AL8">
-        <v>4014</v>
+        <v>4015</v>
       </c>
       <c r="AM8">
-        <v>4147</v>
+        <v>4148</v>
       </c>
       <c r="AN8">
-        <v>4124</v>
+        <v>4128</v>
       </c>
       <c r="AO8">
-        <v>4127</v>
+        <v>4126</v>
       </c>
       <c r="AP8">
-        <v>5141</v>
+        <v>5144</v>
       </c>
       <c r="AQ8">
-        <v>6257</v>
+        <v>6283</v>
       </c>
       <c r="AR8">
-        <v>5433</v>
+        <v>5542</v>
+      </c>
+      <c r="AS8">
+        <v>4863</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2127,7 +2162,7 @@
         <v>243</v>
       </c>
       <c r="AB9">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AC9">
         <v>338</v>
@@ -2136,7 +2171,7 @@
         <v>493</v>
       </c>
       <c r="AE9">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="AF9">
         <v>679</v>
@@ -2145,40 +2180,43 @@
         <v>1270</v>
       </c>
       <c r="AH9">
-        <v>2119</v>
+        <v>2120</v>
       </c>
       <c r="AI9">
-        <v>3956</v>
+        <v>3955</v>
       </c>
       <c r="AJ9">
-        <v>5984</v>
+        <v>5985</v>
       </c>
       <c r="AK9">
-        <v>6845</v>
+        <v>6846</v>
       </c>
       <c r="AL9">
-        <v>6895</v>
+        <v>6899</v>
       </c>
       <c r="AM9">
-        <v>7304</v>
+        <v>7303</v>
       </c>
       <c r="AN9">
-        <v>6982</v>
+        <v>6984</v>
       </c>
       <c r="AO9">
-        <v>7645</v>
+        <v>7647</v>
       </c>
       <c r="AP9">
-        <v>9386</v>
+        <v>9395</v>
       </c>
       <c r="AQ9">
-        <v>10902</v>
+        <v>10933</v>
       </c>
       <c r="AR9">
-        <v>8887</v>
+        <v>9076</v>
+      </c>
+      <c r="AS9">
+        <v>8063</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2198,16 +2236,16 @@
         <v>3668</v>
       </c>
       <c r="G10">
-        <v>2610</v>
+        <v>2609</v>
       </c>
       <c r="H10">
-        <v>1568</v>
+        <v>1566</v>
       </c>
       <c r="I10">
         <v>1060</v>
       </c>
       <c r="J10">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="K10">
         <v>509</v>
@@ -2228,7 +2266,7 @@
         <v>135</v>
       </c>
       <c r="Q10">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="R10">
         <v>203</v>
@@ -2255,7 +2293,7 @@
         <v>326</v>
       </c>
       <c r="Z10">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="AA10">
         <v>353</v>
@@ -2264,55 +2302,58 @@
         <v>390</v>
       </c>
       <c r="AC10">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="AD10">
         <v>761</v>
       </c>
       <c r="AE10">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="AF10">
         <v>1106</v>
       </c>
       <c r="AG10">
-        <v>1865</v>
+        <v>1866</v>
       </c>
       <c r="AH10">
         <v>2998</v>
       </c>
       <c r="AI10">
-        <v>5756</v>
+        <v>5757</v>
       </c>
       <c r="AJ10">
-        <v>8950</v>
+        <v>8952</v>
       </c>
       <c r="AK10">
         <v>10148</v>
       </c>
       <c r="AL10">
-        <v>10296</v>
+        <v>10297</v>
       </c>
       <c r="AM10">
-        <v>10239</v>
+        <v>10236</v>
       </c>
       <c r="AN10">
-        <v>9842</v>
+        <v>9844</v>
       </c>
       <c r="AO10">
-        <v>10330</v>
+        <v>10333</v>
       </c>
       <c r="AP10">
-        <v>12977</v>
+        <v>12999</v>
       </c>
       <c r="AQ10">
-        <v>14840</v>
+        <v>14896</v>
       </c>
       <c r="AR10">
-        <v>11985</v>
+        <v>12232</v>
+      </c>
+      <c r="AS10">
+        <v>10769</v>
       </c>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2320,7 +2361,7 @@
         <v>133</v>
       </c>
       <c r="C11">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="D11">
         <v>3094</v>
@@ -2335,7 +2376,7 @@
         <v>2615</v>
       </c>
       <c r="H11">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="I11">
         <v>990</v>
@@ -2389,10 +2430,10 @@
         <v>474</v>
       </c>
       <c r="Z11">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="AA11">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="AB11">
         <v>555</v>
@@ -2404,54 +2445,57 @@
         <v>897</v>
       </c>
       <c r="AE11">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="AF11">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="AG11">
-        <v>2265</v>
+        <v>2267</v>
       </c>
       <c r="AH11">
         <v>3571</v>
       </c>
       <c r="AI11">
-        <v>6409</v>
+        <v>6408</v>
       </c>
       <c r="AJ11">
-        <v>9764</v>
+        <v>9765</v>
       </c>
       <c r="AK11">
         <v>10941</v>
       </c>
       <c r="AL11">
-        <v>10985</v>
+        <v>10986</v>
       </c>
       <c r="AM11">
-        <v>10823</v>
+        <v>10820</v>
       </c>
       <c r="AN11">
-        <v>10321</v>
+        <v>10319</v>
       </c>
       <c r="AO11">
-        <v>10533</v>
+        <v>10537</v>
       </c>
       <c r="AP11">
-        <v>13190</v>
+        <v>13201</v>
       </c>
       <c r="AQ11">
-        <v>14801</v>
+        <v>14836</v>
       </c>
       <c r="AR11">
-        <v>11660</v>
+        <v>11879</v>
+      </c>
+      <c r="AS11">
+        <v>10250</v>
       </c>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C12">
         <v>745</v>
@@ -2523,13 +2567,13 @@
         <v>574</v>
       </c>
       <c r="Z12">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="AA12">
         <v>606</v>
       </c>
       <c r="AB12">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="AC12">
         <v>696</v>
@@ -2541,46 +2585,49 @@
         <v>898</v>
       </c>
       <c r="AF12">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="AG12">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="AH12">
-        <v>3120</v>
+        <v>3121</v>
       </c>
       <c r="AI12">
-        <v>5805</v>
+        <v>5804</v>
       </c>
       <c r="AJ12">
         <v>8378</v>
       </c>
       <c r="AK12">
-        <v>9466</v>
+        <v>9468</v>
       </c>
       <c r="AL12">
-        <v>9276</v>
+        <v>9279</v>
       </c>
       <c r="AM12">
-        <v>9657</v>
+        <v>9661</v>
       </c>
       <c r="AN12">
-        <v>9036</v>
+        <v>9033</v>
       </c>
       <c r="AO12">
-        <v>9215</v>
+        <v>9221</v>
       </c>
       <c r="AP12">
-        <v>11048</v>
+        <v>11054</v>
       </c>
       <c r="AQ12">
-        <v>12317</v>
+        <v>12348</v>
       </c>
       <c r="AR12">
-        <v>9460</v>
+        <v>9630</v>
+      </c>
+      <c r="AS12">
+        <v>8395</v>
       </c>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2615,7 +2662,7 @@
         <v>405</v>
       </c>
       <c r="L13">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="M13">
         <v>241</v>
@@ -2660,7 +2707,7 @@
         <v>716</v>
       </c>
       <c r="AA13">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="AB13">
         <v>648</v>
@@ -2675,7 +2722,7 @@
         <v>860</v>
       </c>
       <c r="AF13">
-        <v>1043</v>
+        <v>1045</v>
       </c>
       <c r="AG13">
         <v>1869</v>
@@ -2684,37 +2731,40 @@
         <v>2908</v>
       </c>
       <c r="AI13">
-        <v>5299</v>
+        <v>5301</v>
       </c>
       <c r="AJ13">
-        <v>7858</v>
+        <v>7859</v>
       </c>
       <c r="AK13">
-        <v>8853</v>
+        <v>8857</v>
       </c>
       <c r="AL13">
-        <v>8968</v>
+        <v>8971</v>
       </c>
       <c r="AM13">
-        <v>9234</v>
+        <v>9230</v>
       </c>
       <c r="AN13">
-        <v>8776</v>
+        <v>8778</v>
       </c>
       <c r="AO13">
-        <v>8811</v>
+        <v>8810</v>
       </c>
       <c r="AP13">
-        <v>10840</v>
+        <v>10856</v>
       </c>
       <c r="AQ13">
-        <v>11873</v>
+        <v>11907</v>
       </c>
       <c r="AR13">
-        <v>9275</v>
+        <v>9425</v>
+      </c>
+      <c r="AS13">
+        <v>7817</v>
       </c>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -2728,7 +2778,7 @@
         <v>1755</v>
       </c>
       <c r="E14">
-        <v>2387</v>
+        <v>2388</v>
       </c>
       <c r="F14">
         <v>2206</v>
@@ -2773,7 +2823,7 @@
         <v>226</v>
       </c>
       <c r="T14">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="U14">
         <v>251</v>
@@ -2800,55 +2850,58 @@
         <v>647</v>
       </c>
       <c r="AC14">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="AD14">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="AE14">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="AF14">
-        <v>1148</v>
+        <v>1151</v>
       </c>
       <c r="AG14">
         <v>1826</v>
       </c>
       <c r="AH14">
-        <v>3107</v>
+        <v>3105</v>
       </c>
       <c r="AI14">
-        <v>5387</v>
+        <v>5389</v>
       </c>
       <c r="AJ14">
-        <v>8079</v>
+        <v>8078</v>
       </c>
       <c r="AK14">
         <v>8950</v>
       </c>
       <c r="AL14">
-        <v>9175</v>
+        <v>9176</v>
       </c>
       <c r="AM14">
-        <v>9189</v>
+        <v>9188</v>
       </c>
       <c r="AN14">
         <v>8708</v>
       </c>
       <c r="AO14">
-        <v>9118</v>
+        <v>9121</v>
       </c>
       <c r="AP14">
-        <v>10932</v>
+        <v>10948</v>
       </c>
       <c r="AQ14">
-        <v>12099</v>
+        <v>12140</v>
       </c>
       <c r="AR14">
-        <v>9275</v>
+        <v>9442</v>
+      </c>
+      <c r="AS14">
+        <v>7881</v>
       </c>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -2865,13 +2918,13 @@
         <v>2639</v>
       </c>
       <c r="F15">
-        <v>2419</v>
+        <v>2420</v>
       </c>
       <c r="G15">
         <v>1751</v>
       </c>
       <c r="H15">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="I15">
         <v>909</v>
@@ -2913,7 +2966,7 @@
         <v>297</v>
       </c>
       <c r="V15">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="W15">
         <v>424</v>
@@ -2928,16 +2981,16 @@
         <v>946</v>
       </c>
       <c r="AA15">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="AB15">
         <v>938</v>
       </c>
       <c r="AC15">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="AD15">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="AE15">
         <v>1303</v>
@@ -2946,43 +2999,46 @@
         <v>1523</v>
       </c>
       <c r="AG15">
-        <v>2364</v>
+        <v>2365</v>
       </c>
       <c r="AH15">
         <v>3861</v>
       </c>
       <c r="AI15">
-        <v>6706</v>
+        <v>6712</v>
       </c>
       <c r="AJ15">
-        <v>9570</v>
+        <v>9566</v>
       </c>
       <c r="AK15">
-        <v>10468</v>
+        <v>10471</v>
       </c>
       <c r="AL15">
-        <v>10468</v>
+        <v>10472</v>
       </c>
       <c r="AM15">
-        <v>10099</v>
+        <v>10096</v>
       </c>
       <c r="AN15">
-        <v>9349</v>
+        <v>9352</v>
       </c>
       <c r="AO15">
-        <v>9440</v>
+        <v>9448</v>
       </c>
       <c r="AP15">
-        <v>11473</v>
+        <v>11484</v>
       </c>
       <c r="AQ15">
-        <v>12896</v>
+        <v>12943</v>
       </c>
       <c r="AR15">
-        <v>9847</v>
+        <v>9991</v>
+      </c>
+      <c r="AS15">
+        <v>8982</v>
       </c>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -2990,10 +3046,10 @@
         <v>75</v>
       </c>
       <c r="C16">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D16">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="E16">
         <v>2694</v>
@@ -3047,76 +3103,79 @@
         <v>309</v>
       </c>
       <c r="V16">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="W16">
         <v>509</v>
       </c>
       <c r="X16">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="Y16">
         <v>838</v>
       </c>
       <c r="Z16">
-        <v>1192</v>
+        <v>1196</v>
       </c>
       <c r="AA16">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="AB16">
-        <v>1157</v>
+        <v>1159</v>
       </c>
       <c r="AC16">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="AD16">
         <v>1481</v>
       </c>
       <c r="AE16">
-        <v>1435</v>
+        <v>1437</v>
       </c>
       <c r="AF16">
-        <v>1744</v>
+        <v>1745</v>
       </c>
       <c r="AG16">
         <v>2690</v>
       </c>
       <c r="AH16">
-        <v>4476</v>
+        <v>4477</v>
       </c>
       <c r="AI16">
-        <v>7309</v>
+        <v>7307</v>
       </c>
       <c r="AJ16">
         <v>10325</v>
       </c>
       <c r="AK16">
-        <v>11142</v>
+        <v>11145</v>
       </c>
       <c r="AL16">
-        <v>10685</v>
+        <v>10686</v>
       </c>
       <c r="AM16">
-        <v>9931</v>
+        <v>9936</v>
       </c>
       <c r="AN16">
-        <v>8974</v>
+        <v>8976</v>
       </c>
       <c r="AO16">
-        <v>9112</v>
+        <v>9113</v>
       </c>
       <c r="AP16">
-        <v>10754</v>
+        <v>10761</v>
       </c>
       <c r="AQ16">
-        <v>12036</v>
+        <v>12060</v>
       </c>
       <c r="AR16">
-        <v>9261</v>
+        <v>9372</v>
+      </c>
+      <c r="AS16">
+        <v>8302</v>
       </c>
     </row>
-    <row r="17" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -3133,7 +3192,7 @@
         <v>2274</v>
       </c>
       <c r="F17">
-        <v>2245</v>
+        <v>2244</v>
       </c>
       <c r="G17">
         <v>1732</v>
@@ -3190,19 +3249,19 @@
         <v>746</v>
       </c>
       <c r="Y17">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="Z17">
-        <v>1547</v>
+        <v>1549</v>
       </c>
       <c r="AA17">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="AB17">
         <v>1248</v>
       </c>
       <c r="AC17">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="AD17">
         <v>1516</v>
@@ -3211,13 +3270,13 @@
         <v>1583</v>
       </c>
       <c r="AF17">
-        <v>1733</v>
+        <v>1735</v>
       </c>
       <c r="AG17">
-        <v>2790</v>
+        <v>2791</v>
       </c>
       <c r="AH17">
-        <v>4374</v>
+        <v>4375</v>
       </c>
       <c r="AI17">
         <v>7546</v>
@@ -3226,31 +3285,34 @@
         <v>10429</v>
       </c>
       <c r="AK17">
-        <v>11744</v>
+        <v>11745</v>
       </c>
       <c r="AL17">
-        <v>11033</v>
+        <v>11034</v>
       </c>
       <c r="AM17">
         <v>10222</v>
       </c>
       <c r="AN17">
-        <v>8940</v>
+        <v>8937</v>
       </c>
       <c r="AO17">
-        <v>9180</v>
+        <v>9184</v>
       </c>
       <c r="AP17">
-        <v>10755</v>
+        <v>10760</v>
       </c>
       <c r="AQ17">
-        <v>12032</v>
+        <v>12063</v>
       </c>
       <c r="AR17">
-        <v>8902</v>
+        <v>9015</v>
+      </c>
+      <c r="AS17">
+        <v>8458</v>
       </c>
     </row>
-    <row r="18" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -3258,7 +3320,7 @@
         <v>42</v>
       </c>
       <c r="C18">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D18">
         <v>541</v>
@@ -3276,7 +3338,7 @@
         <v>571</v>
       </c>
       <c r="I18">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="J18">
         <v>263</v>
@@ -3321,16 +3383,16 @@
         <v>364</v>
       </c>
       <c r="X18">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="Y18">
         <v>742</v>
       </c>
       <c r="Z18">
-        <v>876</v>
+        <v>881</v>
       </c>
       <c r="AA18">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="AB18">
         <v>768</v>
@@ -3345,48 +3407,51 @@
         <v>1045</v>
       </c>
       <c r="AF18">
-        <v>1326</v>
+        <v>1329</v>
       </c>
       <c r="AG18">
-        <v>2073</v>
+        <v>2074</v>
       </c>
       <c r="AH18">
         <v>2964</v>
       </c>
       <c r="AI18">
-        <v>4850</v>
+        <v>4849</v>
       </c>
       <c r="AJ18">
         <v>7186</v>
       </c>
       <c r="AK18">
-        <v>8399</v>
+        <v>8400</v>
       </c>
       <c r="AL18">
-        <v>8687</v>
+        <v>8689</v>
       </c>
       <c r="AM18">
-        <v>8192</v>
+        <v>8194</v>
       </c>
       <c r="AN18">
-        <v>7451</v>
+        <v>7456</v>
       </c>
       <c r="AO18">
-        <v>7710</v>
+        <v>7717</v>
       </c>
       <c r="AP18">
-        <v>8806</v>
+        <v>8810</v>
       </c>
       <c r="AQ18">
-        <v>8416</v>
+        <v>8427</v>
       </c>
       <c r="AR18">
-        <v>5706</v>
+        <v>5810</v>
+      </c>
+      <c r="AS18">
+        <v>4843</v>
       </c>
     </row>
-    <row r="19" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>41913</v>
+    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="B19">
         <v>21</v>
@@ -3440,7 +3505,7 @@
         <v>146</v>
       </c>
       <c r="S19">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="T19">
         <v>103</v>
@@ -3464,7 +3529,7 @@
         <v>575</v>
       </c>
       <c r="AA19">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="AB19">
         <v>430</v>
@@ -3473,13 +3538,13 @@
         <v>498</v>
       </c>
       <c r="AD19">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="AE19">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="AF19">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="AG19">
         <v>1139</v>
@@ -3488,39 +3553,42 @@
         <v>1652</v>
       </c>
       <c r="AI19">
-        <v>2741</v>
+        <v>2742</v>
       </c>
       <c r="AJ19">
-        <v>4085</v>
+        <v>4083</v>
       </c>
       <c r="AK19">
-        <v>4768</v>
+        <v>4767</v>
       </c>
       <c r="AL19">
         <v>5342</v>
       </c>
       <c r="AM19">
-        <v>5293</v>
+        <v>5294</v>
       </c>
       <c r="AN19">
-        <v>5167</v>
+        <v>5170</v>
       </c>
       <c r="AO19">
-        <v>5141</v>
+        <v>5145</v>
       </c>
       <c r="AP19">
-        <v>5644</v>
+        <v>5658</v>
       </c>
       <c r="AQ19">
-        <v>5217</v>
+        <v>5230</v>
       </c>
       <c r="AR19">
-        <v>3300</v>
+        <v>3346</v>
+      </c>
+      <c r="AS19">
+        <v>2579</v>
       </c>
     </row>
-    <row r="20" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>44079</v>
+    <row r="20" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="B20">
         <v>10</v>
@@ -3598,7 +3666,7 @@
         <v>380</v>
       </c>
       <c r="AA20">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="AB20">
         <v>318</v>
@@ -3610,49 +3678,52 @@
         <v>354</v>
       </c>
       <c r="AE20">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="AF20">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="AG20">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="AH20">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="AI20">
         <v>1834</v>
       </c>
       <c r="AJ20">
-        <v>2792</v>
+        <v>2791</v>
       </c>
       <c r="AK20">
-        <v>3358</v>
+        <v>3360</v>
       </c>
       <c r="AL20">
-        <v>3620</v>
+        <v>3621</v>
       </c>
       <c r="AM20">
-        <v>3906</v>
+        <v>3908</v>
       </c>
       <c r="AN20">
-        <v>3805</v>
+        <v>3806</v>
       </c>
       <c r="AO20">
-        <v>3666</v>
+        <v>3668</v>
       </c>
       <c r="AP20">
-        <v>4234</v>
+        <v>4242</v>
       </c>
       <c r="AQ20">
-        <v>4266</v>
+        <v>4278</v>
       </c>
       <c r="AR20">
-        <v>2961</v>
+        <v>2991</v>
+      </c>
+      <c r="AS20">
+        <v>1895</v>
       </c>
     </row>
-    <row r="21" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -3729,7 +3800,7 @@
         <v>276</v>
       </c>
       <c r="Z21">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="AA21">
         <v>223</v>
@@ -3756,7 +3827,7 @@
         <v>886</v>
       </c>
       <c r="AI21">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="AJ21">
         <v>2247</v>
@@ -3765,44 +3836,46 @@
         <v>2427</v>
       </c>
       <c r="AL21">
-        <v>2428</v>
+        <v>2425</v>
       </c>
       <c r="AM21">
-        <v>2386</v>
+        <v>2383</v>
       </c>
       <c r="AN21">
-        <v>2340</v>
+        <v>2337</v>
       </c>
       <c r="AO21">
-        <v>2321</v>
+        <v>2320</v>
       </c>
       <c r="AP21">
-        <v>2694</v>
+        <v>2696</v>
       </c>
       <c r="AQ21">
         <v>3126</v>
       </c>
       <c r="AR21">
-        <v>2138</v>
+        <v>2127</v>
+      </c>
+      <c r="AS21">
+        <v>1518</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AR21"/>
+  <dimension ref="A1:AS21"/>
   <sheetViews>
-    <sheetView topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:AS1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3935,8 +4008,11 @@
       <c r="AR1">
         <v>52</v>
       </c>
+      <c r="AS1">
+        <v>53</v>
+      </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -3986,7 +4062,7 @@
         <v>2.82</v>
       </c>
       <c r="Q2">
-        <v>4.92</v>
+        <v>4.93</v>
       </c>
       <c r="R2">
         <v>3.86</v>
@@ -4013,10 +4089,10 @@
         <v>9.57</v>
       </c>
       <c r="Z2">
-        <v>11.53</v>
+        <v>11.55</v>
       </c>
       <c r="AA2">
-        <v>10.6</v>
+        <v>10.61</v>
       </c>
       <c r="AB2">
         <v>10.36</v>
@@ -4028,49 +4104,52 @@
         <v>14.76</v>
       </c>
       <c r="AE2">
-        <v>15.7</v>
+        <v>15.72</v>
       </c>
       <c r="AF2">
         <v>19.14</v>
       </c>
       <c r="AG2">
-        <v>31.45</v>
+        <v>31.46</v>
       </c>
       <c r="AH2">
         <v>50.58</v>
       </c>
       <c r="AI2">
-        <v>89.97</v>
+        <v>89.98</v>
       </c>
       <c r="AJ2">
-        <v>133.66</v>
+        <v>133.65</v>
       </c>
       <c r="AK2">
-        <v>151.22999999999999</v>
+        <v>151.26</v>
       </c>
       <c r="AL2">
-        <v>153.72</v>
+        <v>153.76</v>
       </c>
       <c r="AM2">
-        <v>154.55000000000001</v>
+        <v>154.54</v>
       </c>
       <c r="AN2">
-        <v>148.32</v>
+        <v>148.34</v>
       </c>
       <c r="AO2">
-        <v>154.27000000000001</v>
+        <v>154.31</v>
       </c>
       <c r="AP2">
-        <v>187.52</v>
+        <v>187.71</v>
       </c>
       <c r="AQ2">
-        <v>208.59</v>
+        <v>209.3</v>
       </c>
       <c r="AR2">
-        <v>163.5</v>
+        <v>166.23</v>
+      </c>
+      <c r="AS2">
+        <v>144.86000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -4090,7 +4169,7 @@
         <v>142.4</v>
       </c>
       <c r="G3">
-        <v>151.38999999999999</v>
+        <v>151.27000000000001</v>
       </c>
       <c r="H3">
         <v>102.91</v>
@@ -4135,7 +4214,7 @@
         <v>3.28</v>
       </c>
       <c r="V3">
-        <v>2.19</v>
+        <v>2.31</v>
       </c>
       <c r="W3">
         <v>4.74</v>
@@ -4174,37 +4253,40 @@
         <v>52.37</v>
       </c>
       <c r="AI3">
-        <v>107.53</v>
+        <v>107.65</v>
       </c>
       <c r="AJ3">
-        <v>177.88</v>
+        <v>178</v>
       </c>
       <c r="AK3">
-        <v>208.49</v>
+        <v>208.62</v>
       </c>
       <c r="AL3">
-        <v>280.79000000000002</v>
+        <v>281.39</v>
       </c>
       <c r="AM3">
         <v>372.28</v>
       </c>
       <c r="AN3">
-        <v>425.74</v>
+        <v>426.83</v>
       </c>
       <c r="AO3">
-        <v>503.13</v>
+        <v>503.01</v>
       </c>
       <c r="AP3">
-        <v>655.25</v>
+        <v>656.95</v>
       </c>
       <c r="AQ3">
-        <v>709.8</v>
+        <v>718.79</v>
       </c>
       <c r="AR3">
-        <v>619.65</v>
+        <v>633.38</v>
+      </c>
+      <c r="AS3">
+        <v>587.09</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -4224,7 +4306,7 @@
         <v>92.4</v>
       </c>
       <c r="G4">
-        <v>90.74</v>
+        <v>90.8</v>
       </c>
       <c r="H4">
         <v>59.21</v>
@@ -4233,7 +4315,7 @@
         <v>43.74</v>
       </c>
       <c r="J4">
-        <v>20.97</v>
+        <v>21.04</v>
       </c>
       <c r="K4">
         <v>16.82</v>
@@ -4308,37 +4390,40 @@
         <v>36.32</v>
       </c>
       <c r="AI4">
-        <v>72.64</v>
+        <v>72.77</v>
       </c>
       <c r="AJ4">
-        <v>113.82</v>
+        <v>113.76</v>
       </c>
       <c r="AK4">
-        <v>145.93</v>
+        <v>146.25</v>
       </c>
       <c r="AL4">
-        <v>180.78</v>
+        <v>180.9</v>
       </c>
       <c r="AM4">
-        <v>215.24</v>
+        <v>215.37</v>
       </c>
       <c r="AN4">
-        <v>261.54000000000002</v>
+        <v>261.67</v>
       </c>
       <c r="AO4">
-        <v>292.94</v>
+        <v>292.81</v>
       </c>
       <c r="AP4">
-        <v>377.28</v>
+        <v>377.92</v>
       </c>
       <c r="AQ4">
-        <v>436.82</v>
+        <v>440.4</v>
       </c>
       <c r="AR4">
-        <v>362.83</v>
+        <v>372.17</v>
+      </c>
+      <c r="AS4">
+        <v>347.23</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -4346,7 +4431,7 @@
         <v>0.33</v>
       </c>
       <c r="C5">
-        <v>2.4900000000000002</v>
+        <v>2.52</v>
       </c>
       <c r="D5">
         <v>14.21</v>
@@ -4361,7 +4446,7 @@
         <v>52.21</v>
       </c>
       <c r="H5">
-        <v>35.909999999999997</v>
+        <v>35.880000000000003</v>
       </c>
       <c r="I5">
         <v>24.98</v>
@@ -4376,7 +4461,7 @@
         <v>7.47</v>
       </c>
       <c r="M5">
-        <v>4.6100000000000003</v>
+        <v>4.6399999999999997</v>
       </c>
       <c r="N5">
         <v>3.43</v>
@@ -4403,7 +4488,7 @@
         <v>1.18</v>
       </c>
       <c r="V5">
-        <v>1.52</v>
+        <v>1.55</v>
       </c>
       <c r="W5">
         <v>2.7</v>
@@ -4430,7 +4515,7 @@
         <v>5.92</v>
       </c>
       <c r="AE5">
-        <v>6.41</v>
+        <v>6.44</v>
       </c>
       <c r="AF5">
         <v>9.59</v>
@@ -4442,37 +4527,40 @@
         <v>25.95</v>
       </c>
       <c r="AI5">
-        <v>55.67</v>
+        <v>55.73</v>
       </c>
       <c r="AJ5">
-        <v>86.3</v>
+        <v>86.27</v>
       </c>
       <c r="AK5">
-        <v>104.18</v>
+        <v>104.15</v>
       </c>
       <c r="AL5">
-        <v>115.23</v>
+        <v>115.26</v>
       </c>
       <c r="AM5">
-        <v>132.26</v>
+        <v>132.22999999999999</v>
       </c>
       <c r="AN5">
-        <v>145.31</v>
+        <v>145.28</v>
       </c>
       <c r="AO5">
-        <v>164.68</v>
+        <v>164.65</v>
       </c>
       <c r="AP5">
-        <v>213.37</v>
+        <v>213.83</v>
       </c>
       <c r="AQ5">
-        <v>247.82</v>
+        <v>249.61</v>
       </c>
       <c r="AR5">
-        <v>219.2</v>
+        <v>224.36</v>
+      </c>
+      <c r="AS5">
+        <v>202.71</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -4492,7 +4580,7 @@
         <v>46.07</v>
       </c>
       <c r="G6">
-        <v>33.869999999999997</v>
+        <v>33.85</v>
       </c>
       <c r="H6">
         <v>22</v>
@@ -4570,43 +4658,46 @@
         <v>7.89</v>
       </c>
       <c r="AG6">
-        <v>13.03</v>
+        <v>13.05</v>
       </c>
       <c r="AH6">
-        <v>23.37</v>
+        <v>23.35</v>
       </c>
       <c r="AI6">
-        <v>41.89</v>
+        <v>41.92</v>
       </c>
       <c r="AJ6">
-        <v>68.260000000000005</v>
+        <v>68.23</v>
       </c>
       <c r="AK6">
         <v>78.599999999999994</v>
       </c>
       <c r="AL6">
-        <v>84.77</v>
+        <v>84.82</v>
       </c>
       <c r="AM6">
-        <v>87.35</v>
+        <v>87.4</v>
       </c>
       <c r="AN6">
-        <v>90.08</v>
+        <v>90.03</v>
       </c>
       <c r="AO6">
-        <v>102.03</v>
+        <v>102.05</v>
       </c>
       <c r="AP6">
-        <v>128.24</v>
+        <v>128.31</v>
       </c>
       <c r="AQ6">
-        <v>152.28</v>
+        <v>153.11000000000001</v>
       </c>
       <c r="AR6">
-        <v>127.44</v>
+        <v>130.27000000000001</v>
+      </c>
+      <c r="AS6">
+        <v>116.65</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -4614,7 +4705,7 @@
         <v>0.3</v>
       </c>
       <c r="C7">
-        <v>3.95</v>
+        <v>3.92</v>
       </c>
       <c r="D7">
         <v>16.93</v>
@@ -4629,13 +4720,13 @@
         <v>28.61</v>
       </c>
       <c r="H7">
-        <v>17.2</v>
+        <v>17.23</v>
       </c>
       <c r="I7">
         <v>11.54</v>
       </c>
       <c r="J7">
-        <v>7.54</v>
+        <v>7.51</v>
       </c>
       <c r="K7">
         <v>5.63</v>
@@ -4689,7 +4780,7 @@
         <v>2.5299999999999998</v>
       </c>
       <c r="AB7">
-        <v>2.94</v>
+        <v>2.91</v>
       </c>
       <c r="AC7">
         <v>4.1399999999999997</v>
@@ -4698,7 +4789,7 @@
         <v>7.05</v>
       </c>
       <c r="AE7">
-        <v>7.24</v>
+        <v>7.21</v>
       </c>
       <c r="AF7">
         <v>9.5299999999999994</v>
@@ -4707,40 +4798,43 @@
         <v>16.09</v>
       </c>
       <c r="AH7">
-        <v>25.37</v>
+        <v>25.39</v>
       </c>
       <c r="AI7">
-        <v>48.8</v>
+        <v>48.77</v>
       </c>
       <c r="AJ7">
-        <v>78.44</v>
+        <v>78.39</v>
       </c>
       <c r="AK7">
         <v>86.36</v>
       </c>
       <c r="AL7">
-        <v>89.49</v>
+        <v>89.6</v>
       </c>
       <c r="AM7">
-        <v>91.29</v>
+        <v>91.32</v>
       </c>
       <c r="AN7">
-        <v>86.99</v>
+        <v>86.88</v>
       </c>
       <c r="AO7">
         <v>94.53</v>
       </c>
       <c r="AP7">
-        <v>118.83</v>
+        <v>119.05</v>
       </c>
       <c r="AQ7">
-        <v>139.93</v>
+        <v>140.28</v>
       </c>
       <c r="AR7">
-        <v>117.53</v>
+        <v>119.98</v>
+      </c>
+      <c r="AS7">
+        <v>110.04</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -4751,7 +4845,7 @@
         <v>4.88</v>
       </c>
       <c r="D8">
-        <v>18.32</v>
+        <v>18.3</v>
       </c>
       <c r="E8">
         <v>33.96</v>
@@ -4760,7 +4854,7 @@
         <v>34.82</v>
       </c>
       <c r="G8">
-        <v>22.97</v>
+        <v>22.95</v>
       </c>
       <c r="H8">
         <v>13.62</v>
@@ -4832,13 +4926,13 @@
         <v>5.95</v>
       </c>
       <c r="AE8">
-        <v>6.26</v>
+        <v>6.28</v>
       </c>
       <c r="AF8">
-        <v>9.3000000000000007</v>
+        <v>9.32</v>
       </c>
       <c r="AG8">
-        <v>14.12</v>
+        <v>14.1</v>
       </c>
       <c r="AH8">
         <v>26.45</v>
@@ -4847,34 +4941,37 @@
         <v>46.68</v>
       </c>
       <c r="AJ8">
-        <v>73.040000000000006</v>
+        <v>73.06</v>
       </c>
       <c r="AK8">
-        <v>87.24</v>
+        <v>87.22</v>
       </c>
       <c r="AL8">
-        <v>82.61</v>
+        <v>82.63</v>
       </c>
       <c r="AM8">
-        <v>85.35</v>
+        <v>85.37</v>
       </c>
       <c r="AN8">
-        <v>84.87</v>
+        <v>84.96</v>
       </c>
       <c r="AO8">
-        <v>84.93</v>
+        <v>84.91</v>
       </c>
       <c r="AP8">
-        <v>105.8</v>
+        <v>105.86</v>
       </c>
       <c r="AQ8">
-        <v>128.77000000000001</v>
+        <v>129.31</v>
       </c>
       <c r="AR8">
-        <v>111.81</v>
+        <v>114.06</v>
+      </c>
+      <c r="AS8">
+        <v>100.08</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -4957,7 +5054,7 @@
         <v>4.3</v>
       </c>
       <c r="AB9">
-        <v>4.3600000000000003</v>
+        <v>4.37</v>
       </c>
       <c r="AC9">
         <v>5.98</v>
@@ -4966,7 +5063,7 @@
         <v>8.73</v>
       </c>
       <c r="AE9">
-        <v>9.5399999999999991</v>
+        <v>9.58</v>
       </c>
       <c r="AF9">
         <v>12.02</v>
@@ -4975,40 +5072,43 @@
         <v>22.49</v>
       </c>
       <c r="AH9">
-        <v>37.520000000000003</v>
+        <v>37.54</v>
       </c>
       <c r="AI9">
-        <v>70.05</v>
+        <v>70.03</v>
       </c>
       <c r="AJ9">
-        <v>105.95</v>
+        <v>105.97</v>
       </c>
       <c r="AK9">
-        <v>121.2</v>
+        <v>121.22</v>
       </c>
       <c r="AL9">
-        <v>122.08</v>
+        <v>122.15</v>
       </c>
       <c r="AM9">
-        <v>129.33000000000001</v>
+        <v>129.31</v>
       </c>
       <c r="AN9">
-        <v>123.62</v>
+        <v>123.66</v>
       </c>
       <c r="AO9">
-        <v>135.36000000000001</v>
+        <v>135.4</v>
       </c>
       <c r="AP9">
-        <v>166.19</v>
+        <v>166.35</v>
       </c>
       <c r="AQ9">
-        <v>193.03</v>
+        <v>193.58</v>
       </c>
       <c r="AR9">
-        <v>157.35</v>
+        <v>160.69999999999999</v>
+      </c>
+      <c r="AS9">
+        <v>142.76</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -5028,16 +5128,16 @@
         <v>54.44</v>
       </c>
       <c r="G10">
-        <v>38.74</v>
+        <v>38.72</v>
       </c>
       <c r="H10">
-        <v>23.27</v>
+        <v>23.24</v>
       </c>
       <c r="I10">
         <v>15.73</v>
       </c>
       <c r="J10">
-        <v>8.91</v>
+        <v>8.92</v>
       </c>
       <c r="K10">
         <v>7.55</v>
@@ -5058,7 +5158,7 @@
         <v>2</v>
       </c>
       <c r="Q10">
-        <v>2.73</v>
+        <v>2.75</v>
       </c>
       <c r="R10">
         <v>3.01</v>
@@ -5085,7 +5185,7 @@
         <v>4.84</v>
       </c>
       <c r="Z10">
-        <v>6.38</v>
+        <v>6.4</v>
       </c>
       <c r="AA10">
         <v>5.24</v>
@@ -5094,55 +5194,58 @@
         <v>5.79</v>
       </c>
       <c r="AC10">
-        <v>8.2100000000000009</v>
+        <v>8.2200000000000006</v>
       </c>
       <c r="AD10">
         <v>11.3</v>
       </c>
       <c r="AE10">
-        <v>12.82</v>
+        <v>12.84</v>
       </c>
       <c r="AF10">
         <v>16.420000000000002</v>
       </c>
       <c r="AG10">
-        <v>27.68</v>
+        <v>27.7</v>
       </c>
       <c r="AH10">
         <v>44.5</v>
       </c>
       <c r="AI10">
-        <v>85.43</v>
+        <v>85.45</v>
       </c>
       <c r="AJ10">
-        <v>132.84</v>
+        <v>132.87</v>
       </c>
       <c r="AK10">
         <v>150.62</v>
       </c>
       <c r="AL10">
-        <v>152.82</v>
+        <v>152.84</v>
       </c>
       <c r="AM10">
-        <v>151.97</v>
+        <v>151.93</v>
       </c>
       <c r="AN10">
-        <v>146.08000000000001</v>
+        <v>146.11000000000001</v>
       </c>
       <c r="AO10">
-        <v>153.33000000000001</v>
+        <v>153.37</v>
       </c>
       <c r="AP10">
-        <v>192.61</v>
+        <v>192.94</v>
       </c>
       <c r="AQ10">
-        <v>220.27</v>
+        <v>221.1</v>
       </c>
       <c r="AR10">
-        <v>177.89</v>
+        <v>181.56</v>
+      </c>
+      <c r="AS10">
+        <v>159.84</v>
       </c>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -5150,7 +5253,7 @@
         <v>1.98</v>
       </c>
       <c r="C11">
-        <v>14.6</v>
+        <v>14.62</v>
       </c>
       <c r="D11">
         <v>46.11</v>
@@ -5165,7 +5268,7 @@
         <v>38.97</v>
       </c>
       <c r="H11">
-        <v>23.2</v>
+        <v>23.22</v>
       </c>
       <c r="I11">
         <v>14.75</v>
@@ -5219,10 +5322,10 @@
         <v>7.06</v>
       </c>
       <c r="Z11">
-        <v>8.32</v>
+        <v>8.35</v>
       </c>
       <c r="AA11">
-        <v>8.0299999999999994</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="AB11">
         <v>8.27</v>
@@ -5234,54 +5337,57 @@
         <v>13.37</v>
       </c>
       <c r="AE11">
-        <v>14.83</v>
+        <v>14.84</v>
       </c>
       <c r="AF11">
-        <v>17.93</v>
+        <v>17.940000000000001</v>
       </c>
       <c r="AG11">
-        <v>33.75</v>
+        <v>33.78</v>
       </c>
       <c r="AH11">
         <v>53.22</v>
       </c>
       <c r="AI11">
-        <v>95.51</v>
+        <v>95.5</v>
       </c>
       <c r="AJ11">
-        <v>145.51</v>
+        <v>145.52000000000001</v>
       </c>
       <c r="AK11">
         <v>163.05000000000001</v>
       </c>
       <c r="AL11">
-        <v>163.71</v>
+        <v>163.72</v>
       </c>
       <c r="AM11">
-        <v>161.29</v>
+        <v>161.25</v>
       </c>
       <c r="AN11">
-        <v>153.81</v>
+        <v>153.78</v>
       </c>
       <c r="AO11">
-        <v>156.97</v>
+        <v>157.03</v>
       </c>
       <c r="AP11">
-        <v>196.57</v>
+        <v>196.73</v>
       </c>
       <c r="AQ11">
-        <v>220.57</v>
+        <v>221.1</v>
       </c>
       <c r="AR11">
-        <v>173.76</v>
+        <v>177.03</v>
+      </c>
+      <c r="AS11">
+        <v>152.75</v>
       </c>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>1.92</v>
+        <v>1.9</v>
       </c>
       <c r="C12">
         <v>14.13</v>
@@ -5353,13 +5459,13 @@
         <v>10.88</v>
       </c>
       <c r="Z12">
-        <v>13.1</v>
+        <v>13.12</v>
       </c>
       <c r="AA12">
         <v>11.49</v>
       </c>
       <c r="AB12">
-        <v>11.61</v>
+        <v>11.62</v>
       </c>
       <c r="AC12">
         <v>13.2</v>
@@ -5371,46 +5477,49 @@
         <v>17.03</v>
       </c>
       <c r="AF12">
-        <v>22.7</v>
+        <v>22.72</v>
       </c>
       <c r="AG12">
-        <v>38.61</v>
+        <v>38.590000000000003</v>
       </c>
       <c r="AH12">
-        <v>59.17</v>
+        <v>59.18</v>
       </c>
       <c r="AI12">
-        <v>110.08</v>
+        <v>110.06</v>
       </c>
       <c r="AJ12">
         <v>158.87</v>
       </c>
       <c r="AK12">
-        <v>179.51</v>
+        <v>179.54</v>
       </c>
       <c r="AL12">
-        <v>175.9</v>
+        <v>175.96</v>
       </c>
       <c r="AM12">
-        <v>183.13</v>
+        <v>183.2</v>
       </c>
       <c r="AN12">
-        <v>171.35</v>
+        <v>171.3</v>
       </c>
       <c r="AO12">
-        <v>174.75</v>
+        <v>174.86</v>
       </c>
       <c r="AP12">
-        <v>209.51</v>
+        <v>209.62</v>
       </c>
       <c r="AQ12">
-        <v>233.57</v>
+        <v>234.16</v>
       </c>
       <c r="AR12">
-        <v>179.39</v>
+        <v>182.62</v>
+      </c>
+      <c r="AS12">
+        <v>159.19999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -5445,7 +5554,7 @@
         <v>8.25</v>
       </c>
       <c r="L13">
-        <v>7.21</v>
+        <v>7.19</v>
       </c>
       <c r="M13">
         <v>4.91</v>
@@ -5490,7 +5599,7 @@
         <v>14.59</v>
       </c>
       <c r="AA13">
-        <v>13.42</v>
+        <v>13.44</v>
       </c>
       <c r="AB13">
         <v>13.2</v>
@@ -5505,7 +5614,7 @@
         <v>17.52</v>
       </c>
       <c r="AF13">
-        <v>21.25</v>
+        <v>21.29</v>
       </c>
       <c r="AG13">
         <v>38.07</v>
@@ -5514,37 +5623,40 @@
         <v>59.24</v>
       </c>
       <c r="AI13">
-        <v>107.94</v>
+        <v>107.98</v>
       </c>
       <c r="AJ13">
-        <v>160.07</v>
+        <v>160.09</v>
       </c>
       <c r="AK13">
-        <v>180.34</v>
+        <v>180.42</v>
       </c>
       <c r="AL13">
-        <v>182.68</v>
+        <v>182.75</v>
       </c>
       <c r="AM13">
-        <v>188.1</v>
+        <v>188.02</v>
       </c>
       <c r="AN13">
-        <v>178.77</v>
+        <v>178.81</v>
       </c>
       <c r="AO13">
-        <v>179.49</v>
+        <v>179.47</v>
       </c>
       <c r="AP13">
-        <v>220.82</v>
+        <v>221.14</v>
       </c>
       <c r="AQ13">
-        <v>241.86</v>
+        <v>242.55</v>
       </c>
       <c r="AR13">
-        <v>188.94</v>
+        <v>191.99</v>
+      </c>
+      <c r="AS13">
+        <v>159.24</v>
       </c>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -5558,7 +5670,7 @@
         <v>33.18</v>
       </c>
       <c r="E14">
-        <v>45.13</v>
+        <v>45.15</v>
       </c>
       <c r="F14">
         <v>41.71</v>
@@ -5603,7 +5715,7 @@
         <v>4.2699999999999996</v>
       </c>
       <c r="T14">
-        <v>3.88</v>
+        <v>3.89</v>
       </c>
       <c r="U14">
         <v>4.75</v>
@@ -5630,55 +5742,58 @@
         <v>12.23</v>
       </c>
       <c r="AC14">
-        <v>13.16</v>
+        <v>13.18</v>
       </c>
       <c r="AD14">
-        <v>17.02</v>
+        <v>17.03</v>
       </c>
       <c r="AE14">
-        <v>18.98</v>
+        <v>19.02</v>
       </c>
       <c r="AF14">
-        <v>21.7</v>
+        <v>21.76</v>
       </c>
       <c r="AG14">
         <v>34.520000000000003</v>
       </c>
       <c r="AH14">
-        <v>58.74</v>
+        <v>58.7</v>
       </c>
       <c r="AI14">
-        <v>101.85</v>
+        <v>101.89</v>
       </c>
       <c r="AJ14">
-        <v>152.74</v>
+        <v>152.72999999999999</v>
       </c>
       <c r="AK14">
         <v>169.21</v>
       </c>
       <c r="AL14">
-        <v>173.47</v>
+        <v>173.49</v>
       </c>
       <c r="AM14">
-        <v>173.73</v>
+        <v>173.71</v>
       </c>
       <c r="AN14">
         <v>164.64</v>
       </c>
       <c r="AO14">
-        <v>172.39</v>
+        <v>172.45</v>
       </c>
       <c r="AP14">
-        <v>206.68</v>
+        <v>206.99</v>
       </c>
       <c r="AQ14">
-        <v>228.75</v>
+        <v>229.52</v>
       </c>
       <c r="AR14">
-        <v>175.36</v>
+        <v>178.51</v>
+      </c>
+      <c r="AS14">
+        <v>149</v>
       </c>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -5695,13 +5810,13 @@
         <v>48.02</v>
       </c>
       <c r="F15">
-        <v>44.02</v>
+        <v>44.03</v>
       </c>
       <c r="G15">
         <v>31.86</v>
       </c>
       <c r="H15">
-        <v>21.87</v>
+        <v>21.89</v>
       </c>
       <c r="I15">
         <v>16.54</v>
@@ -5743,7 +5858,7 @@
         <v>5.4</v>
       </c>
       <c r="V15">
-        <v>6.97</v>
+        <v>6.99</v>
       </c>
       <c r="W15">
         <v>7.72</v>
@@ -5758,16 +5873,16 @@
         <v>17.21</v>
       </c>
       <c r="AA15">
-        <v>15.52</v>
+        <v>15.54</v>
       </c>
       <c r="AB15">
         <v>17.07</v>
       </c>
       <c r="AC15">
-        <v>17.010000000000002</v>
+        <v>17.03</v>
       </c>
       <c r="AD15">
-        <v>21.91</v>
+        <v>21.89</v>
       </c>
       <c r="AE15">
         <v>23.71</v>
@@ -5776,43 +5891,46 @@
         <v>27.71</v>
       </c>
       <c r="AG15">
-        <v>43.02</v>
+        <v>43.03</v>
       </c>
       <c r="AH15">
         <v>70.25</v>
       </c>
       <c r="AI15">
-        <v>122.02</v>
+        <v>122.13</v>
       </c>
       <c r="AJ15">
-        <v>174.14</v>
+        <v>174.06</v>
       </c>
       <c r="AK15">
-        <v>190.48</v>
+        <v>190.53</v>
       </c>
       <c r="AL15">
-        <v>190.48</v>
+        <v>190.55</v>
       </c>
       <c r="AM15">
-        <v>183.76</v>
+        <v>183.71</v>
       </c>
       <c r="AN15">
-        <v>170.11</v>
+        <v>170.17</v>
       </c>
       <c r="AO15">
-        <v>171.77</v>
+        <v>171.92</v>
       </c>
       <c r="AP15">
-        <v>208.76</v>
+        <v>208.96</v>
       </c>
       <c r="AQ15">
-        <v>234.66</v>
+        <v>235.51</v>
       </c>
       <c r="AR15">
-        <v>179.18</v>
+        <v>181.8</v>
+      </c>
+      <c r="AS15">
+        <v>163.44</v>
       </c>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -5820,10 +5938,10 @@
         <v>1.48</v>
       </c>
       <c r="C16">
-        <v>10.8</v>
+        <v>10.78</v>
       </c>
       <c r="D16">
-        <v>39.47</v>
+        <v>39.49</v>
       </c>
       <c r="E16">
         <v>53.09</v>
@@ -5877,76 +5995,79 @@
         <v>6.09</v>
       </c>
       <c r="V16">
-        <v>8.08</v>
+        <v>8.1</v>
       </c>
       <c r="W16">
         <v>10.029999999999999</v>
       </c>
       <c r="X16">
-        <v>12</v>
+        <v>11.98</v>
       </c>
       <c r="Y16">
         <v>16.510000000000002</v>
       </c>
       <c r="Z16">
-        <v>23.49</v>
+        <v>23.57</v>
       </c>
       <c r="AA16">
-        <v>24.08</v>
+        <v>24.06</v>
       </c>
       <c r="AB16">
-        <v>22.8</v>
+        <v>22.84</v>
       </c>
       <c r="AC16">
-        <v>24.3</v>
+        <v>24.28</v>
       </c>
       <c r="AD16">
         <v>29.19</v>
       </c>
       <c r="AE16">
-        <v>28.28</v>
+        <v>28.32</v>
       </c>
       <c r="AF16">
-        <v>34.369999999999997</v>
+        <v>34.39</v>
       </c>
       <c r="AG16">
         <v>53.01</v>
       </c>
       <c r="AH16">
-        <v>88.21</v>
+        <v>88.23</v>
       </c>
       <c r="AI16">
-        <v>144.03</v>
+        <v>144</v>
       </c>
       <c r="AJ16">
         <v>203.47</v>
       </c>
       <c r="AK16">
-        <v>219.57</v>
+        <v>219.63</v>
       </c>
       <c r="AL16">
-        <v>210.56</v>
+        <v>210.58</v>
       </c>
       <c r="AM16">
-        <v>195.71</v>
+        <v>195.8</v>
       </c>
       <c r="AN16">
-        <v>176.85</v>
+        <v>176.89</v>
       </c>
       <c r="AO16">
-        <v>179.57</v>
+        <v>179.59</v>
       </c>
       <c r="AP16">
-        <v>211.92</v>
+        <v>212.06</v>
       </c>
       <c r="AQ16">
-        <v>237.19</v>
+        <v>237.66</v>
       </c>
       <c r="AR16">
-        <v>182.5</v>
+        <v>184.69</v>
+      </c>
+      <c r="AS16">
+        <v>163.6</v>
       </c>
     </row>
-    <row r="17" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -5963,7 +6084,7 @@
         <v>49.34</v>
       </c>
       <c r="F17">
-        <v>48.72</v>
+        <v>48.69</v>
       </c>
       <c r="G17">
         <v>37.58</v>
@@ -6020,19 +6141,19 @@
         <v>16.190000000000001</v>
       </c>
       <c r="Y17">
-        <v>25.34</v>
+        <v>25.32</v>
       </c>
       <c r="Z17">
-        <v>33.57</v>
+        <v>33.61</v>
       </c>
       <c r="AA17">
-        <v>28.8</v>
+        <v>28.77</v>
       </c>
       <c r="AB17">
         <v>27.08</v>
       </c>
       <c r="AC17">
-        <v>27.97</v>
+        <v>27.95</v>
       </c>
       <c r="AD17">
         <v>32.9</v>
@@ -6041,13 +6162,13 @@
         <v>34.35</v>
       </c>
       <c r="AF17">
-        <v>37.6</v>
+        <v>37.65</v>
       </c>
       <c r="AG17">
-        <v>60.54</v>
+        <v>60.56</v>
       </c>
       <c r="AH17">
-        <v>94.91</v>
+        <v>94.93</v>
       </c>
       <c r="AI17">
         <v>163.74</v>
@@ -6056,31 +6177,34 @@
         <v>226.3</v>
       </c>
       <c r="AK17">
-        <v>254.84</v>
+        <v>254.86</v>
       </c>
       <c r="AL17">
-        <v>239.41</v>
+        <v>239.43</v>
       </c>
       <c r="AM17">
         <v>221.81</v>
       </c>
       <c r="AN17">
-        <v>193.99</v>
+        <v>193.93</v>
       </c>
       <c r="AO17">
-        <v>199.2</v>
+        <v>199.29</v>
       </c>
       <c r="AP17">
-        <v>233.38</v>
+        <v>233.49</v>
       </c>
       <c r="AQ17">
-        <v>261.08999999999997</v>
+        <v>261.76</v>
       </c>
       <c r="AR17">
-        <v>193.17</v>
+        <v>195.62</v>
+      </c>
+      <c r="AS17">
+        <v>183.53</v>
       </c>
     </row>
-    <row r="18" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -6088,7 +6212,7 @@
         <v>1.07</v>
       </c>
       <c r="C18">
-        <v>4.59</v>
+        <v>4.62</v>
       </c>
       <c r="D18">
         <v>13.73</v>
@@ -6106,7 +6230,7 @@
         <v>14.5</v>
       </c>
       <c r="I18">
-        <v>10.210000000000001</v>
+        <v>10.23</v>
       </c>
       <c r="J18">
         <v>6.68</v>
@@ -6151,16 +6275,16 @@
         <v>9.24</v>
       </c>
       <c r="X18">
-        <v>13.78</v>
+        <v>13.81</v>
       </c>
       <c r="Y18">
         <v>18.84</v>
       </c>
       <c r="Z18">
-        <v>22.24</v>
+        <v>22.36</v>
       </c>
       <c r="AA18">
-        <v>21.12</v>
+        <v>21.1</v>
       </c>
       <c r="AB18">
         <v>19.5</v>
@@ -6175,46 +6299,49 @@
         <v>26.53</v>
       </c>
       <c r="AF18">
-        <v>33.659999999999997</v>
+        <v>33.74</v>
       </c>
       <c r="AG18">
-        <v>52.62</v>
+        <v>52.65</v>
       </c>
       <c r="AH18">
         <v>75.239999999999995</v>
       </c>
       <c r="AI18">
-        <v>123.12</v>
+        <v>123.09</v>
       </c>
       <c r="AJ18">
         <v>182.42</v>
       </c>
       <c r="AK18">
-        <v>213.21</v>
+        <v>213.24</v>
       </c>
       <c r="AL18">
-        <v>220.52</v>
+        <v>220.58</v>
       </c>
       <c r="AM18">
-        <v>207.96</v>
+        <v>208.01</v>
       </c>
       <c r="AN18">
-        <v>189.15</v>
+        <v>189.27</v>
       </c>
       <c r="AO18">
-        <v>195.72</v>
+        <v>195.9</v>
       </c>
       <c r="AP18">
-        <v>223.55</v>
+        <v>223.65</v>
       </c>
       <c r="AQ18">
-        <v>213.65</v>
+        <v>213.92</v>
       </c>
       <c r="AR18">
-        <v>144.85</v>
+        <v>147.49</v>
+      </c>
+      <c r="AS18">
+        <v>122.94</v>
       </c>
     </row>
-    <row r="19" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>41913</v>
       </c>
@@ -6270,7 +6397,7 @@
         <v>3.94</v>
       </c>
       <c r="S19">
-        <v>2.81</v>
+        <v>2.84</v>
       </c>
       <c r="T19">
         <v>2.78</v>
@@ -6294,7 +6421,7 @@
         <v>15.53</v>
       </c>
       <c r="AA19">
-        <v>13.04</v>
+        <v>13.07</v>
       </c>
       <c r="AB19">
         <v>11.61</v>
@@ -6303,13 +6430,13 @@
         <v>13.45</v>
       </c>
       <c r="AD19">
-        <v>13.93</v>
+        <v>13.96</v>
       </c>
       <c r="AE19">
-        <v>15.83</v>
+        <v>15.85</v>
       </c>
       <c r="AF19">
-        <v>19.149999999999999</v>
+        <v>19.170000000000002</v>
       </c>
       <c r="AG19">
         <v>30.76</v>
@@ -6318,37 +6445,40 @@
         <v>44.61</v>
       </c>
       <c r="AI19">
-        <v>74.02</v>
+        <v>74.05</v>
       </c>
       <c r="AJ19">
-        <v>110.32</v>
+        <v>110.26</v>
       </c>
       <c r="AK19">
-        <v>128.76</v>
+        <v>128.74</v>
       </c>
       <c r="AL19">
         <v>144.26</v>
       </c>
       <c r="AM19">
-        <v>142.94</v>
+        <v>142.97</v>
       </c>
       <c r="AN19">
-        <v>139.54</v>
+        <v>139.62</v>
       </c>
       <c r="AO19">
-        <v>138.84</v>
+        <v>138.94</v>
       </c>
       <c r="AP19">
-        <v>152.41999999999999</v>
+        <v>152.80000000000001</v>
       </c>
       <c r="AQ19">
-        <v>140.88999999999999</v>
+        <v>141.24</v>
       </c>
       <c r="AR19">
-        <v>89.12</v>
+        <v>90.36</v>
+      </c>
+      <c r="AS19">
+        <v>69.650000000000006</v>
       </c>
     </row>
-    <row r="20" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>44079</v>
       </c>
@@ -6428,7 +6558,7 @@
         <v>10.199999999999999</v>
       </c>
       <c r="AA20">
-        <v>9.44</v>
+        <v>9.4700000000000006</v>
       </c>
       <c r="AB20">
         <v>8.5299999999999994</v>
@@ -6440,49 +6570,52 @@
         <v>9.5</v>
       </c>
       <c r="AE20">
-        <v>10.36</v>
+        <v>10.41</v>
       </c>
       <c r="AF20">
-        <v>11.51</v>
+        <v>11.54</v>
       </c>
       <c r="AG20">
-        <v>16.77</v>
+        <v>16.8</v>
       </c>
       <c r="AH20">
-        <v>26.05</v>
+        <v>26.08</v>
       </c>
       <c r="AI20">
         <v>49.21</v>
       </c>
       <c r="AJ20">
-        <v>74.91</v>
+        <v>74.89</v>
       </c>
       <c r="AK20">
-        <v>90.1</v>
+        <v>90.15</v>
       </c>
       <c r="AL20">
-        <v>97.13</v>
+        <v>97.16</v>
       </c>
       <c r="AM20">
-        <v>104.8</v>
+        <v>104.86</v>
       </c>
       <c r="AN20">
-        <v>102.09</v>
+        <v>102.12</v>
       </c>
       <c r="AO20">
-        <v>98.36</v>
+        <v>98.42</v>
       </c>
       <c r="AP20">
-        <v>113.6</v>
+        <v>113.82</v>
       </c>
       <c r="AQ20">
-        <v>114.46</v>
+        <v>114.78</v>
       </c>
       <c r="AR20">
-        <v>79.45</v>
+        <v>80.25</v>
+      </c>
+      <c r="AS20">
+        <v>50.85</v>
       </c>
     </row>
-    <row r="21" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -6559,7 +6692,7 @@
         <v>6.97</v>
       </c>
       <c r="Z21">
-        <v>7.17</v>
+        <v>7.19</v>
       </c>
       <c r="AA21">
         <v>5.63</v>
@@ -6586,7 +6719,7 @@
         <v>22.37</v>
       </c>
       <c r="AI21">
-        <v>36.96</v>
+        <v>36.979999999999997</v>
       </c>
       <c r="AJ21">
         <v>56.72</v>
@@ -6595,29 +6728,31 @@
         <v>61.27</v>
       </c>
       <c r="AL21">
-        <v>61.29</v>
+        <v>61.22</v>
       </c>
       <c r="AM21">
-        <v>60.23</v>
+        <v>60.16</v>
       </c>
       <c r="AN21">
-        <v>59.07</v>
+        <v>58.99</v>
       </c>
       <c r="AO21">
-        <v>58.59</v>
+        <v>58.57</v>
       </c>
       <c r="AP21">
-        <v>68.010000000000005</v>
+        <v>68.06</v>
       </c>
       <c r="AQ21">
         <v>78.91</v>
       </c>
       <c r="AR21">
-        <v>53.97</v>
+        <v>53.69</v>
+      </c>
+      <c r="AS21">
+        <v>38.32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add RKI data downloaded 2021-01-21--13-35-01
</commit_message>
<xml_diff>
--- a/rki-data/RKI-Altersverteilung.xlsx
+++ b/rki-data/RKI-Altersverteilung.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20368"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE5B920C-A780-4F53-900F-0E65C8FDD25C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466FD17F-3693-4F80-A8DF-2030B8362E82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Erläuterungen" sheetId="3" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="70">
   <si>
     <t>Altersgruppe</t>
   </si>
@@ -225,6 +225,9 @@
   </si>
   <si>
     <t>10-14</t>
+  </si>
+  <si>
+    <t>2021_2</t>
   </si>
 </sst>
 </file>
@@ -1071,7 +1074,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E2FB09-40BA-467A-9A47-7CEA9C443D24}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1106,15 +1109,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1BE48B6-9747-4017-83E5-E7E92A9C8328}">
-  <dimension ref="A1:AT21"/>
+  <dimension ref="A1:AU21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AU2" sqref="AU2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1253,43 +1256,46 @@
       <c r="AT1" t="s">
         <v>66</v>
       </c>
+      <c r="AU1" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="C2">
-        <v>6435</v>
+        <v>6434</v>
       </c>
       <c r="D2">
-        <v>22432</v>
+        <v>22434</v>
       </c>
       <c r="E2">
         <v>34029</v>
       </c>
       <c r="F2">
-        <v>36093</v>
+        <v>36101</v>
       </c>
       <c r="G2">
-        <v>27185</v>
+        <v>27181</v>
       </c>
       <c r="H2">
-        <v>17368</v>
+        <v>17370</v>
       </c>
       <c r="I2">
-        <v>12381</v>
+        <v>12382</v>
       </c>
       <c r="J2">
-        <v>7443</v>
+        <v>7445</v>
       </c>
       <c r="K2">
-        <v>6230</v>
+        <v>6235</v>
       </c>
       <c r="L2">
-        <v>4734</v>
+        <v>4755</v>
       </c>
       <c r="M2">
         <v>3618</v>
@@ -1298,19 +1304,19 @@
         <v>3212</v>
       </c>
       <c r="O2">
-        <v>2361</v>
+        <v>2360</v>
       </c>
       <c r="P2">
         <v>2345</v>
       </c>
       <c r="Q2">
-        <v>4140</v>
+        <v>4135</v>
       </c>
       <c r="R2">
-        <v>3218</v>
+        <v>3214</v>
       </c>
       <c r="S2">
-        <v>2696</v>
+        <v>2697</v>
       </c>
       <c r="T2">
         <v>2428</v>
@@ -1319,82 +1325,85 @@
         <v>3024</v>
       </c>
       <c r="V2">
-        <v>3942</v>
+        <v>3943</v>
       </c>
       <c r="W2">
-        <v>4824</v>
+        <v>4825</v>
       </c>
       <c r="X2">
-        <v>6062</v>
+        <v>6063</v>
       </c>
       <c r="Y2">
-        <v>7955</v>
+        <v>7960</v>
       </c>
       <c r="Z2">
-        <v>9603</v>
+        <v>9606</v>
       </c>
       <c r="AA2">
-        <v>8822</v>
+        <v>8821</v>
       </c>
       <c r="AB2">
-        <v>8621</v>
+        <v>8624</v>
       </c>
       <c r="AC2">
-        <v>9773</v>
+        <v>9775</v>
       </c>
       <c r="AD2">
-        <v>12279</v>
+        <v>12288</v>
       </c>
       <c r="AE2">
-        <v>13070</v>
+        <v>13076</v>
       </c>
       <c r="AF2">
-        <v>15921</v>
+        <v>15925</v>
       </c>
       <c r="AG2">
-        <v>26169</v>
+        <v>26167</v>
       </c>
       <c r="AH2">
-        <v>42075</v>
+        <v>42086</v>
       </c>
       <c r="AI2">
-        <v>74819</v>
+        <v>74822</v>
       </c>
       <c r="AJ2">
-        <v>111143</v>
+        <v>111156</v>
       </c>
       <c r="AK2">
-        <v>125811</v>
+        <v>125812</v>
       </c>
       <c r="AL2">
-        <v>127891</v>
+        <v>127902</v>
       </c>
       <c r="AM2">
-        <v>128528</v>
+        <v>128533</v>
       </c>
       <c r="AN2">
-        <v>123359</v>
+        <v>123379</v>
       </c>
       <c r="AO2">
-        <v>128327</v>
+        <v>128389</v>
       </c>
       <c r="AP2">
-        <v>156158</v>
+        <v>156276</v>
       </c>
       <c r="AQ2">
-        <v>174316</v>
+        <v>174652</v>
       </c>
       <c r="AR2">
-        <v>138538</v>
+        <v>138815</v>
       </c>
       <c r="AS2">
-        <v>122530</v>
+        <v>122936</v>
       </c>
       <c r="AT2">
-        <v>143198</v>
+        <v>144821</v>
+      </c>
+      <c r="AU2">
+        <v>117939</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1405,7 +1414,7 @@
         <v>12</v>
       </c>
       <c r="D3">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E3">
         <v>423</v>
@@ -1480,7 +1489,7 @@
         <v>24</v>
       </c>
       <c r="AC3">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AD3">
         <v>74</v>
@@ -1504,37 +1513,40 @@
         <v>1465</v>
       </c>
       <c r="AK3">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="AL3">
-        <v>2314</v>
+        <v>2316</v>
       </c>
       <c r="AM3">
-        <v>3065</v>
+        <v>3069</v>
       </c>
       <c r="AN3">
-        <v>3517</v>
+        <v>3530</v>
       </c>
       <c r="AO3">
-        <v>4138</v>
+        <v>4153</v>
       </c>
       <c r="AP3">
-        <v>5407</v>
+        <v>5410</v>
       </c>
       <c r="AQ3">
-        <v>5944</v>
+        <v>5983</v>
       </c>
       <c r="AR3">
-        <v>5232</v>
+        <v>5257</v>
       </c>
       <c r="AS3">
-        <v>4939</v>
+        <v>4964</v>
       </c>
       <c r="AT3">
-        <v>5278</v>
+        <v>5380</v>
+      </c>
+      <c r="AU3">
+        <v>4968</v>
       </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1551,13 +1563,13 @@
         <v>738</v>
       </c>
       <c r="F4">
-        <v>1447</v>
+        <v>1450</v>
       </c>
       <c r="G4">
         <v>1421</v>
       </c>
       <c r="H4">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="I4">
         <v>684</v>
@@ -1584,7 +1596,7 @@
         <v>51</v>
       </c>
       <c r="Q4">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="R4">
         <v>34</v>
@@ -1629,52 +1641,55 @@
         <v>121</v>
       </c>
       <c r="AF4">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AG4">
         <v>305</v>
       </c>
       <c r="AH4">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="AI4">
         <v>1137</v>
       </c>
       <c r="AJ4">
-        <v>1780</v>
+        <v>1779</v>
       </c>
       <c r="AK4">
-        <v>2291</v>
+        <v>2290</v>
       </c>
       <c r="AL4">
-        <v>2827</v>
+        <v>2830</v>
       </c>
       <c r="AM4">
-        <v>3366</v>
+        <v>3365</v>
       </c>
       <c r="AN4">
-        <v>4097</v>
+        <v>4112</v>
       </c>
       <c r="AO4">
-        <v>4577</v>
+        <v>4580</v>
       </c>
       <c r="AP4">
-        <v>5894</v>
+        <v>5905</v>
       </c>
       <c r="AQ4">
-        <v>6904</v>
+        <v>6923</v>
       </c>
       <c r="AR4">
-        <v>5826</v>
+        <v>5861</v>
       </c>
       <c r="AS4">
-        <v>5564</v>
+        <v>5591</v>
       </c>
       <c r="AT4">
-        <v>5950</v>
+        <v>6046</v>
+      </c>
+      <c r="AU4">
+        <v>5486</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1691,25 +1706,25 @@
         <v>1285</v>
       </c>
       <c r="F5">
-        <v>1963</v>
+        <v>1964</v>
       </c>
       <c r="G5">
         <v>1719</v>
       </c>
       <c r="H5">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="I5">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="J5">
         <v>451</v>
       </c>
       <c r="K5">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="L5">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="M5">
         <v>152</v>
@@ -1781,40 +1796,43 @@
         <v>1833</v>
       </c>
       <c r="AJ5">
-        <v>2842</v>
+        <v>2841</v>
       </c>
       <c r="AK5">
-        <v>3432</v>
+        <v>3433</v>
       </c>
       <c r="AL5">
-        <v>3799</v>
+        <v>3798</v>
       </c>
       <c r="AM5">
-        <v>4360</v>
+        <v>4364</v>
       </c>
       <c r="AN5">
-        <v>4781</v>
+        <v>4799</v>
       </c>
       <c r="AO5">
         <v>5425</v>
       </c>
       <c r="AP5">
-        <v>7045</v>
+        <v>7056</v>
       </c>
       <c r="AQ5">
-        <v>8228</v>
+        <v>8262</v>
       </c>
       <c r="AR5">
-        <v>7403</v>
+        <v>7432</v>
       </c>
       <c r="AS5">
-        <v>6822</v>
+        <v>6848</v>
       </c>
       <c r="AT5">
-        <v>7550</v>
+        <v>7644</v>
+      </c>
+      <c r="AU5">
+        <v>6587</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1822,22 +1840,22 @@
         <v>24</v>
       </c>
       <c r="C6">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D6">
         <v>571</v>
       </c>
       <c r="E6">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="F6">
-        <v>1786</v>
+        <v>1788</v>
       </c>
       <c r="G6">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="H6">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="I6">
         <v>587</v>
@@ -1849,7 +1867,7 @@
         <v>274</v>
       </c>
       <c r="L6">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="M6">
         <v>105</v>
@@ -1861,7 +1879,7 @@
         <v>58</v>
       </c>
       <c r="P6">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Q6">
         <v>65</v>
@@ -1903,7 +1921,7 @@
         <v>145</v>
       </c>
       <c r="AD6">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="AE6">
         <v>231</v>
@@ -1915,46 +1933,49 @@
         <v>507</v>
       </c>
       <c r="AH6">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="AI6">
-        <v>1627</v>
+        <v>1628</v>
       </c>
       <c r="AJ6">
-        <v>2645</v>
+        <v>2646</v>
       </c>
       <c r="AK6">
-        <v>3045</v>
+        <v>3049</v>
       </c>
       <c r="AL6">
         <v>3289</v>
       </c>
       <c r="AM6">
-        <v>3387</v>
+        <v>3391</v>
       </c>
       <c r="AN6">
-        <v>3492</v>
+        <v>3494</v>
       </c>
       <c r="AO6">
-        <v>3956</v>
+        <v>3962</v>
       </c>
       <c r="AP6">
-        <v>4974</v>
+        <v>4985</v>
       </c>
       <c r="AQ6">
-        <v>5940</v>
+        <v>5958</v>
       </c>
       <c r="AR6">
-        <v>5068</v>
+        <v>5081</v>
       </c>
       <c r="AS6">
-        <v>4603</v>
+        <v>4618</v>
       </c>
       <c r="AT6">
-        <v>5145</v>
+        <v>5213</v>
+      </c>
+      <c r="AU6">
+        <v>4297</v>
       </c>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1962,19 +1983,19 @@
         <v>11</v>
       </c>
       <c r="C7">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D7">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="E7">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="F7">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="G7">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="H7">
         <v>632</v>
@@ -1989,7 +2010,7 @@
         <v>207</v>
       </c>
       <c r="L7">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="M7">
         <v>92</v>
@@ -2001,7 +2022,7 @@
         <v>47</v>
       </c>
       <c r="P7">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q7">
         <v>58</v>
@@ -2034,7 +2055,7 @@
         <v>96</v>
       </c>
       <c r="AA7">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AB7">
         <v>107</v>
@@ -2052,19 +2073,19 @@
         <v>350</v>
       </c>
       <c r="AG7">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="AH7">
         <v>932</v>
       </c>
       <c r="AI7">
-        <v>1791</v>
+        <v>1793</v>
       </c>
       <c r="AJ7">
-        <v>2880</v>
+        <v>2881</v>
       </c>
       <c r="AK7">
-        <v>3172</v>
+        <v>3174</v>
       </c>
       <c r="AL7">
         <v>3291</v>
@@ -2073,48 +2094,51 @@
         <v>3356</v>
       </c>
       <c r="AN7">
-        <v>3196</v>
+        <v>3209</v>
       </c>
       <c r="AO7">
-        <v>3470</v>
+        <v>3477</v>
       </c>
       <c r="AP7">
-        <v>4374</v>
+        <v>4381</v>
       </c>
       <c r="AQ7">
-        <v>5154</v>
+        <v>5164</v>
       </c>
       <c r="AR7">
-        <v>4422</v>
+        <v>4433</v>
       </c>
       <c r="AS7">
-        <v>4119</v>
+        <v>4134</v>
       </c>
       <c r="AT7">
-        <v>4757</v>
+        <v>4801</v>
+      </c>
+      <c r="AU7">
+        <v>3649</v>
       </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8">
         <v>237</v>
       </c>
       <c r="D8">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="E8">
         <v>1650</v>
       </c>
       <c r="F8">
-        <v>1692</v>
+        <v>1693</v>
       </c>
       <c r="G8">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="H8">
         <v>662</v>
@@ -2129,7 +2153,7 @@
         <v>208</v>
       </c>
       <c r="L8">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="M8">
         <v>124</v>
@@ -2183,7 +2207,7 @@
         <v>224</v>
       </c>
       <c r="AD8">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="AE8">
         <v>305</v>
@@ -2198,43 +2222,46 @@
         <v>1285</v>
       </c>
       <c r="AI8">
-        <v>2267</v>
+        <v>2269</v>
       </c>
       <c r="AJ8">
-        <v>3551</v>
+        <v>3552</v>
       </c>
       <c r="AK8">
-        <v>4238</v>
+        <v>4237</v>
       </c>
       <c r="AL8">
-        <v>4018</v>
+        <v>4016</v>
       </c>
       <c r="AM8">
-        <v>4148</v>
+        <v>4147</v>
       </c>
       <c r="AN8">
-        <v>4131</v>
+        <v>4139</v>
       </c>
       <c r="AO8">
-        <v>4127</v>
+        <v>4125</v>
       </c>
       <c r="AP8">
-        <v>5146</v>
+        <v>5154</v>
       </c>
       <c r="AQ8">
-        <v>6301</v>
+        <v>6324</v>
       </c>
       <c r="AR8">
-        <v>5555</v>
+        <v>5567</v>
       </c>
       <c r="AS8">
-        <v>4942</v>
+        <v>4960</v>
       </c>
       <c r="AT8">
-        <v>5620</v>
+        <v>5684</v>
+      </c>
+      <c r="AU8">
+        <v>4363</v>
       </c>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2245,22 +2272,22 @@
         <v>431</v>
       </c>
       <c r="D9">
-        <v>1598</v>
+        <v>1597</v>
       </c>
       <c r="E9">
-        <v>2526</v>
+        <v>2528</v>
       </c>
       <c r="F9">
         <v>2784</v>
       </c>
       <c r="G9">
-        <v>1799</v>
+        <v>1798</v>
       </c>
       <c r="H9">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="I9">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="J9">
         <v>406</v>
@@ -2308,7 +2335,7 @@
         <v>204</v>
       </c>
       <c r="Y9">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="Z9">
         <v>237</v>
@@ -2332,49 +2359,52 @@
         <v>680</v>
       </c>
       <c r="AG9">
-        <v>1269</v>
+        <v>1271</v>
       </c>
       <c r="AH9">
-        <v>2119</v>
+        <v>2121</v>
       </c>
       <c r="AI9">
-        <v>3952</v>
+        <v>3953</v>
       </c>
       <c r="AJ9">
-        <v>5987</v>
+        <v>5989</v>
       </c>
       <c r="AK9">
-        <v>6845</v>
+        <v>6846</v>
       </c>
       <c r="AL9">
-        <v>6898</v>
+        <v>6902</v>
       </c>
       <c r="AM9">
-        <v>7304</v>
+        <v>7306</v>
       </c>
       <c r="AN9">
-        <v>6986</v>
+        <v>6994</v>
       </c>
       <c r="AO9">
-        <v>7651</v>
+        <v>7652</v>
       </c>
       <c r="AP9">
-        <v>9397</v>
+        <v>9413</v>
       </c>
       <c r="AQ9">
-        <v>10958</v>
+        <v>10987</v>
       </c>
       <c r="AR9">
-        <v>9105</v>
+        <v>9127</v>
       </c>
       <c r="AS9">
-        <v>8208</v>
+        <v>8241</v>
       </c>
       <c r="AT9">
-        <v>9091</v>
+        <v>9205</v>
+      </c>
+      <c r="AU9">
+        <v>7464</v>
       </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2385,19 +2415,19 @@
         <v>752</v>
       </c>
       <c r="D10">
-        <v>2599</v>
+        <v>2598</v>
       </c>
       <c r="E10">
-        <v>3596</v>
+        <v>3595</v>
       </c>
       <c r="F10">
         <v>3667</v>
       </c>
       <c r="G10">
-        <v>2610</v>
+        <v>2611</v>
       </c>
       <c r="H10">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="I10">
         <v>1060</v>
@@ -2406,13 +2436,13 @@
         <v>600</v>
       </c>
       <c r="K10">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="L10">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="M10">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="N10">
         <v>237</v>
@@ -2451,70 +2481,73 @@
         <v>326</v>
       </c>
       <c r="Z10">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="AA10">
         <v>353</v>
       </c>
       <c r="AB10">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="AC10">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="AD10">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="AE10">
-        <v>864</v>
+        <v>866</v>
       </c>
       <c r="AF10">
         <v>1106</v>
       </c>
       <c r="AG10">
-        <v>1867</v>
+        <v>1866</v>
       </c>
       <c r="AH10">
-        <v>2999</v>
+        <v>2998</v>
       </c>
       <c r="AI10">
-        <v>5756</v>
+        <v>5753</v>
       </c>
       <c r="AJ10">
-        <v>8957</v>
+        <v>8964</v>
       </c>
       <c r="AK10">
-        <v>10154</v>
+        <v>10155</v>
       </c>
       <c r="AL10">
-        <v>10302</v>
+        <v>10304</v>
       </c>
       <c r="AM10">
-        <v>10230</v>
+        <v>10236</v>
       </c>
       <c r="AN10">
-        <v>9846</v>
+        <v>9859</v>
       </c>
       <c r="AO10">
-        <v>10332</v>
+        <v>10341</v>
       </c>
       <c r="AP10">
-        <v>13007</v>
+        <v>13024</v>
       </c>
       <c r="AQ10">
-        <v>14926</v>
+        <v>14962</v>
       </c>
       <c r="AR10">
-        <v>12269</v>
+        <v>12297</v>
       </c>
       <c r="AS10">
-        <v>10976</v>
+        <v>11032</v>
       </c>
       <c r="AT10">
-        <v>12058</v>
+        <v>12222</v>
+      </c>
+      <c r="AU10">
+        <v>9916</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2531,13 +2564,13 @@
         <v>4001</v>
       </c>
       <c r="F11">
-        <v>3702</v>
+        <v>3700</v>
       </c>
       <c r="G11">
-        <v>2615</v>
+        <v>2614</v>
       </c>
       <c r="H11">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="I11">
         <v>991</v>
@@ -2549,10 +2582,10 @@
         <v>520</v>
       </c>
       <c r="L11">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="M11">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="N11">
         <v>239</v>
@@ -2564,7 +2597,7 @@
         <v>147</v>
       </c>
       <c r="Q11">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="R11">
         <v>268</v>
@@ -2585,19 +2618,19 @@
         <v>352</v>
       </c>
       <c r="X11">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="Y11">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="Z11">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="AA11">
         <v>540</v>
       </c>
       <c r="AB11">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="AC11">
         <v>668</v>
@@ -2606,55 +2639,58 @@
         <v>896</v>
       </c>
       <c r="AE11">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="AF11">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="AG11">
-        <v>2268</v>
+        <v>2267</v>
       </c>
       <c r="AH11">
-        <v>3571</v>
+        <v>3572</v>
       </c>
       <c r="AI11">
-        <v>6409</v>
+        <v>6411</v>
       </c>
       <c r="AJ11">
-        <v>9764</v>
+        <v>9770</v>
       </c>
       <c r="AK11">
-        <v>10944</v>
+        <v>10949</v>
       </c>
       <c r="AL11">
-        <v>10992</v>
+        <v>10991</v>
       </c>
       <c r="AM11">
-        <v>10821</v>
+        <v>10823</v>
       </c>
       <c r="AN11">
-        <v>10317</v>
+        <v>10338</v>
       </c>
       <c r="AO11">
-        <v>10534</v>
+        <v>10538</v>
       </c>
       <c r="AP11">
-        <v>13212</v>
+        <v>13228</v>
       </c>
       <c r="AQ11">
-        <v>14856</v>
+        <v>14886</v>
       </c>
       <c r="AR11">
-        <v>11915</v>
+        <v>11942</v>
       </c>
       <c r="AS11">
-        <v>10419</v>
+        <v>10471</v>
       </c>
       <c r="AT11">
-        <v>11877</v>
+        <v>12033</v>
+      </c>
+      <c r="AU11">
+        <v>9682</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2662,7 +2698,7 @@
         <v>100</v>
       </c>
       <c r="C12">
-        <v>745</v>
+        <v>742</v>
       </c>
       <c r="D12">
         <v>2097</v>
@@ -2671,10 +2707,10 @@
         <v>2924</v>
       </c>
       <c r="F12">
-        <v>2720</v>
+        <v>2722</v>
       </c>
       <c r="G12">
-        <v>1919</v>
+        <v>1920</v>
       </c>
       <c r="H12">
         <v>1174</v>
@@ -2686,7 +2722,7 @@
         <v>468</v>
       </c>
       <c r="K12">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="L12">
         <v>330</v>
@@ -2704,7 +2740,7 @@
         <v>144</v>
       </c>
       <c r="Q12">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="R12">
         <v>277</v>
@@ -2731,13 +2767,13 @@
         <v>574</v>
       </c>
       <c r="Z12">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="AA12">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="AB12">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="AC12">
         <v>695</v>
@@ -2752,49 +2788,52 @@
         <v>1198</v>
       </c>
       <c r="AG12">
-        <v>2035</v>
+        <v>2038</v>
       </c>
       <c r="AH12">
-        <v>3125</v>
+        <v>3127</v>
       </c>
       <c r="AI12">
-        <v>5804</v>
+        <v>5805</v>
       </c>
       <c r="AJ12">
-        <v>8378</v>
+        <v>8381</v>
       </c>
       <c r="AK12">
-        <v>9470</v>
+        <v>9471</v>
       </c>
       <c r="AL12">
-        <v>9280</v>
+        <v>9283</v>
       </c>
       <c r="AM12">
-        <v>9664</v>
+        <v>9665</v>
       </c>
       <c r="AN12">
-        <v>9039</v>
+        <v>9054</v>
       </c>
       <c r="AO12">
-        <v>9228</v>
+        <v>9232</v>
       </c>
       <c r="AP12">
-        <v>11065</v>
+        <v>11066</v>
       </c>
       <c r="AQ12">
-        <v>12382</v>
+        <v>12409</v>
       </c>
       <c r="AR12">
-        <v>9660</v>
+        <v>9692</v>
       </c>
       <c r="AS12">
-        <v>8506</v>
+        <v>8520</v>
       </c>
       <c r="AT12">
-        <v>9600</v>
+        <v>9728</v>
+      </c>
+      <c r="AU12">
+        <v>7928</v>
       </c>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2802,10 +2841,10 @@
         <v>86</v>
       </c>
       <c r="C13">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D13">
-        <v>1803</v>
+        <v>1804</v>
       </c>
       <c r="E13">
         <v>2330</v>
@@ -2829,7 +2868,7 @@
         <v>405</v>
       </c>
       <c r="L13">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="M13">
         <v>241</v>
@@ -2838,13 +2877,13 @@
         <v>213</v>
       </c>
       <c r="O13">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="P13">
         <v>158</v>
       </c>
       <c r="Q13">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="R13">
         <v>272</v>
@@ -2862,79 +2901,82 @@
         <v>322</v>
       </c>
       <c r="W13">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="X13">
         <v>488</v>
       </c>
       <c r="Y13">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="Z13">
         <v>716</v>
       </c>
       <c r="AA13">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="AB13">
         <v>648</v>
       </c>
       <c r="AC13">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="AD13">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="AE13">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="AF13">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="AG13">
         <v>1869</v>
       </c>
       <c r="AH13">
-        <v>2908</v>
+        <v>2907</v>
       </c>
       <c r="AI13">
-        <v>5299</v>
+        <v>5300</v>
       </c>
       <c r="AJ13">
-        <v>7856</v>
+        <v>7865</v>
       </c>
       <c r="AK13">
-        <v>8859</v>
+        <v>8862</v>
       </c>
       <c r="AL13">
-        <v>8976</v>
+        <v>8978</v>
       </c>
       <c r="AM13">
-        <v>9229</v>
+        <v>9231</v>
       </c>
       <c r="AN13">
-        <v>8777</v>
+        <v>8792</v>
       </c>
       <c r="AO13">
-        <v>8804</v>
+        <v>8818</v>
       </c>
       <c r="AP13">
-        <v>10864</v>
+        <v>10875</v>
       </c>
       <c r="AQ13">
-        <v>11931</v>
+        <v>11967</v>
       </c>
       <c r="AR13">
-        <v>9460</v>
+        <v>9480</v>
       </c>
       <c r="AS13">
-        <v>7979</v>
+        <v>8025</v>
       </c>
       <c r="AT13">
-        <v>9373</v>
+        <v>9472</v>
+      </c>
+      <c r="AU13">
+        <v>7480</v>
       </c>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -2942,19 +2984,19 @@
         <v>66</v>
       </c>
       <c r="C14">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="D14">
-        <v>1754</v>
+        <v>1755</v>
       </c>
       <c r="E14">
-        <v>2387</v>
+        <v>2386</v>
       </c>
       <c r="F14">
         <v>2205</v>
       </c>
       <c r="G14">
-        <v>1653</v>
+        <v>1652</v>
       </c>
       <c r="H14">
         <v>984</v>
@@ -2966,10 +3008,10 @@
         <v>464</v>
       </c>
       <c r="K14">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="L14">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="M14">
         <v>275</v>
@@ -2984,13 +3026,13 @@
         <v>195</v>
       </c>
       <c r="Q14">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="R14">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="S14">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="T14">
         <v>206</v>
@@ -3011,70 +3053,73 @@
         <v>645</v>
       </c>
       <c r="Z14">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="AA14">
         <v>715</v>
       </c>
       <c r="AB14">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="AC14">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="AD14">
         <v>901</v>
       </c>
       <c r="AE14">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="AF14">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="AG14">
         <v>1826</v>
       </c>
       <c r="AH14">
-        <v>3105</v>
+        <v>3107</v>
       </c>
       <c r="AI14">
-        <v>5387</v>
+        <v>5388</v>
       </c>
       <c r="AJ14">
-        <v>8079</v>
+        <v>8089</v>
       </c>
       <c r="AK14">
-        <v>8952</v>
+        <v>8954</v>
       </c>
       <c r="AL14">
-        <v>9181</v>
+        <v>9180</v>
       </c>
       <c r="AM14">
-        <v>9190</v>
+        <v>9196</v>
       </c>
       <c r="AN14">
-        <v>8707</v>
+        <v>8722</v>
       </c>
       <c r="AO14">
-        <v>9127</v>
+        <v>9140</v>
       </c>
       <c r="AP14">
-        <v>10958</v>
+        <v>10970</v>
       </c>
       <c r="AQ14">
-        <v>12165</v>
+        <v>12187</v>
       </c>
       <c r="AR14">
-        <v>9457</v>
+        <v>9479</v>
       </c>
       <c r="AS14">
-        <v>8050</v>
+        <v>8081</v>
       </c>
       <c r="AT14">
-        <v>9959</v>
+        <v>10062</v>
+      </c>
+      <c r="AU14">
+        <v>7925</v>
       </c>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -3082,10 +3127,10 @@
         <v>69</v>
       </c>
       <c r="C15">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D15">
-        <v>2050</v>
+        <v>2049</v>
       </c>
       <c r="E15">
         <v>2640</v>
@@ -3094,7 +3139,7 @@
         <v>2419</v>
       </c>
       <c r="G15">
-        <v>1749</v>
+        <v>1750</v>
       </c>
       <c r="H15">
         <v>1203</v>
@@ -3109,7 +3154,7 @@
         <v>488</v>
       </c>
       <c r="L15">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="M15">
         <v>323</v>
@@ -3133,7 +3178,7 @@
         <v>260</v>
       </c>
       <c r="T15">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="U15">
         <v>297</v>
@@ -3151,70 +3196,73 @@
         <v>700</v>
       </c>
       <c r="Z15">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="AA15">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="AB15">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="AC15">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="AD15">
         <v>1205</v>
       </c>
       <c r="AE15">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="AF15">
-        <v>1523</v>
+        <v>1524</v>
       </c>
       <c r="AG15">
-        <v>2366</v>
+        <v>2365</v>
       </c>
       <c r="AH15">
-        <v>3863</v>
+        <v>3864</v>
       </c>
       <c r="AI15">
-        <v>6711</v>
+        <v>6712</v>
       </c>
       <c r="AJ15">
-        <v>9569</v>
+        <v>9574</v>
       </c>
       <c r="AK15">
-        <v>10470</v>
+        <v>10475</v>
       </c>
       <c r="AL15">
-        <v>10476</v>
+        <v>10482</v>
       </c>
       <c r="AM15">
         <v>10100</v>
       </c>
       <c r="AN15">
-        <v>9350</v>
+        <v>9370</v>
       </c>
       <c r="AO15">
-        <v>9448</v>
+        <v>9457</v>
       </c>
       <c r="AP15">
-        <v>11495</v>
+        <v>11509</v>
       </c>
       <c r="AQ15">
-        <v>12957</v>
+        <v>12982</v>
       </c>
       <c r="AR15">
-        <v>10009</v>
+        <v>10036</v>
       </c>
       <c r="AS15">
-        <v>9139</v>
+        <v>9169</v>
       </c>
       <c r="AT15">
-        <v>11416</v>
+        <v>11523</v>
+      </c>
+      <c r="AU15">
+        <v>8976</v>
       </c>
     </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -3225,7 +3273,7 @@
         <v>547</v>
       </c>
       <c r="D16">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="E16">
         <v>2693</v>
@@ -3240,16 +3288,16 @@
         <v>1297</v>
       </c>
       <c r="I16">
-        <v>996</v>
+        <v>998</v>
       </c>
       <c r="J16">
         <v>680</v>
       </c>
       <c r="K16">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="L16">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="M16">
         <v>350</v>
@@ -3288,73 +3336,76 @@
         <v>608</v>
       </c>
       <c r="Y16">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="Z16">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="AA16">
-        <v>1221</v>
+        <v>1223</v>
       </c>
       <c r="AB16">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="AC16">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="AD16">
-        <v>1481</v>
+        <v>1482</v>
       </c>
       <c r="AE16">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="AF16">
-        <v>1745</v>
+        <v>1746</v>
       </c>
       <c r="AG16">
-        <v>2690</v>
+        <v>2692</v>
       </c>
       <c r="AH16">
-        <v>4478</v>
+        <v>4479</v>
       </c>
       <c r="AI16">
-        <v>7306</v>
+        <v>7309</v>
       </c>
       <c r="AJ16">
-        <v>10320</v>
+        <v>10325</v>
       </c>
       <c r="AK16">
-        <v>11148</v>
+        <v>11150</v>
       </c>
       <c r="AL16">
-        <v>10687</v>
+        <v>10694</v>
       </c>
       <c r="AM16">
-        <v>9939</v>
+        <v>9942</v>
       </c>
       <c r="AN16">
-        <v>8982</v>
+        <v>8995</v>
       </c>
       <c r="AO16">
-        <v>9114</v>
+        <v>9131</v>
       </c>
       <c r="AP16">
-        <v>10770</v>
+        <v>10781</v>
       </c>
       <c r="AQ16">
-        <v>12075</v>
+        <v>12089</v>
       </c>
       <c r="AR16">
-        <v>9397</v>
+        <v>9396</v>
       </c>
       <c r="AS16">
-        <v>8399</v>
+        <v>8427</v>
       </c>
       <c r="AT16">
-        <v>10638</v>
+        <v>10759</v>
+      </c>
+      <c r="AU16">
+        <v>8475</v>
       </c>
     </row>
-    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -3362,16 +3413,16 @@
         <v>70</v>
       </c>
       <c r="C17">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="D17">
         <v>1447</v>
       </c>
       <c r="E17">
-        <v>2273</v>
+        <v>2274</v>
       </c>
       <c r="F17">
-        <v>2243</v>
+        <v>2245</v>
       </c>
       <c r="G17">
         <v>1732</v>
@@ -3380,7 +3431,7 @@
         <v>1233</v>
       </c>
       <c r="I17">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="J17">
         <v>595</v>
@@ -3389,7 +3440,7 @@
         <v>508</v>
       </c>
       <c r="L17">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="M17">
         <v>314</v>
@@ -3401,13 +3452,13 @@
         <v>229</v>
       </c>
       <c r="P17">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="Q17">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="R17">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="S17">
         <v>258</v>
@@ -3419,7 +3470,7 @@
         <v>302</v>
       </c>
       <c r="V17">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="W17">
         <v>521</v>
@@ -3431,22 +3482,22 @@
         <v>1166</v>
       </c>
       <c r="Z17">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="AA17">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="AB17">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="AC17">
         <v>1291</v>
       </c>
       <c r="AD17">
-        <v>1516</v>
+        <v>1519</v>
       </c>
       <c r="AE17">
-        <v>1583</v>
+        <v>1585</v>
       </c>
       <c r="AF17">
         <v>1735</v>
@@ -3455,46 +3506,49 @@
         <v>2792</v>
       </c>
       <c r="AH17">
-        <v>4375</v>
+        <v>4380</v>
       </c>
       <c r="AI17">
-        <v>7544</v>
+        <v>7551</v>
       </c>
       <c r="AJ17">
-        <v>10428</v>
+        <v>10430</v>
       </c>
       <c r="AK17">
-        <v>11739</v>
+        <v>11745</v>
       </c>
       <c r="AL17">
-        <v>11032</v>
+        <v>11045</v>
       </c>
       <c r="AM17">
-        <v>10222</v>
+        <v>10227</v>
       </c>
       <c r="AN17">
-        <v>8933</v>
+        <v>8950</v>
       </c>
       <c r="AO17">
-        <v>9185</v>
+        <v>9187</v>
       </c>
       <c r="AP17">
-        <v>10762</v>
+        <v>10777</v>
       </c>
       <c r="AQ17">
-        <v>12082</v>
+        <v>12105</v>
       </c>
       <c r="AR17">
-        <v>9035</v>
+        <v>9047</v>
       </c>
       <c r="AS17">
-        <v>8573</v>
+        <v>8592</v>
       </c>
       <c r="AT17">
-        <v>10763</v>
+        <v>10868</v>
+      </c>
+      <c r="AU17">
+        <v>8439</v>
       </c>
     </row>
-    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -3502,7 +3556,7 @@
         <v>42</v>
       </c>
       <c r="C18">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D18">
         <v>541</v>
@@ -3514,7 +3568,7 @@
         <v>1080</v>
       </c>
       <c r="G18">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="H18">
         <v>572</v>
@@ -3523,7 +3577,7 @@
         <v>403</v>
       </c>
       <c r="J18">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="K18">
         <v>258</v>
@@ -3544,7 +3598,7 @@
         <v>111</v>
       </c>
       <c r="Q18">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="R18">
         <v>169</v>
@@ -3571,70 +3625,73 @@
         <v>742</v>
       </c>
       <c r="Z18">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="AA18">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="AB18">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="AC18">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="AD18">
         <v>1034</v>
       </c>
       <c r="AE18">
-        <v>1046</v>
+        <v>1049</v>
       </c>
       <c r="AF18">
-        <v>1329</v>
+        <v>1331</v>
       </c>
       <c r="AG18">
-        <v>2074</v>
+        <v>2077</v>
       </c>
       <c r="AH18">
-        <v>2965</v>
+        <v>2968</v>
       </c>
       <c r="AI18">
-        <v>4848</v>
+        <v>4851</v>
       </c>
       <c r="AJ18">
-        <v>7187</v>
+        <v>7186</v>
       </c>
       <c r="AK18">
-        <v>8406</v>
+        <v>8410</v>
       </c>
       <c r="AL18">
-        <v>8691</v>
+        <v>8699</v>
       </c>
       <c r="AM18">
-        <v>8196</v>
+        <v>8203</v>
       </c>
       <c r="AN18">
-        <v>7451</v>
+        <v>7464</v>
       </c>
       <c r="AO18">
-        <v>7713</v>
+        <v>7718</v>
       </c>
       <c r="AP18">
-        <v>8814</v>
+        <v>8823</v>
       </c>
       <c r="AQ18">
-        <v>8441</v>
+        <v>8456</v>
       </c>
       <c r="AR18">
-        <v>5831</v>
+        <v>5844</v>
       </c>
       <c r="AS18">
-        <v>4934</v>
+        <v>4959</v>
       </c>
       <c r="AT18">
-        <v>6257</v>
+        <v>6330</v>
+      </c>
+      <c r="AU18">
+        <v>5360</v>
       </c>
     </row>
-    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>68</v>
       </c>
@@ -3708,13 +3765,13 @@
         <v>364</v>
       </c>
       <c r="Y19">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="Z19">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="AA19">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="AB19">
         <v>430</v>
@@ -3723,7 +3780,7 @@
         <v>498</v>
       </c>
       <c r="AD19">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="AE19">
         <v>587</v>
@@ -3732,49 +3789,52 @@
         <v>710</v>
       </c>
       <c r="AG19">
-        <v>1140</v>
+        <v>1142</v>
       </c>
       <c r="AH19">
         <v>1653</v>
       </c>
       <c r="AI19">
-        <v>2744</v>
+        <v>2745</v>
       </c>
       <c r="AJ19">
-        <v>4080</v>
+        <v>4082</v>
       </c>
       <c r="AK19">
-        <v>4772</v>
+        <v>4775</v>
       </c>
       <c r="AL19">
-        <v>5339</v>
+        <v>5342</v>
       </c>
       <c r="AM19">
-        <v>5297</v>
+        <v>5305</v>
       </c>
       <c r="AN19">
-        <v>5174</v>
+        <v>5181</v>
       </c>
       <c r="AO19">
         <v>5153</v>
       </c>
       <c r="AP19">
-        <v>5663</v>
+        <v>5673</v>
       </c>
       <c r="AQ19">
-        <v>5244</v>
+        <v>5253</v>
       </c>
       <c r="AR19">
-        <v>3359</v>
+        <v>3366</v>
       </c>
       <c r="AS19">
-        <v>2630</v>
+        <v>2634</v>
       </c>
       <c r="AT19">
-        <v>3242</v>
+        <v>3291</v>
+      </c>
+      <c r="AU19">
+        <v>2691</v>
       </c>
     </row>
-    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>67</v>
       </c>
@@ -3803,7 +3863,7 @@
         <v>153</v>
       </c>
       <c r="J20">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K20">
         <v>105</v>
@@ -3818,7 +3878,7 @@
         <v>113</v>
       </c>
       <c r="O20">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P20">
         <v>123</v>
@@ -3827,7 +3887,7 @@
         <v>176</v>
       </c>
       <c r="R20">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S20">
         <v>124</v>
@@ -3866,10 +3926,10 @@
         <v>354</v>
       </c>
       <c r="AE20">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="AF20">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="AG20">
         <v>626</v>
@@ -3878,43 +3938,46 @@
         <v>971</v>
       </c>
       <c r="AI20">
-        <v>1834</v>
+        <v>1833</v>
       </c>
       <c r="AJ20">
         <v>2790</v>
       </c>
       <c r="AK20">
-        <v>3361</v>
+        <v>3360</v>
       </c>
       <c r="AL20">
-        <v>3620</v>
+        <v>3616</v>
       </c>
       <c r="AM20">
-        <v>3912</v>
+        <v>3915</v>
       </c>
       <c r="AN20">
-        <v>3806</v>
+        <v>3813</v>
       </c>
       <c r="AO20">
-        <v>3669</v>
+        <v>3674</v>
       </c>
       <c r="AP20">
         <v>4242</v>
       </c>
       <c r="AQ20">
-        <v>4286</v>
+        <v>4290</v>
       </c>
       <c r="AR20">
-        <v>2992</v>
+        <v>2998</v>
       </c>
       <c r="AS20">
-        <v>1925</v>
+        <v>1931</v>
       </c>
       <c r="AT20">
-        <v>2355</v>
+        <v>2372</v>
+      </c>
+      <c r="AU20">
+        <v>2177</v>
       </c>
     </row>
-    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -3928,7 +3991,7 @@
         <v>143</v>
       </c>
       <c r="E21">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F21">
         <v>273</v>
@@ -3961,7 +4024,7 @@
         <v>108</v>
       </c>
       <c r="P21">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q21">
         <v>160</v>
@@ -3973,7 +4036,7 @@
         <v>141</v>
       </c>
       <c r="T21">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="U21">
         <v>140</v>
@@ -3991,7 +4054,7 @@
         <v>276</v>
       </c>
       <c r="Z21">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="AA21">
         <v>223</v>
@@ -4000,25 +4063,25 @@
         <v>229</v>
       </c>
       <c r="AC21">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AD21">
         <v>290</v>
       </c>
       <c r="AE21">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="AF21">
         <v>324</v>
       </c>
       <c r="AG21">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="AH21">
         <v>886</v>
       </c>
       <c r="AI21">
-        <v>1466</v>
+        <v>1463</v>
       </c>
       <c r="AJ21">
         <v>2248</v>
@@ -4027,31 +4090,34 @@
         <v>2422</v>
       </c>
       <c r="AL21">
-        <v>2426</v>
+        <v>2427</v>
       </c>
       <c r="AM21">
-        <v>2383</v>
+        <v>2381</v>
       </c>
       <c r="AN21">
         <v>2336</v>
       </c>
       <c r="AO21">
-        <v>2315</v>
+        <v>2319</v>
       </c>
       <c r="AP21">
-        <v>2695</v>
+        <v>2692</v>
       </c>
       <c r="AQ21">
-        <v>3115</v>
+        <v>3117</v>
       </c>
       <c r="AR21">
-        <v>2118</v>
+        <v>2117</v>
       </c>
       <c r="AS21">
-        <v>1533</v>
+        <v>1532</v>
       </c>
       <c r="AT21">
-        <v>1898</v>
+        <v>1918</v>
+      </c>
+      <c r="AU21">
+        <v>1836</v>
       </c>
     </row>
   </sheetData>
@@ -4062,15 +4128,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A5C854-B8B9-4F3F-88F5-F4BF0588EB40}">
-  <dimension ref="A1:AT21"/>
+  <dimension ref="A1:AU21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AU2" sqref="AU2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4209,13 +4275,16 @@
       <c r="AT1" t="s">
         <v>66</v>
       </c>
+      <c r="AU1" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1.08</v>
+        <v>1.07</v>
       </c>
       <c r="C2">
         <v>7.74</v>
@@ -4227,13 +4296,13 @@
         <v>40.92</v>
       </c>
       <c r="F2">
-        <v>43.4</v>
+        <v>43.41</v>
       </c>
       <c r="G2">
-        <v>32.69</v>
+        <v>32.68</v>
       </c>
       <c r="H2">
-        <v>20.88</v>
+        <v>20.89</v>
       </c>
       <c r="I2">
         <v>14.89</v>
@@ -4242,10 +4311,10 @@
         <v>8.9499999999999993</v>
       </c>
       <c r="K2">
-        <v>7.49</v>
+        <v>7.5</v>
       </c>
       <c r="L2">
-        <v>5.69</v>
+        <v>5.72</v>
       </c>
       <c r="M2">
         <v>4.3499999999999996</v>
@@ -4260,10 +4329,10 @@
         <v>2.82</v>
       </c>
       <c r="Q2">
-        <v>4.9800000000000004</v>
+        <v>4.97</v>
       </c>
       <c r="R2">
-        <v>3.87</v>
+        <v>3.86</v>
       </c>
       <c r="S2">
         <v>3.24</v>
@@ -4299,58 +4368,61 @@
         <v>11.75</v>
       </c>
       <c r="AD2">
-        <v>14.76</v>
+        <v>14.78</v>
       </c>
       <c r="AE2">
         <v>15.72</v>
       </c>
       <c r="AF2">
-        <v>19.14</v>
+        <v>19.149999999999999</v>
       </c>
       <c r="AG2">
-        <v>31.47</v>
+        <v>31.46</v>
       </c>
       <c r="AH2">
-        <v>50.59</v>
+        <v>50.6</v>
       </c>
       <c r="AI2">
-        <v>89.96</v>
+        <v>89.97</v>
       </c>
       <c r="AJ2">
-        <v>133.63999999999999</v>
+        <v>133.65</v>
       </c>
       <c r="AK2">
         <v>151.28</v>
       </c>
       <c r="AL2">
-        <v>153.78</v>
+        <v>153.79</v>
       </c>
       <c r="AM2">
-        <v>154.54</v>
+        <v>154.55000000000001</v>
       </c>
       <c r="AN2">
-        <v>148.33000000000001</v>
+        <v>148.35</v>
       </c>
       <c r="AO2">
-        <v>154.30000000000001</v>
+        <v>154.38</v>
       </c>
       <c r="AP2">
-        <v>187.77</v>
+        <v>187.91</v>
       </c>
       <c r="AQ2">
-        <v>209.6</v>
+        <v>210</v>
       </c>
       <c r="AR2">
-        <v>166.58</v>
+        <v>166.91</v>
       </c>
       <c r="AS2">
-        <v>147.33000000000001</v>
+        <v>147.82</v>
       </c>
       <c r="AT2">
-        <v>172.18</v>
+        <v>174.13</v>
+      </c>
+      <c r="AU2">
+        <v>141.81</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -4361,7 +4433,7 @@
         <v>1.46</v>
       </c>
       <c r="D3">
-        <v>12.03</v>
+        <v>12.15</v>
       </c>
       <c r="E3">
         <v>51.39</v>
@@ -4436,7 +4508,7 @@
         <v>2.92</v>
       </c>
       <c r="AC3">
-        <v>5.35</v>
+        <v>5.47</v>
       </c>
       <c r="AD3">
         <v>8.99</v>
@@ -4460,37 +4532,40 @@
         <v>178</v>
       </c>
       <c r="AK3">
-        <v>208.98</v>
+        <v>208.86</v>
       </c>
       <c r="AL3">
-        <v>281.14999999999998</v>
+        <v>281.39</v>
       </c>
       <c r="AM3">
-        <v>372.4</v>
+        <v>372.88</v>
       </c>
       <c r="AN3">
-        <v>427.31</v>
+        <v>428.89</v>
       </c>
       <c r="AO3">
-        <v>502.77</v>
+        <v>504.59</v>
       </c>
       <c r="AP3">
-        <v>656.95</v>
+        <v>657.31</v>
       </c>
       <c r="AQ3">
-        <v>722.19</v>
+        <v>726.93</v>
       </c>
       <c r="AR3">
-        <v>635.69000000000005</v>
+        <v>638.72</v>
       </c>
       <c r="AS3">
-        <v>600.09</v>
+        <v>603.12</v>
       </c>
       <c r="AT3">
-        <v>641.28</v>
+        <v>653.66999999999996</v>
+      </c>
+      <c r="AU3">
+        <v>603.61</v>
       </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -4507,13 +4582,13 @@
         <v>47.19</v>
       </c>
       <c r="F4">
-        <v>92.53</v>
+        <v>92.72</v>
       </c>
       <c r="G4">
         <v>90.87</v>
       </c>
       <c r="H4">
-        <v>59.21</v>
+        <v>59.28</v>
       </c>
       <c r="I4">
         <v>43.74</v>
@@ -4540,7 +4615,7 @@
         <v>3.26</v>
       </c>
       <c r="Q4">
-        <v>2.88</v>
+        <v>2.94</v>
       </c>
       <c r="R4">
         <v>2.17</v>
@@ -4585,52 +4660,55 @@
         <v>7.74</v>
       </c>
       <c r="AF4">
-        <v>10.42</v>
+        <v>10.49</v>
       </c>
       <c r="AG4">
         <v>19.5</v>
       </c>
       <c r="AH4">
-        <v>36.450000000000003</v>
+        <v>36.58</v>
       </c>
       <c r="AI4">
         <v>72.709999999999994</v>
       </c>
       <c r="AJ4">
-        <v>113.82</v>
+        <v>113.76</v>
       </c>
       <c r="AK4">
-        <v>146.5</v>
+        <v>146.44</v>
       </c>
       <c r="AL4">
-        <v>180.78</v>
+        <v>180.97</v>
       </c>
       <c r="AM4">
-        <v>215.24</v>
+        <v>215.18</v>
       </c>
       <c r="AN4">
-        <v>261.99</v>
+        <v>262.95</v>
       </c>
       <c r="AO4">
-        <v>292.68</v>
+        <v>292.88</v>
       </c>
       <c r="AP4">
-        <v>376.9</v>
+        <v>377.6</v>
       </c>
       <c r="AQ4">
-        <v>441.49</v>
+        <v>442.7</v>
       </c>
       <c r="AR4">
-        <v>372.55</v>
+        <v>374.79</v>
       </c>
       <c r="AS4">
-        <v>355.8</v>
+        <v>357.52</v>
       </c>
       <c r="AT4">
-        <v>380.48</v>
+        <v>386.62</v>
+      </c>
+      <c r="AU4">
+        <v>350.81</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -4647,25 +4725,25 @@
         <v>39.01</v>
       </c>
       <c r="F5">
-        <v>59.59</v>
+        <v>59.62</v>
       </c>
       <c r="G5">
         <v>52.18</v>
       </c>
       <c r="H5">
-        <v>35.880000000000003</v>
+        <v>35.85</v>
       </c>
       <c r="I5">
-        <v>24.98</v>
+        <v>25.01</v>
       </c>
       <c r="J5">
         <v>13.69</v>
       </c>
       <c r="K5">
-        <v>9.08</v>
+        <v>9.11</v>
       </c>
       <c r="L5">
-        <v>7.47</v>
+        <v>7.5</v>
       </c>
       <c r="M5">
         <v>4.6100000000000003</v>
@@ -4737,40 +4815,43 @@
         <v>55.64</v>
       </c>
       <c r="AJ5">
-        <v>86.27</v>
+        <v>86.24</v>
       </c>
       <c r="AK5">
-        <v>104.18</v>
+        <v>104.21</v>
       </c>
       <c r="AL5">
-        <v>115.32</v>
+        <v>115.29</v>
       </c>
       <c r="AM5">
-        <v>132.35</v>
+        <v>132.47</v>
       </c>
       <c r="AN5">
-        <v>145.13</v>
+        <v>145.68</v>
       </c>
       <c r="AO5">
         <v>164.68</v>
       </c>
       <c r="AP5">
-        <v>213.86</v>
+        <v>214.19</v>
       </c>
       <c r="AQ5">
-        <v>249.77</v>
+        <v>250.8</v>
       </c>
       <c r="AR5">
-        <v>224.72</v>
+        <v>225.6</v>
       </c>
       <c r="AS5">
-        <v>207.09</v>
+        <v>207.88</v>
       </c>
       <c r="AT5">
-        <v>229.19</v>
+        <v>232.04</v>
+      </c>
+      <c r="AU5">
+        <v>199.95</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -4778,22 +4859,22 @@
         <v>0.62</v>
       </c>
       <c r="C6">
-        <v>2.89</v>
+        <v>2.92</v>
       </c>
       <c r="D6">
         <v>14.73</v>
       </c>
       <c r="E6">
-        <v>36.299999999999997</v>
+        <v>36.270000000000003</v>
       </c>
       <c r="F6">
-        <v>46.07</v>
+        <v>46.13</v>
       </c>
       <c r="G6">
-        <v>33.85</v>
+        <v>33.82</v>
       </c>
       <c r="H6">
-        <v>22</v>
+        <v>22.03</v>
       </c>
       <c r="I6">
         <v>15.14</v>
@@ -4805,7 +4886,7 @@
         <v>7.07</v>
       </c>
       <c r="L6">
-        <v>4.46</v>
+        <v>4.51</v>
       </c>
       <c r="M6">
         <v>2.71</v>
@@ -4817,7 +4898,7 @@
         <v>1.5</v>
       </c>
       <c r="P6">
-        <v>1.1399999999999999</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="Q6">
         <v>1.68</v>
@@ -4859,7 +4940,7 @@
         <v>3.74</v>
       </c>
       <c r="AD6">
-        <v>4.6399999999999997</v>
+        <v>4.67</v>
       </c>
       <c r="AE6">
         <v>5.96</v>
@@ -4871,46 +4952,49 @@
         <v>13.08</v>
       </c>
       <c r="AH6">
-        <v>23.35</v>
+        <v>23.32</v>
       </c>
       <c r="AI6">
-        <v>41.97</v>
+        <v>42</v>
       </c>
       <c r="AJ6">
-        <v>68.23</v>
+        <v>68.260000000000005</v>
       </c>
       <c r="AK6">
-        <v>78.55</v>
+        <v>78.66</v>
       </c>
       <c r="AL6">
         <v>84.85</v>
       </c>
       <c r="AM6">
-        <v>87.37</v>
+        <v>87.48</v>
       </c>
       <c r="AN6">
-        <v>90.08</v>
+        <v>90.13</v>
       </c>
       <c r="AO6">
-        <v>102.05</v>
+        <v>102.21</v>
       </c>
       <c r="AP6">
-        <v>128.31</v>
+        <v>128.6</v>
       </c>
       <c r="AQ6">
-        <v>153.22999999999999</v>
+        <v>153.69999999999999</v>
       </c>
       <c r="AR6">
-        <v>130.74</v>
+        <v>131.07</v>
       </c>
       <c r="AS6">
-        <v>118.74</v>
+        <v>119.13</v>
       </c>
       <c r="AT6">
-        <v>132.72999999999999</v>
+        <v>134.47999999999999</v>
+      </c>
+      <c r="AU6">
+        <v>110.85</v>
       </c>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -4918,19 +5002,19 @@
         <v>0.3</v>
       </c>
       <c r="C7">
-        <v>3.92</v>
+        <v>3.95</v>
       </c>
       <c r="D7">
-        <v>16.93</v>
+        <v>16.96</v>
       </c>
       <c r="E7">
-        <v>36.090000000000003</v>
+        <v>36.119999999999997</v>
       </c>
       <c r="F7">
-        <v>38.54</v>
+        <v>38.51</v>
       </c>
       <c r="G7">
-        <v>28.61</v>
+        <v>28.58</v>
       </c>
       <c r="H7">
         <v>17.2</v>
@@ -4945,7 +5029,7 @@
         <v>5.63</v>
       </c>
       <c r="L7">
-        <v>3.48</v>
+        <v>3.51</v>
       </c>
       <c r="M7">
         <v>2.5</v>
@@ -4957,7 +5041,7 @@
         <v>1.28</v>
       </c>
       <c r="P7">
-        <v>1.0900000000000001</v>
+        <v>1.06</v>
       </c>
       <c r="Q7">
         <v>1.58</v>
@@ -4990,7 +5074,7 @@
         <v>2.61</v>
       </c>
       <c r="AA7">
-        <v>2.5299999999999998</v>
+        <v>2.5</v>
       </c>
       <c r="AB7">
         <v>2.91</v>
@@ -5008,19 +5092,19 @@
         <v>9.5299999999999994</v>
       </c>
       <c r="AG7">
-        <v>16.11</v>
+        <v>16.059999999999999</v>
       </c>
       <c r="AH7">
         <v>25.37</v>
       </c>
       <c r="AI7">
-        <v>48.75</v>
+        <v>48.8</v>
       </c>
       <c r="AJ7">
-        <v>78.39</v>
+        <v>78.41</v>
       </c>
       <c r="AK7">
-        <v>86.33</v>
+        <v>86.39</v>
       </c>
       <c r="AL7">
         <v>89.57</v>
@@ -5029,48 +5113,51 @@
         <v>91.34</v>
       </c>
       <c r="AN7">
-        <v>86.99</v>
+        <v>87.34</v>
       </c>
       <c r="AO7">
-        <v>94.45</v>
+        <v>94.64</v>
       </c>
       <c r="AP7">
-        <v>119.05</v>
+        <v>119.24</v>
       </c>
       <c r="AQ7">
-        <v>140.28</v>
+        <v>140.55000000000001</v>
       </c>
       <c r="AR7">
-        <v>120.36</v>
+        <v>120.66</v>
       </c>
       <c r="AS7">
-        <v>112.11</v>
+        <v>112.52</v>
       </c>
       <c r="AT7">
-        <v>129.47</v>
+        <v>130.66999999999999</v>
+      </c>
+      <c r="AU7">
+        <v>99.32</v>
       </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0.51</v>
+        <v>0.49</v>
       </c>
       <c r="C8">
         <v>4.88</v>
       </c>
       <c r="D8">
-        <v>18.32</v>
+        <v>18.3</v>
       </c>
       <c r="E8">
         <v>33.96</v>
       </c>
       <c r="F8">
-        <v>34.82</v>
+        <v>34.840000000000003</v>
       </c>
       <c r="G8">
-        <v>22.97</v>
+        <v>22.95</v>
       </c>
       <c r="H8">
         <v>13.62</v>
@@ -5085,7 +5172,7 @@
         <v>4.28</v>
       </c>
       <c r="L8">
-        <v>2.96</v>
+        <v>3.03</v>
       </c>
       <c r="M8">
         <v>2.5499999999999998</v>
@@ -5139,7 +5226,7 @@
         <v>4.6100000000000003</v>
       </c>
       <c r="AD8">
-        <v>5.95</v>
+        <v>5.97</v>
       </c>
       <c r="AE8">
         <v>6.28</v>
@@ -5154,43 +5241,46 @@
         <v>26.45</v>
       </c>
       <c r="AI8">
-        <v>46.66</v>
+        <v>46.7</v>
       </c>
       <c r="AJ8">
-        <v>73.08</v>
+        <v>73.099999999999994</v>
       </c>
       <c r="AK8">
-        <v>87.22</v>
+        <v>87.2</v>
       </c>
       <c r="AL8">
-        <v>82.69</v>
+        <v>82.65</v>
       </c>
       <c r="AM8">
-        <v>85.37</v>
+        <v>85.35</v>
       </c>
       <c r="AN8">
-        <v>85.02</v>
+        <v>85.18</v>
       </c>
       <c r="AO8">
-        <v>84.93</v>
+        <v>84.89</v>
       </c>
       <c r="AP8">
-        <v>105.91</v>
+        <v>106.07</v>
       </c>
       <c r="AQ8">
-        <v>129.68</v>
+        <v>130.15</v>
       </c>
       <c r="AR8">
-        <v>114.32</v>
+        <v>114.57</v>
       </c>
       <c r="AS8">
-        <v>101.71</v>
+        <v>102.08</v>
       </c>
       <c r="AT8">
-        <v>115.66</v>
+        <v>116.98</v>
+      </c>
+      <c r="AU8">
+        <v>89.79</v>
       </c>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -5201,22 +5291,22 @@
         <v>7.63</v>
       </c>
       <c r="D9">
-        <v>28.29</v>
+        <v>28.28</v>
       </c>
       <c r="E9">
-        <v>44.73</v>
+        <v>44.76</v>
       </c>
       <c r="F9">
         <v>49.29</v>
       </c>
       <c r="G9">
-        <v>31.85</v>
+        <v>31.84</v>
       </c>
       <c r="H9">
-        <v>19.23</v>
+        <v>19.25</v>
       </c>
       <c r="I9">
-        <v>11.93</v>
+        <v>11.92</v>
       </c>
       <c r="J9">
         <v>7.19</v>
@@ -5264,7 +5354,7 @@
         <v>3.61</v>
       </c>
       <c r="Y9">
-        <v>3.42</v>
+        <v>3.43</v>
       </c>
       <c r="Z9">
         <v>4.2</v>
@@ -5288,49 +5378,52 @@
         <v>12.04</v>
       </c>
       <c r="AG9">
-        <v>22.47</v>
+        <v>22.5</v>
       </c>
       <c r="AH9">
-        <v>37.520000000000003</v>
+        <v>37.549999999999997</v>
       </c>
       <c r="AI9">
-        <v>69.97</v>
+        <v>69.989999999999995</v>
       </c>
       <c r="AJ9">
-        <v>106.01</v>
+        <v>106.04</v>
       </c>
       <c r="AK9">
-        <v>121.2</v>
+        <v>121.22</v>
       </c>
       <c r="AL9">
-        <v>122.14</v>
+        <v>122.21</v>
       </c>
       <c r="AM9">
-        <v>129.33000000000001</v>
+        <v>129.36000000000001</v>
       </c>
       <c r="AN9">
-        <v>123.69</v>
+        <v>123.84</v>
       </c>
       <c r="AO9">
-        <v>135.47</v>
+        <v>135.49</v>
       </c>
       <c r="AP9">
-        <v>166.38</v>
+        <v>166.67</v>
       </c>
       <c r="AQ9">
-        <v>194.02</v>
+        <v>194.54</v>
       </c>
       <c r="AR9">
-        <v>161.21</v>
+        <v>161.6</v>
       </c>
       <c r="AS9">
-        <v>145.33000000000001</v>
+        <v>145.91999999999999</v>
       </c>
       <c r="AT9">
-        <v>160.97</v>
+        <v>162.97999999999999</v>
+      </c>
+      <c r="AU9">
+        <v>132.16</v>
       </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -5341,19 +5434,19 @@
         <v>11.16</v>
       </c>
       <c r="D10">
-        <v>38.58</v>
+        <v>38.56</v>
       </c>
       <c r="E10">
-        <v>53.37</v>
+        <v>53.36</v>
       </c>
       <c r="F10">
         <v>54.43</v>
       </c>
       <c r="G10">
-        <v>38.74</v>
+        <v>38.75</v>
       </c>
       <c r="H10">
-        <v>23.26</v>
+        <v>23.24</v>
       </c>
       <c r="I10">
         <v>15.73</v>
@@ -5362,13 +5455,13 @@
         <v>8.91</v>
       </c>
       <c r="K10">
-        <v>7.55</v>
+        <v>7.57</v>
       </c>
       <c r="L10">
-        <v>5.28</v>
+        <v>5.34</v>
       </c>
       <c r="M10">
-        <v>3.96</v>
+        <v>3.95</v>
       </c>
       <c r="N10">
         <v>3.52</v>
@@ -5407,70 +5500,73 @@
         <v>4.84</v>
       </c>
       <c r="Z10">
-        <v>6.4</v>
+        <v>6.41</v>
       </c>
       <c r="AA10">
         <v>5.24</v>
       </c>
       <c r="AB10">
-        <v>5.82</v>
+        <v>5.83</v>
       </c>
       <c r="AC10">
-        <v>8.2100000000000009</v>
+        <v>8.2200000000000006</v>
       </c>
       <c r="AD10">
-        <v>11.28</v>
+        <v>11.3</v>
       </c>
       <c r="AE10">
-        <v>12.82</v>
+        <v>12.85</v>
       </c>
       <c r="AF10">
         <v>16.420000000000002</v>
       </c>
       <c r="AG10">
-        <v>27.71</v>
+        <v>27.7</v>
       </c>
       <c r="AH10">
-        <v>44.51</v>
+        <v>44.5</v>
       </c>
       <c r="AI10">
-        <v>85.43</v>
+        <v>85.39</v>
       </c>
       <c r="AJ10">
-        <v>132.94999999999999</v>
+        <v>133.05000000000001</v>
       </c>
       <c r="AK10">
-        <v>150.71</v>
+        <v>150.72999999999999</v>
       </c>
       <c r="AL10">
-        <v>152.91</v>
+        <v>152.94</v>
       </c>
       <c r="AM10">
-        <v>151.84</v>
+        <v>151.93</v>
       </c>
       <c r="AN10">
-        <v>146.13999999999999</v>
+        <v>146.33000000000001</v>
       </c>
       <c r="AO10">
-        <v>153.36000000000001</v>
+        <v>153.49</v>
       </c>
       <c r="AP10">
-        <v>193.06</v>
+        <v>193.31</v>
       </c>
       <c r="AQ10">
-        <v>221.54</v>
+        <v>222.08</v>
       </c>
       <c r="AR10">
-        <v>182.11</v>
+        <v>182.52</v>
       </c>
       <c r="AS10">
-        <v>162.91</v>
+        <v>163.74</v>
       </c>
       <c r="AT10">
-        <v>178.97</v>
+        <v>181.41</v>
+      </c>
+      <c r="AU10">
+        <v>147.18</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -5487,13 +5583,13 @@
         <v>59.63</v>
       </c>
       <c r="F11">
-        <v>55.17</v>
+        <v>55.14</v>
       </c>
       <c r="G11">
-        <v>38.97</v>
+        <v>38.96</v>
       </c>
       <c r="H11">
-        <v>23.23</v>
+        <v>23.25</v>
       </c>
       <c r="I11">
         <v>14.77</v>
@@ -5505,10 +5601,10 @@
         <v>7.75</v>
       </c>
       <c r="L11">
-        <v>5.53</v>
+        <v>5.56</v>
       </c>
       <c r="M11">
-        <v>3.74</v>
+        <v>3.76</v>
       </c>
       <c r="N11">
         <v>3.56</v>
@@ -5520,7 +5616,7 @@
         <v>2.19</v>
       </c>
       <c r="Q11">
-        <v>4.75</v>
+        <v>4.74</v>
       </c>
       <c r="R11">
         <v>3.99</v>
@@ -5541,19 +5637,19 @@
         <v>5.25</v>
       </c>
       <c r="X11">
-        <v>6.21</v>
+        <v>6.23</v>
       </c>
       <c r="Y11">
-        <v>7.06</v>
+        <v>7.08</v>
       </c>
       <c r="Z11">
-        <v>8.35</v>
+        <v>8.36</v>
       </c>
       <c r="AA11">
         <v>8.0500000000000007</v>
       </c>
       <c r="AB11">
-        <v>8.27</v>
+        <v>8.26</v>
       </c>
       <c r="AC11">
         <v>9.9499999999999993</v>
@@ -5562,55 +5658,58 @@
         <v>13.35</v>
       </c>
       <c r="AE11">
-        <v>14.84</v>
+        <v>14.86</v>
       </c>
       <c r="AF11">
-        <v>17.940000000000001</v>
+        <v>17.96</v>
       </c>
       <c r="AG11">
-        <v>33.799999999999997</v>
+        <v>33.78</v>
       </c>
       <c r="AH11">
-        <v>53.22</v>
+        <v>53.23</v>
       </c>
       <c r="AI11">
-        <v>95.51</v>
+        <v>95.54</v>
       </c>
       <c r="AJ11">
-        <v>145.51</v>
+        <v>145.6</v>
       </c>
       <c r="AK11">
-        <v>163.09</v>
+        <v>163.16999999999999</v>
       </c>
       <c r="AL11">
-        <v>163.81</v>
+        <v>163.79</v>
       </c>
       <c r="AM11">
-        <v>161.26</v>
+        <v>161.29</v>
       </c>
       <c r="AN11">
-        <v>153.75</v>
+        <v>154.06</v>
       </c>
       <c r="AO11">
-        <v>156.97999999999999</v>
+        <v>157.04</v>
       </c>
       <c r="AP11">
-        <v>196.89</v>
+        <v>197.13</v>
       </c>
       <c r="AQ11">
-        <v>221.39</v>
+        <v>221.84</v>
       </c>
       <c r="AR11">
-        <v>177.56</v>
+        <v>177.97</v>
       </c>
       <c r="AS11">
-        <v>155.27000000000001</v>
+        <v>156.05000000000001</v>
       </c>
       <c r="AT11">
-        <v>177</v>
+        <v>179.32</v>
+      </c>
+      <c r="AU11">
+        <v>144.29</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -5618,7 +5717,7 @@
         <v>1.9</v>
       </c>
       <c r="C12">
-        <v>14.13</v>
+        <v>14.07</v>
       </c>
       <c r="D12">
         <v>39.770000000000003</v>
@@ -5627,10 +5726,10 @@
         <v>55.45</v>
       </c>
       <c r="F12">
-        <v>51.58</v>
+        <v>51.62</v>
       </c>
       <c r="G12">
-        <v>36.39</v>
+        <v>36.409999999999997</v>
       </c>
       <c r="H12">
         <v>22.26</v>
@@ -5642,7 +5741,7 @@
         <v>8.8699999999999992</v>
       </c>
       <c r="K12">
-        <v>8.48</v>
+        <v>8.5</v>
       </c>
       <c r="L12">
         <v>6.26</v>
@@ -5660,7 +5759,7 @@
         <v>2.73</v>
       </c>
       <c r="Q12">
-        <v>7.17</v>
+        <v>7.15</v>
       </c>
       <c r="R12">
         <v>5.25</v>
@@ -5687,13 +5786,13 @@
         <v>10.88</v>
       </c>
       <c r="Z12">
-        <v>13.12</v>
+        <v>13.14</v>
       </c>
       <c r="AA12">
-        <v>11.47</v>
+        <v>11.45</v>
       </c>
       <c r="AB12">
-        <v>11.62</v>
+        <v>11.66</v>
       </c>
       <c r="AC12">
         <v>13.18</v>
@@ -5708,49 +5807,52 @@
         <v>22.72</v>
       </c>
       <c r="AG12">
-        <v>38.590000000000003</v>
+        <v>38.65</v>
       </c>
       <c r="AH12">
-        <v>59.26</v>
+        <v>59.3</v>
       </c>
       <c r="AI12">
-        <v>110.06</v>
+        <v>110.08</v>
       </c>
       <c r="AJ12">
-        <v>158.87</v>
+        <v>158.93</v>
       </c>
       <c r="AK12">
-        <v>179.58</v>
+        <v>179.6</v>
       </c>
       <c r="AL12">
-        <v>175.98</v>
+        <v>176.04</v>
       </c>
       <c r="AM12">
-        <v>183.26</v>
+        <v>183.28</v>
       </c>
       <c r="AN12">
-        <v>171.41</v>
+        <v>171.69</v>
       </c>
       <c r="AO12">
-        <v>174.99</v>
+        <v>175.07</v>
       </c>
       <c r="AP12">
-        <v>209.83</v>
+        <v>209.85</v>
       </c>
       <c r="AQ12">
-        <v>234.8</v>
+        <v>235.31</v>
       </c>
       <c r="AR12">
-        <v>183.18</v>
+        <v>183.79</v>
       </c>
       <c r="AS12">
-        <v>161.30000000000001</v>
+        <v>161.57</v>
       </c>
       <c r="AT12">
-        <v>182.05</v>
+        <v>184.47</v>
+      </c>
+      <c r="AU12">
+        <v>150.34</v>
       </c>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -5758,10 +5860,10 @@
         <v>1.75</v>
       </c>
       <c r="C13">
-        <v>11.63</v>
+        <v>11.61</v>
       </c>
       <c r="D13">
-        <v>36.729999999999997</v>
+        <v>36.75</v>
       </c>
       <c r="E13">
         <v>47.46</v>
@@ -5785,7 +5887,7 @@
         <v>8.25</v>
       </c>
       <c r="L13">
-        <v>7.21</v>
+        <v>7.27</v>
       </c>
       <c r="M13">
         <v>4.91</v>
@@ -5794,13 +5896,13 @@
         <v>4.34</v>
       </c>
       <c r="O13">
-        <v>3.54</v>
+        <v>3.56</v>
       </c>
       <c r="P13">
         <v>3.22</v>
       </c>
       <c r="Q13">
-        <v>9.2899999999999991</v>
+        <v>9.27</v>
       </c>
       <c r="R13">
         <v>5.54</v>
@@ -5818,79 +5920,82 @@
         <v>6.56</v>
       </c>
       <c r="W13">
-        <v>8.7200000000000006</v>
+        <v>8.74</v>
       </c>
       <c r="X13">
         <v>9.94</v>
       </c>
       <c r="Y13">
-        <v>13.06</v>
+        <v>13.08</v>
       </c>
       <c r="Z13">
         <v>14.59</v>
       </c>
       <c r="AA13">
-        <v>13.44</v>
+        <v>13.46</v>
       </c>
       <c r="AB13">
         <v>13.2</v>
       </c>
       <c r="AC13">
-        <v>13.99</v>
+        <v>14.02</v>
       </c>
       <c r="AD13">
-        <v>17.13</v>
+        <v>17.170000000000002</v>
       </c>
       <c r="AE13">
-        <v>17.54</v>
+        <v>17.52</v>
       </c>
       <c r="AF13">
-        <v>21.31</v>
+        <v>21.33</v>
       </c>
       <c r="AG13">
         <v>38.07</v>
       </c>
       <c r="AH13">
-        <v>59.24</v>
+        <v>59.22</v>
       </c>
       <c r="AI13">
-        <v>107.94</v>
+        <v>107.96</v>
       </c>
       <c r="AJ13">
-        <v>160.03</v>
+        <v>160.22</v>
       </c>
       <c r="AK13">
-        <v>180.46</v>
+        <v>180.52</v>
       </c>
       <c r="AL13">
-        <v>182.85</v>
+        <v>182.89</v>
       </c>
       <c r="AM13">
-        <v>188</v>
+        <v>188.04</v>
       </c>
       <c r="AN13">
-        <v>178.79</v>
+        <v>179.1</v>
       </c>
       <c r="AO13">
-        <v>179.34</v>
+        <v>179.63</v>
       </c>
       <c r="AP13">
-        <v>221.31</v>
+        <v>221.53</v>
       </c>
       <c r="AQ13">
-        <v>243.04</v>
+        <v>243.78</v>
       </c>
       <c r="AR13">
-        <v>192.71</v>
+        <v>193.11</v>
       </c>
       <c r="AS13">
-        <v>162.54</v>
+        <v>163.47</v>
       </c>
       <c r="AT13">
-        <v>190.93</v>
+        <v>192.95</v>
+      </c>
+      <c r="AU13">
+        <v>152.37</v>
       </c>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -5898,19 +6003,19 @@
         <v>1.25</v>
       </c>
       <c r="C14">
-        <v>10.34</v>
+        <v>10.36</v>
       </c>
       <c r="D14">
-        <v>33.159999999999997</v>
+        <v>33.18</v>
       </c>
       <c r="E14">
-        <v>45.13</v>
+        <v>45.11</v>
       </c>
       <c r="F14">
         <v>41.69</v>
       </c>
       <c r="G14">
-        <v>31.25</v>
+        <v>31.23</v>
       </c>
       <c r="H14">
         <v>18.600000000000001</v>
@@ -5922,10 +6027,10 @@
         <v>8.77</v>
       </c>
       <c r="K14">
-        <v>7.96</v>
+        <v>7.98</v>
       </c>
       <c r="L14">
-        <v>6.62</v>
+        <v>6.66</v>
       </c>
       <c r="M14">
         <v>5.2</v>
@@ -5940,13 +6045,13 @@
         <v>3.69</v>
       </c>
       <c r="Q14">
-        <v>7.28</v>
+        <v>7.26</v>
       </c>
       <c r="R14">
-        <v>5.69</v>
+        <v>5.65</v>
       </c>
       <c r="S14">
-        <v>4.2699999999999996</v>
+        <v>4.29</v>
       </c>
       <c r="T14">
         <v>3.89</v>
@@ -5967,70 +6072,73 @@
         <v>12.19</v>
       </c>
       <c r="Z14">
-        <v>14.39</v>
+        <v>14.41</v>
       </c>
       <c r="AA14">
         <v>13.52</v>
       </c>
       <c r="AB14">
-        <v>12.25</v>
+        <v>12.27</v>
       </c>
       <c r="AC14">
-        <v>13.18</v>
+        <v>13.2</v>
       </c>
       <c r="AD14">
         <v>17.03</v>
       </c>
       <c r="AE14">
-        <v>19.02</v>
+        <v>19.04</v>
       </c>
       <c r="AF14">
-        <v>21.76</v>
+        <v>21.78</v>
       </c>
       <c r="AG14">
         <v>34.520000000000003</v>
       </c>
       <c r="AH14">
-        <v>58.7</v>
+        <v>58.74</v>
       </c>
       <c r="AI14">
-        <v>101.85</v>
+        <v>101.87</v>
       </c>
       <c r="AJ14">
-        <v>152.74</v>
+        <v>152.93</v>
       </c>
       <c r="AK14">
-        <v>169.25</v>
+        <v>169.29</v>
       </c>
       <c r="AL14">
-        <v>173.58</v>
+        <v>173.56</v>
       </c>
       <c r="AM14">
-        <v>173.75</v>
+        <v>173.86</v>
       </c>
       <c r="AN14">
-        <v>164.62</v>
+        <v>164.9</v>
       </c>
       <c r="AO14">
-        <v>172.56</v>
+        <v>172.8</v>
       </c>
       <c r="AP14">
-        <v>207.18</v>
+        <v>207.4</v>
       </c>
       <c r="AQ14">
-        <v>230</v>
+        <v>230.41</v>
       </c>
       <c r="AR14">
-        <v>178.8</v>
+        <v>179.21</v>
       </c>
       <c r="AS14">
-        <v>152.19999999999999</v>
+        <v>152.78</v>
       </c>
       <c r="AT14">
-        <v>188.29</v>
+        <v>190.24</v>
+      </c>
+      <c r="AU14">
+        <v>149.83000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -6038,10 +6146,10 @@
         <v>1.26</v>
       </c>
       <c r="C15">
-        <v>9.7200000000000006</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="D15">
-        <v>37.299999999999997</v>
+        <v>37.28</v>
       </c>
       <c r="E15">
         <v>48.04</v>
@@ -6050,7 +6158,7 @@
         <v>44.02</v>
       </c>
       <c r="G15">
-        <v>31.82</v>
+        <v>31.84</v>
       </c>
       <c r="H15">
         <v>21.89</v>
@@ -6065,7 +6173,7 @@
         <v>8.8800000000000008</v>
       </c>
       <c r="L15">
-        <v>7.17</v>
+        <v>7.15</v>
       </c>
       <c r="M15">
         <v>5.88</v>
@@ -6089,7 +6197,7 @@
         <v>4.7300000000000004</v>
       </c>
       <c r="T15">
-        <v>4.7300000000000004</v>
+        <v>4.71</v>
       </c>
       <c r="U15">
         <v>5.4</v>
@@ -6107,70 +6215,73 @@
         <v>12.74</v>
       </c>
       <c r="Z15">
-        <v>17.21</v>
+        <v>17.23</v>
       </c>
       <c r="AA15">
-        <v>15.56</v>
+        <v>15.54</v>
       </c>
       <c r="AB15">
-        <v>17.07</v>
+        <v>17.05</v>
       </c>
       <c r="AC15">
-        <v>17.09</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="AD15">
         <v>21.93</v>
       </c>
       <c r="AE15">
-        <v>23.71</v>
+        <v>23.69</v>
       </c>
       <c r="AF15">
-        <v>27.71</v>
+        <v>27.73</v>
       </c>
       <c r="AG15">
-        <v>43.05</v>
+        <v>43.03</v>
       </c>
       <c r="AH15">
-        <v>70.290000000000006</v>
+        <v>70.31</v>
       </c>
       <c r="AI15">
-        <v>122.11</v>
+        <v>122.13</v>
       </c>
       <c r="AJ15">
-        <v>174.12</v>
+        <v>174.21</v>
       </c>
       <c r="AK15">
-        <v>190.51</v>
+        <v>190.6</v>
       </c>
       <c r="AL15">
-        <v>190.62</v>
+        <v>190.73</v>
       </c>
       <c r="AM15">
         <v>183.78</v>
       </c>
       <c r="AN15">
-        <v>170.13</v>
+        <v>170.5</v>
       </c>
       <c r="AO15">
-        <v>171.92</v>
+        <v>172.08</v>
       </c>
       <c r="AP15">
-        <v>209.16</v>
+        <v>209.42</v>
       </c>
       <c r="AQ15">
-        <v>235.77</v>
+        <v>236.22</v>
       </c>
       <c r="AR15">
-        <v>182.12</v>
+        <v>182.61</v>
       </c>
       <c r="AS15">
-        <v>166.29</v>
+        <v>166.84</v>
       </c>
       <c r="AT15">
-        <v>207.73</v>
+        <v>209.67</v>
+      </c>
+      <c r="AU15">
+        <v>163.33000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -6181,7 +6292,7 @@
         <v>10.78</v>
       </c>
       <c r="D16">
-        <v>39.49</v>
+        <v>39.51</v>
       </c>
       <c r="E16">
         <v>53.07</v>
@@ -6196,16 +6307,16 @@
         <v>25.56</v>
       </c>
       <c r="I16">
-        <v>19.63</v>
+        <v>19.670000000000002</v>
       </c>
       <c r="J16">
         <v>13.4</v>
       </c>
       <c r="K16">
-        <v>10.210000000000001</v>
+        <v>10.23</v>
       </c>
       <c r="L16">
-        <v>7.65</v>
+        <v>7.69</v>
       </c>
       <c r="M16">
         <v>6.9</v>
@@ -6244,73 +6355,76 @@
         <v>11.98</v>
       </c>
       <c r="Y16">
-        <v>16.510000000000002</v>
+        <v>16.53</v>
       </c>
       <c r="Z16">
-        <v>23.57</v>
+        <v>23.55</v>
       </c>
       <c r="AA16">
-        <v>24.06</v>
+        <v>24.1</v>
       </c>
       <c r="AB16">
-        <v>22.84</v>
+        <v>22.86</v>
       </c>
       <c r="AC16">
-        <v>24.3</v>
+        <v>24.28</v>
       </c>
       <c r="AD16">
-        <v>29.19</v>
+        <v>29.21</v>
       </c>
       <c r="AE16">
-        <v>28.32</v>
+        <v>28.34</v>
       </c>
       <c r="AF16">
-        <v>34.39</v>
+        <v>34.409999999999997</v>
       </c>
       <c r="AG16">
-        <v>53.01</v>
+        <v>53.05</v>
       </c>
       <c r="AH16">
-        <v>88.25</v>
+        <v>88.27</v>
       </c>
       <c r="AI16">
-        <v>143.97999999999999</v>
+        <v>144.03</v>
       </c>
       <c r="AJ16">
-        <v>203.37</v>
+        <v>203.47</v>
       </c>
       <c r="AK16">
-        <v>219.69</v>
+        <v>219.73</v>
       </c>
       <c r="AL16">
-        <v>210.6</v>
+        <v>210.74</v>
       </c>
       <c r="AM16">
-        <v>195.86</v>
+        <v>195.92</v>
       </c>
       <c r="AN16">
-        <v>177</v>
+        <v>177.26</v>
       </c>
       <c r="AO16">
-        <v>179.6</v>
+        <v>179.94</v>
       </c>
       <c r="AP16">
-        <v>212.24</v>
+        <v>212.46</v>
       </c>
       <c r="AQ16">
-        <v>237.96</v>
+        <v>238.23</v>
       </c>
       <c r="AR16">
-        <v>185.18</v>
+        <v>185.16</v>
       </c>
       <c r="AS16">
-        <v>165.51</v>
+        <v>166.07</v>
       </c>
       <c r="AT16">
-        <v>209.64</v>
+        <v>212.02</v>
+      </c>
+      <c r="AU16">
+        <v>167.01</v>
       </c>
     </row>
-    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -6318,16 +6432,16 @@
         <v>1.52</v>
       </c>
       <c r="C17">
-        <v>7.01</v>
+        <v>7.05</v>
       </c>
       <c r="D17">
         <v>31.4</v>
       </c>
       <c r="E17">
-        <v>49.32</v>
+        <v>49.34</v>
       </c>
       <c r="F17">
-        <v>48.67</v>
+        <v>48.72</v>
       </c>
       <c r="G17">
         <v>37.58</v>
@@ -6336,7 +6450,7 @@
         <v>26.76</v>
       </c>
       <c r="I17">
-        <v>20.9</v>
+        <v>20.87</v>
       </c>
       <c r="J17">
         <v>12.91</v>
@@ -6345,7 +6459,7 @@
         <v>11.02</v>
       </c>
       <c r="L17">
-        <v>8.98</v>
+        <v>9.0299999999999994</v>
       </c>
       <c r="M17">
         <v>6.81</v>
@@ -6357,13 +6471,13 @@
         <v>4.97</v>
       </c>
       <c r="P17">
-        <v>5.38</v>
+        <v>5.4</v>
       </c>
       <c r="Q17">
-        <v>8.18</v>
+        <v>8.16</v>
       </c>
       <c r="R17">
-        <v>5.66</v>
+        <v>5.64</v>
       </c>
       <c r="S17">
         <v>5.6</v>
@@ -6375,7 +6489,7 @@
         <v>6.55</v>
       </c>
       <c r="V17">
-        <v>8.18</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="W17">
         <v>11.31</v>
@@ -6387,22 +6501,22 @@
         <v>25.3</v>
       </c>
       <c r="Z17">
-        <v>33.61</v>
+        <v>33.630000000000003</v>
       </c>
       <c r="AA17">
-        <v>28.77</v>
+        <v>28.8</v>
       </c>
       <c r="AB17">
-        <v>27.08</v>
+        <v>27.1</v>
       </c>
       <c r="AC17">
         <v>28.01</v>
       </c>
       <c r="AD17">
-        <v>32.9</v>
+        <v>32.96</v>
       </c>
       <c r="AE17">
-        <v>34.35</v>
+        <v>34.39</v>
       </c>
       <c r="AF17">
         <v>37.65</v>
@@ -6411,46 +6525,49 @@
         <v>60.58</v>
       </c>
       <c r="AH17">
-        <v>94.93</v>
+        <v>95.04</v>
       </c>
       <c r="AI17">
-        <v>163.69999999999999</v>
+        <v>163.85</v>
       </c>
       <c r="AJ17">
-        <v>226.28</v>
+        <v>226.32</v>
       </c>
       <c r="AK17">
-        <v>254.73</v>
+        <v>254.86</v>
       </c>
       <c r="AL17">
-        <v>239.39</v>
+        <v>239.67</v>
       </c>
       <c r="AM17">
-        <v>221.81</v>
+        <v>221.92</v>
       </c>
       <c r="AN17">
-        <v>193.84</v>
+        <v>194.21</v>
       </c>
       <c r="AO17">
-        <v>199.31</v>
+        <v>199.35</v>
       </c>
       <c r="AP17">
-        <v>233.53</v>
+        <v>233.85</v>
       </c>
       <c r="AQ17">
-        <v>262.17</v>
+        <v>262.67</v>
       </c>
       <c r="AR17">
-        <v>196.05</v>
+        <v>196.31</v>
       </c>
       <c r="AS17">
-        <v>186.03</v>
+        <v>186.44</v>
       </c>
       <c r="AT17">
-        <v>233.55</v>
+        <v>235.83</v>
+      </c>
+      <c r="AU17">
+        <v>183.12</v>
       </c>
     </row>
-    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -6458,7 +6575,7 @@
         <v>1.07</v>
       </c>
       <c r="C18">
-        <v>4.62</v>
+        <v>4.59</v>
       </c>
       <c r="D18">
         <v>13.73</v>
@@ -6470,7 +6587,7 @@
         <v>27.42</v>
       </c>
       <c r="G18">
-        <v>21.78</v>
+        <v>21.76</v>
       </c>
       <c r="H18">
         <v>14.52</v>
@@ -6479,7 +6596,7 @@
         <v>10.23</v>
       </c>
       <c r="J18">
-        <v>6.7</v>
+        <v>6.73</v>
       </c>
       <c r="K18">
         <v>6.55</v>
@@ -6500,7 +6617,7 @@
         <v>2.82</v>
       </c>
       <c r="Q18">
-        <v>6.17</v>
+        <v>6.14</v>
       </c>
       <c r="R18">
         <v>4.29</v>
@@ -6527,70 +6644,73 @@
         <v>18.84</v>
       </c>
       <c r="Z18">
-        <v>22.36</v>
+        <v>22.39</v>
       </c>
       <c r="AA18">
-        <v>21.1</v>
+        <v>21.12</v>
       </c>
       <c r="AB18">
-        <v>19.5</v>
+        <v>19.52</v>
       </c>
       <c r="AC18">
-        <v>21.12</v>
+        <v>21.15</v>
       </c>
       <c r="AD18">
         <v>26.25</v>
       </c>
       <c r="AE18">
-        <v>26.55</v>
+        <v>26.63</v>
       </c>
       <c r="AF18">
-        <v>33.74</v>
+        <v>33.79</v>
       </c>
       <c r="AG18">
-        <v>52.65</v>
+        <v>52.73</v>
       </c>
       <c r="AH18">
-        <v>75.27</v>
+        <v>75.34</v>
       </c>
       <c r="AI18">
-        <v>123.07</v>
+        <v>123.15</v>
       </c>
       <c r="AJ18">
-        <v>182.45</v>
+        <v>182.42</v>
       </c>
       <c r="AK18">
-        <v>213.39</v>
+        <v>213.49</v>
       </c>
       <c r="AL18">
-        <v>220.63</v>
+        <v>220.83</v>
       </c>
       <c r="AM18">
-        <v>208.06</v>
+        <v>208.24</v>
       </c>
       <c r="AN18">
-        <v>189.15</v>
+        <v>189.48</v>
       </c>
       <c r="AO18">
-        <v>195.8</v>
+        <v>195.93</v>
       </c>
       <c r="AP18">
-        <v>223.75</v>
+        <v>223.98</v>
       </c>
       <c r="AQ18">
-        <v>214.28</v>
+        <v>214.66</v>
       </c>
       <c r="AR18">
-        <v>148.02000000000001</v>
+        <v>148.35</v>
       </c>
       <c r="AS18">
-        <v>125.25</v>
+        <v>125.89</v>
       </c>
       <c r="AT18">
-        <v>158.84</v>
+        <v>160.69</v>
+      </c>
+      <c r="AU18">
+        <v>136.07</v>
       </c>
     </row>
-    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>68</v>
       </c>
@@ -6664,13 +6784,13 @@
         <v>9.83</v>
       </c>
       <c r="Y19">
-        <v>14.72</v>
+        <v>14.75</v>
       </c>
       <c r="Z19">
-        <v>15.53</v>
+        <v>15.56</v>
       </c>
       <c r="AA19">
-        <v>13.07</v>
+        <v>13.04</v>
       </c>
       <c r="AB19">
         <v>11.61</v>
@@ -6679,7 +6799,7 @@
         <v>13.45</v>
       </c>
       <c r="AD19">
-        <v>13.96</v>
+        <v>14.02</v>
       </c>
       <c r="AE19">
         <v>15.85</v>
@@ -6688,49 +6808,52 @@
         <v>19.170000000000002</v>
       </c>
       <c r="AG19">
-        <v>30.79</v>
+        <v>30.84</v>
       </c>
       <c r="AH19">
         <v>44.64</v>
       </c>
       <c r="AI19">
-        <v>74.099999999999994</v>
+        <v>74.13</v>
       </c>
       <c r="AJ19">
-        <v>110.18</v>
+        <v>110.24</v>
       </c>
       <c r="AK19">
-        <v>128.87</v>
+        <v>128.94999999999999</v>
       </c>
       <c r="AL19">
-        <v>144.18</v>
+        <v>144.26</v>
       </c>
       <c r="AM19">
-        <v>143.05000000000001</v>
+        <v>143.27000000000001</v>
       </c>
       <c r="AN19">
-        <v>139.72999999999999</v>
+        <v>139.91999999999999</v>
       </c>
       <c r="AO19">
         <v>139.16</v>
       </c>
       <c r="AP19">
-        <v>152.93</v>
+        <v>153.19999999999999</v>
       </c>
       <c r="AQ19">
-        <v>141.62</v>
+        <v>141.86000000000001</v>
       </c>
       <c r="AR19">
-        <v>90.71</v>
+        <v>90.9</v>
       </c>
       <c r="AS19">
-        <v>71.03</v>
+        <v>71.13</v>
       </c>
       <c r="AT19">
-        <v>87.55</v>
+        <v>88.88</v>
+      </c>
+      <c r="AU19">
+        <v>72.67</v>
       </c>
     </row>
-    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>67</v>
       </c>
@@ -6759,7 +6882,7 @@
         <v>4.1100000000000003</v>
       </c>
       <c r="J20">
-        <v>3.19</v>
+        <v>3.22</v>
       </c>
       <c r="K20">
         <v>2.82</v>
@@ -6774,7 +6897,7 @@
         <v>3.03</v>
       </c>
       <c r="O20">
-        <v>2.68</v>
+        <v>2.66</v>
       </c>
       <c r="P20">
         <v>3.3</v>
@@ -6783,7 +6906,7 @@
         <v>4.72</v>
       </c>
       <c r="R20">
-        <v>3.76</v>
+        <v>3.73</v>
       </c>
       <c r="S20">
         <v>3.33</v>
@@ -6822,10 +6945,10 @@
         <v>9.5</v>
       </c>
       <c r="AE20">
-        <v>10.41</v>
+        <v>10.44</v>
       </c>
       <c r="AF20">
-        <v>11.54</v>
+        <v>11.56</v>
       </c>
       <c r="AG20">
         <v>16.8</v>
@@ -6834,43 +6957,46 @@
         <v>26.05</v>
       </c>
       <c r="AI20">
-        <v>49.21</v>
+        <v>49.18</v>
       </c>
       <c r="AJ20">
         <v>74.86</v>
       </c>
       <c r="AK20">
-        <v>90.18</v>
+        <v>90.15</v>
       </c>
       <c r="AL20">
-        <v>97.13</v>
+        <v>97.02</v>
       </c>
       <c r="AM20">
-        <v>104.96</v>
+        <v>105.05</v>
       </c>
       <c r="AN20">
-        <v>102.12</v>
+        <v>102.31</v>
       </c>
       <c r="AO20">
-        <v>98.44</v>
+        <v>98.58</v>
       </c>
       <c r="AP20">
         <v>113.82</v>
       </c>
       <c r="AQ20">
-        <v>115</v>
+        <v>115.11</v>
       </c>
       <c r="AR20">
-        <v>80.28</v>
+        <v>80.44</v>
       </c>
       <c r="AS20">
-        <v>51.65</v>
+        <v>51.81</v>
       </c>
       <c r="AT20">
-        <v>63.19</v>
+        <v>63.64</v>
+      </c>
+      <c r="AU20">
+        <v>58.41</v>
       </c>
     </row>
-    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -6884,7 +7010,7 @@
         <v>3.61</v>
       </c>
       <c r="E21">
-        <v>6.46</v>
+        <v>6.44</v>
       </c>
       <c r="F21">
         <v>6.89</v>
@@ -6917,7 +7043,7 @@
         <v>2.73</v>
       </c>
       <c r="P21">
-        <v>2.8</v>
+        <v>2.78</v>
       </c>
       <c r="Q21">
         <v>4.04</v>
@@ -6929,7 +7055,7 @@
         <v>3.56</v>
       </c>
       <c r="T21">
-        <v>3.69</v>
+        <v>3.71</v>
       </c>
       <c r="U21">
         <v>3.53</v>
@@ -6947,7 +7073,7 @@
         <v>6.97</v>
       </c>
       <c r="Z21">
-        <v>7.19</v>
+        <v>7.17</v>
       </c>
       <c r="AA21">
         <v>5.63</v>
@@ -6956,25 +7082,25 @@
         <v>5.78</v>
       </c>
       <c r="AC21">
-        <v>5.78</v>
+        <v>5.76</v>
       </c>
       <c r="AD21">
         <v>7.32</v>
       </c>
       <c r="AE21">
-        <v>7.65</v>
+        <v>7.62</v>
       </c>
       <c r="AF21">
         <v>8.18</v>
       </c>
       <c r="AG21">
-        <v>13.25</v>
+        <v>13.2</v>
       </c>
       <c r="AH21">
         <v>22.37</v>
       </c>
       <c r="AI21">
-        <v>37.01</v>
+        <v>36.93</v>
       </c>
       <c r="AJ21">
         <v>56.75</v>
@@ -6983,31 +7109,34 @@
         <v>61.14</v>
       </c>
       <c r="AL21">
-        <v>61.24</v>
+        <v>61.27</v>
       </c>
       <c r="AM21">
-        <v>60.16</v>
+        <v>60.11</v>
       </c>
       <c r="AN21">
         <v>58.97</v>
       </c>
       <c r="AO21">
-        <v>58.44</v>
+        <v>58.54</v>
       </c>
       <c r="AP21">
-        <v>68.03</v>
+        <v>67.959999999999994</v>
       </c>
       <c r="AQ21">
-        <v>78.63</v>
+        <v>78.680000000000007</v>
       </c>
       <c r="AR21">
-        <v>53.47</v>
+        <v>53.44</v>
       </c>
       <c r="AS21">
-        <v>38.700000000000003</v>
+        <v>38.67</v>
       </c>
       <c r="AT21">
-        <v>47.91</v>
+        <v>48.42</v>
+      </c>
+      <c r="AU21">
+        <v>46.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add RKI data downloaded 2021-01-28--13-35-01
</commit_message>
<xml_diff>
--- a/rki-data/RKI-Altersverteilung.xlsx
+++ b/rki-data/RKI-Altersverteilung.xlsx
@@ -2,22 +2,27 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20368"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466FD17F-3693-4F80-A8DF-2030B8362E82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Wissdaten\RKI_nCoV-Lage\3.Kommunikation\3.7.Lageberichte\2021-01-26\Tabellen für webmaster\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B58E7572-CD29-42BB-9F60-E1B609845612}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14028" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Erläuterungen" sheetId="3" r:id="rId1"/>
-    <sheet name="Fallzahlen" sheetId="5" r:id="rId2"/>
-    <sheet name="Inzidenz" sheetId="6" r:id="rId3"/>
+    <sheet name="Fallzahlen" sheetId="7" r:id="rId2"/>
+    <sheet name="Inzidenzen" sheetId="8" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="71">
   <si>
     <t>Altersgruppe</t>
   </si>
@@ -228,6 +233,9 @@
   </si>
   <si>
     <t>2021_2</t>
+  </si>
+  <si>
+    <t>2021_3</t>
   </si>
 </sst>
 </file>
@@ -1074,50 +1082,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E2FB09-40BA-467A-9A47-7CEA9C443D24}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.42578125" customWidth="1"/>
+    <col min="1" max="1" width="48.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1BE48B6-9747-4017-83E5-E7E92A9C8328}">
-  <dimension ref="A1:AU21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72991CAA-386D-459B-B35F-6BD6022CE7C5}">
+  <dimension ref="A1:AV21"/>
   <sheetViews>
-    <sheetView topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="AU2" sqref="AU2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AJ16" sqref="AJ16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1259,49 +1266,52 @@
       <c r="AU1" t="s">
         <v>69</v>
       </c>
+      <c r="AV1" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="C2">
-        <v>6434</v>
+        <v>6433</v>
       </c>
       <c r="D2">
-        <v>22434</v>
+        <v>22439</v>
       </c>
       <c r="E2">
-        <v>34029</v>
+        <v>34026</v>
       </c>
       <c r="F2">
-        <v>36101</v>
+        <v>36099</v>
       </c>
       <c r="G2">
-        <v>27181</v>
+        <v>27185</v>
       </c>
       <c r="H2">
-        <v>17370</v>
+        <v>17371</v>
       </c>
       <c r="I2">
-        <v>12382</v>
+        <v>12380</v>
       </c>
       <c r="J2">
-        <v>7445</v>
+        <v>7447</v>
       </c>
       <c r="K2">
         <v>6235</v>
       </c>
       <c r="L2">
-        <v>4755</v>
+        <v>4756</v>
       </c>
       <c r="M2">
-        <v>3618</v>
+        <v>3620</v>
       </c>
       <c r="N2">
-        <v>3212</v>
+        <v>3210</v>
       </c>
       <c r="O2">
         <v>2360</v>
@@ -1310,100 +1320,103 @@
         <v>2345</v>
       </c>
       <c r="Q2">
-        <v>4135</v>
+        <v>4131</v>
       </c>
       <c r="R2">
-        <v>3214</v>
+        <v>3212</v>
       </c>
       <c r="S2">
-        <v>2697</v>
+        <v>2695</v>
       </c>
       <c r="T2">
         <v>2428</v>
       </c>
       <c r="U2">
-        <v>3024</v>
+        <v>3026</v>
       </c>
       <c r="V2">
-        <v>3943</v>
+        <v>3944</v>
       </c>
       <c r="W2">
-        <v>4825</v>
+        <v>4824</v>
       </c>
       <c r="X2">
-        <v>6063</v>
+        <v>6062</v>
       </c>
       <c r="Y2">
-        <v>7960</v>
+        <v>7959</v>
       </c>
       <c r="Z2">
-        <v>9606</v>
+        <v>9604</v>
       </c>
       <c r="AA2">
-        <v>8821</v>
+        <v>8819</v>
       </c>
       <c r="AB2">
-        <v>8624</v>
+        <v>8626</v>
       </c>
       <c r="AC2">
-        <v>9775</v>
+        <v>9774</v>
       </c>
       <c r="AD2">
-        <v>12288</v>
+        <v>12292</v>
       </c>
       <c r="AE2">
-        <v>13076</v>
+        <v>13077</v>
       </c>
       <c r="AF2">
-        <v>15925</v>
+        <v>15926</v>
       </c>
       <c r="AG2">
-        <v>26167</v>
+        <v>26155</v>
       </c>
       <c r="AH2">
-        <v>42086</v>
+        <v>42085</v>
       </c>
       <c r="AI2">
-        <v>74822</v>
+        <v>74845</v>
       </c>
       <c r="AJ2">
-        <v>111156</v>
+        <v>111147</v>
       </c>
       <c r="AK2">
-        <v>125812</v>
+        <v>125795</v>
       </c>
       <c r="AL2">
-        <v>127902</v>
+        <v>127858</v>
       </c>
       <c r="AM2">
-        <v>128533</v>
+        <v>128513</v>
       </c>
       <c r="AN2">
-        <v>123379</v>
+        <v>123363</v>
       </c>
       <c r="AO2">
-        <v>128389</v>
+        <v>128465</v>
       </c>
       <c r="AP2">
-        <v>156276</v>
+        <v>156406</v>
       </c>
       <c r="AQ2">
-        <v>174652</v>
+        <v>174793</v>
       </c>
       <c r="AR2">
-        <v>138815</v>
+        <v>138973</v>
       </c>
       <c r="AS2">
-        <v>122936</v>
+        <v>123143</v>
       </c>
       <c r="AT2">
-        <v>144821</v>
+        <v>145427</v>
       </c>
       <c r="AU2">
-        <v>117939</v>
+        <v>118979</v>
+      </c>
+      <c r="AV2">
+        <v>94934</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1423,7 +1436,7 @@
         <v>1172</v>
       </c>
       <c r="G3">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="H3">
         <v>848</v>
@@ -1474,7 +1487,7 @@
         <v>39</v>
       </c>
       <c r="X3">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Y3">
         <v>25</v>
@@ -1504,49 +1517,52 @@
         <v>187</v>
       </c>
       <c r="AH3">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="AI3">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="AJ3">
         <v>1465</v>
       </c>
       <c r="AK3">
-        <v>1719</v>
+        <v>1720</v>
       </c>
       <c r="AL3">
-        <v>2316</v>
+        <v>2320</v>
       </c>
       <c r="AM3">
-        <v>3069</v>
+        <v>3074</v>
       </c>
       <c r="AN3">
-        <v>3530</v>
+        <v>3522</v>
       </c>
       <c r="AO3">
-        <v>4153</v>
+        <v>4177</v>
       </c>
       <c r="AP3">
-        <v>5410</v>
+        <v>5412</v>
       </c>
       <c r="AQ3">
-        <v>5983</v>
+        <v>5984</v>
       </c>
       <c r="AR3">
-        <v>5257</v>
+        <v>5258</v>
       </c>
       <c r="AS3">
-        <v>4964</v>
+        <v>4975</v>
       </c>
       <c r="AT3">
-        <v>5380</v>
+        <v>5397</v>
       </c>
       <c r="AU3">
-        <v>4968</v>
+        <v>5024</v>
+      </c>
+      <c r="AV3">
+        <v>3912</v>
       </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1557,7 +1573,7 @@
         <v>38</v>
       </c>
       <c r="D4">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E4">
         <v>738</v>
@@ -1575,7 +1591,7 @@
         <v>684</v>
       </c>
       <c r="J4">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="K4">
         <v>263</v>
@@ -1587,7 +1603,7 @@
         <v>127</v>
       </c>
       <c r="N4">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O4">
         <v>51</v>
@@ -1647,49 +1663,52 @@
         <v>305</v>
       </c>
       <c r="AH4">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="AI4">
-        <v>1137</v>
+        <v>1140</v>
       </c>
       <c r="AJ4">
-        <v>1779</v>
+        <v>1780</v>
       </c>
       <c r="AK4">
-        <v>2290</v>
+        <v>2291</v>
       </c>
       <c r="AL4">
-        <v>2830</v>
+        <v>2829</v>
       </c>
       <c r="AM4">
-        <v>3365</v>
+        <v>3370</v>
       </c>
       <c r="AN4">
-        <v>4112</v>
+        <v>4110</v>
       </c>
       <c r="AO4">
-        <v>4580</v>
+        <v>4589</v>
       </c>
       <c r="AP4">
-        <v>5905</v>
+        <v>5911</v>
       </c>
       <c r="AQ4">
-        <v>6923</v>
+        <v>6940</v>
       </c>
       <c r="AR4">
-        <v>5861</v>
+        <v>5859</v>
       </c>
       <c r="AS4">
-        <v>5591</v>
+        <v>5605</v>
       </c>
       <c r="AT4">
-        <v>6046</v>
+        <v>6076</v>
       </c>
       <c r="AU4">
-        <v>5486</v>
+        <v>5559</v>
+      </c>
+      <c r="AV4">
+        <v>4424</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1697,13 +1716,13 @@
         <v>12</v>
       </c>
       <c r="C5">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D5">
         <v>468</v>
       </c>
       <c r="E5">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="F5">
         <v>1964</v>
@@ -1718,13 +1737,13 @@
         <v>824</v>
       </c>
       <c r="J5">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="K5">
         <v>300</v>
       </c>
       <c r="L5">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="M5">
         <v>152</v>
@@ -1736,7 +1755,7 @@
         <v>76</v>
       </c>
       <c r="P5">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q5">
         <v>62</v>
@@ -1787,52 +1806,55 @@
         <v>316</v>
       </c>
       <c r="AG5">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="AH5">
-        <v>856</v>
+        <v>858</v>
       </c>
       <c r="AI5">
-        <v>1833</v>
+        <v>1835</v>
       </c>
       <c r="AJ5">
-        <v>2841</v>
+        <v>2842</v>
       </c>
       <c r="AK5">
-        <v>3433</v>
+        <v>3436</v>
       </c>
       <c r="AL5">
         <v>3798</v>
       </c>
       <c r="AM5">
-        <v>4364</v>
+        <v>4367</v>
       </c>
       <c r="AN5">
-        <v>4799</v>
+        <v>4796</v>
       </c>
       <c r="AO5">
-        <v>5425</v>
+        <v>5441</v>
       </c>
       <c r="AP5">
-        <v>7056</v>
+        <v>7070</v>
       </c>
       <c r="AQ5">
-        <v>8262</v>
+        <v>8268</v>
       </c>
       <c r="AR5">
-        <v>7432</v>
+        <v>7443</v>
       </c>
       <c r="AS5">
-        <v>6848</v>
+        <v>6872</v>
       </c>
       <c r="AT5">
-        <v>7644</v>
+        <v>7668</v>
       </c>
       <c r="AU5">
-        <v>6587</v>
+        <v>6677</v>
+      </c>
+      <c r="AV5">
+        <v>5310</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1852,7 +1874,7 @@
         <v>1788</v>
       </c>
       <c r="G6">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="H6">
         <v>854</v>
@@ -1861,7 +1883,7 @@
         <v>587</v>
       </c>
       <c r="J6">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="K6">
         <v>274</v>
@@ -1879,7 +1901,7 @@
         <v>58</v>
       </c>
       <c r="P6">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="Q6">
         <v>65</v>
@@ -1927,7 +1949,7 @@
         <v>231</v>
       </c>
       <c r="AF6">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AG6">
         <v>507</v>
@@ -1939,43 +1961,46 @@
         <v>1628</v>
       </c>
       <c r="AJ6">
-        <v>2646</v>
+        <v>2650</v>
       </c>
       <c r="AK6">
-        <v>3049</v>
+        <v>3050</v>
       </c>
       <c r="AL6">
-        <v>3289</v>
+        <v>3285</v>
       </c>
       <c r="AM6">
+        <v>3392</v>
+      </c>
+      <c r="AN6">
+        <v>3495</v>
+      </c>
+      <c r="AO6">
+        <v>3969</v>
+      </c>
+      <c r="AP6">
+        <v>4993</v>
+      </c>
+      <c r="AQ6">
+        <v>5950</v>
+      </c>
+      <c r="AR6">
+        <v>5094</v>
+      </c>
+      <c r="AS6">
+        <v>4637</v>
+      </c>
+      <c r="AT6">
+        <v>5233</v>
+      </c>
+      <c r="AU6">
+        <v>4325</v>
+      </c>
+      <c r="AV6">
         <v>3391</v>
       </c>
-      <c r="AN6">
-        <v>3494</v>
-      </c>
-      <c r="AO6">
-        <v>3962</v>
-      </c>
-      <c r="AP6">
-        <v>4985</v>
-      </c>
-      <c r="AQ6">
-        <v>5958</v>
-      </c>
-      <c r="AR6">
-        <v>5081</v>
-      </c>
-      <c r="AS6">
-        <v>4618</v>
-      </c>
-      <c r="AT6">
-        <v>5213</v>
-      </c>
-      <c r="AU6">
-        <v>4297</v>
-      </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1986,7 +2011,7 @@
         <v>145</v>
       </c>
       <c r="D7">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E7">
         <v>1327</v>
@@ -2010,7 +2035,7 @@
         <v>207</v>
       </c>
       <c r="L7">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M7">
         <v>92</v>
@@ -2061,7 +2086,7 @@
         <v>107</v>
       </c>
       <c r="AC7">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AD7">
         <v>259</v>
@@ -2070,60 +2095,63 @@
         <v>265</v>
       </c>
       <c r="AF7">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AG7">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="AH7">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="AI7">
         <v>1793</v>
       </c>
       <c r="AJ7">
-        <v>2881</v>
+        <v>2882</v>
       </c>
       <c r="AK7">
         <v>3174</v>
       </c>
       <c r="AL7">
-        <v>3291</v>
+        <v>3292</v>
       </c>
       <c r="AM7">
-        <v>3356</v>
+        <v>3359</v>
       </c>
       <c r="AN7">
-        <v>3209</v>
+        <v>3206</v>
       </c>
       <c r="AO7">
-        <v>3477</v>
+        <v>3482</v>
       </c>
       <c r="AP7">
-        <v>4381</v>
+        <v>4390</v>
       </c>
       <c r="AQ7">
-        <v>5164</v>
+        <v>5168</v>
       </c>
       <c r="AR7">
-        <v>4433</v>
+        <v>4436</v>
       </c>
       <c r="AS7">
-        <v>4134</v>
+        <v>4138</v>
       </c>
       <c r="AT7">
-        <v>4801</v>
+        <v>4825</v>
       </c>
       <c r="AU7">
-        <v>3649</v>
+        <v>3661</v>
+      </c>
+      <c r="AV7">
+        <v>3050</v>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8">
         <v>237</v>
@@ -2132,19 +2160,19 @@
         <v>889</v>
       </c>
       <c r="E8">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="F8">
         <v>1693</v>
       </c>
       <c r="G8">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="H8">
         <v>662</v>
       </c>
       <c r="I8">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="J8">
         <v>266</v>
@@ -2153,13 +2181,13 @@
         <v>208</v>
       </c>
       <c r="L8">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M8">
         <v>124</v>
       </c>
       <c r="N8">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O8">
         <v>60</v>
@@ -2216,52 +2244,55 @@
         <v>453</v>
       </c>
       <c r="AG8">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="AH8">
         <v>1285</v>
       </c>
       <c r="AI8">
-        <v>2269</v>
+        <v>2271</v>
       </c>
       <c r="AJ8">
         <v>3552</v>
       </c>
       <c r="AK8">
-        <v>4237</v>
+        <v>4243</v>
       </c>
       <c r="AL8">
-        <v>4016</v>
+        <v>4017</v>
       </c>
       <c r="AM8">
-        <v>4147</v>
+        <v>4146</v>
       </c>
       <c r="AN8">
-        <v>4139</v>
+        <v>4136</v>
       </c>
       <c r="AO8">
-        <v>4125</v>
+        <v>4127</v>
       </c>
       <c r="AP8">
-        <v>5154</v>
+        <v>5164</v>
       </c>
       <c r="AQ8">
-        <v>6324</v>
+        <v>6335</v>
       </c>
       <c r="AR8">
-        <v>5567</v>
+        <v>5581</v>
       </c>
       <c r="AS8">
-        <v>4960</v>
+        <v>4967</v>
       </c>
       <c r="AT8">
-        <v>5684</v>
+        <v>5698</v>
       </c>
       <c r="AU8">
-        <v>4363</v>
+        <v>4413</v>
+      </c>
+      <c r="AV8">
+        <v>3573</v>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2269,19 +2300,19 @@
         <v>62</v>
       </c>
       <c r="C9">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D9">
-        <v>1597</v>
+        <v>1598</v>
       </c>
       <c r="E9">
-        <v>2528</v>
+        <v>2527</v>
       </c>
       <c r="F9">
         <v>2784</v>
       </c>
       <c r="G9">
-        <v>1798</v>
+        <v>1797</v>
       </c>
       <c r="H9">
         <v>1087</v>
@@ -2305,7 +2336,7 @@
         <v>169</v>
       </c>
       <c r="O9">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="P9">
         <v>91</v>
@@ -2329,7 +2360,7 @@
         <v>153</v>
       </c>
       <c r="W9">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="X9">
         <v>204</v>
@@ -2347,13 +2378,13 @@
         <v>247</v>
       </c>
       <c r="AC9">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AD9">
         <v>493</v>
       </c>
       <c r="AE9">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="AF9">
         <v>680</v>
@@ -2362,49 +2393,52 @@
         <v>1271</v>
       </c>
       <c r="AH9">
-        <v>2121</v>
+        <v>2120</v>
       </c>
       <c r="AI9">
-        <v>3953</v>
+        <v>3954</v>
       </c>
       <c r="AJ9">
-        <v>5989</v>
+        <v>5992</v>
       </c>
       <c r="AK9">
-        <v>6846</v>
+        <v>6849</v>
       </c>
       <c r="AL9">
         <v>6902</v>
       </c>
       <c r="AM9">
-        <v>7306</v>
+        <v>7305</v>
       </c>
       <c r="AN9">
-        <v>6994</v>
+        <v>6999</v>
       </c>
       <c r="AO9">
-        <v>7652</v>
+        <v>7655</v>
       </c>
       <c r="AP9">
-        <v>9413</v>
+        <v>9422</v>
       </c>
       <c r="AQ9">
-        <v>10987</v>
+        <v>11005</v>
       </c>
       <c r="AR9">
-        <v>9127</v>
+        <v>9156</v>
       </c>
       <c r="AS9">
-        <v>8241</v>
+        <v>8267</v>
       </c>
       <c r="AT9">
-        <v>9205</v>
+        <v>9255</v>
       </c>
       <c r="AU9">
-        <v>7464</v>
+        <v>7527</v>
+      </c>
+      <c r="AV9">
+        <v>6185</v>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2415,7 +2449,7 @@
         <v>752</v>
       </c>
       <c r="D10">
-        <v>2598</v>
+        <v>2600</v>
       </c>
       <c r="E10">
         <v>3595</v>
@@ -2433,13 +2467,13 @@
         <v>1060</v>
       </c>
       <c r="J10">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="K10">
         <v>510</v>
       </c>
       <c r="L10">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="M10">
         <v>266</v>
@@ -2448,16 +2482,16 @@
         <v>237</v>
       </c>
       <c r="O10">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="P10">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Q10">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="R10">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="S10">
         <v>156</v>
@@ -2493,7 +2527,7 @@
         <v>554</v>
       </c>
       <c r="AD10">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="AE10">
         <v>866</v>
@@ -2508,46 +2542,49 @@
         <v>2998</v>
       </c>
       <c r="AI10">
-        <v>5753</v>
+        <v>5755</v>
       </c>
       <c r="AJ10">
-        <v>8964</v>
+        <v>8961</v>
       </c>
       <c r="AK10">
         <v>10155</v>
       </c>
       <c r="AL10">
-        <v>10304</v>
+        <v>10301</v>
       </c>
       <c r="AM10">
-        <v>10236</v>
+        <v>10237</v>
       </c>
       <c r="AN10">
-        <v>9859</v>
+        <v>9862</v>
       </c>
       <c r="AO10">
-        <v>10341</v>
+        <v>10358</v>
       </c>
       <c r="AP10">
-        <v>13024</v>
+        <v>13045</v>
       </c>
       <c r="AQ10">
-        <v>14962</v>
+        <v>14980</v>
       </c>
       <c r="AR10">
-        <v>12297</v>
+        <v>12319</v>
       </c>
       <c r="AS10">
-        <v>11032</v>
+        <v>11055</v>
       </c>
       <c r="AT10">
-        <v>12222</v>
+        <v>12304</v>
       </c>
       <c r="AU10">
-        <v>9916</v>
+        <v>10020</v>
+      </c>
+      <c r="AV10">
+        <v>8286</v>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2558,10 +2595,10 @@
         <v>980</v>
       </c>
       <c r="D11">
-        <v>3095</v>
+        <v>3094</v>
       </c>
       <c r="E11">
-        <v>4001</v>
+        <v>4000</v>
       </c>
       <c r="F11">
         <v>3700</v>
@@ -2576,16 +2613,16 @@
         <v>991</v>
       </c>
       <c r="J11">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="K11">
         <v>520</v>
       </c>
       <c r="L11">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="M11">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="N11">
         <v>239</v>
@@ -2609,7 +2646,7 @@
         <v>172</v>
       </c>
       <c r="U11">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="V11">
         <v>294</v>
@@ -2624,10 +2661,10 @@
         <v>475</v>
       </c>
       <c r="Z11">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="AA11">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="AB11">
         <v>554</v>
@@ -2648,49 +2685,52 @@
         <v>2267</v>
       </c>
       <c r="AH11">
-        <v>3572</v>
+        <v>3571</v>
       </c>
       <c r="AI11">
-        <v>6411</v>
+        <v>6415</v>
       </c>
       <c r="AJ11">
-        <v>9770</v>
+        <v>9773</v>
       </c>
       <c r="AK11">
-        <v>10949</v>
+        <v>10946</v>
       </c>
       <c r="AL11">
-        <v>10991</v>
+        <v>10987</v>
       </c>
       <c r="AM11">
-        <v>10823</v>
+        <v>10822</v>
       </c>
       <c r="AN11">
-        <v>10338</v>
+        <v>10342</v>
       </c>
       <c r="AO11">
-        <v>10538</v>
+        <v>10548</v>
       </c>
       <c r="AP11">
-        <v>13228</v>
+        <v>13236</v>
       </c>
       <c r="AQ11">
-        <v>14886</v>
+        <v>14902</v>
       </c>
       <c r="AR11">
-        <v>11942</v>
+        <v>11955</v>
       </c>
       <c r="AS11">
-        <v>10471</v>
+        <v>10501</v>
       </c>
       <c r="AT11">
-        <v>12033</v>
+        <v>12085</v>
       </c>
       <c r="AU11">
-        <v>9682</v>
+        <v>9780</v>
+      </c>
+      <c r="AV11">
+        <v>8099</v>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2698,19 +2738,19 @@
         <v>100</v>
       </c>
       <c r="C12">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="D12">
-        <v>2097</v>
+        <v>2098</v>
       </c>
       <c r="E12">
-        <v>2924</v>
+        <v>2923</v>
       </c>
       <c r="F12">
         <v>2722</v>
       </c>
       <c r="G12">
-        <v>1920</v>
+        <v>1921</v>
       </c>
       <c r="H12">
         <v>1174</v>
@@ -2719,7 +2759,7 @@
         <v>788</v>
       </c>
       <c r="J12">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="K12">
         <v>448</v>
@@ -2731,16 +2771,16 @@
         <v>254</v>
       </c>
       <c r="N12">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="O12">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="P12">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="Q12">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="R12">
         <v>277</v>
@@ -2767,10 +2807,10 @@
         <v>574</v>
       </c>
       <c r="Z12">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="AA12">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="AB12">
         <v>615</v>
@@ -2791,49 +2831,52 @@
         <v>2038</v>
       </c>
       <c r="AH12">
-        <v>3127</v>
+        <v>3128</v>
       </c>
       <c r="AI12">
-        <v>5805</v>
+        <v>5809</v>
       </c>
       <c r="AJ12">
-        <v>8381</v>
+        <v>8384</v>
       </c>
       <c r="AK12">
-        <v>9471</v>
+        <v>9466</v>
       </c>
       <c r="AL12">
         <v>9283</v>
       </c>
       <c r="AM12">
-        <v>9665</v>
+        <v>9670</v>
       </c>
       <c r="AN12">
-        <v>9054</v>
+        <v>9059</v>
       </c>
       <c r="AO12">
-        <v>9232</v>
+        <v>9231</v>
       </c>
       <c r="AP12">
-        <v>11066</v>
+        <v>11079</v>
       </c>
       <c r="AQ12">
-        <v>12409</v>
+        <v>12423</v>
       </c>
       <c r="AR12">
-        <v>9692</v>
+        <v>9713</v>
       </c>
       <c r="AS12">
-        <v>8520</v>
+        <v>8537</v>
       </c>
       <c r="AT12">
-        <v>9728</v>
+        <v>9772</v>
       </c>
       <c r="AU12">
-        <v>7928</v>
+        <v>7978</v>
+      </c>
+      <c r="AV12">
+        <v>6411</v>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2841,13 +2884,13 @@
         <v>86</v>
       </c>
       <c r="C13">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D13">
-        <v>1804</v>
+        <v>1805</v>
       </c>
       <c r="E13">
-        <v>2330</v>
+        <v>2331</v>
       </c>
       <c r="F13">
         <v>2310</v>
@@ -2859,10 +2902,10 @@
         <v>1024</v>
       </c>
       <c r="I13">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J13">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="K13">
         <v>405</v>
@@ -2871,7 +2914,7 @@
         <v>357</v>
       </c>
       <c r="M13">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="N13">
         <v>213</v>
@@ -2883,7 +2926,7 @@
         <v>158</v>
       </c>
       <c r="Q13">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="R13">
         <v>272</v>
@@ -2898,7 +2941,7 @@
         <v>253</v>
       </c>
       <c r="V13">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="W13">
         <v>429</v>
@@ -2913,7 +2956,7 @@
         <v>716</v>
       </c>
       <c r="AA13">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="AB13">
         <v>648</v>
@@ -2925,10 +2968,10 @@
         <v>843</v>
       </c>
       <c r="AE13">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="AF13">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="AG13">
         <v>1869</v>
@@ -2937,46 +2980,49 @@
         <v>2907</v>
       </c>
       <c r="AI13">
-        <v>5300</v>
+        <v>5298</v>
       </c>
       <c r="AJ13">
-        <v>7865</v>
+        <v>7869</v>
       </c>
       <c r="AK13">
-        <v>8862</v>
+        <v>8866</v>
       </c>
       <c r="AL13">
-        <v>8978</v>
+        <v>8984</v>
       </c>
       <c r="AM13">
-        <v>9231</v>
+        <v>9235</v>
       </c>
       <c r="AN13">
-        <v>8792</v>
+        <v>8798</v>
       </c>
       <c r="AO13">
-        <v>8818</v>
+        <v>8825</v>
       </c>
       <c r="AP13">
-        <v>10875</v>
+        <v>10884</v>
       </c>
       <c r="AQ13">
-        <v>11967</v>
+        <v>11979</v>
       </c>
       <c r="AR13">
-        <v>9480</v>
+        <v>9493</v>
       </c>
       <c r="AS13">
-        <v>8025</v>
+        <v>8031</v>
       </c>
       <c r="AT13">
-        <v>9472</v>
+        <v>9516</v>
       </c>
       <c r="AU13">
-        <v>7480</v>
+        <v>7560</v>
+      </c>
+      <c r="AV13">
+        <v>6163</v>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -2987,7 +3033,7 @@
         <v>548</v>
       </c>
       <c r="D14">
-        <v>1755</v>
+        <v>1756</v>
       </c>
       <c r="E14">
         <v>2386</v>
@@ -2996,7 +3042,7 @@
         <v>2205</v>
       </c>
       <c r="G14">
-        <v>1652</v>
+        <v>1653</v>
       </c>
       <c r="H14">
         <v>984</v>
@@ -3011,25 +3057,25 @@
         <v>422</v>
       </c>
       <c r="L14">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="M14">
         <v>275</v>
       </c>
       <c r="N14">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="O14">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="P14">
         <v>195</v>
       </c>
       <c r="Q14">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="R14">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="S14">
         <v>227</v>
@@ -3041,7 +3087,7 @@
         <v>251</v>
       </c>
       <c r="V14">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="W14">
         <v>383</v>
@@ -3050,22 +3096,22 @@
         <v>514</v>
       </c>
       <c r="Y14">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="Z14">
         <v>762</v>
       </c>
       <c r="AA14">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="AB14">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="AC14">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="AD14">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="AE14">
         <v>1007</v>
@@ -3074,52 +3120,55 @@
         <v>1152</v>
       </c>
       <c r="AG14">
-        <v>1826</v>
+        <v>1825</v>
       </c>
       <c r="AH14">
-        <v>3107</v>
+        <v>3105</v>
       </c>
       <c r="AI14">
-        <v>5388</v>
+        <v>5393</v>
       </c>
       <c r="AJ14">
-        <v>8089</v>
+        <v>8084</v>
       </c>
       <c r="AK14">
-        <v>8954</v>
+        <v>8952</v>
       </c>
       <c r="AL14">
-        <v>9180</v>
+        <v>9178</v>
       </c>
       <c r="AM14">
-        <v>9196</v>
+        <v>9193</v>
       </c>
       <c r="AN14">
-        <v>8722</v>
+        <v>8723</v>
       </c>
       <c r="AO14">
-        <v>9140</v>
+        <v>9142</v>
       </c>
       <c r="AP14">
-        <v>10970</v>
+        <v>10979</v>
       </c>
       <c r="AQ14">
-        <v>12187</v>
+        <v>12206</v>
       </c>
       <c r="AR14">
-        <v>9479</v>
+        <v>9496</v>
       </c>
       <c r="AS14">
-        <v>8081</v>
+        <v>8097</v>
       </c>
       <c r="AT14">
-        <v>10062</v>
+        <v>10117</v>
       </c>
       <c r="AU14">
-        <v>7925</v>
+        <v>8012</v>
+      </c>
+      <c r="AV14">
+        <v>6279</v>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -3127,13 +3176,13 @@
         <v>69</v>
       </c>
       <c r="C15">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="D15">
-        <v>2049</v>
+        <v>2050</v>
       </c>
       <c r="E15">
-        <v>2640</v>
+        <v>2639</v>
       </c>
       <c r="F15">
         <v>2419</v>
@@ -3148,7 +3197,7 @@
         <v>909</v>
       </c>
       <c r="J15">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="K15">
         <v>488</v>
@@ -3157,13 +3206,13 @@
         <v>393</v>
       </c>
       <c r="M15">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="N15">
         <v>269</v>
       </c>
       <c r="O15">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="P15">
         <v>223</v>
@@ -3184,7 +3233,7 @@
         <v>297</v>
       </c>
       <c r="V15">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="W15">
         <v>424</v>
@@ -3196,16 +3245,16 @@
         <v>700</v>
       </c>
       <c r="Z15">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="AA15">
-        <v>854</v>
+        <v>857</v>
       </c>
       <c r="AB15">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="AC15">
-        <v>940</v>
+        <v>942</v>
       </c>
       <c r="AD15">
         <v>1205</v>
@@ -3214,55 +3263,58 @@
         <v>1302</v>
       </c>
       <c r="AF15">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="AG15">
-        <v>2365</v>
+        <v>2364</v>
       </c>
       <c r="AH15">
-        <v>3864</v>
+        <v>3863</v>
       </c>
       <c r="AI15">
-        <v>6712</v>
+        <v>6715</v>
       </c>
       <c r="AJ15">
-        <v>9574</v>
+        <v>9576</v>
       </c>
       <c r="AK15">
+        <v>10476</v>
+      </c>
+      <c r="AL15">
         <v>10475</v>
       </c>
-      <c r="AL15">
-        <v>10482</v>
-      </c>
       <c r="AM15">
-        <v>10100</v>
+        <v>10096</v>
       </c>
       <c r="AN15">
-        <v>9370</v>
+        <v>9377</v>
       </c>
       <c r="AO15">
-        <v>9457</v>
+        <v>9460</v>
       </c>
       <c r="AP15">
-        <v>11509</v>
+        <v>11526</v>
       </c>
       <c r="AQ15">
-        <v>12982</v>
+        <v>13000</v>
       </c>
       <c r="AR15">
-        <v>10036</v>
+        <v>10039</v>
       </c>
       <c r="AS15">
-        <v>9169</v>
+        <v>9179</v>
       </c>
       <c r="AT15">
-        <v>11523</v>
+        <v>11575</v>
       </c>
       <c r="AU15">
-        <v>8976</v>
+        <v>9051</v>
+      </c>
+      <c r="AV15">
+        <v>6950</v>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -3273,7 +3325,7 @@
         <v>547</v>
       </c>
       <c r="D16">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="E16">
         <v>2693</v>
@@ -3282,16 +3334,16 @@
         <v>2489</v>
       </c>
       <c r="G16">
-        <v>1935</v>
+        <v>1933</v>
       </c>
       <c r="H16">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="I16">
         <v>998</v>
       </c>
       <c r="J16">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="K16">
         <v>519</v>
@@ -3318,7 +3370,7 @@
         <v>325</v>
       </c>
       <c r="S16">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="T16">
         <v>227</v>
@@ -3333,7 +3385,7 @@
         <v>509</v>
       </c>
       <c r="X16">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="Y16">
         <v>839</v>
@@ -3348,64 +3400,67 @@
         <v>1160</v>
       </c>
       <c r="AC16">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="AD16">
-        <v>1482</v>
+        <v>1483</v>
       </c>
       <c r="AE16">
         <v>1438</v>
       </c>
       <c r="AF16">
-        <v>1746</v>
+        <v>1744</v>
       </c>
       <c r="AG16">
         <v>2692</v>
       </c>
       <c r="AH16">
-        <v>4479</v>
+        <v>4477</v>
       </c>
       <c r="AI16">
-        <v>7309</v>
+        <v>7311</v>
       </c>
       <c r="AJ16">
-        <v>10325</v>
+        <v>10327</v>
       </c>
       <c r="AK16">
-        <v>11150</v>
+        <v>11147</v>
       </c>
       <c r="AL16">
-        <v>10694</v>
+        <v>10699</v>
       </c>
       <c r="AM16">
-        <v>9942</v>
+        <v>9946</v>
       </c>
       <c r="AN16">
-        <v>8995</v>
+        <v>8993</v>
       </c>
       <c r="AO16">
-        <v>9131</v>
+        <v>9130</v>
       </c>
       <c r="AP16">
         <v>10781</v>
       </c>
       <c r="AQ16">
-        <v>12089</v>
+        <v>12103</v>
       </c>
       <c r="AR16">
-        <v>9396</v>
+        <v>9412</v>
       </c>
       <c r="AS16">
-        <v>8427</v>
+        <v>8433</v>
       </c>
       <c r="AT16">
-        <v>10759</v>
+        <v>10787</v>
       </c>
       <c r="AU16">
-        <v>8475</v>
+        <v>8526</v>
+      </c>
+      <c r="AV16">
+        <v>6368</v>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -3413,22 +3468,22 @@
         <v>70</v>
       </c>
       <c r="C17">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D17">
-        <v>1447</v>
+        <v>1449</v>
       </c>
       <c r="E17">
         <v>2274</v>
       </c>
       <c r="F17">
-        <v>2245</v>
+        <v>2243</v>
       </c>
       <c r="G17">
-        <v>1732</v>
+        <v>1733</v>
       </c>
       <c r="H17">
-        <v>1233</v>
+        <v>1235</v>
       </c>
       <c r="I17">
         <v>962</v>
@@ -3440,7 +3495,7 @@
         <v>508</v>
       </c>
       <c r="L17">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="M17">
         <v>314</v>
@@ -3455,7 +3510,7 @@
         <v>249</v>
       </c>
       <c r="Q17">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="R17">
         <v>260</v>
@@ -3467,10 +3522,10 @@
         <v>237</v>
       </c>
       <c r="U17">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="V17">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="W17">
         <v>521</v>
@@ -3482,10 +3537,10 @@
         <v>1166</v>
       </c>
       <c r="Z17">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="AA17">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="AB17">
         <v>1249</v>
@@ -3497,13 +3552,13 @@
         <v>1519</v>
       </c>
       <c r="AE17">
-        <v>1585</v>
+        <v>1583</v>
       </c>
       <c r="AF17">
-        <v>1735</v>
+        <v>1737</v>
       </c>
       <c r="AG17">
-        <v>2792</v>
+        <v>2793</v>
       </c>
       <c r="AH17">
         <v>4380</v>
@@ -3512,43 +3567,46 @@
         <v>7551</v>
       </c>
       <c r="AJ17">
-        <v>10430</v>
+        <v>10433</v>
       </c>
       <c r="AK17">
-        <v>11745</v>
+        <v>11744</v>
       </c>
       <c r="AL17">
-        <v>11045</v>
+        <v>11041</v>
       </c>
       <c r="AM17">
-        <v>10227</v>
+        <v>10221</v>
       </c>
       <c r="AN17">
-        <v>8950</v>
+        <v>8949</v>
       </c>
       <c r="AO17">
-        <v>9187</v>
+        <v>9182</v>
       </c>
       <c r="AP17">
-        <v>10777</v>
+        <v>10790</v>
       </c>
       <c r="AQ17">
-        <v>12105</v>
+        <v>12095</v>
       </c>
       <c r="AR17">
-        <v>9047</v>
+        <v>9053</v>
       </c>
       <c r="AS17">
-        <v>8592</v>
+        <v>8600</v>
       </c>
       <c r="AT17">
-        <v>10868</v>
+        <v>10895</v>
       </c>
       <c r="AU17">
-        <v>8439</v>
+        <v>8502</v>
+      </c>
+      <c r="AV17">
+        <v>6441</v>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -3556,7 +3614,7 @@
         <v>42</v>
       </c>
       <c r="C18">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D18">
         <v>541</v>
@@ -3565,7 +3623,7 @@
         <v>940</v>
       </c>
       <c r="F18">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="G18">
         <v>857</v>
@@ -3592,19 +3650,19 @@
         <v>162</v>
       </c>
       <c r="O18">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P18">
         <v>111</v>
       </c>
       <c r="Q18">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="R18">
         <v>169</v>
       </c>
       <c r="S18">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="T18">
         <v>149</v>
@@ -3613,7 +3671,7 @@
         <v>191</v>
       </c>
       <c r="V18">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="W18">
         <v>364</v>
@@ -3637,7 +3695,7 @@
         <v>833</v>
       </c>
       <c r="AD18">
-        <v>1034</v>
+        <v>1036</v>
       </c>
       <c r="AE18">
         <v>1049</v>
@@ -3646,52 +3704,55 @@
         <v>1331</v>
       </c>
       <c r="AG18">
-        <v>2077</v>
+        <v>2070</v>
       </c>
       <c r="AH18">
-        <v>2968</v>
+        <v>2965</v>
       </c>
       <c r="AI18">
-        <v>4851</v>
+        <v>4852</v>
       </c>
       <c r="AJ18">
-        <v>7186</v>
+        <v>7188</v>
       </c>
       <c r="AK18">
-        <v>8410</v>
+        <v>8408</v>
       </c>
       <c r="AL18">
-        <v>8699</v>
+        <v>8697</v>
       </c>
       <c r="AM18">
         <v>8203</v>
       </c>
       <c r="AN18">
-        <v>7464</v>
+        <v>7462</v>
       </c>
       <c r="AO18">
         <v>7718</v>
       </c>
       <c r="AP18">
-        <v>8823</v>
+        <v>8831</v>
       </c>
       <c r="AQ18">
-        <v>8456</v>
+        <v>8460</v>
       </c>
       <c r="AR18">
         <v>5844</v>
       </c>
       <c r="AS18">
-        <v>4959</v>
+        <v>4965</v>
       </c>
       <c r="AT18">
-        <v>6330</v>
+        <v>6366</v>
       </c>
       <c r="AU18">
-        <v>5360</v>
+        <v>5403</v>
+      </c>
+      <c r="AV18">
+        <v>4168</v>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>68</v>
       </c>
@@ -3729,7 +3790,7 @@
         <v>117</v>
       </c>
       <c r="M19">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="N19">
         <v>119</v>
@@ -3777,64 +3838,67 @@
         <v>430</v>
       </c>
       <c r="AC19">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="AD19">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="AE19">
         <v>587</v>
       </c>
       <c r="AF19">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="AG19">
         <v>1142</v>
       </c>
       <c r="AH19">
-        <v>1653</v>
+        <v>1655</v>
       </c>
       <c r="AI19">
-        <v>2745</v>
+        <v>2748</v>
       </c>
       <c r="AJ19">
-        <v>4082</v>
+        <v>4081</v>
       </c>
       <c r="AK19">
         <v>4775</v>
       </c>
       <c r="AL19">
-        <v>5342</v>
+        <v>5340</v>
       </c>
       <c r="AM19">
-        <v>5305</v>
+        <v>5303</v>
       </c>
       <c r="AN19">
-        <v>5181</v>
+        <v>5185</v>
       </c>
       <c r="AO19">
-        <v>5153</v>
+        <v>5156</v>
       </c>
       <c r="AP19">
-        <v>5673</v>
+        <v>5674</v>
       </c>
       <c r="AQ19">
-        <v>5253</v>
+        <v>5258</v>
       </c>
       <c r="AR19">
-        <v>3366</v>
+        <v>3371</v>
       </c>
       <c r="AS19">
-        <v>2634</v>
+        <v>2640</v>
       </c>
       <c r="AT19">
-        <v>3291</v>
+        <v>3306</v>
       </c>
       <c r="AU19">
-        <v>2691</v>
+        <v>2718</v>
+      </c>
+      <c r="AV19">
+        <v>2201</v>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>67</v>
       </c>
@@ -3851,7 +3915,7 @@
         <v>249</v>
       </c>
       <c r="F20">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="G20">
         <v>236</v>
@@ -3941,43 +4005,46 @@
         <v>1833</v>
       </c>
       <c r="AJ20">
-        <v>2790</v>
+        <v>2792</v>
       </c>
       <c r="AK20">
         <v>3360</v>
       </c>
       <c r="AL20">
-        <v>3616</v>
+        <v>3617</v>
       </c>
       <c r="AM20">
-        <v>3915</v>
+        <v>3914</v>
       </c>
       <c r="AN20">
         <v>3813</v>
       </c>
       <c r="AO20">
-        <v>3674</v>
+        <v>3677</v>
       </c>
       <c r="AP20">
-        <v>4242</v>
+        <v>4252</v>
       </c>
       <c r="AQ20">
-        <v>4290</v>
+        <v>4304</v>
       </c>
       <c r="AR20">
-        <v>2998</v>
+        <v>3005</v>
       </c>
       <c r="AS20">
-        <v>1931</v>
+        <v>1935</v>
       </c>
       <c r="AT20">
-        <v>2372</v>
+        <v>2394</v>
       </c>
       <c r="AU20">
-        <v>2177</v>
+        <v>2199</v>
+      </c>
+      <c r="AV20">
+        <v>1882</v>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -3988,7 +4055,7 @@
         <v>36</v>
       </c>
       <c r="D21">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E21">
         <v>255</v>
@@ -3997,7 +4064,7 @@
         <v>273</v>
       </c>
       <c r="G21">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="H21">
         <v>161</v>
@@ -4048,7 +4115,7 @@
         <v>151</v>
       </c>
       <c r="X21">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="Y21">
         <v>276</v>
@@ -4072,7 +4139,7 @@
         <v>302</v>
       </c>
       <c r="AF21">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="AG21">
         <v>523</v>
@@ -4084,59 +4151,61 @@
         <v>1463</v>
       </c>
       <c r="AJ21">
-        <v>2248</v>
+        <v>2251</v>
       </c>
       <c r="AK21">
-        <v>2422</v>
+        <v>2419</v>
       </c>
       <c r="AL21">
-        <v>2427</v>
+        <v>2428</v>
       </c>
       <c r="AM21">
-        <v>2381</v>
+        <v>2377</v>
       </c>
       <c r="AN21">
         <v>2336</v>
       </c>
       <c r="AO21">
-        <v>2319</v>
+        <v>2315</v>
       </c>
       <c r="AP21">
-        <v>2692</v>
+        <v>2691</v>
       </c>
       <c r="AQ21">
-        <v>3117</v>
+        <v>3116</v>
       </c>
       <c r="AR21">
-        <v>2117</v>
+        <v>2120</v>
       </c>
       <c r="AS21">
-        <v>1532</v>
+        <v>1537</v>
       </c>
       <c r="AT21">
-        <v>1918</v>
+        <v>1926</v>
       </c>
       <c r="AU21">
-        <v>1836</v>
+        <v>1860</v>
+      </c>
+      <c r="AV21">
+        <v>1691</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A5C854-B8B9-4F3F-88F5-F4BF0588EB40}">
-  <dimension ref="A1:AU21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6507039-E9D0-4988-A28C-0DAF62A64674}">
+  <dimension ref="A1:AV21"/>
   <sheetViews>
-    <sheetView topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="AU2" sqref="AU2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4278,28 +4347,31 @@
       <c r="AU1" t="s">
         <v>69</v>
       </c>
+      <c r="AV1" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1.07</v>
+        <v>1.08</v>
       </c>
       <c r="C2">
         <v>7.74</v>
       </c>
       <c r="D2">
-        <v>26.97</v>
+        <v>26.98</v>
       </c>
       <c r="E2">
-        <v>40.92</v>
+        <v>40.909999999999997</v>
       </c>
       <c r="F2">
         <v>43.41</v>
       </c>
       <c r="G2">
-        <v>32.68</v>
+        <v>32.69</v>
       </c>
       <c r="H2">
         <v>20.89</v>
@@ -4359,7 +4431,7 @@
         <v>11.55</v>
       </c>
       <c r="AA2">
-        <v>10.61</v>
+        <v>10.6</v>
       </c>
       <c r="AB2">
         <v>10.37</v>
@@ -4377,52 +4449,55 @@
         <v>19.149999999999999</v>
       </c>
       <c r="AG2">
-        <v>31.46</v>
+        <v>31.45</v>
       </c>
       <c r="AH2">
         <v>50.6</v>
       </c>
       <c r="AI2">
-        <v>89.97</v>
+        <v>89.99</v>
       </c>
       <c r="AJ2">
-        <v>133.65</v>
+        <v>133.63999999999999</v>
       </c>
       <c r="AK2">
-        <v>151.28</v>
+        <v>151.26</v>
       </c>
       <c r="AL2">
-        <v>153.79</v>
+        <v>153.74</v>
       </c>
       <c r="AM2">
-        <v>154.55000000000001</v>
+        <v>154.52000000000001</v>
       </c>
       <c r="AN2">
-        <v>148.35</v>
+        <v>148.33000000000001</v>
       </c>
       <c r="AO2">
-        <v>154.38</v>
+        <v>154.47</v>
       </c>
       <c r="AP2">
-        <v>187.91</v>
+        <v>188.06</v>
       </c>
       <c r="AQ2">
-        <v>210</v>
+        <v>210.17</v>
       </c>
       <c r="AR2">
-        <v>166.91</v>
+        <v>167.1</v>
       </c>
       <c r="AS2">
-        <v>147.82</v>
+        <v>148.07</v>
       </c>
       <c r="AT2">
-        <v>174.13</v>
+        <v>174.86</v>
       </c>
       <c r="AU2">
-        <v>141.81</v>
+        <v>143.06</v>
+      </c>
+      <c r="AV2">
+        <v>114.15</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -4442,7 +4517,7 @@
         <v>142.4</v>
       </c>
       <c r="G3">
-        <v>151.27000000000001</v>
+        <v>151.38999999999999</v>
       </c>
       <c r="H3">
         <v>103.03</v>
@@ -4493,7 +4568,7 @@
         <v>4.74</v>
       </c>
       <c r="X3">
-        <v>3.4</v>
+        <v>3.52</v>
       </c>
       <c r="Y3">
         <v>3.04</v>
@@ -4523,49 +4598,52 @@
         <v>22.72</v>
       </c>
       <c r="AH3">
-        <v>52.24</v>
+        <v>52.73</v>
       </c>
       <c r="AI3">
-        <v>107.65</v>
+        <v>107.77</v>
       </c>
       <c r="AJ3">
         <v>178</v>
       </c>
       <c r="AK3">
-        <v>208.86</v>
+        <v>208.98</v>
       </c>
       <c r="AL3">
-        <v>281.39</v>
+        <v>281.88</v>
       </c>
       <c r="AM3">
-        <v>372.88</v>
+        <v>373.49</v>
       </c>
       <c r="AN3">
-        <v>428.89</v>
+        <v>427.92</v>
       </c>
       <c r="AO3">
-        <v>504.59</v>
+        <v>507.5</v>
       </c>
       <c r="AP3">
-        <v>657.31</v>
+        <v>657.56</v>
       </c>
       <c r="AQ3">
-        <v>726.93</v>
+        <v>727.05</v>
       </c>
       <c r="AR3">
-        <v>638.72</v>
+        <v>638.85</v>
       </c>
       <c r="AS3">
-        <v>603.12</v>
+        <v>604.46</v>
       </c>
       <c r="AT3">
-        <v>653.66999999999996</v>
+        <v>655.73</v>
       </c>
       <c r="AU3">
-        <v>603.61</v>
+        <v>610.41</v>
+      </c>
+      <c r="AV3">
+        <v>475.31</v>
       </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -4576,7 +4654,7 @@
         <v>2.4300000000000002</v>
       </c>
       <c r="D4">
-        <v>13.94</v>
+        <v>14</v>
       </c>
       <c r="E4">
         <v>47.19</v>
@@ -4594,7 +4672,7 @@
         <v>43.74</v>
       </c>
       <c r="J4">
-        <v>21.04</v>
+        <v>20.97</v>
       </c>
       <c r="K4">
         <v>16.82</v>
@@ -4606,7 +4684,7 @@
         <v>8.1199999999999992</v>
       </c>
       <c r="N4">
-        <v>5.5</v>
+        <v>5.44</v>
       </c>
       <c r="O4">
         <v>3.26</v>
@@ -4666,49 +4744,52 @@
         <v>19.5</v>
       </c>
       <c r="AH4">
-        <v>36.58</v>
+        <v>36.51</v>
       </c>
       <c r="AI4">
-        <v>72.709999999999994</v>
+        <v>72.900000000000006</v>
       </c>
       <c r="AJ4">
-        <v>113.76</v>
+        <v>113.82</v>
       </c>
       <c r="AK4">
-        <v>146.44</v>
+        <v>146.5</v>
       </c>
       <c r="AL4">
-        <v>180.97</v>
+        <v>180.9</v>
       </c>
       <c r="AM4">
-        <v>215.18</v>
+        <v>215.5</v>
       </c>
       <c r="AN4">
-        <v>262.95</v>
+        <v>262.82</v>
       </c>
       <c r="AO4">
-        <v>292.88</v>
+        <v>293.45</v>
       </c>
       <c r="AP4">
-        <v>377.6</v>
+        <v>377.99</v>
       </c>
       <c r="AQ4">
-        <v>442.7</v>
+        <v>443.79</v>
       </c>
       <c r="AR4">
-        <v>374.79</v>
+        <v>374.66</v>
       </c>
       <c r="AS4">
-        <v>357.52</v>
+        <v>358.42</v>
       </c>
       <c r="AT4">
-        <v>386.62</v>
+        <v>388.54</v>
       </c>
       <c r="AU4">
-        <v>350.81</v>
+        <v>355.48</v>
+      </c>
+      <c r="AV4">
+        <v>282.89999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -4716,13 +4797,13 @@
         <v>0.36</v>
       </c>
       <c r="C5">
-        <v>2.52</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="D5">
         <v>14.21</v>
       </c>
       <c r="E5">
-        <v>39.01</v>
+        <v>39.04</v>
       </c>
       <c r="F5">
         <v>59.62</v>
@@ -4737,13 +4818,13 @@
         <v>25.01</v>
       </c>
       <c r="J5">
-        <v>13.69</v>
+        <v>13.72</v>
       </c>
       <c r="K5">
         <v>9.11</v>
       </c>
       <c r="L5">
-        <v>7.5</v>
+        <v>7.47</v>
       </c>
       <c r="M5">
         <v>4.6100000000000003</v>
@@ -4755,7 +4836,7 @@
         <v>2.31</v>
       </c>
       <c r="P5">
-        <v>1.91</v>
+        <v>1.88</v>
       </c>
       <c r="Q5">
         <v>1.88</v>
@@ -4806,52 +4887,55 @@
         <v>9.59</v>
       </c>
       <c r="AG5">
-        <v>14.36</v>
+        <v>14.33</v>
       </c>
       <c r="AH5">
-        <v>25.98</v>
+        <v>26.05</v>
       </c>
       <c r="AI5">
-        <v>55.64</v>
+        <v>55.7</v>
       </c>
       <c r="AJ5">
-        <v>86.24</v>
+        <v>86.27</v>
       </c>
       <c r="AK5">
-        <v>104.21</v>
+        <v>104.3</v>
       </c>
       <c r="AL5">
         <v>115.29</v>
       </c>
       <c r="AM5">
-        <v>132.47</v>
+        <v>132.56</v>
       </c>
       <c r="AN5">
-        <v>145.68</v>
+        <v>145.59</v>
       </c>
       <c r="AO5">
-        <v>164.68</v>
+        <v>165.17</v>
       </c>
       <c r="AP5">
-        <v>214.19</v>
+        <v>214.61</v>
       </c>
       <c r="AQ5">
-        <v>250.8</v>
+        <v>250.98</v>
       </c>
       <c r="AR5">
-        <v>225.6</v>
+        <v>225.94</v>
       </c>
       <c r="AS5">
-        <v>207.88</v>
+        <v>208.6</v>
       </c>
       <c r="AT5">
-        <v>232.04</v>
+        <v>232.77</v>
       </c>
       <c r="AU5">
-        <v>199.95</v>
+        <v>202.68</v>
+      </c>
+      <c r="AV5">
+        <v>161.19</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -4871,7 +4955,7 @@
         <v>46.13</v>
       </c>
       <c r="G6">
-        <v>33.82</v>
+        <v>33.85</v>
       </c>
       <c r="H6">
         <v>22.03</v>
@@ -4880,7 +4964,7 @@
         <v>15.14</v>
       </c>
       <c r="J6">
-        <v>9.08</v>
+        <v>9.0500000000000007</v>
       </c>
       <c r="K6">
         <v>7.07</v>
@@ -4898,7 +4982,7 @@
         <v>1.5</v>
       </c>
       <c r="P6">
-        <v>1.1599999999999999</v>
+        <v>1.19</v>
       </c>
       <c r="Q6">
         <v>1.68</v>
@@ -4946,7 +5030,7 @@
         <v>5.96</v>
       </c>
       <c r="AF6">
-        <v>7.89</v>
+        <v>7.92</v>
       </c>
       <c r="AG6">
         <v>13.08</v>
@@ -4958,43 +5042,46 @@
         <v>42</v>
       </c>
       <c r="AJ6">
-        <v>68.260000000000005</v>
+        <v>68.36</v>
       </c>
       <c r="AK6">
-        <v>78.66</v>
+        <v>78.680000000000007</v>
       </c>
       <c r="AL6">
-        <v>84.85</v>
+        <v>84.74</v>
       </c>
       <c r="AM6">
+        <v>87.5</v>
+      </c>
+      <c r="AN6">
+        <v>90.16</v>
+      </c>
+      <c r="AO6">
+        <v>102.39</v>
+      </c>
+      <c r="AP6">
+        <v>128.80000000000001</v>
+      </c>
+      <c r="AQ6">
+        <v>153.49</v>
+      </c>
+      <c r="AR6">
+        <v>131.41</v>
+      </c>
+      <c r="AS6">
+        <v>119.62</v>
+      </c>
+      <c r="AT6">
+        <v>135</v>
+      </c>
+      <c r="AU6">
+        <v>111.57</v>
+      </c>
+      <c r="AV6">
         <v>87.48</v>
       </c>
-      <c r="AN6">
-        <v>90.13</v>
-      </c>
-      <c r="AO6">
-        <v>102.21</v>
-      </c>
-      <c r="AP6">
-        <v>128.6</v>
-      </c>
-      <c r="AQ6">
-        <v>153.69999999999999</v>
-      </c>
-      <c r="AR6">
-        <v>131.07</v>
-      </c>
-      <c r="AS6">
-        <v>119.13</v>
-      </c>
-      <c r="AT6">
-        <v>134.47999999999999</v>
-      </c>
-      <c r="AU6">
-        <v>110.85</v>
-      </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -5005,7 +5092,7 @@
         <v>3.95</v>
       </c>
       <c r="D7">
-        <v>16.96</v>
+        <v>16.93</v>
       </c>
       <c r="E7">
         <v>36.119999999999997</v>
@@ -5029,7 +5116,7 @@
         <v>5.63</v>
       </c>
       <c r="L7">
-        <v>3.51</v>
+        <v>3.48</v>
       </c>
       <c r="M7">
         <v>2.5</v>
@@ -5080,7 +5167,7 @@
         <v>2.91</v>
       </c>
       <c r="AC7">
-        <v>4.1399999999999997</v>
+        <v>4.1100000000000003</v>
       </c>
       <c r="AD7">
         <v>7.05</v>
@@ -5089,60 +5176,63 @@
         <v>7.21</v>
       </c>
       <c r="AF7">
-        <v>9.5299999999999994</v>
+        <v>9.5</v>
       </c>
       <c r="AG7">
-        <v>16.059999999999999</v>
+        <v>16.03</v>
       </c>
       <c r="AH7">
-        <v>25.37</v>
+        <v>25.39</v>
       </c>
       <c r="AI7">
         <v>48.8</v>
       </c>
       <c r="AJ7">
-        <v>78.41</v>
+        <v>78.44</v>
       </c>
       <c r="AK7">
         <v>86.39</v>
       </c>
       <c r="AL7">
-        <v>89.57</v>
+        <v>89.6</v>
       </c>
       <c r="AM7">
-        <v>91.34</v>
+        <v>91.42</v>
       </c>
       <c r="AN7">
-        <v>87.34</v>
+        <v>87.26</v>
       </c>
       <c r="AO7">
-        <v>94.64</v>
+        <v>94.77</v>
       </c>
       <c r="AP7">
-        <v>119.24</v>
+        <v>119.49</v>
       </c>
       <c r="AQ7">
-        <v>140.55000000000001</v>
+        <v>140.66</v>
       </c>
       <c r="AR7">
-        <v>120.66</v>
+        <v>120.74</v>
       </c>
       <c r="AS7">
-        <v>112.52</v>
+        <v>112.63</v>
       </c>
       <c r="AT7">
-        <v>130.66999999999999</v>
+        <v>131.32</v>
       </c>
       <c r="AU7">
-        <v>99.32</v>
+        <v>99.64</v>
+      </c>
+      <c r="AV7">
+        <v>83.01</v>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0.49</v>
+        <v>0.51</v>
       </c>
       <c r="C8">
         <v>4.88</v>
@@ -5151,19 +5241,19 @@
         <v>18.3</v>
       </c>
       <c r="E8">
-        <v>33.96</v>
+        <v>33.94</v>
       </c>
       <c r="F8">
         <v>34.840000000000003</v>
       </c>
       <c r="G8">
-        <v>22.95</v>
+        <v>22.97</v>
       </c>
       <c r="H8">
         <v>13.62</v>
       </c>
       <c r="I8">
-        <v>10.41</v>
+        <v>10.39</v>
       </c>
       <c r="J8">
         <v>5.47</v>
@@ -5172,13 +5262,13 @@
         <v>4.28</v>
       </c>
       <c r="L8">
-        <v>3.03</v>
+        <v>3</v>
       </c>
       <c r="M8">
         <v>2.5499999999999998</v>
       </c>
       <c r="N8">
-        <v>2.2200000000000002</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="O8">
         <v>1.23</v>
@@ -5235,52 +5325,55 @@
         <v>9.32</v>
       </c>
       <c r="AG8">
-        <v>14.1</v>
+        <v>14.06</v>
       </c>
       <c r="AH8">
         <v>26.45</v>
       </c>
       <c r="AI8">
-        <v>46.7</v>
+        <v>46.74</v>
       </c>
       <c r="AJ8">
         <v>73.099999999999994</v>
       </c>
       <c r="AK8">
-        <v>87.2</v>
+        <v>87.32</v>
       </c>
       <c r="AL8">
-        <v>82.65</v>
+        <v>82.67</v>
       </c>
       <c r="AM8">
-        <v>85.35</v>
+        <v>85.33</v>
       </c>
       <c r="AN8">
-        <v>85.18</v>
+        <v>85.12</v>
       </c>
       <c r="AO8">
-        <v>84.89</v>
+        <v>84.93</v>
       </c>
       <c r="AP8">
-        <v>106.07</v>
+        <v>106.28</v>
       </c>
       <c r="AQ8">
-        <v>130.15</v>
+        <v>130.38</v>
       </c>
       <c r="AR8">
-        <v>114.57</v>
+        <v>114.86</v>
       </c>
       <c r="AS8">
-        <v>102.08</v>
+        <v>102.22</v>
       </c>
       <c r="AT8">
-        <v>116.98</v>
+        <v>117.27</v>
       </c>
       <c r="AU8">
-        <v>89.79</v>
+        <v>90.82</v>
+      </c>
+      <c r="AV8">
+        <v>73.53</v>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -5288,19 +5381,19 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C9">
-        <v>7.63</v>
+        <v>7.61</v>
       </c>
       <c r="D9">
-        <v>28.28</v>
+        <v>28.29</v>
       </c>
       <c r="E9">
-        <v>44.76</v>
+        <v>44.74</v>
       </c>
       <c r="F9">
         <v>49.29</v>
       </c>
       <c r="G9">
-        <v>31.84</v>
+        <v>31.82</v>
       </c>
       <c r="H9">
         <v>19.25</v>
@@ -5324,7 +5417,7 @@
         <v>2.99</v>
       </c>
       <c r="O9">
-        <v>1.91</v>
+        <v>1.89</v>
       </c>
       <c r="P9">
         <v>1.61</v>
@@ -5348,7 +5441,7 @@
         <v>2.71</v>
       </c>
       <c r="W9">
-        <v>2.71</v>
+        <v>2.69</v>
       </c>
       <c r="X9">
         <v>3.61</v>
@@ -5366,13 +5459,13 @@
         <v>4.37</v>
       </c>
       <c r="AC9">
-        <v>5.98</v>
+        <v>5.97</v>
       </c>
       <c r="AD9">
         <v>8.73</v>
       </c>
       <c r="AE9">
-        <v>9.58</v>
+        <v>9.61</v>
       </c>
       <c r="AF9">
         <v>12.04</v>
@@ -5381,49 +5474,52 @@
         <v>22.5</v>
       </c>
       <c r="AH9">
-        <v>37.549999999999997</v>
+        <v>37.54</v>
       </c>
       <c r="AI9">
-        <v>69.989999999999995</v>
+        <v>70.010000000000005</v>
       </c>
       <c r="AJ9">
-        <v>106.04</v>
+        <v>106.09</v>
       </c>
       <c r="AK9">
-        <v>121.22</v>
+        <v>121.27</v>
       </c>
       <c r="AL9">
         <v>122.21</v>
       </c>
       <c r="AM9">
-        <v>129.36000000000001</v>
+        <v>129.34</v>
       </c>
       <c r="AN9">
-        <v>123.84</v>
+        <v>123.92</v>
       </c>
       <c r="AO9">
-        <v>135.49</v>
+        <v>135.54</v>
       </c>
       <c r="AP9">
-        <v>166.67</v>
+        <v>166.83</v>
       </c>
       <c r="AQ9">
-        <v>194.54</v>
+        <v>194.86</v>
       </c>
       <c r="AR9">
-        <v>161.6</v>
+        <v>162.12</v>
       </c>
       <c r="AS9">
-        <v>145.91999999999999</v>
+        <v>146.38</v>
       </c>
       <c r="AT9">
-        <v>162.97999999999999</v>
+        <v>163.87</v>
       </c>
       <c r="AU9">
-        <v>132.16</v>
+        <v>133.27000000000001</v>
+      </c>
+      <c r="AV9">
+        <v>109.51</v>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -5434,7 +5530,7 @@
         <v>11.16</v>
       </c>
       <c r="D10">
-        <v>38.56</v>
+        <v>38.590000000000003</v>
       </c>
       <c r="E10">
         <v>53.36</v>
@@ -5452,13 +5548,13 @@
         <v>15.73</v>
       </c>
       <c r="J10">
-        <v>8.91</v>
+        <v>8.89</v>
       </c>
       <c r="K10">
         <v>7.57</v>
       </c>
       <c r="L10">
-        <v>5.34</v>
+        <v>5.36</v>
       </c>
       <c r="M10">
         <v>3.95</v>
@@ -5467,16 +5563,16 @@
         <v>3.52</v>
       </c>
       <c r="O10">
-        <v>2.11</v>
+        <v>2.12</v>
       </c>
       <c r="P10">
-        <v>2</v>
+        <v>1.99</v>
       </c>
       <c r="Q10">
-        <v>2.75</v>
+        <v>2.76</v>
       </c>
       <c r="R10">
-        <v>3.01</v>
+        <v>3</v>
       </c>
       <c r="S10">
         <v>2.3199999999999998</v>
@@ -5512,7 +5608,7 @@
         <v>8.2200000000000006</v>
       </c>
       <c r="AD10">
-        <v>11.3</v>
+        <v>11.31</v>
       </c>
       <c r="AE10">
         <v>12.85</v>
@@ -5527,46 +5623,49 @@
         <v>44.5</v>
       </c>
       <c r="AI10">
-        <v>85.39</v>
+        <v>85.42</v>
       </c>
       <c r="AJ10">
-        <v>133.05000000000001</v>
+        <v>133.01</v>
       </c>
       <c r="AK10">
         <v>150.72999999999999</v>
       </c>
       <c r="AL10">
-        <v>152.94</v>
+        <v>152.88999999999999</v>
       </c>
       <c r="AM10">
-        <v>151.93</v>
+        <v>151.94999999999999</v>
       </c>
       <c r="AN10">
-        <v>146.33000000000001</v>
+        <v>146.38</v>
       </c>
       <c r="AO10">
-        <v>153.49</v>
+        <v>153.74</v>
       </c>
       <c r="AP10">
-        <v>193.31</v>
+        <v>193.62</v>
       </c>
       <c r="AQ10">
-        <v>222.08</v>
+        <v>222.34</v>
       </c>
       <c r="AR10">
-        <v>182.52</v>
+        <v>182.85</v>
       </c>
       <c r="AS10">
-        <v>163.74</v>
+        <v>164.09</v>
       </c>
       <c r="AT10">
-        <v>181.41</v>
+        <v>182.62</v>
       </c>
       <c r="AU10">
-        <v>147.18</v>
+        <v>148.72</v>
+      </c>
+      <c r="AV10">
+        <v>122.99</v>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -5577,10 +5676,10 @@
         <v>14.6</v>
       </c>
       <c r="D11">
-        <v>46.12</v>
+        <v>46.11</v>
       </c>
       <c r="E11">
-        <v>59.63</v>
+        <v>59.61</v>
       </c>
       <c r="F11">
         <v>55.14</v>
@@ -5595,16 +5694,16 @@
         <v>14.77</v>
       </c>
       <c r="J11">
-        <v>8.99</v>
+        <v>9.02</v>
       </c>
       <c r="K11">
         <v>7.75</v>
       </c>
       <c r="L11">
-        <v>5.56</v>
+        <v>5.57</v>
       </c>
       <c r="M11">
-        <v>3.76</v>
+        <v>3.77</v>
       </c>
       <c r="N11">
         <v>3.56</v>
@@ -5628,7 +5727,7 @@
         <v>2.56</v>
       </c>
       <c r="U11">
-        <v>3.11</v>
+        <v>3.13</v>
       </c>
       <c r="V11">
         <v>4.38</v>
@@ -5643,10 +5742,10 @@
         <v>7.08</v>
       </c>
       <c r="Z11">
-        <v>8.36</v>
+        <v>8.35</v>
       </c>
       <c r="AA11">
-        <v>8.0500000000000007</v>
+        <v>8.0299999999999994</v>
       </c>
       <c r="AB11">
         <v>8.26</v>
@@ -5667,49 +5766,52 @@
         <v>33.78</v>
       </c>
       <c r="AH11">
-        <v>53.23</v>
+        <v>53.22</v>
       </c>
       <c r="AI11">
-        <v>95.54</v>
+        <v>95.6</v>
       </c>
       <c r="AJ11">
-        <v>145.6</v>
+        <v>145.63999999999999</v>
       </c>
       <c r="AK11">
-        <v>163.16999999999999</v>
+        <v>163.12</v>
       </c>
       <c r="AL11">
-        <v>163.79</v>
+        <v>163.72999999999999</v>
       </c>
       <c r="AM11">
-        <v>161.29</v>
+        <v>161.28</v>
       </c>
       <c r="AN11">
-        <v>154.06</v>
+        <v>154.12</v>
       </c>
       <c r="AO11">
-        <v>157.04</v>
+        <v>157.19</v>
       </c>
       <c r="AP11">
-        <v>197.13</v>
+        <v>197.25</v>
       </c>
       <c r="AQ11">
-        <v>221.84</v>
+        <v>222.08</v>
       </c>
       <c r="AR11">
-        <v>177.97</v>
+        <v>178.16</v>
       </c>
       <c r="AS11">
-        <v>156.05000000000001</v>
+        <v>156.49</v>
       </c>
       <c r="AT11">
-        <v>179.32</v>
+        <v>180.1</v>
       </c>
       <c r="AU11">
-        <v>144.29</v>
+        <v>145.75</v>
+      </c>
+      <c r="AV11">
+        <v>120.7</v>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -5717,19 +5819,19 @@
         <v>1.9</v>
       </c>
       <c r="C12">
-        <v>14.07</v>
+        <v>14.05</v>
       </c>
       <c r="D12">
-        <v>39.770000000000003</v>
+        <v>39.78</v>
       </c>
       <c r="E12">
-        <v>55.45</v>
+        <v>55.43</v>
       </c>
       <c r="F12">
         <v>51.62</v>
       </c>
       <c r="G12">
-        <v>36.409999999999997</v>
+        <v>36.43</v>
       </c>
       <c r="H12">
         <v>22.26</v>
@@ -5738,7 +5840,7 @@
         <v>14.94</v>
       </c>
       <c r="J12">
-        <v>8.8699999999999992</v>
+        <v>8.89</v>
       </c>
       <c r="K12">
         <v>8.5</v>
@@ -5750,16 +5852,16 @@
         <v>4.82</v>
       </c>
       <c r="N12">
-        <v>4.04</v>
+        <v>4.0599999999999996</v>
       </c>
       <c r="O12">
-        <v>3.09</v>
+        <v>3.11</v>
       </c>
       <c r="P12">
-        <v>2.73</v>
+        <v>2.75</v>
       </c>
       <c r="Q12">
-        <v>7.15</v>
+        <v>7.13</v>
       </c>
       <c r="R12">
         <v>5.25</v>
@@ -5786,10 +5888,10 @@
         <v>10.88</v>
       </c>
       <c r="Z12">
-        <v>13.14</v>
+        <v>13.16</v>
       </c>
       <c r="AA12">
-        <v>11.45</v>
+        <v>11.42</v>
       </c>
       <c r="AB12">
         <v>11.66</v>
@@ -5810,49 +5912,52 @@
         <v>38.65</v>
       </c>
       <c r="AH12">
-        <v>59.3</v>
+        <v>59.32</v>
       </c>
       <c r="AI12">
-        <v>110.08</v>
+        <v>110.16</v>
       </c>
       <c r="AJ12">
-        <v>158.93</v>
+        <v>158.99</v>
       </c>
       <c r="AK12">
-        <v>179.6</v>
+        <v>179.51</v>
       </c>
       <c r="AL12">
         <v>176.04</v>
       </c>
       <c r="AM12">
-        <v>183.28</v>
+        <v>183.37</v>
       </c>
       <c r="AN12">
-        <v>171.69</v>
+        <v>171.79</v>
       </c>
       <c r="AO12">
-        <v>175.07</v>
+        <v>175.05</v>
       </c>
       <c r="AP12">
-        <v>209.85</v>
+        <v>210.09</v>
       </c>
       <c r="AQ12">
-        <v>235.31</v>
+        <v>235.58</v>
       </c>
       <c r="AR12">
-        <v>183.79</v>
+        <v>184.19</v>
       </c>
       <c r="AS12">
-        <v>161.57</v>
+        <v>161.88999999999999</v>
       </c>
       <c r="AT12">
-        <v>184.47</v>
+        <v>185.31</v>
       </c>
       <c r="AU12">
-        <v>150.34</v>
+        <v>151.29</v>
+      </c>
+      <c r="AV12">
+        <v>121.57</v>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -5860,13 +5965,13 @@
         <v>1.75</v>
       </c>
       <c r="C13">
-        <v>11.61</v>
+        <v>11.59</v>
       </c>
       <c r="D13">
-        <v>36.75</v>
+        <v>36.770000000000003</v>
       </c>
       <c r="E13">
-        <v>47.46</v>
+        <v>47.48</v>
       </c>
       <c r="F13">
         <v>47.06</v>
@@ -5878,10 +5983,10 @@
         <v>20.86</v>
       </c>
       <c r="I13">
-        <v>14.24</v>
+        <v>14.22</v>
       </c>
       <c r="J13">
-        <v>9.27</v>
+        <v>9.2899999999999991</v>
       </c>
       <c r="K13">
         <v>8.25</v>
@@ -5890,7 +5995,7 @@
         <v>7.27</v>
       </c>
       <c r="M13">
-        <v>4.91</v>
+        <v>4.95</v>
       </c>
       <c r="N13">
         <v>4.34</v>
@@ -5902,7 +6007,7 @@
         <v>3.22</v>
       </c>
       <c r="Q13">
-        <v>9.27</v>
+        <v>9.25</v>
       </c>
       <c r="R13">
         <v>5.54</v>
@@ -5917,7 +6022,7 @@
         <v>5.15</v>
       </c>
       <c r="V13">
-        <v>6.56</v>
+        <v>6.54</v>
       </c>
       <c r="W13">
         <v>8.74</v>
@@ -5932,7 +6037,7 @@
         <v>14.59</v>
       </c>
       <c r="AA13">
-        <v>13.46</v>
+        <v>13.44</v>
       </c>
       <c r="AB13">
         <v>13.2</v>
@@ -5944,10 +6049,10 @@
         <v>17.170000000000002</v>
       </c>
       <c r="AE13">
-        <v>17.52</v>
+        <v>17.54</v>
       </c>
       <c r="AF13">
-        <v>21.33</v>
+        <v>21.35</v>
       </c>
       <c r="AG13">
         <v>38.07</v>
@@ -5956,46 +6061,49 @@
         <v>59.22</v>
       </c>
       <c r="AI13">
-        <v>107.96</v>
+        <v>107.92</v>
       </c>
       <c r="AJ13">
-        <v>160.22</v>
+        <v>160.30000000000001</v>
       </c>
       <c r="AK13">
-        <v>180.52</v>
+        <v>180.61</v>
       </c>
       <c r="AL13">
-        <v>182.89</v>
+        <v>183.01</v>
       </c>
       <c r="AM13">
-        <v>188.04</v>
+        <v>188.12</v>
       </c>
       <c r="AN13">
-        <v>179.1</v>
+        <v>179.22</v>
       </c>
       <c r="AO13">
-        <v>179.63</v>
+        <v>179.77</v>
       </c>
       <c r="AP13">
-        <v>221.53</v>
+        <v>221.71</v>
       </c>
       <c r="AQ13">
-        <v>243.78</v>
+        <v>244.02</v>
       </c>
       <c r="AR13">
-        <v>193.11</v>
+        <v>193.38</v>
       </c>
       <c r="AS13">
-        <v>163.47</v>
+        <v>163.6</v>
       </c>
       <c r="AT13">
-        <v>192.95</v>
+        <v>193.85</v>
       </c>
       <c r="AU13">
-        <v>152.37</v>
+        <v>154</v>
+      </c>
+      <c r="AV13">
+        <v>125.54</v>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -6006,7 +6114,7 @@
         <v>10.36</v>
       </c>
       <c r="D14">
-        <v>33.18</v>
+        <v>33.200000000000003</v>
       </c>
       <c r="E14">
         <v>45.11</v>
@@ -6015,7 +6123,7 @@
         <v>41.69</v>
       </c>
       <c r="G14">
-        <v>31.23</v>
+        <v>31.25</v>
       </c>
       <c r="H14">
         <v>18.600000000000001</v>
@@ -6030,25 +6138,25 @@
         <v>7.98</v>
       </c>
       <c r="L14">
-        <v>6.66</v>
+        <v>6.67</v>
       </c>
       <c r="M14">
         <v>5.2</v>
       </c>
       <c r="N14">
-        <v>4.5599999999999996</v>
+        <v>4.54</v>
       </c>
       <c r="O14">
-        <v>2.95</v>
+        <v>2.97</v>
       </c>
       <c r="P14">
         <v>3.69</v>
       </c>
       <c r="Q14">
-        <v>7.26</v>
+        <v>7.24</v>
       </c>
       <c r="R14">
-        <v>5.65</v>
+        <v>5.63</v>
       </c>
       <c r="S14">
         <v>4.29</v>
@@ -6060,7 +6168,7 @@
         <v>4.75</v>
       </c>
       <c r="V14">
-        <v>6.84</v>
+        <v>6.86</v>
       </c>
       <c r="W14">
         <v>7.24</v>
@@ -6069,22 +6177,22 @@
         <v>9.7200000000000006</v>
       </c>
       <c r="Y14">
-        <v>12.19</v>
+        <v>12.18</v>
       </c>
       <c r="Z14">
         <v>14.41</v>
       </c>
       <c r="AA14">
-        <v>13.52</v>
+        <v>13.54</v>
       </c>
       <c r="AB14">
-        <v>12.27</v>
+        <v>12.29</v>
       </c>
       <c r="AC14">
-        <v>13.2</v>
+        <v>13.22</v>
       </c>
       <c r="AD14">
-        <v>17.03</v>
+        <v>17.05</v>
       </c>
       <c r="AE14">
         <v>19.04</v>
@@ -6093,52 +6201,55 @@
         <v>21.78</v>
       </c>
       <c r="AG14">
-        <v>34.520000000000003</v>
+        <v>34.5</v>
       </c>
       <c r="AH14">
-        <v>58.74</v>
+        <v>58.7</v>
       </c>
       <c r="AI14">
-        <v>101.87</v>
+        <v>101.96</v>
       </c>
       <c r="AJ14">
-        <v>152.93</v>
+        <v>152.84</v>
       </c>
       <c r="AK14">
-        <v>169.29</v>
+        <v>169.25</v>
       </c>
       <c r="AL14">
-        <v>173.56</v>
+        <v>173.52</v>
       </c>
       <c r="AM14">
-        <v>173.86</v>
+        <v>173.81</v>
       </c>
       <c r="AN14">
-        <v>164.9</v>
+        <v>164.92</v>
       </c>
       <c r="AO14">
-        <v>172.8</v>
+        <v>172.84</v>
       </c>
       <c r="AP14">
-        <v>207.4</v>
+        <v>207.57</v>
       </c>
       <c r="AQ14">
-        <v>230.41</v>
+        <v>230.77</v>
       </c>
       <c r="AR14">
-        <v>179.21</v>
+        <v>179.54</v>
       </c>
       <c r="AS14">
-        <v>152.78</v>
+        <v>153.09</v>
       </c>
       <c r="AT14">
-        <v>190.24</v>
+        <v>191.28</v>
       </c>
       <c r="AU14">
-        <v>149.83000000000001</v>
+        <v>151.47999999999999</v>
+      </c>
+      <c r="AV14">
+        <v>118.71</v>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -6146,13 +6257,13 @@
         <v>1.26</v>
       </c>
       <c r="C15">
-        <v>9.6999999999999993</v>
+        <v>9.7200000000000006</v>
       </c>
       <c r="D15">
-        <v>37.28</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="E15">
-        <v>48.04</v>
+        <v>48.02</v>
       </c>
       <c r="F15">
         <v>44.02</v>
@@ -6167,7 +6278,7 @@
         <v>16.54</v>
       </c>
       <c r="J15">
-        <v>10.24</v>
+        <v>10.23</v>
       </c>
       <c r="K15">
         <v>8.8800000000000008</v>
@@ -6176,13 +6287,13 @@
         <v>7.15</v>
       </c>
       <c r="M15">
-        <v>5.88</v>
+        <v>5.84</v>
       </c>
       <c r="N15">
         <v>4.8899999999999997</v>
       </c>
       <c r="O15">
-        <v>3.77</v>
+        <v>3.75</v>
       </c>
       <c r="P15">
         <v>4.0599999999999996</v>
@@ -6203,7 +6314,7 @@
         <v>5.4</v>
       </c>
       <c r="V15">
-        <v>6.99</v>
+        <v>7.01</v>
       </c>
       <c r="W15">
         <v>7.72</v>
@@ -6215,16 +6326,16 @@
         <v>12.74</v>
       </c>
       <c r="Z15">
-        <v>17.23</v>
+        <v>17.21</v>
       </c>
       <c r="AA15">
-        <v>15.54</v>
+        <v>15.59</v>
       </c>
       <c r="AB15">
-        <v>17.05</v>
+        <v>17.07</v>
       </c>
       <c r="AC15">
-        <v>17.100000000000001</v>
+        <v>17.14</v>
       </c>
       <c r="AD15">
         <v>21.93</v>
@@ -6233,55 +6344,58 @@
         <v>23.69</v>
       </c>
       <c r="AF15">
-        <v>27.73</v>
+        <v>27.75</v>
       </c>
       <c r="AG15">
-        <v>43.03</v>
+        <v>43.02</v>
       </c>
       <c r="AH15">
-        <v>70.31</v>
+        <v>70.290000000000006</v>
       </c>
       <c r="AI15">
-        <v>122.13</v>
+        <v>122.19</v>
       </c>
       <c r="AJ15">
-        <v>174.21</v>
+        <v>174.24</v>
       </c>
       <c r="AK15">
+        <v>190.62</v>
+      </c>
+      <c r="AL15">
         <v>190.6</v>
       </c>
-      <c r="AL15">
-        <v>190.73</v>
-      </c>
       <c r="AM15">
-        <v>183.78</v>
+        <v>183.71</v>
       </c>
       <c r="AN15">
-        <v>170.5</v>
+        <v>170.62</v>
       </c>
       <c r="AO15">
-        <v>172.08</v>
+        <v>172.13</v>
       </c>
       <c r="AP15">
-        <v>209.42</v>
+        <v>209.73</v>
       </c>
       <c r="AQ15">
-        <v>236.22</v>
+        <v>236.55</v>
       </c>
       <c r="AR15">
-        <v>182.61</v>
+        <v>182.67</v>
       </c>
       <c r="AS15">
-        <v>166.84</v>
+        <v>167.02</v>
       </c>
       <c r="AT15">
-        <v>209.67</v>
+        <v>210.62</v>
       </c>
       <c r="AU15">
-        <v>163.33000000000001</v>
+        <v>164.69</v>
+      </c>
+      <c r="AV15">
+        <v>126.46</v>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -6292,7 +6406,7 @@
         <v>10.78</v>
       </c>
       <c r="D16">
-        <v>39.51</v>
+        <v>39.49</v>
       </c>
       <c r="E16">
         <v>53.07</v>
@@ -6301,16 +6415,16 @@
         <v>49.05</v>
       </c>
       <c r="G16">
-        <v>38.130000000000003</v>
+        <v>38.090000000000003</v>
       </c>
       <c r="H16">
-        <v>25.56</v>
+        <v>25.54</v>
       </c>
       <c r="I16">
         <v>19.670000000000002</v>
       </c>
       <c r="J16">
-        <v>13.4</v>
+        <v>13.42</v>
       </c>
       <c r="K16">
         <v>10.23</v>
@@ -6337,7 +6451,7 @@
         <v>6.4</v>
       </c>
       <c r="S16">
-        <v>6.23</v>
+        <v>6.21</v>
       </c>
       <c r="T16">
         <v>4.47</v>
@@ -6352,7 +6466,7 @@
         <v>10.029999999999999</v>
       </c>
       <c r="X16">
-        <v>11.98</v>
+        <v>11.96</v>
       </c>
       <c r="Y16">
         <v>16.53</v>
@@ -6367,64 +6481,67 @@
         <v>22.86</v>
       </c>
       <c r="AC16">
-        <v>24.28</v>
+        <v>24.26</v>
       </c>
       <c r="AD16">
-        <v>29.21</v>
+        <v>29.22</v>
       </c>
       <c r="AE16">
         <v>28.34</v>
       </c>
       <c r="AF16">
-        <v>34.409999999999997</v>
+        <v>34.369999999999997</v>
       </c>
       <c r="AG16">
         <v>53.05</v>
       </c>
       <c r="AH16">
-        <v>88.27</v>
+        <v>88.23</v>
       </c>
       <c r="AI16">
-        <v>144.03</v>
+        <v>144.07</v>
       </c>
       <c r="AJ16">
-        <v>203.47</v>
+        <v>203.51</v>
       </c>
       <c r="AK16">
-        <v>219.73</v>
+        <v>219.67</v>
       </c>
       <c r="AL16">
-        <v>210.74</v>
+        <v>210.84</v>
       </c>
       <c r="AM16">
-        <v>195.92</v>
+        <v>196</v>
       </c>
       <c r="AN16">
-        <v>177.26</v>
+        <v>177.22</v>
       </c>
       <c r="AO16">
-        <v>179.94</v>
+        <v>179.92</v>
       </c>
       <c r="AP16">
         <v>212.46</v>
       </c>
       <c r="AQ16">
-        <v>238.23</v>
+        <v>238.51</v>
       </c>
       <c r="AR16">
-        <v>185.16</v>
+        <v>185.48</v>
       </c>
       <c r="AS16">
-        <v>166.07</v>
+        <v>166.18</v>
       </c>
       <c r="AT16">
-        <v>212.02</v>
+        <v>212.57</v>
       </c>
       <c r="AU16">
-        <v>167.01</v>
+        <v>168.02</v>
+      </c>
+      <c r="AV16">
+        <v>125.49</v>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -6432,22 +6549,22 @@
         <v>1.52</v>
       </c>
       <c r="C17">
-        <v>7.05</v>
+        <v>7.03</v>
       </c>
       <c r="D17">
-        <v>31.4</v>
+        <v>31.44</v>
       </c>
       <c r="E17">
         <v>49.34</v>
       </c>
       <c r="F17">
-        <v>48.72</v>
+        <v>48.67</v>
       </c>
       <c r="G17">
-        <v>37.58</v>
+        <v>37.6</v>
       </c>
       <c r="H17">
-        <v>26.76</v>
+        <v>26.8</v>
       </c>
       <c r="I17">
         <v>20.87</v>
@@ -6459,7 +6576,7 @@
         <v>11.02</v>
       </c>
       <c r="L17">
-        <v>9.0299999999999994</v>
+        <v>9.0500000000000007</v>
       </c>
       <c r="M17">
         <v>6.81</v>
@@ -6474,7 +6591,7 @@
         <v>5.4</v>
       </c>
       <c r="Q17">
-        <v>8.16</v>
+        <v>8.14</v>
       </c>
       <c r="R17">
         <v>5.64</v>
@@ -6486,10 +6603,10 @@
         <v>5.14</v>
       </c>
       <c r="U17">
-        <v>6.55</v>
+        <v>6.57</v>
       </c>
       <c r="V17">
-        <v>8.1999999999999993</v>
+        <v>8.2200000000000006</v>
       </c>
       <c r="W17">
         <v>11.31</v>
@@ -6501,10 +6618,10 @@
         <v>25.3</v>
       </c>
       <c r="Z17">
-        <v>33.630000000000003</v>
+        <v>33.61</v>
       </c>
       <c r="AA17">
-        <v>28.8</v>
+        <v>28.75</v>
       </c>
       <c r="AB17">
         <v>27.1</v>
@@ -6516,13 +6633,13 @@
         <v>32.96</v>
       </c>
       <c r="AE17">
-        <v>34.39</v>
+        <v>34.35</v>
       </c>
       <c r="AF17">
-        <v>37.65</v>
+        <v>37.69</v>
       </c>
       <c r="AG17">
-        <v>60.58</v>
+        <v>60.61</v>
       </c>
       <c r="AH17">
         <v>95.04</v>
@@ -6531,43 +6648,46 @@
         <v>163.85</v>
       </c>
       <c r="AJ17">
-        <v>226.32</v>
+        <v>226.39</v>
       </c>
       <c r="AK17">
-        <v>254.86</v>
+        <v>254.84</v>
       </c>
       <c r="AL17">
-        <v>239.67</v>
+        <v>239.58</v>
       </c>
       <c r="AM17">
-        <v>221.92</v>
+        <v>221.79</v>
       </c>
       <c r="AN17">
-        <v>194.21</v>
+        <v>194.19</v>
       </c>
       <c r="AO17">
-        <v>199.35</v>
+        <v>199.24</v>
       </c>
       <c r="AP17">
-        <v>233.85</v>
+        <v>234.14</v>
       </c>
       <c r="AQ17">
-        <v>262.67</v>
+        <v>262.45</v>
       </c>
       <c r="AR17">
-        <v>196.31</v>
+        <v>196.44</v>
       </c>
       <c r="AS17">
-        <v>186.44</v>
+        <v>186.61</v>
       </c>
       <c r="AT17">
-        <v>235.83</v>
+        <v>236.41</v>
       </c>
       <c r="AU17">
-        <v>183.12</v>
+        <v>184.49</v>
+      </c>
+      <c r="AV17">
+        <v>139.77000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -6575,7 +6695,7 @@
         <v>1.07</v>
       </c>
       <c r="C18">
-        <v>4.59</v>
+        <v>4.62</v>
       </c>
       <c r="D18">
         <v>13.73</v>
@@ -6584,7 +6704,7 @@
         <v>23.86</v>
       </c>
       <c r="F18">
-        <v>27.42</v>
+        <v>27.39</v>
       </c>
       <c r="G18">
         <v>21.76</v>
@@ -6611,19 +6731,19 @@
         <v>4.1100000000000003</v>
       </c>
       <c r="O18">
-        <v>4.1100000000000003</v>
+        <v>4.09</v>
       </c>
       <c r="P18">
         <v>2.82</v>
       </c>
       <c r="Q18">
-        <v>6.14</v>
+        <v>6.12</v>
       </c>
       <c r="R18">
         <v>4.29</v>
       </c>
       <c r="S18">
-        <v>3.53</v>
+        <v>3.5</v>
       </c>
       <c r="T18">
         <v>3.78</v>
@@ -6632,7 +6752,7 @@
         <v>4.8499999999999996</v>
       </c>
       <c r="V18">
-        <v>6.3</v>
+        <v>6.27</v>
       </c>
       <c r="W18">
         <v>9.24</v>
@@ -6656,7 +6776,7 @@
         <v>21.15</v>
       </c>
       <c r="AD18">
-        <v>26.25</v>
+        <v>26.3</v>
       </c>
       <c r="AE18">
         <v>26.63</v>
@@ -6665,52 +6785,55 @@
         <v>33.79</v>
       </c>
       <c r="AG18">
-        <v>52.73</v>
+        <v>52.55</v>
       </c>
       <c r="AH18">
-        <v>75.34</v>
+        <v>75.27</v>
       </c>
       <c r="AI18">
-        <v>123.15</v>
+        <v>123.17</v>
       </c>
       <c r="AJ18">
-        <v>182.42</v>
+        <v>182.47</v>
       </c>
       <c r="AK18">
-        <v>213.49</v>
+        <v>213.44</v>
       </c>
       <c r="AL18">
-        <v>220.83</v>
+        <v>220.78</v>
       </c>
       <c r="AM18">
         <v>208.24</v>
       </c>
       <c r="AN18">
-        <v>189.48</v>
+        <v>189.43</v>
       </c>
       <c r="AO18">
         <v>195.93</v>
       </c>
       <c r="AP18">
-        <v>223.98</v>
+        <v>224.18</v>
       </c>
       <c r="AQ18">
-        <v>214.66</v>
+        <v>214.76</v>
       </c>
       <c r="AR18">
         <v>148.35</v>
       </c>
       <c r="AS18">
-        <v>125.89</v>
+        <v>126.04</v>
       </c>
       <c r="AT18">
-        <v>160.69</v>
+        <v>161.6</v>
       </c>
       <c r="AU18">
-        <v>136.07</v>
+        <v>137.16</v>
+      </c>
+      <c r="AV18">
+        <v>105.81</v>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>68</v>
       </c>
@@ -6748,7 +6871,7 @@
         <v>3.16</v>
       </c>
       <c r="M19">
-        <v>2.92</v>
+        <v>2.94</v>
       </c>
       <c r="N19">
         <v>3.21</v>
@@ -6796,64 +6919,67 @@
         <v>11.61</v>
       </c>
       <c r="AC19">
-        <v>13.45</v>
+        <v>13.42</v>
       </c>
       <c r="AD19">
-        <v>14.02</v>
+        <v>13.99</v>
       </c>
       <c r="AE19">
         <v>15.85</v>
       </c>
       <c r="AF19">
-        <v>19.170000000000002</v>
+        <v>19.149999999999999</v>
       </c>
       <c r="AG19">
         <v>30.84</v>
       </c>
       <c r="AH19">
-        <v>44.64</v>
+        <v>44.69</v>
       </c>
       <c r="AI19">
-        <v>74.13</v>
+        <v>74.209999999999994</v>
       </c>
       <c r="AJ19">
-        <v>110.24</v>
+        <v>110.21</v>
       </c>
       <c r="AK19">
         <v>128.94999999999999</v>
       </c>
       <c r="AL19">
-        <v>144.26</v>
+        <v>144.21</v>
       </c>
       <c r="AM19">
-        <v>143.27000000000001</v>
+        <v>143.21</v>
       </c>
       <c r="AN19">
-        <v>139.91999999999999</v>
+        <v>140.02000000000001</v>
       </c>
       <c r="AO19">
-        <v>139.16</v>
+        <v>139.24</v>
       </c>
       <c r="AP19">
-        <v>153.19999999999999</v>
+        <v>153.22999999999999</v>
       </c>
       <c r="AQ19">
-        <v>141.86000000000001</v>
+        <v>142</v>
       </c>
       <c r="AR19">
-        <v>90.9</v>
+        <v>91.04</v>
       </c>
       <c r="AS19">
-        <v>71.13</v>
+        <v>71.3</v>
       </c>
       <c r="AT19">
-        <v>88.88</v>
+        <v>89.28</v>
       </c>
       <c r="AU19">
-        <v>72.67</v>
+        <v>73.400000000000006</v>
+      </c>
+      <c r="AV19">
+        <v>59.44</v>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>67</v>
       </c>
@@ -6870,7 +6996,7 @@
         <v>6.68</v>
       </c>
       <c r="F20">
-        <v>7.83</v>
+        <v>7.86</v>
       </c>
       <c r="G20">
         <v>6.33</v>
@@ -6960,43 +7086,46 @@
         <v>49.18</v>
       </c>
       <c r="AJ20">
-        <v>74.86</v>
+        <v>74.91</v>
       </c>
       <c r="AK20">
         <v>90.15</v>
       </c>
       <c r="AL20">
-        <v>97.02</v>
+        <v>97.05</v>
       </c>
       <c r="AM20">
-        <v>105.05</v>
+        <v>105.02</v>
       </c>
       <c r="AN20">
         <v>102.31</v>
       </c>
       <c r="AO20">
-        <v>98.58</v>
+        <v>98.66</v>
       </c>
       <c r="AP20">
-        <v>113.82</v>
+        <v>114.09</v>
       </c>
       <c r="AQ20">
-        <v>115.11</v>
+        <v>115.48</v>
       </c>
       <c r="AR20">
-        <v>80.44</v>
+        <v>80.63</v>
       </c>
       <c r="AS20">
-        <v>51.81</v>
+        <v>51.92</v>
       </c>
       <c r="AT20">
-        <v>63.64</v>
+        <v>64.23</v>
       </c>
       <c r="AU20">
-        <v>58.41</v>
+        <v>59</v>
+      </c>
+      <c r="AV20">
+        <v>50.5</v>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -7007,7 +7136,7 @@
         <v>0.91</v>
       </c>
       <c r="D21">
-        <v>3.61</v>
+        <v>3.58</v>
       </c>
       <c r="E21">
         <v>6.44</v>
@@ -7016,7 +7145,7 @@
         <v>6.89</v>
       </c>
       <c r="G21">
-        <v>5.93</v>
+        <v>5.96</v>
       </c>
       <c r="H21">
         <v>4.0599999999999996</v>
@@ -7067,7 +7196,7 @@
         <v>3.81</v>
       </c>
       <c r="X21">
-        <v>4.8</v>
+        <v>4.7699999999999996</v>
       </c>
       <c r="Y21">
         <v>6.97</v>
@@ -7091,7 +7220,7 @@
         <v>7.62</v>
       </c>
       <c r="AF21">
-        <v>8.18</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="AG21">
         <v>13.2</v>
@@ -7103,44 +7232,46 @@
         <v>36.93</v>
       </c>
       <c r="AJ21">
-        <v>56.75</v>
+        <v>56.82</v>
       </c>
       <c r="AK21">
-        <v>61.14</v>
+        <v>61.06</v>
       </c>
       <c r="AL21">
-        <v>61.27</v>
+        <v>61.29</v>
       </c>
       <c r="AM21">
-        <v>60.11</v>
+        <v>60</v>
       </c>
       <c r="AN21">
         <v>58.97</v>
       </c>
       <c r="AO21">
-        <v>58.54</v>
+        <v>58.44</v>
       </c>
       <c r="AP21">
-        <v>67.959999999999994</v>
+        <v>67.930000000000007</v>
       </c>
       <c r="AQ21">
-        <v>78.680000000000007</v>
+        <v>78.66</v>
       </c>
       <c r="AR21">
-        <v>53.44</v>
+        <v>53.52</v>
       </c>
       <c r="AS21">
-        <v>38.67</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="AT21">
-        <v>48.42</v>
+        <v>48.62</v>
       </c>
       <c r="AU21">
-        <v>46.35</v>
+        <v>46.95</v>
+      </c>
+      <c r="AV21">
+        <v>42.69</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add RKI data downloaded 2021-02-15--13-35-01
</commit_message>
<xml_diff>
--- a/rki-data/RKI-Altersverteilung.xlsx
+++ b/rki-data/RKI-Altersverteilung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20368"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20367"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Wissdaten\RKI_nCoV-Lage\3.Kommunikation\3.7.Lageberichte\2021-02-02\Tabellen für den WEbmaster\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Wissdaten\RKI_nCoV-Lage\3.Kommunikation\3.7.Lageberichte\2021-02-09\Tabellen_für_webmaster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF5C69C-7C6C-42E8-88A4-8CC4C6F1BCAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8068A6C1-62B8-473F-8811-861C309744D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6825" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Erläuterungen" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="73">
   <si>
     <t>Altersgruppe</t>
   </si>
@@ -239,6 +239,9 @@
   </si>
   <si>
     <t>Zur besseren Übersicht werden mit Berichtswoche 46 die altersspezifischen Anteile als 7-Tage-Inzidenz pro 100.000 Einwohner nach Meldewoche dargestellt.</t>
+  </si>
+  <si>
+    <t>2021_5</t>
   </si>
 </sst>
 </file>
@@ -1085,7 +1088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B89A279-CE5A-41E1-B3A8-F46B8367BF07}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1107,7 +1110,7 @@
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
     </row>
-    <row r="4" spans="1:1" ht="165" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>70</v>
       </c>
@@ -1119,15 +1122,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AW21"/>
+  <dimension ref="A1:AX21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="B1" sqref="B1:AX21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1275,52 +1278,55 @@
       <c r="AW1" t="s">
         <v>48</v>
       </c>
+      <c r="AX1" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>49</v>
       </c>
       <c r="B2">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="C2">
-        <v>6431</v>
+        <v>6429</v>
       </c>
       <c r="D2">
-        <v>22436</v>
+        <v>22438</v>
       </c>
       <c r="E2">
-        <v>34021</v>
+        <v>34015</v>
       </c>
       <c r="F2">
-        <v>36097</v>
+        <v>36096</v>
       </c>
       <c r="G2">
-        <v>27189</v>
+        <v>27188</v>
       </c>
       <c r="H2">
-        <v>17370</v>
+        <v>17371</v>
       </c>
       <c r="I2">
         <v>12381</v>
       </c>
       <c r="J2">
-        <v>7456</v>
+        <v>7446</v>
       </c>
       <c r="K2">
-        <v>6236</v>
+        <v>6237</v>
       </c>
       <c r="L2">
-        <v>4754</v>
+        <v>4755</v>
       </c>
       <c r="M2">
         <v>3620</v>
       </c>
       <c r="N2">
-        <v>3210</v>
+        <v>3208</v>
       </c>
       <c r="O2">
-        <v>2359</v>
+        <v>2360</v>
       </c>
       <c r="P2">
         <v>2343</v>
@@ -1332,7 +1338,7 @@
         <v>3213</v>
       </c>
       <c r="S2">
-        <v>2695</v>
+        <v>2696</v>
       </c>
       <c r="T2">
         <v>2427</v>
@@ -1341,91 +1347,94 @@
         <v>3025</v>
       </c>
       <c r="V2">
-        <v>3941</v>
+        <v>3939</v>
       </c>
       <c r="W2">
         <v>4823</v>
       </c>
       <c r="X2">
-        <v>6062</v>
+        <v>6061</v>
       </c>
       <c r="Y2">
-        <v>7959</v>
+        <v>7960</v>
       </c>
       <c r="Z2">
-        <v>9602</v>
+        <v>9601</v>
       </c>
       <c r="AA2">
         <v>8822</v>
       </c>
       <c r="AB2">
-        <v>8625</v>
+        <v>8626</v>
       </c>
       <c r="AC2">
-        <v>9775</v>
+        <v>9777</v>
       </c>
       <c r="AD2">
-        <v>12295</v>
+        <v>12298</v>
       </c>
       <c r="AE2">
         <v>13078</v>
       </c>
       <c r="AF2">
-        <v>15930</v>
+        <v>15933</v>
       </c>
       <c r="AG2">
-        <v>26155</v>
+        <v>26154</v>
       </c>
       <c r="AH2">
-        <v>42097</v>
+        <v>42098</v>
       </c>
       <c r="AI2">
-        <v>74864</v>
+        <v>74872</v>
       </c>
       <c r="AJ2">
-        <v>111149</v>
+        <v>111173</v>
       </c>
       <c r="AK2">
-        <v>125817</v>
+        <v>125830</v>
       </c>
       <c r="AL2">
-        <v>127872</v>
+        <v>127897</v>
       </c>
       <c r="AM2">
-        <v>128501</v>
+        <v>128503</v>
       </c>
       <c r="AN2">
-        <v>123332</v>
+        <v>123351</v>
       </c>
       <c r="AO2">
-        <v>128481</v>
+        <v>128508</v>
       </c>
       <c r="AP2">
-        <v>156473</v>
+        <v>156495</v>
       </c>
       <c r="AQ2">
-        <v>175062</v>
+        <v>175072</v>
       </c>
       <c r="AR2">
-        <v>139328</v>
+        <v>139432</v>
       </c>
       <c r="AS2">
-        <v>123296</v>
+        <v>123372</v>
       </c>
       <c r="AT2">
-        <v>145635</v>
+        <v>145701</v>
       </c>
       <c r="AU2">
-        <v>119135</v>
+        <v>119233</v>
       </c>
       <c r="AV2">
-        <v>95779</v>
+        <v>95768</v>
       </c>
       <c r="AW2">
-        <v>78124</v>
+        <v>78515</v>
+      </c>
+      <c r="AX2">
+        <v>64440</v>
       </c>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -1433,7 +1442,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3">
         <v>100</v>
@@ -1451,16 +1460,16 @@
         <v>848</v>
       </c>
       <c r="I3">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="J3">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="K3">
         <v>208</v>
       </c>
       <c r="L3">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="M3">
         <v>103</v>
@@ -1523,58 +1532,61 @@
         <v>119</v>
       </c>
       <c r="AG3">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AH3">
         <v>436</v>
       </c>
       <c r="AI3">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="AJ3">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="AK3">
-        <v>1717</v>
+        <v>1719</v>
       </c>
       <c r="AL3">
-        <v>2323</v>
+        <v>2325</v>
       </c>
       <c r="AM3">
-        <v>3071</v>
+        <v>3075</v>
       </c>
       <c r="AN3">
-        <v>3518</v>
+        <v>3517</v>
       </c>
       <c r="AO3">
-        <v>4194</v>
+        <v>4196</v>
       </c>
       <c r="AP3">
-        <v>5413</v>
+        <v>5412</v>
       </c>
       <c r="AQ3">
-        <v>5993</v>
+        <v>5989</v>
       </c>
       <c r="AR3">
-        <v>5285</v>
+        <v>5289</v>
       </c>
       <c r="AS3">
-        <v>4981</v>
+        <v>4988</v>
       </c>
       <c r="AT3">
-        <v>5404</v>
+        <v>5427</v>
       </c>
       <c r="AU3">
-        <v>5045</v>
+        <v>5055</v>
       </c>
       <c r="AV3">
-        <v>3968</v>
+        <v>3964</v>
       </c>
       <c r="AW3">
-        <v>2886</v>
+        <v>2894</v>
+      </c>
+      <c r="AX3">
+        <v>1939</v>
       </c>
     </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -1600,16 +1612,16 @@
         <v>927</v>
       </c>
       <c r="I4">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="J4">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="K4">
         <v>263</v>
       </c>
       <c r="L4">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M4">
         <v>127</v>
@@ -1639,7 +1651,7 @@
         <v>24</v>
       </c>
       <c r="V4">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="W4">
         <v>41</v>
@@ -1681,49 +1693,52 @@
         <v>1144</v>
       </c>
       <c r="AJ4">
-        <v>1778</v>
+        <v>1779</v>
       </c>
       <c r="AK4">
         <v>2293</v>
       </c>
       <c r="AL4">
-        <v>2833</v>
+        <v>2836</v>
       </c>
       <c r="AM4">
-        <v>3368</v>
+        <v>3371</v>
       </c>
       <c r="AN4">
-        <v>4105</v>
+        <v>4102</v>
       </c>
       <c r="AO4">
-        <v>4600</v>
+        <v>4599</v>
       </c>
       <c r="AP4">
-        <v>5913</v>
+        <v>5915</v>
       </c>
       <c r="AQ4">
-        <v>6954</v>
+        <v>6957</v>
       </c>
       <c r="AR4">
-        <v>5864</v>
+        <v>5865</v>
       </c>
       <c r="AS4">
         <v>5609</v>
       </c>
       <c r="AT4">
-        <v>6087</v>
+        <v>6093</v>
       </c>
       <c r="AU4">
         <v>5572</v>
       </c>
       <c r="AV4">
-        <v>4462</v>
+        <v>4461</v>
       </c>
       <c r="AW4">
-        <v>3317</v>
+        <v>3332</v>
+      </c>
+      <c r="AX4">
+        <v>2579</v>
       </c>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -1731,19 +1746,19 @@
         <v>12</v>
       </c>
       <c r="C5">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D5">
         <v>468</v>
       </c>
       <c r="E5">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="F5">
         <v>1964</v>
       </c>
       <c r="G5">
-        <v>1719</v>
+        <v>1720</v>
       </c>
       <c r="H5">
         <v>1182</v>
@@ -1764,7 +1779,7 @@
         <v>152</v>
       </c>
       <c r="N5">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="O5">
         <v>76</v>
@@ -1827,7 +1842,7 @@
         <v>857</v>
       </c>
       <c r="AI5">
-        <v>1837</v>
+        <v>1835</v>
       </c>
       <c r="AJ5">
         <v>2843</v>
@@ -1836,7 +1851,7 @@
         <v>3436</v>
       </c>
       <c r="AL5">
-        <v>3806</v>
+        <v>3807</v>
       </c>
       <c r="AM5">
         <v>4361</v>
@@ -1845,34 +1860,37 @@
         <v>4792</v>
       </c>
       <c r="AO5">
-        <v>5442</v>
+        <v>5444</v>
       </c>
       <c r="AP5">
-        <v>7076</v>
+        <v>7079</v>
       </c>
       <c r="AQ5">
         <v>8286</v>
       </c>
       <c r="AR5">
-        <v>7450</v>
+        <v>7457</v>
       </c>
       <c r="AS5">
-        <v>6881</v>
+        <v>6900</v>
       </c>
       <c r="AT5">
-        <v>7679</v>
+        <v>7683</v>
       </c>
       <c r="AU5">
-        <v>6696</v>
+        <v>6705</v>
       </c>
       <c r="AV5">
-        <v>5341</v>
+        <v>5333</v>
       </c>
       <c r="AW5">
-        <v>4169</v>
+        <v>4207</v>
+      </c>
+      <c r="AX5">
+        <v>3128</v>
       </c>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -1901,7 +1919,7 @@
         <v>587</v>
       </c>
       <c r="J6">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="K6">
         <v>274</v>
@@ -1910,7 +1928,7 @@
         <v>176</v>
       </c>
       <c r="M6">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="N6">
         <v>82</v>
@@ -1967,7 +1985,7 @@
         <v>232</v>
       </c>
       <c r="AF6">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="AG6">
         <v>507</v>
@@ -1976,52 +1994,55 @@
         <v>903</v>
       </c>
       <c r="AI6">
-        <v>1630</v>
+        <v>1629</v>
       </c>
       <c r="AJ6">
-        <v>2650</v>
+        <v>2651</v>
       </c>
       <c r="AK6">
-        <v>3050</v>
+        <v>3054</v>
       </c>
       <c r="AL6">
-        <v>3291</v>
+        <v>3293</v>
       </c>
       <c r="AM6">
-        <v>3384</v>
+        <v>3386</v>
       </c>
       <c r="AN6">
         <v>3494</v>
       </c>
       <c r="AO6">
-        <v>3972</v>
+        <v>3971</v>
       </c>
       <c r="AP6">
-        <v>4996</v>
+        <v>5000</v>
       </c>
       <c r="AQ6">
-        <v>5953</v>
+        <v>5950</v>
       </c>
       <c r="AR6">
-        <v>5111</v>
+        <v>5119</v>
       </c>
       <c r="AS6">
-        <v>4645</v>
+        <v>4642</v>
       </c>
       <c r="AT6">
-        <v>5241</v>
+        <v>5243</v>
       </c>
       <c r="AU6">
-        <v>4323</v>
+        <v>4320</v>
       </c>
       <c r="AV6">
-        <v>3423</v>
+        <v>3418</v>
       </c>
       <c r="AW6">
-        <v>2802</v>
+        <v>2821</v>
+      </c>
+      <c r="AX6">
+        <v>2192</v>
       </c>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -2032,7 +2053,7 @@
         <v>145</v>
       </c>
       <c r="D7">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="E7">
         <v>1327</v>
@@ -2050,13 +2071,13 @@
         <v>424</v>
       </c>
       <c r="J7">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K7">
         <v>207</v>
       </c>
       <c r="L7">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="M7">
         <v>92</v>
@@ -2086,10 +2107,10 @@
         <v>61</v>
       </c>
       <c r="V7">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="W7">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="X7">
         <v>91</v>
@@ -2125,16 +2146,16 @@
         <v>933</v>
       </c>
       <c r="AI7">
-        <v>1795</v>
+        <v>1796</v>
       </c>
       <c r="AJ7">
-        <v>2882</v>
+        <v>2887</v>
       </c>
       <c r="AK7">
         <v>3176</v>
       </c>
       <c r="AL7">
-        <v>3293</v>
+        <v>3291</v>
       </c>
       <c r="AM7">
         <v>3362</v>
@@ -2143,34 +2164,37 @@
         <v>3202</v>
       </c>
       <c r="AO7">
-        <v>3479</v>
+        <v>3481</v>
       </c>
       <c r="AP7">
-        <v>4393</v>
+        <v>4395</v>
       </c>
       <c r="AQ7">
-        <v>5175</v>
+        <v>5180</v>
       </c>
       <c r="AR7">
-        <v>4454</v>
+        <v>4461</v>
       </c>
       <c r="AS7">
-        <v>4143</v>
+        <v>4149</v>
       </c>
       <c r="AT7">
-        <v>4837</v>
+        <v>4832</v>
       </c>
       <c r="AU7">
-        <v>3661</v>
+        <v>3668</v>
       </c>
       <c r="AV7">
-        <v>3082</v>
+        <v>3078</v>
       </c>
       <c r="AW7">
         <v>2491</v>
       </c>
+      <c r="AX7">
+        <v>2051</v>
+      </c>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -2187,7 +2211,7 @@
         <v>1647</v>
       </c>
       <c r="F8">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="G8">
         <v>1116</v>
@@ -2196,7 +2220,7 @@
         <v>662</v>
       </c>
       <c r="I8">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="J8">
         <v>266</v>
@@ -2208,7 +2232,7 @@
         <v>146</v>
       </c>
       <c r="M8">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N8">
         <v>107</v>
@@ -2220,7 +2244,7 @@
         <v>51</v>
       </c>
       <c r="Q8">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="R8">
         <v>65</v>
@@ -2238,7 +2262,7 @@
         <v>85</v>
       </c>
       <c r="W8">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="X8">
         <v>121</v>
@@ -2256,7 +2280,7 @@
         <v>128</v>
       </c>
       <c r="AC8">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="AD8">
         <v>290</v>
@@ -2274,52 +2298,55 @@
         <v>1286</v>
       </c>
       <c r="AI8">
-        <v>2270</v>
+        <v>2271</v>
       </c>
       <c r="AJ8">
-        <v>3550</v>
+        <v>3551</v>
       </c>
       <c r="AK8">
-        <v>4250</v>
+        <v>4249</v>
       </c>
       <c r="AL8">
         <v>4017</v>
       </c>
       <c r="AM8">
-        <v>4148</v>
+        <v>4151</v>
       </c>
       <c r="AN8">
         <v>4138</v>
       </c>
       <c r="AO8">
-        <v>4129</v>
+        <v>4126</v>
       </c>
       <c r="AP8">
-        <v>5165</v>
+        <v>5171</v>
       </c>
       <c r="AQ8">
-        <v>6352</v>
+        <v>6350</v>
       </c>
       <c r="AR8">
-        <v>5592</v>
+        <v>5594</v>
       </c>
       <c r="AS8">
-        <v>4979</v>
+        <v>4982</v>
       </c>
       <c r="AT8">
-        <v>5713</v>
+        <v>5717</v>
       </c>
       <c r="AU8">
-        <v>4421</v>
+        <v>4420</v>
       </c>
       <c r="AV8">
-        <v>3629</v>
+        <v>3627</v>
       </c>
       <c r="AW8">
-        <v>3108</v>
+        <v>3137</v>
+      </c>
+      <c r="AX8">
+        <v>2508</v>
       </c>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -2348,7 +2375,7 @@
         <v>674</v>
       </c>
       <c r="J9">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="K9">
         <v>332</v>
@@ -2417,58 +2444,61 @@
         <v>682</v>
       </c>
       <c r="AG9">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="AH9">
         <v>2120</v>
       </c>
       <c r="AI9">
-        <v>3958</v>
+        <v>3959</v>
       </c>
       <c r="AJ9">
-        <v>5995</v>
+        <v>5996</v>
       </c>
       <c r="AK9">
-        <v>6850</v>
+        <v>6852</v>
       </c>
       <c r="AL9">
-        <v>6905</v>
+        <v>6907</v>
       </c>
       <c r="AM9">
-        <v>7302</v>
+        <v>7306</v>
       </c>
       <c r="AN9">
-        <v>6998</v>
+        <v>6999</v>
       </c>
       <c r="AO9">
-        <v>7655</v>
+        <v>7656</v>
       </c>
       <c r="AP9">
         <v>9426</v>
       </c>
       <c r="AQ9">
-        <v>11028</v>
+        <v>11029</v>
       </c>
       <c r="AR9">
-        <v>9186</v>
+        <v>9199</v>
       </c>
       <c r="AS9">
-        <v>8277</v>
+        <v>8279</v>
       </c>
       <c r="AT9">
-        <v>9273</v>
+        <v>9277</v>
       </c>
       <c r="AU9">
-        <v>7525</v>
+        <v>7535</v>
       </c>
       <c r="AV9">
-        <v>6228</v>
+        <v>6239</v>
       </c>
       <c r="AW9">
-        <v>5105</v>
+        <v>5137</v>
+      </c>
+      <c r="AX9">
+        <v>4188</v>
       </c>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -2476,16 +2506,16 @@
         <v>75</v>
       </c>
       <c r="C10">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="D10">
-        <v>2600</v>
+        <v>2599</v>
       </c>
       <c r="E10">
         <v>3595</v>
       </c>
       <c r="F10">
-        <v>3667</v>
+        <v>3668</v>
       </c>
       <c r="G10">
         <v>2610</v>
@@ -2497,7 +2527,7 @@
         <v>1060</v>
       </c>
       <c r="J10">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="K10">
         <v>511</v>
@@ -2539,7 +2569,7 @@
         <v>285</v>
       </c>
       <c r="X10">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="Y10">
         <v>326</v>
@@ -2554,19 +2584,19 @@
         <v>393</v>
       </c>
       <c r="AC10">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="AD10">
         <v>762</v>
       </c>
       <c r="AE10">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="AF10">
         <v>1107</v>
       </c>
       <c r="AG10">
-        <v>1870</v>
+        <v>1871</v>
       </c>
       <c r="AH10">
         <v>2999</v>
@@ -2575,10 +2605,10 @@
         <v>5758</v>
       </c>
       <c r="AJ10">
-        <v>8965</v>
+        <v>8971</v>
       </c>
       <c r="AK10">
-        <v>10156</v>
+        <v>10157</v>
       </c>
       <c r="AL10">
         <v>10303</v>
@@ -2587,37 +2617,40 @@
         <v>10242</v>
       </c>
       <c r="AN10">
-        <v>9872</v>
+        <v>9880</v>
       </c>
       <c r="AO10">
-        <v>10353</v>
+        <v>10364</v>
       </c>
       <c r="AP10">
-        <v>13063</v>
+        <v>13065</v>
       </c>
       <c r="AQ10">
-        <v>15005</v>
+        <v>15014</v>
       </c>
       <c r="AR10">
-        <v>12364</v>
+        <v>12377</v>
       </c>
       <c r="AS10">
-        <v>11082</v>
+        <v>11088</v>
       </c>
       <c r="AT10">
-        <v>12326</v>
+        <v>12335</v>
       </c>
       <c r="AU10">
-        <v>10041</v>
+        <v>10048</v>
       </c>
       <c r="AV10">
-        <v>8366</v>
+        <v>8363</v>
       </c>
       <c r="AW10">
-        <v>6999</v>
+        <v>7047</v>
+      </c>
+      <c r="AX10">
+        <v>5802</v>
       </c>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -2628,10 +2661,10 @@
         <v>980</v>
       </c>
       <c r="D11">
-        <v>3094</v>
+        <v>3092</v>
       </c>
       <c r="E11">
-        <v>4000</v>
+        <v>3999</v>
       </c>
       <c r="F11">
         <v>3700</v>
@@ -2643,7 +2676,7 @@
         <v>1560</v>
       </c>
       <c r="I11">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="J11">
         <v>605</v>
@@ -2682,7 +2715,7 @@
         <v>211</v>
       </c>
       <c r="V11">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="W11">
         <v>352</v>
@@ -2703,7 +2736,7 @@
         <v>553</v>
       </c>
       <c r="AC11">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="AD11">
         <v>897</v>
@@ -2715,7 +2748,7 @@
         <v>1206</v>
       </c>
       <c r="AG11">
-        <v>2267</v>
+        <v>2268</v>
       </c>
       <c r="AH11">
         <v>3571</v>
@@ -2724,63 +2757,66 @@
         <v>6415</v>
       </c>
       <c r="AJ11">
-        <v>9776</v>
+        <v>9780</v>
       </c>
       <c r="AK11">
-        <v>10953</v>
+        <v>10957</v>
       </c>
       <c r="AL11">
-        <v>10991</v>
+        <v>11002</v>
       </c>
       <c r="AM11">
-        <v>10829</v>
+        <v>10824</v>
       </c>
       <c r="AN11">
-        <v>10338</v>
+        <v>10345</v>
       </c>
       <c r="AO11">
-        <v>10550</v>
+        <v>10552</v>
       </c>
       <c r="AP11">
-        <v>13244</v>
+        <v>13245</v>
       </c>
       <c r="AQ11">
-        <v>14914</v>
+        <v>14922</v>
       </c>
       <c r="AR11">
-        <v>11980</v>
+        <v>11997</v>
       </c>
       <c r="AS11">
-        <v>10520</v>
+        <v>10537</v>
       </c>
       <c r="AT11">
-        <v>12084</v>
+        <v>12085</v>
       </c>
       <c r="AU11">
-        <v>9788</v>
+        <v>9795</v>
       </c>
       <c r="AV11">
         <v>8181</v>
       </c>
       <c r="AW11">
-        <v>6665</v>
+        <v>6693</v>
+      </c>
+      <c r="AX11">
+        <v>5278</v>
       </c>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>59</v>
       </c>
       <c r="B12">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C12">
         <v>740</v>
       </c>
       <c r="D12">
-        <v>2099</v>
+        <v>2102</v>
       </c>
       <c r="E12">
-        <v>2923</v>
+        <v>2922</v>
       </c>
       <c r="F12">
         <v>2721</v>
@@ -2792,7 +2828,7 @@
         <v>1174</v>
       </c>
       <c r="I12">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="J12">
         <v>469</v>
@@ -2852,7 +2888,7 @@
         <v>614</v>
       </c>
       <c r="AC12">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="AD12">
         <v>874</v>
@@ -2864,19 +2900,19 @@
         <v>1199</v>
       </c>
       <c r="AG12">
-        <v>2039</v>
+        <v>2040</v>
       </c>
       <c r="AH12">
-        <v>3131</v>
+        <v>3132</v>
       </c>
       <c r="AI12">
-        <v>5811</v>
+        <v>5810</v>
       </c>
       <c r="AJ12">
-        <v>8386</v>
+        <v>8388</v>
       </c>
       <c r="AK12">
-        <v>9474</v>
+        <v>9471</v>
       </c>
       <c r="AL12">
         <v>9288</v>
@@ -2885,69 +2921,72 @@
         <v>9670</v>
       </c>
       <c r="AN12">
-        <v>9060</v>
+        <v>9064</v>
       </c>
       <c r="AO12">
-        <v>9230</v>
+        <v>9233</v>
       </c>
       <c r="AP12">
-        <v>11087</v>
+        <v>11088</v>
       </c>
       <c r="AQ12">
-        <v>12437</v>
+        <v>12441</v>
       </c>
       <c r="AR12">
-        <v>9726</v>
+        <v>9729</v>
       </c>
       <c r="AS12">
-        <v>8543</v>
+        <v>8556</v>
       </c>
       <c r="AT12">
-        <v>9796</v>
+        <v>9799</v>
       </c>
       <c r="AU12">
-        <v>7975</v>
+        <v>7985</v>
       </c>
       <c r="AV12">
-        <v>6460</v>
+        <v>6469</v>
       </c>
       <c r="AW12">
-        <v>5292</v>
+        <v>5330</v>
+      </c>
+      <c r="AX12">
+        <v>4473</v>
       </c>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>60</v>
       </c>
       <c r="B13">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C13">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D13">
         <v>1804</v>
       </c>
       <c r="E13">
-        <v>2331</v>
+        <v>2330</v>
       </c>
       <c r="F13">
-        <v>2310</v>
+        <v>2309</v>
       </c>
       <c r="G13">
         <v>1675</v>
       </c>
       <c r="H13">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="I13">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="J13">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="K13">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="L13">
         <v>356</v>
@@ -2980,13 +3019,13 @@
         <v>252</v>
       </c>
       <c r="V13">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="W13">
         <v>429</v>
       </c>
       <c r="X13">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="Y13">
         <v>642</v>
@@ -2998,13 +3037,13 @@
         <v>661</v>
       </c>
       <c r="AB13">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="AC13">
         <v>688</v>
       </c>
       <c r="AD13">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="AE13">
         <v>861</v>
@@ -3013,58 +3052,61 @@
         <v>1050</v>
       </c>
       <c r="AG13">
-        <v>1868</v>
+        <v>1870</v>
       </c>
       <c r="AH13">
-        <v>2907</v>
+        <v>2908</v>
       </c>
       <c r="AI13">
-        <v>5298</v>
+        <v>5301</v>
       </c>
       <c r="AJ13">
-        <v>7872</v>
+        <v>7874</v>
       </c>
       <c r="AK13">
-        <v>8874</v>
+        <v>8877</v>
       </c>
       <c r="AL13">
-        <v>8980</v>
+        <v>8981</v>
       </c>
       <c r="AM13">
         <v>9236</v>
       </c>
       <c r="AN13">
-        <v>8800</v>
+        <v>8804</v>
       </c>
       <c r="AO13">
-        <v>8827</v>
+        <v>8831</v>
       </c>
       <c r="AP13">
-        <v>10892</v>
+        <v>10893</v>
       </c>
       <c r="AQ13">
-        <v>12001</v>
+        <v>12006</v>
       </c>
       <c r="AR13">
-        <v>9515</v>
+        <v>9532</v>
       </c>
       <c r="AS13">
-        <v>8039</v>
+        <v>8043</v>
       </c>
       <c r="AT13">
-        <v>9524</v>
+        <v>9522</v>
       </c>
       <c r="AU13">
         <v>7568</v>
       </c>
       <c r="AV13">
-        <v>6238</v>
+        <v>6239</v>
       </c>
       <c r="AW13">
-        <v>5121</v>
+        <v>5135</v>
+      </c>
+      <c r="AX13">
+        <v>4275</v>
       </c>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>61</v>
       </c>
@@ -3072,13 +3114,13 @@
         <v>66</v>
       </c>
       <c r="C14">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D14">
-        <v>1756</v>
+        <v>1755</v>
       </c>
       <c r="E14">
-        <v>2385</v>
+        <v>2384</v>
       </c>
       <c r="F14">
         <v>2206</v>
@@ -3120,7 +3162,7 @@
         <v>298</v>
       </c>
       <c r="S14">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="T14">
         <v>206</v>
@@ -3159,61 +3201,64 @@
         <v>1007</v>
       </c>
       <c r="AF14">
-        <v>1153</v>
+        <v>1155</v>
       </c>
       <c r="AG14">
-        <v>1825</v>
+        <v>1827</v>
       </c>
       <c r="AH14">
         <v>3106</v>
       </c>
       <c r="AI14">
-        <v>5393</v>
+        <v>5395</v>
       </c>
       <c r="AJ14">
-        <v>8081</v>
+        <v>8082</v>
       </c>
       <c r="AK14">
-        <v>8953</v>
+        <v>8955</v>
       </c>
       <c r="AL14">
-        <v>9176</v>
+        <v>9179</v>
       </c>
       <c r="AM14">
-        <v>9194</v>
+        <v>9198</v>
       </c>
       <c r="AN14">
-        <v>8723</v>
+        <v>8718</v>
       </c>
       <c r="AO14">
-        <v>9137</v>
+        <v>9139</v>
       </c>
       <c r="AP14">
-        <v>10982</v>
+        <v>10992</v>
       </c>
       <c r="AQ14">
-        <v>12224</v>
+        <v>12228</v>
       </c>
       <c r="AR14">
-        <v>9513</v>
+        <v>9524</v>
       </c>
       <c r="AS14">
-        <v>8102</v>
+        <v>8106</v>
       </c>
       <c r="AT14">
-        <v>10126</v>
+        <v>10134</v>
       </c>
       <c r="AU14">
-        <v>8027</v>
+        <v>8036</v>
       </c>
       <c r="AV14">
-        <v>6352</v>
+        <v>6355</v>
       </c>
       <c r="AW14">
-        <v>5215</v>
+        <v>5228</v>
+      </c>
+      <c r="AX14">
+        <v>4448</v>
       </c>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -3224,10 +3269,10 @@
         <v>534</v>
       </c>
       <c r="D15">
-        <v>2050</v>
+        <v>2051</v>
       </c>
       <c r="E15">
-        <v>2639</v>
+        <v>2638</v>
       </c>
       <c r="F15">
         <v>2419</v>
@@ -3269,7 +3314,7 @@
         <v>334</v>
       </c>
       <c r="S15">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="T15">
         <v>259</v>
@@ -3284,7 +3329,7 @@
         <v>424</v>
       </c>
       <c r="X15">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="Y15">
         <v>700</v>
@@ -3296,81 +3341,84 @@
         <v>856</v>
       </c>
       <c r="AB15">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="AC15">
         <v>942</v>
       </c>
       <c r="AD15">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="AE15">
         <v>1303</v>
       </c>
       <c r="AF15">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="AG15">
-        <v>2365</v>
+        <v>2363</v>
       </c>
       <c r="AH15">
         <v>3863</v>
       </c>
       <c r="AI15">
-        <v>6715</v>
+        <v>6718</v>
       </c>
       <c r="AJ15">
         <v>9576</v>
       </c>
       <c r="AK15">
-        <v>10479</v>
+        <v>10477</v>
       </c>
       <c r="AL15">
-        <v>10482</v>
+        <v>10488</v>
       </c>
       <c r="AM15">
-        <v>10098</v>
+        <v>10094</v>
       </c>
       <c r="AN15">
         <v>9381</v>
       </c>
       <c r="AO15">
-        <v>9465</v>
+        <v>9472</v>
       </c>
       <c r="AP15">
-        <v>11530</v>
+        <v>11532</v>
       </c>
       <c r="AQ15">
-        <v>13025</v>
+        <v>13024</v>
       </c>
       <c r="AR15">
-        <v>10053</v>
+        <v>10059</v>
       </c>
       <c r="AS15">
-        <v>9191</v>
+        <v>9193</v>
       </c>
       <c r="AT15">
-        <v>11601</v>
+        <v>11611</v>
       </c>
       <c r="AU15">
-        <v>9061</v>
+        <v>9067</v>
       </c>
       <c r="AV15">
-        <v>7025</v>
+        <v>7039</v>
       </c>
       <c r="AW15">
-        <v>5771</v>
+        <v>5804</v>
+      </c>
+      <c r="AX15">
+        <v>4906</v>
       </c>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>63</v>
       </c>
       <c r="B16">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C16">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D16">
         <v>2004</v>
@@ -3379,10 +3427,10 @@
         <v>2693</v>
       </c>
       <c r="F16">
-        <v>2489</v>
+        <v>2488</v>
       </c>
       <c r="G16">
-        <v>1935</v>
+        <v>1934</v>
       </c>
       <c r="H16">
         <v>1296</v>
@@ -3397,7 +3445,7 @@
         <v>519</v>
       </c>
       <c r="L16">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="M16">
         <v>350</v>
@@ -3427,19 +3475,19 @@
         <v>308</v>
       </c>
       <c r="V16">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="W16">
         <v>509</v>
       </c>
       <c r="X16">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="Y16">
         <v>839</v>
       </c>
       <c r="Z16">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="AA16">
         <v>1223</v>
@@ -3448,7 +3496,7 @@
         <v>1160</v>
       </c>
       <c r="AC16">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="AD16">
         <v>1484</v>
@@ -3457,61 +3505,64 @@
         <v>1440</v>
       </c>
       <c r="AF16">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="AG16">
-        <v>2691</v>
+        <v>2689</v>
       </c>
       <c r="AH16">
-        <v>4478</v>
+        <v>4479</v>
       </c>
       <c r="AI16">
-        <v>7314</v>
+        <v>7317</v>
       </c>
       <c r="AJ16">
-        <v>10328</v>
+        <v>10334</v>
       </c>
       <c r="AK16">
-        <v>11146</v>
+        <v>11147</v>
       </c>
       <c r="AL16">
-        <v>10702</v>
+        <v>10703</v>
       </c>
       <c r="AM16">
-        <v>9941</v>
+        <v>9944</v>
       </c>
       <c r="AN16">
-        <v>8999</v>
+        <v>9001</v>
       </c>
       <c r="AO16">
-        <v>9133</v>
+        <v>9137</v>
       </c>
       <c r="AP16">
-        <v>10789</v>
+        <v>10792</v>
       </c>
       <c r="AQ16">
-        <v>12119</v>
+        <v>12121</v>
       </c>
       <c r="AR16">
-        <v>9441</v>
+        <v>9444</v>
       </c>
       <c r="AS16">
-        <v>8445</v>
+        <v>8440</v>
       </c>
       <c r="AT16">
-        <v>10802</v>
+        <v>10804</v>
       </c>
       <c r="AU16">
-        <v>8545</v>
+        <v>8559</v>
       </c>
       <c r="AV16">
-        <v>6407</v>
+        <v>6413</v>
       </c>
       <c r="AW16">
-        <v>5335</v>
+        <v>5359</v>
+      </c>
+      <c r="AX16">
+        <v>4477</v>
       </c>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>64</v>
       </c>
@@ -3522,22 +3573,22 @@
         <v>325</v>
       </c>
       <c r="D17">
-        <v>1448</v>
+        <v>1450</v>
       </c>
       <c r="E17">
         <v>2274</v>
       </c>
       <c r="F17">
-        <v>2242</v>
+        <v>2243</v>
       </c>
       <c r="G17">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="H17">
         <v>1235</v>
       </c>
       <c r="I17">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="J17">
         <v>595</v>
@@ -3555,19 +3606,19 @@
         <v>289</v>
       </c>
       <c r="O17">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="P17">
         <v>249</v>
       </c>
       <c r="Q17">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="R17">
         <v>260</v>
       </c>
       <c r="S17">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="T17">
         <v>237</v>
@@ -3585,7 +3636,7 @@
         <v>746</v>
       </c>
       <c r="Y17">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="Z17">
         <v>1548</v>
@@ -3594,19 +3645,19 @@
         <v>1325</v>
       </c>
       <c r="AB17">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="AC17">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="AD17">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="AE17">
         <v>1584</v>
       </c>
       <c r="AF17">
-        <v>1739</v>
+        <v>1741</v>
       </c>
       <c r="AG17">
         <v>2792</v>
@@ -3615,52 +3666,55 @@
         <v>4381</v>
       </c>
       <c r="AI17">
-        <v>7556</v>
+        <v>7557</v>
       </c>
       <c r="AJ17">
-        <v>10433</v>
+        <v>10437</v>
       </c>
       <c r="AK17">
-        <v>11746</v>
+        <v>11745</v>
       </c>
       <c r="AL17">
-        <v>11034</v>
+        <v>11035</v>
       </c>
       <c r="AM17">
-        <v>10219</v>
+        <v>10218</v>
       </c>
       <c r="AN17">
-        <v>8945</v>
+        <v>8946</v>
       </c>
       <c r="AO17">
         <v>9185</v>
       </c>
       <c r="AP17">
-        <v>10786</v>
+        <v>10790</v>
       </c>
       <c r="AQ17">
         <v>12111</v>
       </c>
       <c r="AR17">
-        <v>9073</v>
+        <v>9077</v>
       </c>
       <c r="AS17">
-        <v>8603</v>
+        <v>8610</v>
       </c>
       <c r="AT17">
-        <v>10891</v>
+        <v>10900</v>
       </c>
       <c r="AU17">
-        <v>8517</v>
+        <v>8532</v>
       </c>
       <c r="AV17">
-        <v>6470</v>
+        <v>6459</v>
       </c>
       <c r="AW17">
-        <v>5238</v>
+        <v>5259</v>
+      </c>
+      <c r="AX17">
+        <v>4403</v>
       </c>
     </row>
-    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -3671,7 +3725,7 @@
         <v>183</v>
       </c>
       <c r="D18">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="E18">
         <v>938</v>
@@ -3749,67 +3803,70 @@
         <v>833</v>
       </c>
       <c r="AD18">
-        <v>1036</v>
+        <v>1039</v>
       </c>
       <c r="AE18">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="AF18">
         <v>1329</v>
       </c>
       <c r="AG18">
-        <v>2070</v>
+        <v>2069</v>
       </c>
       <c r="AH18">
-        <v>2967</v>
+        <v>2966</v>
       </c>
       <c r="AI18">
-        <v>4854</v>
+        <v>4855</v>
       </c>
       <c r="AJ18">
-        <v>7188</v>
+        <v>7192</v>
       </c>
       <c r="AK18">
-        <v>8410</v>
+        <v>8408</v>
       </c>
       <c r="AL18">
-        <v>8703</v>
+        <v>8704</v>
       </c>
       <c r="AM18">
-        <v>8205</v>
+        <v>8202</v>
       </c>
       <c r="AN18">
-        <v>7459</v>
+        <v>7461</v>
       </c>
       <c r="AO18">
-        <v>7716</v>
+        <v>7719</v>
       </c>
       <c r="AP18">
-        <v>8831</v>
+        <v>8837</v>
       </c>
       <c r="AQ18">
-        <v>8472</v>
+        <v>8467</v>
       </c>
       <c r="AR18">
-        <v>5866</v>
+        <v>5869</v>
       </c>
       <c r="AS18">
-        <v>4968</v>
+        <v>4967</v>
       </c>
       <c r="AT18">
         <v>6378</v>
       </c>
       <c r="AU18">
-        <v>5415</v>
+        <v>5412</v>
       </c>
       <c r="AV18">
-        <v>4214</v>
+        <v>4216</v>
       </c>
       <c r="AW18">
-        <v>3469</v>
+        <v>3489</v>
+      </c>
+      <c r="AX18">
+        <v>2894</v>
       </c>
     </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>67</v>
       </c>
@@ -3913,52 +3970,55 @@
         <v>1656</v>
       </c>
       <c r="AI19">
-        <v>2747</v>
+        <v>2745</v>
       </c>
       <c r="AJ19">
-        <v>4083</v>
+        <v>4082</v>
       </c>
       <c r="AK19">
-        <v>4772</v>
+        <v>4773</v>
       </c>
       <c r="AL19">
-        <v>5342</v>
+        <v>5343</v>
       </c>
       <c r="AM19">
-        <v>5302</v>
+        <v>5300</v>
       </c>
       <c r="AN19">
-        <v>5184</v>
+        <v>5186</v>
       </c>
       <c r="AO19">
         <v>5157</v>
       </c>
       <c r="AP19">
-        <v>5678</v>
+        <v>5677</v>
       </c>
       <c r="AQ19">
-        <v>5276</v>
+        <v>5277</v>
       </c>
       <c r="AR19">
-        <v>3378</v>
+        <v>3377</v>
       </c>
       <c r="AS19">
-        <v>2644</v>
+        <v>2645</v>
       </c>
       <c r="AT19">
-        <v>3311</v>
+        <v>3314</v>
       </c>
       <c r="AU19">
-        <v>2726</v>
+        <v>2733</v>
       </c>
       <c r="AV19">
-        <v>2217</v>
+        <v>2219</v>
       </c>
       <c r="AW19">
-        <v>1873</v>
+        <v>1889</v>
+      </c>
+      <c r="AX19">
+        <v>1704</v>
       </c>
     </row>
-    <row r="20" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>68</v>
       </c>
@@ -4065,10 +4125,10 @@
         <v>1833</v>
       </c>
       <c r="AJ20">
-        <v>2792</v>
+        <v>2793</v>
       </c>
       <c r="AK20">
-        <v>3358</v>
+        <v>3359</v>
       </c>
       <c r="AL20">
         <v>3617</v>
@@ -4077,37 +4137,40 @@
         <v>3915</v>
       </c>
       <c r="AN20">
-        <v>3812</v>
+        <v>3814</v>
       </c>
       <c r="AO20">
-        <v>3675</v>
+        <v>3677</v>
       </c>
       <c r="AP20">
-        <v>4256</v>
+        <v>4255</v>
       </c>
       <c r="AQ20">
-        <v>4310</v>
+        <v>4307</v>
       </c>
       <c r="AR20">
-        <v>3022</v>
+        <v>3025</v>
       </c>
       <c r="AS20">
-        <v>1940</v>
+        <v>1939</v>
       </c>
       <c r="AT20">
-        <v>2403</v>
+        <v>2402</v>
       </c>
       <c r="AU20">
-        <v>2201</v>
+        <v>2202</v>
       </c>
       <c r="AV20">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="AW20">
-        <v>1624</v>
+        <v>1638</v>
+      </c>
+      <c r="AX20">
+        <v>1593</v>
       </c>
     </row>
-    <row r="21" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>66</v>
       </c>
@@ -4133,7 +4196,7 @@
         <v>161</v>
       </c>
       <c r="I21">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J21">
         <v>132</v>
@@ -4214,46 +4277,49 @@
         <v>1463</v>
       </c>
       <c r="AJ21">
-        <v>2249</v>
+        <v>2246</v>
       </c>
       <c r="AK21">
-        <v>2423</v>
+        <v>2425</v>
       </c>
       <c r="AL21">
-        <v>2425</v>
+        <v>2426</v>
       </c>
       <c r="AM21">
         <v>2379</v>
       </c>
       <c r="AN21">
-        <v>2331</v>
+        <v>2328</v>
       </c>
       <c r="AO21">
-        <v>2313</v>
+        <v>2307</v>
       </c>
       <c r="AP21">
-        <v>2684</v>
+        <v>2678</v>
       </c>
       <c r="AQ21">
         <v>3112</v>
       </c>
       <c r="AR21">
-        <v>2127</v>
+        <v>2121</v>
       </c>
       <c r="AS21">
-        <v>1537</v>
+        <v>1536</v>
       </c>
       <c r="AT21">
-        <v>1932</v>
+        <v>1929</v>
       </c>
       <c r="AU21">
-        <v>1861</v>
+        <v>1864</v>
       </c>
       <c r="AV21">
-        <v>1708</v>
+        <v>1704</v>
       </c>
       <c r="AW21">
-        <v>1533</v>
+        <v>1543</v>
+      </c>
+      <c r="AX21">
+        <v>1503</v>
       </c>
     </row>
   </sheetData>
@@ -4263,15 +4329,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AW21"/>
+  <dimension ref="A1:AX21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:AX21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4419,13 +4485,16 @@
       <c r="AW1" t="s">
         <v>48</v>
       </c>
+      <c r="AX1" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>49</v>
       </c>
       <c r="B2">
-        <v>1.08</v>
+        <v>1.07</v>
       </c>
       <c r="C2">
         <v>7.73</v>
@@ -4434,7 +4503,7 @@
         <v>26.98</v>
       </c>
       <c r="E2">
-        <v>40.909999999999997</v>
+        <v>40.9</v>
       </c>
       <c r="F2">
         <v>43.4</v>
@@ -4449,7 +4518,7 @@
         <v>14.89</v>
       </c>
       <c r="J2">
-        <v>8.9700000000000006</v>
+        <v>8.9499999999999993</v>
       </c>
       <c r="K2">
         <v>7.5</v>
@@ -4497,7 +4566,7 @@
         <v>9.57</v>
       </c>
       <c r="Z2">
-        <v>11.55</v>
+        <v>11.54</v>
       </c>
       <c r="AA2">
         <v>10.61</v>
@@ -4506,16 +4575,16 @@
         <v>10.37</v>
       </c>
       <c r="AC2">
-        <v>11.75</v>
+        <v>11.76</v>
       </c>
       <c r="AD2">
-        <v>14.78</v>
+        <v>14.79</v>
       </c>
       <c r="AE2">
         <v>15.73</v>
       </c>
       <c r="AF2">
-        <v>19.149999999999999</v>
+        <v>19.16</v>
       </c>
       <c r="AG2">
         <v>31.45</v>
@@ -4524,52 +4593,55 @@
         <v>50.62</v>
       </c>
       <c r="AI2">
-        <v>90.02</v>
+        <v>90.03</v>
       </c>
       <c r="AJ2">
-        <v>133.65</v>
+        <v>133.66999999999999</v>
       </c>
       <c r="AK2">
-        <v>151.28</v>
+        <v>151.30000000000001</v>
       </c>
       <c r="AL2">
-        <v>153.75</v>
+        <v>153.78</v>
       </c>
       <c r="AM2">
         <v>154.51</v>
       </c>
       <c r="AN2">
-        <v>148.29</v>
+        <v>148.32</v>
       </c>
       <c r="AO2">
-        <v>154.49</v>
+        <v>154.52000000000001</v>
       </c>
       <c r="AP2">
-        <v>188.14</v>
+        <v>188.17</v>
       </c>
       <c r="AQ2">
-        <v>210.5</v>
+        <v>210.51</v>
       </c>
       <c r="AR2">
-        <v>167.53</v>
+        <v>167.65</v>
       </c>
       <c r="AS2">
-        <v>148.25</v>
+        <v>148.34</v>
       </c>
       <c r="AT2">
-        <v>175.11</v>
+        <v>175.19</v>
       </c>
       <c r="AU2">
-        <v>143.25</v>
+        <v>143.37</v>
       </c>
       <c r="AV2">
-        <v>115.17</v>
+        <v>115.15</v>
       </c>
       <c r="AW2">
-        <v>93.94</v>
+        <v>94.41</v>
+      </c>
+      <c r="AX2">
+        <v>77.48</v>
       </c>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -4577,7 +4649,7 @@
         <v>0.12</v>
       </c>
       <c r="C3">
-        <v>1.46</v>
+        <v>1.58</v>
       </c>
       <c r="D3">
         <v>12.15</v>
@@ -4595,16 +4667,16 @@
         <v>103.03</v>
       </c>
       <c r="I3">
-        <v>70.709999999999994</v>
+        <v>70.83</v>
       </c>
       <c r="J3">
-        <v>34.869999999999997</v>
+        <v>34.630000000000003</v>
       </c>
       <c r="K3">
         <v>25.27</v>
       </c>
       <c r="L3">
-        <v>17.13</v>
+        <v>17.37</v>
       </c>
       <c r="M3">
         <v>12.51</v>
@@ -4667,58 +4739,61 @@
         <v>14.46</v>
       </c>
       <c r="AG3">
-        <v>22.6</v>
+        <v>22.48</v>
       </c>
       <c r="AH3">
         <v>52.97</v>
       </c>
       <c r="AI3">
-        <v>107.53</v>
+        <v>107.65</v>
       </c>
       <c r="AJ3">
-        <v>177.88</v>
+        <v>178</v>
       </c>
       <c r="AK3">
-        <v>208.62</v>
+        <v>208.86</v>
       </c>
       <c r="AL3">
-        <v>282.24</v>
+        <v>282.49</v>
       </c>
       <c r="AM3">
-        <v>373.13</v>
+        <v>373.61</v>
       </c>
       <c r="AN3">
-        <v>427.44</v>
+        <v>427.31</v>
       </c>
       <c r="AO3">
-        <v>509.57</v>
+        <v>509.81</v>
       </c>
       <c r="AP3">
-        <v>657.68</v>
+        <v>657.56</v>
       </c>
       <c r="AQ3">
-        <v>728.15</v>
+        <v>727.66</v>
       </c>
       <c r="AR3">
-        <v>642.13</v>
+        <v>642.61</v>
       </c>
       <c r="AS3">
-        <v>605.19000000000005</v>
+        <v>606.04</v>
       </c>
       <c r="AT3">
-        <v>656.58</v>
+        <v>659.38</v>
       </c>
       <c r="AU3">
-        <v>612.97</v>
+        <v>614.17999999999995</v>
       </c>
       <c r="AV3">
-        <v>482.11</v>
+        <v>481.62</v>
       </c>
       <c r="AW3">
-        <v>350.65</v>
+        <v>351.62</v>
+      </c>
+      <c r="AX3">
+        <v>235.59</v>
       </c>
     </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -4744,16 +4819,16 @@
         <v>59.28</v>
       </c>
       <c r="I4">
-        <v>43.74</v>
+        <v>43.68</v>
       </c>
       <c r="J4">
-        <v>21.04</v>
+        <v>20.91</v>
       </c>
       <c r="K4">
         <v>16.82</v>
       </c>
       <c r="L4">
-        <v>11.51</v>
+        <v>11.45</v>
       </c>
       <c r="M4">
         <v>8.1199999999999992</v>
@@ -4783,7 +4858,7 @@
         <v>1.53</v>
       </c>
       <c r="V4">
-        <v>2.2999999999999998</v>
+        <v>2.2400000000000002</v>
       </c>
       <c r="W4">
         <v>2.62</v>
@@ -4825,49 +4900,52 @@
         <v>73.150000000000006</v>
       </c>
       <c r="AJ4">
-        <v>113.7</v>
+        <v>113.76</v>
       </c>
       <c r="AK4">
         <v>146.63</v>
       </c>
       <c r="AL4">
-        <v>181.16</v>
+        <v>181.35</v>
       </c>
       <c r="AM4">
-        <v>215.37</v>
+        <v>215.56</v>
       </c>
       <c r="AN4">
-        <v>262.5</v>
+        <v>262.31</v>
       </c>
       <c r="AO4">
-        <v>294.14999999999998</v>
+        <v>294.08999999999997</v>
       </c>
       <c r="AP4">
-        <v>378.12</v>
+        <v>378.24</v>
       </c>
       <c r="AQ4">
-        <v>444.68</v>
+        <v>444.88</v>
       </c>
       <c r="AR4">
-        <v>374.98</v>
+        <v>375.05</v>
       </c>
       <c r="AS4">
         <v>358.68</v>
       </c>
       <c r="AT4">
-        <v>389.24</v>
+        <v>389.63</v>
       </c>
       <c r="AU4">
         <v>356.31</v>
       </c>
       <c r="AV4">
-        <v>285.33</v>
+        <v>285.27</v>
       </c>
       <c r="AW4">
-        <v>212.11</v>
+        <v>213.07</v>
+      </c>
+      <c r="AX4">
+        <v>164.92</v>
       </c>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -4875,19 +4953,19 @@
         <v>0.36</v>
       </c>
       <c r="C5">
-        <v>2.5499999999999998</v>
+        <v>2.58</v>
       </c>
       <c r="D5">
         <v>14.21</v>
       </c>
       <c r="E5">
-        <v>39.04</v>
+        <v>39.01</v>
       </c>
       <c r="F5">
         <v>59.62</v>
       </c>
       <c r="G5">
-        <v>52.18</v>
+        <v>52.21</v>
       </c>
       <c r="H5">
         <v>35.880000000000003</v>
@@ -4908,7 +4986,7 @@
         <v>4.6100000000000003</v>
       </c>
       <c r="N5">
-        <v>3.43</v>
+        <v>3.37</v>
       </c>
       <c r="O5">
         <v>2.31</v>
@@ -4971,7 +5049,7 @@
         <v>26.01</v>
       </c>
       <c r="AI5">
-        <v>55.76</v>
+        <v>55.7</v>
       </c>
       <c r="AJ5">
         <v>86.3</v>
@@ -4980,7 +5058,7 @@
         <v>104.3</v>
       </c>
       <c r="AL5">
-        <v>115.53</v>
+        <v>115.56</v>
       </c>
       <c r="AM5">
         <v>132.38</v>
@@ -4989,34 +5067,37 @@
         <v>145.46</v>
       </c>
       <c r="AO5">
-        <v>165.2</v>
+        <v>165.26</v>
       </c>
       <c r="AP5">
-        <v>214.8</v>
+        <v>214.89</v>
       </c>
       <c r="AQ5">
         <v>251.53</v>
       </c>
       <c r="AR5">
-        <v>226.15</v>
+        <v>226.36</v>
       </c>
       <c r="AS5">
-        <v>208.88</v>
+        <v>209.45</v>
       </c>
       <c r="AT5">
-        <v>233.1</v>
+        <v>233.22</v>
       </c>
       <c r="AU5">
-        <v>203.26</v>
+        <v>203.53</v>
       </c>
       <c r="AV5">
-        <v>162.13</v>
+        <v>161.88999999999999</v>
       </c>
       <c r="AW5">
-        <v>126.55</v>
+        <v>127.71</v>
+      </c>
+      <c r="AX5">
+        <v>94.95</v>
       </c>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -5045,7 +5126,7 @@
         <v>15.14</v>
       </c>
       <c r="J6">
-        <v>9.08</v>
+        <v>9.0500000000000007</v>
       </c>
       <c r="K6">
         <v>7.07</v>
@@ -5054,7 +5135,7 @@
         <v>4.54</v>
       </c>
       <c r="M6">
-        <v>2.71</v>
+        <v>2.73</v>
       </c>
       <c r="N6">
         <v>2.12</v>
@@ -5111,7 +5192,7 @@
         <v>5.98</v>
       </c>
       <c r="AF6">
-        <v>7.97</v>
+        <v>8</v>
       </c>
       <c r="AG6">
         <v>13.08</v>
@@ -5120,52 +5201,55 @@
         <v>23.29</v>
       </c>
       <c r="AI6">
-        <v>42.05</v>
+        <v>42.02</v>
       </c>
       <c r="AJ6">
-        <v>68.36</v>
+        <v>68.39</v>
       </c>
       <c r="AK6">
-        <v>78.680000000000007</v>
+        <v>78.78</v>
       </c>
       <c r="AL6">
-        <v>84.9</v>
+        <v>84.95</v>
       </c>
       <c r="AM6">
-        <v>87.3</v>
+        <v>87.35</v>
       </c>
       <c r="AN6">
         <v>90.13</v>
       </c>
       <c r="AO6">
-        <v>102.47</v>
+        <v>102.44</v>
       </c>
       <c r="AP6">
-        <v>128.88</v>
+        <v>128.97999999999999</v>
       </c>
       <c r="AQ6">
-        <v>153.57</v>
+        <v>153.49</v>
       </c>
       <c r="AR6">
-        <v>131.85</v>
+        <v>132.05000000000001</v>
       </c>
       <c r="AS6">
-        <v>119.83</v>
+        <v>119.75</v>
       </c>
       <c r="AT6">
-        <v>135.19999999999999</v>
+        <v>135.25</v>
       </c>
       <c r="AU6">
-        <v>111.52</v>
+        <v>111.44</v>
       </c>
       <c r="AV6">
-        <v>88.3</v>
+        <v>88.17</v>
       </c>
       <c r="AW6">
-        <v>72.28</v>
+        <v>72.77</v>
+      </c>
+      <c r="AX6">
+        <v>56.55</v>
       </c>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -5176,7 +5260,7 @@
         <v>3.95</v>
       </c>
       <c r="D7">
-        <v>16.899999999999999</v>
+        <v>16.87</v>
       </c>
       <c r="E7">
         <v>36.119999999999997</v>
@@ -5194,13 +5278,13 @@
         <v>11.54</v>
       </c>
       <c r="J7">
-        <v>7.54</v>
+        <v>7.51</v>
       </c>
       <c r="K7">
         <v>5.63</v>
       </c>
       <c r="L7">
-        <v>3.48</v>
+        <v>3.51</v>
       </c>
       <c r="M7">
         <v>2.5</v>
@@ -5230,10 +5314,10 @@
         <v>1.66</v>
       </c>
       <c r="V7">
-        <v>1.69</v>
+        <v>1.71</v>
       </c>
       <c r="W7">
-        <v>2.4500000000000002</v>
+        <v>2.42</v>
       </c>
       <c r="X7">
         <v>2.48</v>
@@ -5269,16 +5353,16 @@
         <v>25.39</v>
       </c>
       <c r="AI7">
-        <v>48.86</v>
+        <v>48.88</v>
       </c>
       <c r="AJ7">
-        <v>78.44</v>
+        <v>78.58</v>
       </c>
       <c r="AK7">
         <v>86.44</v>
       </c>
       <c r="AL7">
-        <v>89.63</v>
+        <v>89.57</v>
       </c>
       <c r="AM7">
         <v>91.51</v>
@@ -5287,34 +5371,37 @@
         <v>87.15</v>
       </c>
       <c r="AO7">
-        <v>94.69</v>
+        <v>94.74</v>
       </c>
       <c r="AP7">
-        <v>119.57</v>
+        <v>119.62</v>
       </c>
       <c r="AQ7">
-        <v>140.85</v>
+        <v>140.99</v>
       </c>
       <c r="AR7">
-        <v>121.23</v>
+        <v>121.42</v>
       </c>
       <c r="AS7">
-        <v>112.76</v>
+        <v>112.93</v>
       </c>
       <c r="AT7">
-        <v>131.65</v>
+        <v>131.52000000000001</v>
       </c>
       <c r="AU7">
-        <v>99.64</v>
+        <v>99.83</v>
       </c>
       <c r="AV7">
-        <v>83.88</v>
+        <v>83.78</v>
       </c>
       <c r="AW7">
         <v>67.8</v>
       </c>
+      <c r="AX7">
+        <v>55.82</v>
+      </c>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -5331,7 +5418,7 @@
         <v>33.9</v>
       </c>
       <c r="F8">
-        <v>34.840000000000003</v>
+        <v>34.82</v>
       </c>
       <c r="G8">
         <v>22.97</v>
@@ -5340,7 +5427,7 @@
         <v>13.62</v>
       </c>
       <c r="I8">
-        <v>10.39</v>
+        <v>10.37</v>
       </c>
       <c r="J8">
         <v>5.47</v>
@@ -5352,7 +5439,7 @@
         <v>3</v>
       </c>
       <c r="M8">
-        <v>2.5499999999999998</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="N8">
         <v>2.2000000000000002</v>
@@ -5364,7 +5451,7 @@
         <v>1.05</v>
       </c>
       <c r="Q8">
-        <v>1.44</v>
+        <v>1.42</v>
       </c>
       <c r="R8">
         <v>1.34</v>
@@ -5382,7 +5469,7 @@
         <v>1.75</v>
       </c>
       <c r="W8">
-        <v>1.75</v>
+        <v>1.77</v>
       </c>
       <c r="X8">
         <v>2.4900000000000002</v>
@@ -5400,7 +5487,7 @@
         <v>2.63</v>
       </c>
       <c r="AC8">
-        <v>4.6100000000000003</v>
+        <v>4.63</v>
       </c>
       <c r="AD8">
         <v>5.97</v>
@@ -5418,52 +5505,55 @@
         <v>26.47</v>
       </c>
       <c r="AI8">
-        <v>46.72</v>
+        <v>46.74</v>
       </c>
       <c r="AJ8">
-        <v>73.06</v>
+        <v>73.08</v>
       </c>
       <c r="AK8">
-        <v>87.47</v>
+        <v>87.45</v>
       </c>
       <c r="AL8">
         <v>82.67</v>
       </c>
       <c r="AM8">
-        <v>85.37</v>
+        <v>85.43</v>
       </c>
       <c r="AN8">
         <v>85.16</v>
       </c>
       <c r="AO8">
-        <v>84.98</v>
+        <v>84.91</v>
       </c>
       <c r="AP8">
-        <v>106.3</v>
+        <v>106.42</v>
       </c>
       <c r="AQ8">
-        <v>130.72999999999999</v>
+        <v>130.68</v>
       </c>
       <c r="AR8">
-        <v>115.08</v>
+        <v>115.13</v>
       </c>
       <c r="AS8">
-        <v>102.47</v>
+        <v>102.53</v>
       </c>
       <c r="AT8">
-        <v>117.57</v>
+        <v>117.66</v>
       </c>
       <c r="AU8">
-        <v>90.99</v>
+        <v>90.96</v>
       </c>
       <c r="AV8">
-        <v>74.69</v>
+        <v>74.64</v>
       </c>
       <c r="AW8">
-        <v>63.96</v>
+        <v>64.56</v>
+      </c>
+      <c r="AX8">
+        <v>51.62</v>
       </c>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -5492,7 +5582,7 @@
         <v>11.93</v>
       </c>
       <c r="J9">
-        <v>7.19</v>
+        <v>7.17</v>
       </c>
       <c r="K9">
         <v>5.88</v>
@@ -5561,58 +5651,61 @@
         <v>12.08</v>
       </c>
       <c r="AG9">
-        <v>22.56</v>
+        <v>22.54</v>
       </c>
       <c r="AH9">
         <v>37.54</v>
       </c>
       <c r="AI9">
-        <v>70.08</v>
+        <v>70.099999999999994</v>
       </c>
       <c r="AJ9">
-        <v>106.15</v>
+        <v>106.17</v>
       </c>
       <c r="AK9">
-        <v>121.29</v>
+        <v>121.32</v>
       </c>
       <c r="AL9">
-        <v>122.26</v>
+        <v>122.3</v>
       </c>
       <c r="AM9">
-        <v>129.29</v>
+        <v>129.36000000000001</v>
       </c>
       <c r="AN9">
-        <v>123.91</v>
+        <v>123.92</v>
       </c>
       <c r="AO9">
-        <v>135.54</v>
+        <v>135.56</v>
       </c>
       <c r="AP9">
         <v>166.9</v>
       </c>
       <c r="AQ9">
-        <v>195.26</v>
+        <v>195.28</v>
       </c>
       <c r="AR9">
-        <v>162.65</v>
+        <v>162.88</v>
       </c>
       <c r="AS9">
-        <v>146.55000000000001</v>
+        <v>146.59</v>
       </c>
       <c r="AT9">
-        <v>164.19</v>
+        <v>164.26</v>
       </c>
       <c r="AU9">
-        <v>133.24</v>
+        <v>133.41999999999999</v>
       </c>
       <c r="AV9">
-        <v>110.27</v>
+        <v>110.47</v>
       </c>
       <c r="AW9">
-        <v>90.39</v>
+        <v>90.96</v>
+      </c>
+      <c r="AX9">
+        <v>74.150000000000006</v>
       </c>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -5620,16 +5713,16 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="C10">
-        <v>11.18</v>
+        <v>11.16</v>
       </c>
       <c r="D10">
-        <v>38.590000000000003</v>
+        <v>38.58</v>
       </c>
       <c r="E10">
         <v>53.36</v>
       </c>
       <c r="F10">
-        <v>54.43</v>
+        <v>54.44</v>
       </c>
       <c r="G10">
         <v>38.74</v>
@@ -5641,7 +5734,7 @@
         <v>15.73</v>
       </c>
       <c r="J10">
-        <v>8.94</v>
+        <v>8.91</v>
       </c>
       <c r="K10">
         <v>7.58</v>
@@ -5683,7 +5776,7 @@
         <v>4.2300000000000004</v>
       </c>
       <c r="X10">
-        <v>4.57</v>
+        <v>4.59</v>
       </c>
       <c r="Y10">
         <v>4.84</v>
@@ -5698,19 +5791,19 @@
         <v>5.83</v>
       </c>
       <c r="AC10">
-        <v>8.2200000000000006</v>
+        <v>8.24</v>
       </c>
       <c r="AD10">
         <v>11.31</v>
       </c>
       <c r="AE10">
-        <v>12.84</v>
+        <v>12.85</v>
       </c>
       <c r="AF10">
         <v>16.43</v>
       </c>
       <c r="AG10">
-        <v>27.76</v>
+        <v>27.77</v>
       </c>
       <c r="AH10">
         <v>44.51</v>
@@ -5719,10 +5812,10 @@
         <v>85.46</v>
       </c>
       <c r="AJ10">
-        <v>133.07</v>
+        <v>133.15</v>
       </c>
       <c r="AK10">
-        <v>150.74</v>
+        <v>150.76</v>
       </c>
       <c r="AL10">
         <v>152.91999999999999</v>
@@ -5731,37 +5824,40 @@
         <v>152.02000000000001</v>
       </c>
       <c r="AN10">
-        <v>146.53</v>
+        <v>146.65</v>
       </c>
       <c r="AO10">
-        <v>153.66999999999999</v>
+        <v>153.83000000000001</v>
       </c>
       <c r="AP10">
-        <v>193.89</v>
+        <v>193.92</v>
       </c>
       <c r="AQ10">
-        <v>222.72</v>
+        <v>222.85</v>
       </c>
       <c r="AR10">
-        <v>183.52</v>
+        <v>183.71</v>
       </c>
       <c r="AS10">
-        <v>164.49</v>
+        <v>164.58</v>
       </c>
       <c r="AT10">
-        <v>182.95</v>
+        <v>183.09</v>
       </c>
       <c r="AU10">
-        <v>149.04</v>
+        <v>149.13999999999999</v>
       </c>
       <c r="AV10">
-        <v>124.17</v>
+        <v>124.13</v>
       </c>
       <c r="AW10">
-        <v>103.88</v>
+        <v>104.6</v>
+      </c>
+      <c r="AX10">
+        <v>86.12</v>
       </c>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -5772,10 +5868,10 @@
         <v>14.6</v>
       </c>
       <c r="D11">
-        <v>46.11</v>
+        <v>46.08</v>
       </c>
       <c r="E11">
-        <v>59.61</v>
+        <v>59.6</v>
       </c>
       <c r="F11">
         <v>55.14</v>
@@ -5787,7 +5883,7 @@
         <v>23.25</v>
       </c>
       <c r="I11">
-        <v>14.77</v>
+        <v>14.78</v>
       </c>
       <c r="J11">
         <v>9.02</v>
@@ -5826,7 +5922,7 @@
         <v>3.14</v>
       </c>
       <c r="V11">
-        <v>4.4000000000000004</v>
+        <v>4.38</v>
       </c>
       <c r="W11">
         <v>5.25</v>
@@ -5847,7 +5943,7 @@
         <v>8.24</v>
       </c>
       <c r="AC11">
-        <v>9.9499999999999993</v>
+        <v>9.9700000000000006</v>
       </c>
       <c r="AD11">
         <v>13.37</v>
@@ -5859,7 +5955,7 @@
         <v>17.97</v>
       </c>
       <c r="AG11">
-        <v>33.78</v>
+        <v>33.799999999999997</v>
       </c>
       <c r="AH11">
         <v>53.22</v>
@@ -5868,63 +5964,66 @@
         <v>95.6</v>
       </c>
       <c r="AJ11">
-        <v>145.69</v>
+        <v>145.75</v>
       </c>
       <c r="AK11">
-        <v>163.22999999999999</v>
+        <v>163.29</v>
       </c>
       <c r="AL11">
-        <v>163.79</v>
+        <v>163.96</v>
       </c>
       <c r="AM11">
-        <v>161.38</v>
+        <v>161.31</v>
       </c>
       <c r="AN11">
-        <v>154.06</v>
+        <v>154.16999999999999</v>
       </c>
       <c r="AO11">
-        <v>157.22</v>
+        <v>157.25</v>
       </c>
       <c r="AP11">
-        <v>197.37</v>
+        <v>197.39</v>
       </c>
       <c r="AQ11">
-        <v>222.26</v>
+        <v>222.38</v>
       </c>
       <c r="AR11">
-        <v>178.53</v>
+        <v>178.79</v>
       </c>
       <c r="AS11">
-        <v>156.78</v>
+        <v>157.03</v>
       </c>
       <c r="AT11">
-        <v>180.08</v>
+        <v>180.1</v>
       </c>
       <c r="AU11">
-        <v>145.87</v>
+        <v>145.97</v>
       </c>
       <c r="AV11">
         <v>121.92</v>
       </c>
       <c r="AW11">
-        <v>99.33</v>
+        <v>99.74</v>
+      </c>
+      <c r="AX11">
+        <v>78.66</v>
       </c>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>59</v>
       </c>
       <c r="B12">
-        <v>1.9</v>
+        <v>1.88</v>
       </c>
       <c r="C12">
         <v>14.03</v>
       </c>
       <c r="D12">
-        <v>39.799999999999997</v>
+        <v>39.86</v>
       </c>
       <c r="E12">
-        <v>55.43</v>
+        <v>55.41</v>
       </c>
       <c r="F12">
         <v>51.6</v>
@@ -5936,7 +6035,7 @@
         <v>22.26</v>
       </c>
       <c r="I12">
-        <v>14.94</v>
+        <v>14.96</v>
       </c>
       <c r="J12">
         <v>8.89</v>
@@ -5996,7 +6095,7 @@
         <v>11.64</v>
       </c>
       <c r="AC12">
-        <v>13.18</v>
+        <v>13.16</v>
       </c>
       <c r="AD12">
         <v>16.57</v>
@@ -6008,19 +6107,19 @@
         <v>22.74</v>
       </c>
       <c r="AG12">
-        <v>38.67</v>
+        <v>38.69</v>
       </c>
       <c r="AH12">
-        <v>59.37</v>
+        <v>59.39</v>
       </c>
       <c r="AI12">
-        <v>110.2</v>
+        <v>110.18</v>
       </c>
       <c r="AJ12">
-        <v>159.03</v>
+        <v>159.06</v>
       </c>
       <c r="AK12">
-        <v>179.66</v>
+        <v>179.6</v>
       </c>
       <c r="AL12">
         <v>176.13</v>
@@ -6029,69 +6128,72 @@
         <v>183.37</v>
       </c>
       <c r="AN12">
-        <v>171.81</v>
+        <v>171.88</v>
       </c>
       <c r="AO12">
-        <v>175.03</v>
+        <v>175.09</v>
       </c>
       <c r="AP12">
-        <v>210.25</v>
+        <v>210.26</v>
       </c>
       <c r="AQ12">
-        <v>235.85</v>
+        <v>235.92</v>
       </c>
       <c r="AR12">
-        <v>184.44</v>
+        <v>184.49</v>
       </c>
       <c r="AS12">
-        <v>162</v>
+        <v>162.25</v>
       </c>
       <c r="AT12">
-        <v>185.76</v>
+        <v>185.82</v>
       </c>
       <c r="AU12">
-        <v>151.22999999999999</v>
+        <v>151.41999999999999</v>
       </c>
       <c r="AV12">
-        <v>122.5</v>
+        <v>122.67</v>
       </c>
       <c r="AW12">
-        <v>100.35</v>
+        <v>101.07</v>
+      </c>
+      <c r="AX12">
+        <v>84.82</v>
       </c>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>60</v>
       </c>
       <c r="B13">
-        <v>1.75</v>
+        <v>1.73</v>
       </c>
       <c r="C13">
-        <v>11.59</v>
+        <v>11.57</v>
       </c>
       <c r="D13">
         <v>36.75</v>
       </c>
       <c r="E13">
-        <v>47.48</v>
+        <v>47.46</v>
       </c>
       <c r="F13">
-        <v>47.06</v>
+        <v>47.04</v>
       </c>
       <c r="G13">
         <v>34.119999999999997</v>
       </c>
       <c r="H13">
-        <v>20.86</v>
+        <v>20.88</v>
       </c>
       <c r="I13">
-        <v>14.22</v>
+        <v>14.2</v>
       </c>
       <c r="J13">
-        <v>9.2899999999999991</v>
+        <v>9.27</v>
       </c>
       <c r="K13">
-        <v>8.23</v>
+        <v>8.25</v>
       </c>
       <c r="L13">
         <v>7.25</v>
@@ -6124,13 +6226,13 @@
         <v>5.13</v>
       </c>
       <c r="V13">
-        <v>6.54</v>
+        <v>6.56</v>
       </c>
       <c r="W13">
         <v>8.74</v>
       </c>
       <c r="X13">
-        <v>9.94</v>
+        <v>9.9600000000000009</v>
       </c>
       <c r="Y13">
         <v>13.08</v>
@@ -6142,13 +6244,13 @@
         <v>13.46</v>
       </c>
       <c r="AB13">
-        <v>13.2</v>
+        <v>13.18</v>
       </c>
       <c r="AC13">
         <v>14.02</v>
       </c>
       <c r="AD13">
-        <v>17.190000000000001</v>
+        <v>17.21</v>
       </c>
       <c r="AE13">
         <v>17.54</v>
@@ -6157,58 +6259,61 @@
         <v>21.39</v>
       </c>
       <c r="AG13">
-        <v>38.049999999999997</v>
+        <v>38.090000000000003</v>
       </c>
       <c r="AH13">
-        <v>59.22</v>
+        <v>59.24</v>
       </c>
       <c r="AI13">
-        <v>107.92</v>
+        <v>107.98</v>
       </c>
       <c r="AJ13">
-        <v>160.36000000000001</v>
+        <v>160.4</v>
       </c>
       <c r="AK13">
-        <v>180.77</v>
+        <v>180.83</v>
       </c>
       <c r="AL13">
-        <v>182.93</v>
+        <v>182.95</v>
       </c>
       <c r="AM13">
         <v>188.14</v>
       </c>
       <c r="AN13">
-        <v>179.26</v>
+        <v>179.34</v>
       </c>
       <c r="AO13">
-        <v>179.81</v>
+        <v>179.89</v>
       </c>
       <c r="AP13">
-        <v>221.88</v>
+        <v>221.9</v>
       </c>
       <c r="AQ13">
-        <v>244.47</v>
+        <v>244.57</v>
       </c>
       <c r="AR13">
-        <v>193.83</v>
+        <v>194.17</v>
       </c>
       <c r="AS13">
-        <v>163.76</v>
+        <v>163.84</v>
       </c>
       <c r="AT13">
-        <v>194.01</v>
+        <v>193.97</v>
       </c>
       <c r="AU13">
         <v>154.16999999999999</v>
       </c>
       <c r="AV13">
-        <v>127.07</v>
+        <v>127.09</v>
       </c>
       <c r="AW13">
-        <v>104.32</v>
+        <v>104.6</v>
+      </c>
+      <c r="AX13">
+        <v>87.08</v>
       </c>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>61</v>
       </c>
@@ -6216,13 +6321,13 @@
         <v>1.25</v>
       </c>
       <c r="C14">
-        <v>10.36</v>
+        <v>10.34</v>
       </c>
       <c r="D14">
-        <v>33.200000000000003</v>
+        <v>33.18</v>
       </c>
       <c r="E14">
-        <v>45.09</v>
+        <v>45.07</v>
       </c>
       <c r="F14">
         <v>41.71</v>
@@ -6264,7 +6369,7 @@
         <v>5.63</v>
       </c>
       <c r="S14">
-        <v>4.29</v>
+        <v>4.2699999999999996</v>
       </c>
       <c r="T14">
         <v>3.89</v>
@@ -6303,61 +6408,64 @@
         <v>19.04</v>
       </c>
       <c r="AF14">
-        <v>21.8</v>
+        <v>21.84</v>
       </c>
       <c r="AG14">
-        <v>34.5</v>
+        <v>34.54</v>
       </c>
       <c r="AH14">
         <v>58.72</v>
       </c>
       <c r="AI14">
-        <v>101.96</v>
+        <v>102</v>
       </c>
       <c r="AJ14">
-        <v>152.78</v>
+        <v>152.80000000000001</v>
       </c>
       <c r="AK14">
-        <v>169.27</v>
+        <v>169.31</v>
       </c>
       <c r="AL14">
-        <v>173.49</v>
+        <v>173.54</v>
       </c>
       <c r="AM14">
-        <v>173.83</v>
+        <v>173.9</v>
       </c>
       <c r="AN14">
-        <v>164.92</v>
+        <v>164.83</v>
       </c>
       <c r="AO14">
-        <v>172.75</v>
+        <v>172.79</v>
       </c>
       <c r="AP14">
-        <v>207.63</v>
+        <v>207.82</v>
       </c>
       <c r="AQ14">
-        <v>231.11</v>
+        <v>231.19</v>
       </c>
       <c r="AR14">
-        <v>179.86</v>
+        <v>180.06</v>
       </c>
       <c r="AS14">
-        <v>153.18</v>
+        <v>153.26</v>
       </c>
       <c r="AT14">
-        <v>191.45</v>
+        <v>191.6</v>
       </c>
       <c r="AU14">
-        <v>151.76</v>
+        <v>151.93</v>
       </c>
       <c r="AV14">
-        <v>120.09</v>
+        <v>120.15</v>
       </c>
       <c r="AW14">
-        <v>98.6</v>
+        <v>98.84</v>
+      </c>
+      <c r="AX14">
+        <v>84.1</v>
       </c>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -6368,10 +6476,10 @@
         <v>9.7200000000000006</v>
       </c>
       <c r="D15">
-        <v>37.299999999999997</v>
+        <v>37.32</v>
       </c>
       <c r="E15">
-        <v>48.02</v>
+        <v>48</v>
       </c>
       <c r="F15">
         <v>44.02</v>
@@ -6413,7 +6521,7 @@
         <v>6.08</v>
       </c>
       <c r="S15">
-        <v>4.7300000000000004</v>
+        <v>4.75</v>
       </c>
       <c r="T15">
         <v>4.71</v>
@@ -6428,7 +6536,7 @@
         <v>7.72</v>
       </c>
       <c r="X15">
-        <v>9.3699999999999992</v>
+        <v>9.35</v>
       </c>
       <c r="Y15">
         <v>12.74</v>
@@ -6440,81 +6548,84 @@
         <v>15.58</v>
       </c>
       <c r="AB15">
-        <v>17.09</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="AC15">
         <v>17.14</v>
       </c>
       <c r="AD15">
-        <v>21.93</v>
+        <v>21.94</v>
       </c>
       <c r="AE15">
         <v>23.71</v>
       </c>
       <c r="AF15">
-        <v>27.75</v>
+        <v>27.77</v>
       </c>
       <c r="AG15">
-        <v>43.03</v>
+        <v>43</v>
       </c>
       <c r="AH15">
         <v>70.290000000000006</v>
       </c>
       <c r="AI15">
-        <v>122.19</v>
+        <v>122.24</v>
       </c>
       <c r="AJ15">
         <v>174.24</v>
       </c>
       <c r="AK15">
-        <v>190.68</v>
+        <v>190.64</v>
       </c>
       <c r="AL15">
-        <v>190.73</v>
+        <v>190.84</v>
       </c>
       <c r="AM15">
-        <v>183.74</v>
+        <v>183.67</v>
       </c>
       <c r="AN15">
         <v>170.7</v>
       </c>
       <c r="AO15">
-        <v>172.22</v>
+        <v>172.35</v>
       </c>
       <c r="AP15">
-        <v>209.8</v>
+        <v>209.84</v>
       </c>
       <c r="AQ15">
-        <v>237</v>
+        <v>236.98</v>
       </c>
       <c r="AR15">
-        <v>182.92</v>
+        <v>183.03</v>
       </c>
       <c r="AS15">
-        <v>167.24</v>
+        <v>167.28</v>
       </c>
       <c r="AT15">
-        <v>211.09</v>
+        <v>211.27</v>
       </c>
       <c r="AU15">
-        <v>164.87</v>
+        <v>164.98</v>
       </c>
       <c r="AV15">
-        <v>127.83</v>
+        <v>128.08000000000001</v>
       </c>
       <c r="AW15">
-        <v>105.01</v>
+        <v>105.61</v>
+      </c>
+      <c r="AX15">
+        <v>89.27</v>
       </c>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>63</v>
       </c>
       <c r="B16">
-        <v>1.5</v>
+        <v>1.52</v>
       </c>
       <c r="C16">
-        <v>10.78</v>
+        <v>10.76</v>
       </c>
       <c r="D16">
         <v>39.49</v>
@@ -6523,10 +6634,10 @@
         <v>53.07</v>
       </c>
       <c r="F16">
-        <v>49.05</v>
+        <v>49.03</v>
       </c>
       <c r="G16">
-        <v>38.130000000000003</v>
+        <v>38.11</v>
       </c>
       <c r="H16">
         <v>25.54</v>
@@ -6541,7 +6652,7 @@
         <v>10.23</v>
       </c>
       <c r="L16">
-        <v>7.69</v>
+        <v>7.67</v>
       </c>
       <c r="M16">
         <v>6.9</v>
@@ -6571,19 +6682,19 @@
         <v>6.07</v>
       </c>
       <c r="V16">
-        <v>8.1</v>
+        <v>8.08</v>
       </c>
       <c r="W16">
         <v>10.029999999999999</v>
       </c>
       <c r="X16">
-        <v>11.96</v>
+        <v>11.94</v>
       </c>
       <c r="Y16">
         <v>16.53</v>
       </c>
       <c r="Z16">
-        <v>23.57</v>
+        <v>23.55</v>
       </c>
       <c r="AA16">
         <v>24.1</v>
@@ -6592,7 +6703,7 @@
         <v>22.86</v>
       </c>
       <c r="AC16">
-        <v>24.28</v>
+        <v>24.26</v>
       </c>
       <c r="AD16">
         <v>29.24</v>
@@ -6601,61 +6712,64 @@
         <v>28.38</v>
       </c>
       <c r="AF16">
-        <v>34.35</v>
+        <v>34.33</v>
       </c>
       <c r="AG16">
-        <v>53.03</v>
+        <v>52.99</v>
       </c>
       <c r="AH16">
-        <v>88.25</v>
+        <v>88.27</v>
       </c>
       <c r="AI16">
-        <v>144.13</v>
+        <v>144.19</v>
       </c>
       <c r="AJ16">
-        <v>203.53</v>
+        <v>203.65</v>
       </c>
       <c r="AK16">
-        <v>219.65</v>
+        <v>219.67</v>
       </c>
       <c r="AL16">
-        <v>210.9</v>
+        <v>210.92</v>
       </c>
       <c r="AM16">
-        <v>195.9</v>
+        <v>195.96</v>
       </c>
       <c r="AN16">
-        <v>177.34</v>
+        <v>177.38</v>
       </c>
       <c r="AO16">
-        <v>179.98</v>
+        <v>180.06</v>
       </c>
       <c r="AP16">
-        <v>212.61</v>
+        <v>212.67</v>
       </c>
       <c r="AQ16">
-        <v>238.82</v>
+        <v>238.86</v>
       </c>
       <c r="AR16">
-        <v>186.05</v>
+        <v>186.11</v>
       </c>
       <c r="AS16">
-        <v>166.42</v>
+        <v>166.32</v>
       </c>
       <c r="AT16">
-        <v>212.87</v>
+        <v>212.91</v>
       </c>
       <c r="AU16">
-        <v>168.39</v>
+        <v>168.67</v>
       </c>
       <c r="AV16">
-        <v>126.26</v>
+        <v>126.38</v>
       </c>
       <c r="AW16">
-        <v>105.13</v>
+        <v>105.61</v>
+      </c>
+      <c r="AX16">
+        <v>88.23</v>
       </c>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>64</v>
       </c>
@@ -6666,22 +6780,22 @@
         <v>7.05</v>
       </c>
       <c r="D17">
-        <v>31.42</v>
+        <v>31.46</v>
       </c>
       <c r="E17">
         <v>49.34</v>
       </c>
       <c r="F17">
-        <v>48.65</v>
+        <v>48.67</v>
       </c>
       <c r="G17">
-        <v>37.67</v>
+        <v>37.65</v>
       </c>
       <c r="H17">
         <v>26.8</v>
       </c>
       <c r="I17">
-        <v>20.87</v>
+        <v>20.85</v>
       </c>
       <c r="J17">
         <v>12.91</v>
@@ -6699,19 +6813,19 @@
         <v>6.27</v>
       </c>
       <c r="O17">
-        <v>4.97</v>
+        <v>4.99</v>
       </c>
       <c r="P17">
         <v>5.4</v>
       </c>
       <c r="Q17">
-        <v>8.14</v>
+        <v>8.16</v>
       </c>
       <c r="R17">
         <v>5.64</v>
       </c>
       <c r="S17">
-        <v>5.6</v>
+        <v>5.62</v>
       </c>
       <c r="T17">
         <v>5.14</v>
@@ -6729,7 +6843,7 @@
         <v>16.190000000000001</v>
       </c>
       <c r="Y17">
-        <v>25.3</v>
+        <v>25.32</v>
       </c>
       <c r="Z17">
         <v>33.590000000000003</v>
@@ -6738,19 +6852,19 @@
         <v>28.75</v>
       </c>
       <c r="AB17">
-        <v>27.1</v>
+        <v>27.12</v>
       </c>
       <c r="AC17">
-        <v>28.01</v>
+        <v>28.04</v>
       </c>
       <c r="AD17">
-        <v>32.96</v>
+        <v>32.94</v>
       </c>
       <c r="AE17">
         <v>34.369999999999997</v>
       </c>
       <c r="AF17">
-        <v>37.74</v>
+        <v>37.78</v>
       </c>
       <c r="AG17">
         <v>60.58</v>
@@ -6759,52 +6873,55 @@
         <v>95.06</v>
       </c>
       <c r="AI17">
-        <v>163.96</v>
+        <v>163.98</v>
       </c>
       <c r="AJ17">
-        <v>226.39</v>
+        <v>226.48</v>
       </c>
       <c r="AK17">
-        <v>254.88</v>
+        <v>254.86</v>
       </c>
       <c r="AL17">
-        <v>239.43</v>
+        <v>239.45</v>
       </c>
       <c r="AM17">
-        <v>221.75</v>
+        <v>221.72</v>
       </c>
       <c r="AN17">
-        <v>194.1</v>
+        <v>194.12</v>
       </c>
       <c r="AO17">
         <v>199.31</v>
       </c>
       <c r="AP17">
-        <v>234.05</v>
+        <v>234.14</v>
       </c>
       <c r="AQ17">
         <v>262.8</v>
       </c>
       <c r="AR17">
-        <v>196.88</v>
+        <v>196.97</v>
       </c>
       <c r="AS17">
-        <v>186.68</v>
+        <v>186.83</v>
       </c>
       <c r="AT17">
-        <v>236.33</v>
+        <v>236.52</v>
       </c>
       <c r="AU17">
-        <v>184.81</v>
+        <v>185.14</v>
       </c>
       <c r="AV17">
-        <v>140.38999999999999</v>
+        <v>140.16</v>
       </c>
       <c r="AW17">
-        <v>113.66</v>
+        <v>114.12</v>
+      </c>
+      <c r="AX17">
+        <v>95.54</v>
       </c>
     </row>
-    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -6815,7 +6932,7 @@
         <v>4.6500000000000004</v>
       </c>
       <c r="D18">
-        <v>13.73</v>
+        <v>13.76</v>
       </c>
       <c r="E18">
         <v>23.81</v>
@@ -6893,67 +7010,70 @@
         <v>21.15</v>
       </c>
       <c r="AD18">
-        <v>26.3</v>
+        <v>26.38</v>
       </c>
       <c r="AE18">
-        <v>26.6</v>
+        <v>26.58</v>
       </c>
       <c r="AF18">
         <v>33.74</v>
       </c>
       <c r="AG18">
-        <v>52.55</v>
+        <v>52.52</v>
       </c>
       <c r="AH18">
-        <v>75.319999999999993</v>
+        <v>75.290000000000006</v>
       </c>
       <c r="AI18">
-        <v>123.22</v>
+        <v>123.25</v>
       </c>
       <c r="AJ18">
-        <v>182.47</v>
+        <v>182.57</v>
       </c>
       <c r="AK18">
-        <v>213.49</v>
+        <v>213.44</v>
       </c>
       <c r="AL18">
-        <v>220.93</v>
+        <v>220.96</v>
       </c>
       <c r="AM18">
-        <v>208.29</v>
+        <v>208.21</v>
       </c>
       <c r="AN18">
-        <v>189.35</v>
+        <v>189.4</v>
       </c>
       <c r="AO18">
-        <v>195.88</v>
+        <v>195.95</v>
       </c>
       <c r="AP18">
-        <v>224.18</v>
+        <v>224.33</v>
       </c>
       <c r="AQ18">
-        <v>215.07</v>
+        <v>214.94</v>
       </c>
       <c r="AR18">
-        <v>148.91</v>
+        <v>148.99</v>
       </c>
       <c r="AS18">
-        <v>126.12</v>
+        <v>126.09</v>
       </c>
       <c r="AT18">
         <v>161.91</v>
       </c>
       <c r="AU18">
-        <v>137.46</v>
+        <v>137.38999999999999</v>
       </c>
       <c r="AV18">
-        <v>106.97</v>
+        <v>107.03</v>
       </c>
       <c r="AW18">
-        <v>88.06</v>
+        <v>88.57</v>
+      </c>
+      <c r="AX18">
+        <v>73.47</v>
       </c>
     </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>67</v>
       </c>
@@ -7057,52 +7177,55 @@
         <v>44.72</v>
       </c>
       <c r="AI19">
-        <v>74.180000000000007</v>
+        <v>74.13</v>
       </c>
       <c r="AJ19">
-        <v>110.26</v>
+        <v>110.24</v>
       </c>
       <c r="AK19">
-        <v>128.87</v>
+        <v>128.9</v>
       </c>
       <c r="AL19">
-        <v>144.26</v>
+        <v>144.29</v>
       </c>
       <c r="AM19">
-        <v>143.18</v>
+        <v>143.13</v>
       </c>
       <c r="AN19">
-        <v>140</v>
+        <v>140.05000000000001</v>
       </c>
       <c r="AO19">
         <v>139.27000000000001</v>
       </c>
       <c r="AP19">
-        <v>153.34</v>
+        <v>153.31</v>
       </c>
       <c r="AQ19">
-        <v>142.47999999999999</v>
+        <v>142.51</v>
       </c>
       <c r="AR19">
-        <v>91.23</v>
+        <v>91.2</v>
       </c>
       <c r="AS19">
-        <v>71.400000000000006</v>
+        <v>71.430000000000007</v>
       </c>
       <c r="AT19">
-        <v>89.42</v>
+        <v>89.5</v>
       </c>
       <c r="AU19">
-        <v>73.62</v>
+        <v>73.81</v>
       </c>
       <c r="AV19">
-        <v>59.87</v>
+        <v>59.93</v>
       </c>
       <c r="AW19">
-        <v>50.58</v>
+        <v>51.01</v>
+      </c>
+      <c r="AX19">
+        <v>46.02</v>
       </c>
     </row>
-    <row r="20" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>68</v>
       </c>
@@ -7209,10 +7332,10 @@
         <v>49.18</v>
       </c>
       <c r="AJ20">
-        <v>74.91</v>
+        <v>74.94</v>
       </c>
       <c r="AK20">
-        <v>90.1</v>
+        <v>90.13</v>
       </c>
       <c r="AL20">
         <v>97.05</v>
@@ -7221,37 +7344,40 @@
         <v>105.05</v>
       </c>
       <c r="AN20">
-        <v>102.28</v>
+        <v>102.34</v>
       </c>
       <c r="AO20">
-        <v>98.61</v>
+        <v>98.66</v>
       </c>
       <c r="AP20">
-        <v>114.19</v>
+        <v>114.17</v>
       </c>
       <c r="AQ20">
-        <v>115.64</v>
+        <v>115.56</v>
       </c>
       <c r="AR20">
-        <v>81.08</v>
+        <v>81.17</v>
       </c>
       <c r="AS20">
-        <v>52.05</v>
+        <v>52.03</v>
       </c>
       <c r="AT20">
-        <v>64.48</v>
+        <v>64.45</v>
       </c>
       <c r="AU20">
-        <v>59.06</v>
+        <v>59.08</v>
       </c>
       <c r="AV20">
-        <v>51.11</v>
+        <v>51.09</v>
       </c>
       <c r="AW20">
-        <v>43.57</v>
+        <v>43.95</v>
+      </c>
+      <c r="AX20">
+        <v>42.74</v>
       </c>
     </row>
-    <row r="21" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>66</v>
       </c>
@@ -7277,7 +7403,7 @@
         <v>4.0599999999999996</v>
       </c>
       <c r="I21">
-        <v>4.6399999999999997</v>
+        <v>4.67</v>
       </c>
       <c r="J21">
         <v>3.33</v>
@@ -7358,46 +7484,49 @@
         <v>36.93</v>
       </c>
       <c r="AJ21">
-        <v>56.77</v>
+        <v>56.7</v>
       </c>
       <c r="AK21">
-        <v>61.17</v>
+        <v>61.22</v>
       </c>
       <c r="AL21">
-        <v>61.22</v>
+        <v>61.24</v>
       </c>
       <c r="AM21">
         <v>60.05</v>
       </c>
       <c r="AN21">
-        <v>58.84</v>
+        <v>58.77</v>
       </c>
       <c r="AO21">
-        <v>58.39</v>
+        <v>58.24</v>
       </c>
       <c r="AP21">
-        <v>67.75</v>
+        <v>67.599999999999994</v>
       </c>
       <c r="AQ21">
         <v>78.56</v>
       </c>
       <c r="AR21">
-        <v>53.69</v>
+        <v>53.54</v>
       </c>
       <c r="AS21">
-        <v>38.799999999999997</v>
+        <v>38.770000000000003</v>
       </c>
       <c r="AT21">
-        <v>48.77</v>
+        <v>48.7</v>
       </c>
       <c r="AU21">
-        <v>46.98</v>
+        <v>47.05</v>
       </c>
       <c r="AV21">
-        <v>43.12</v>
+        <v>43.02</v>
       </c>
       <c r="AW21">
-        <v>38.700000000000003</v>
+        <v>38.950000000000003</v>
+      </c>
+      <c r="AX21">
+        <v>37.94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add RKI data downloaded 2021-03-14--19-15-01
</commit_message>
<xml_diff>
--- a/rki-data/RKI-Altersverteilung.xlsx
+++ b/rki-data/RKI-Altersverteilung.xlsx
@@ -3,19 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20371"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CC46B5-4B01-4725-950F-F757083D1A63}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C21DF6-2C27-4142-93BD-8D581B78BE40}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23235" windowHeight="9165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23235" windowHeight="9165" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="inzidenz_tabelle" sheetId="1" r:id="rId1"/>
+    <sheet name="Erläuterungen" sheetId="3" r:id="rId1"/>
+    <sheet name="Fallzahlen" sheetId="2" r:id="rId2"/>
+    <sheet name="7-Tage-Inzidenzen" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="76">
   <si>
     <t>Altersgruppe</t>
   </si>
@@ -234,6 +236,16 @@
   </si>
   <si>
     <t>10 - 14</t>
+  </si>
+  <si>
+    <t>Zur besseren Übersicht werden mit Berichtswoche 46 die altersspezifischen Anteile als 7-Tage-Inzidenz pro 100.000 Einwohner nach Meldewoche dargestellt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auf den folgenden Tabellenblättern finden sich die altersspezifischen Fallzahlen sowie die altersspezifischen 7-Tage-Inzidenzen. </t>
+  </si>
+  <si>
+    <t>Für die Berechnung von Inzidenzen wurde die Bevölkerungsstatistik
+mit Stand 31.12.2019 herangezogen.</t>
   </si>
 </sst>
 </file>
@@ -717,9 +729,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1074,11 +1089,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62335572-56F4-4D6E-B05A-2B52239D257C}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+    </row>
+    <row r="4" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D90D7B9-2525-4D74-A23A-F28E2F015D7A}">
   <dimension ref="A1:BA21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
-      <selection activeCell="AZ24" sqref="AZ24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1249,6 +1301,3403 @@
         <v>53</v>
       </c>
       <c r="B2">
+        <v>6424</v>
+      </c>
+      <c r="C2">
+        <v>22431</v>
+      </c>
+      <c r="D2">
+        <v>34006</v>
+      </c>
+      <c r="E2">
+        <v>36086</v>
+      </c>
+      <c r="F2">
+        <v>27187</v>
+      </c>
+      <c r="G2">
+        <v>17369</v>
+      </c>
+      <c r="H2">
+        <v>12376</v>
+      </c>
+      <c r="I2">
+        <v>7445</v>
+      </c>
+      <c r="J2">
+        <v>6241</v>
+      </c>
+      <c r="K2">
+        <v>4753</v>
+      </c>
+      <c r="L2">
+        <v>3621</v>
+      </c>
+      <c r="M2">
+        <v>3208</v>
+      </c>
+      <c r="N2">
+        <v>2358</v>
+      </c>
+      <c r="O2">
+        <v>2344</v>
+      </c>
+      <c r="P2">
+        <v>4129</v>
+      </c>
+      <c r="Q2">
+        <v>3216</v>
+      </c>
+      <c r="R2">
+        <v>2697</v>
+      </c>
+      <c r="S2">
+        <v>2428</v>
+      </c>
+      <c r="T2">
+        <v>3016</v>
+      </c>
+      <c r="U2">
+        <v>3933</v>
+      </c>
+      <c r="V2">
+        <v>4820</v>
+      </c>
+      <c r="W2">
+        <v>6055</v>
+      </c>
+      <c r="X2">
+        <v>7950</v>
+      </c>
+      <c r="Y2">
+        <v>9595</v>
+      </c>
+      <c r="Z2">
+        <v>8819</v>
+      </c>
+      <c r="AA2">
+        <v>8623</v>
+      </c>
+      <c r="AB2">
+        <v>9772</v>
+      </c>
+      <c r="AC2">
+        <v>12293</v>
+      </c>
+      <c r="AD2">
+        <v>13071</v>
+      </c>
+      <c r="AE2">
+        <v>15930</v>
+      </c>
+      <c r="AF2">
+        <v>26128</v>
+      </c>
+      <c r="AG2">
+        <v>42084</v>
+      </c>
+      <c r="AH2">
+        <v>74859</v>
+      </c>
+      <c r="AI2">
+        <v>111133</v>
+      </c>
+      <c r="AJ2">
+        <v>125836</v>
+      </c>
+      <c r="AK2">
+        <v>127918</v>
+      </c>
+      <c r="AL2">
+        <v>128506</v>
+      </c>
+      <c r="AM2">
+        <v>123313</v>
+      </c>
+      <c r="AN2">
+        <v>128513</v>
+      </c>
+      <c r="AO2">
+        <v>156556</v>
+      </c>
+      <c r="AP2">
+        <v>174967</v>
+      </c>
+      <c r="AQ2">
+        <v>139293</v>
+      </c>
+      <c r="AR2">
+        <v>123231</v>
+      </c>
+      <c r="AS2">
+        <v>145545</v>
+      </c>
+      <c r="AT2">
+        <v>119016</v>
+      </c>
+      <c r="AU2">
+        <v>95606</v>
+      </c>
+      <c r="AV2">
+        <v>78311</v>
+      </c>
+      <c r="AW2">
+        <v>64655</v>
+      </c>
+      <c r="AX2">
+        <v>50888</v>
+      </c>
+      <c r="AY2">
+        <v>52504</v>
+      </c>
+      <c r="AZ2">
+        <v>56471</v>
+      </c>
+      <c r="BA2">
+        <v>57979</v>
+      </c>
+    </row>
+    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>101</v>
+      </c>
+      <c r="D3">
+        <v>424</v>
+      </c>
+      <c r="E3">
+        <v>1171</v>
+      </c>
+      <c r="F3">
+        <v>1244</v>
+      </c>
+      <c r="G3">
+        <v>848</v>
+      </c>
+      <c r="H3">
+        <v>581</v>
+      </c>
+      <c r="I3">
+        <v>285</v>
+      </c>
+      <c r="J3">
+        <v>208</v>
+      </c>
+      <c r="K3">
+        <v>143</v>
+      </c>
+      <c r="L3">
+        <v>103</v>
+      </c>
+      <c r="M3">
+        <v>72</v>
+      </c>
+      <c r="N3">
+        <v>42</v>
+      </c>
+      <c r="O3">
+        <v>46</v>
+      </c>
+      <c r="P3">
+        <v>37</v>
+      </c>
+      <c r="Q3">
+        <v>28</v>
+      </c>
+      <c r="R3">
+        <v>24</v>
+      </c>
+      <c r="S3">
+        <v>15</v>
+      </c>
+      <c r="T3">
+        <v>27</v>
+      </c>
+      <c r="U3">
+        <v>17</v>
+      </c>
+      <c r="V3">
+        <v>39</v>
+      </c>
+      <c r="W3">
+        <v>28</v>
+      </c>
+      <c r="X3">
+        <v>25</v>
+      </c>
+      <c r="Y3">
+        <v>18</v>
+      </c>
+      <c r="Z3">
+        <v>29</v>
+      </c>
+      <c r="AA3">
+        <v>24</v>
+      </c>
+      <c r="AB3">
+        <v>45</v>
+      </c>
+      <c r="AC3">
+        <v>74</v>
+      </c>
+      <c r="AD3">
+        <v>94</v>
+      </c>
+      <c r="AE3">
+        <v>118</v>
+      </c>
+      <c r="AF3">
+        <v>184</v>
+      </c>
+      <c r="AG3">
+        <v>438</v>
+      </c>
+      <c r="AH3">
+        <v>884</v>
+      </c>
+      <c r="AI3">
+        <v>1467</v>
+      </c>
+      <c r="AJ3">
+        <v>1724</v>
+      </c>
+      <c r="AK3">
+        <v>2320</v>
+      </c>
+      <c r="AL3">
+        <v>3072</v>
+      </c>
+      <c r="AM3">
+        <v>3516</v>
+      </c>
+      <c r="AN3">
+        <v>4185</v>
+      </c>
+      <c r="AO3">
+        <v>5412</v>
+      </c>
+      <c r="AP3">
+        <v>5978</v>
+      </c>
+      <c r="AQ3">
+        <v>5264</v>
+      </c>
+      <c r="AR3">
+        <v>4976</v>
+      </c>
+      <c r="AS3">
+        <v>5412</v>
+      </c>
+      <c r="AT3">
+        <v>5040</v>
+      </c>
+      <c r="AU3">
+        <v>3945</v>
+      </c>
+      <c r="AV3">
+        <v>2884</v>
+      </c>
+      <c r="AW3">
+        <v>1939</v>
+      </c>
+      <c r="AX3">
+        <v>1310</v>
+      </c>
+      <c r="AY3">
+        <v>1080</v>
+      </c>
+      <c r="AZ3">
+        <v>830</v>
+      </c>
+      <c r="BA3">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4">
+        <v>38</v>
+      </c>
+      <c r="C4">
+        <v>220</v>
+      </c>
+      <c r="D4">
+        <v>738</v>
+      </c>
+      <c r="E4">
+        <v>1448</v>
+      </c>
+      <c r="F4">
+        <v>1423</v>
+      </c>
+      <c r="G4">
+        <v>926</v>
+      </c>
+      <c r="H4">
+        <v>681</v>
+      </c>
+      <c r="I4">
+        <v>326</v>
+      </c>
+      <c r="J4">
+        <v>263</v>
+      </c>
+      <c r="K4">
+        <v>179</v>
+      </c>
+      <c r="L4">
+        <v>127</v>
+      </c>
+      <c r="M4">
+        <v>85</v>
+      </c>
+      <c r="N4">
+        <v>51</v>
+      </c>
+      <c r="O4">
+        <v>51</v>
+      </c>
+      <c r="P4">
+        <v>47</v>
+      </c>
+      <c r="Q4">
+        <v>34</v>
+      </c>
+      <c r="R4">
+        <v>28</v>
+      </c>
+      <c r="S4">
+        <v>20</v>
+      </c>
+      <c r="T4">
+        <v>24</v>
+      </c>
+      <c r="U4">
+        <v>34</v>
+      </c>
+      <c r="V4">
+        <v>41</v>
+      </c>
+      <c r="W4">
+        <v>40</v>
+      </c>
+      <c r="X4">
+        <v>56</v>
+      </c>
+      <c r="Y4">
+        <v>23</v>
+      </c>
+      <c r="Z4">
+        <v>33</v>
+      </c>
+      <c r="AA4">
+        <v>25</v>
+      </c>
+      <c r="AB4">
+        <v>84</v>
+      </c>
+      <c r="AC4">
+        <v>103</v>
+      </c>
+      <c r="AD4">
+        <v>121</v>
+      </c>
+      <c r="AE4">
+        <v>165</v>
+      </c>
+      <c r="AF4">
+        <v>306</v>
+      </c>
+      <c r="AG4">
+        <v>575</v>
+      </c>
+      <c r="AH4">
+        <v>1146</v>
+      </c>
+      <c r="AI4">
+        <v>1786</v>
+      </c>
+      <c r="AJ4">
+        <v>2293</v>
+      </c>
+      <c r="AK4">
+        <v>2831</v>
+      </c>
+      <c r="AL4">
+        <v>3373</v>
+      </c>
+      <c r="AM4">
+        <v>4098</v>
+      </c>
+      <c r="AN4">
+        <v>4600</v>
+      </c>
+      <c r="AO4">
+        <v>5931</v>
+      </c>
+      <c r="AP4">
+        <v>6954</v>
+      </c>
+      <c r="AQ4">
+        <v>5865</v>
+      </c>
+      <c r="AR4">
+        <v>5598</v>
+      </c>
+      <c r="AS4">
+        <v>6083</v>
+      </c>
+      <c r="AT4">
+        <v>5554</v>
+      </c>
+      <c r="AU4">
+        <v>4450</v>
+      </c>
+      <c r="AV4">
+        <v>3330</v>
+      </c>
+      <c r="AW4">
+        <v>2580</v>
+      </c>
+      <c r="AX4">
+        <v>1656</v>
+      </c>
+      <c r="AY4">
+        <v>1462</v>
+      </c>
+      <c r="AZ4">
+        <v>1208</v>
+      </c>
+      <c r="BA4">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5">
+        <v>85</v>
+      </c>
+      <c r="C5">
+        <v>468</v>
+      </c>
+      <c r="D5">
+        <v>1282</v>
+      </c>
+      <c r="E5">
+        <v>1966</v>
+      </c>
+      <c r="F5">
+        <v>1717</v>
+      </c>
+      <c r="G5">
+        <v>1181</v>
+      </c>
+      <c r="H5">
+        <v>822</v>
+      </c>
+      <c r="I5">
+        <v>452</v>
+      </c>
+      <c r="J5">
+        <v>299</v>
+      </c>
+      <c r="K5">
+        <v>246</v>
+      </c>
+      <c r="L5">
+        <v>153</v>
+      </c>
+      <c r="M5">
+        <v>112</v>
+      </c>
+      <c r="N5">
+        <v>76</v>
+      </c>
+      <c r="O5">
+        <v>62</v>
+      </c>
+      <c r="P5">
+        <v>62</v>
+      </c>
+      <c r="Q5">
+        <v>51</v>
+      </c>
+      <c r="R5">
+        <v>49</v>
+      </c>
+      <c r="S5">
+        <v>36</v>
+      </c>
+      <c r="T5">
+        <v>38</v>
+      </c>
+      <c r="U5">
+        <v>51</v>
+      </c>
+      <c r="V5">
+        <v>90</v>
+      </c>
+      <c r="W5">
+        <v>69</v>
+      </c>
+      <c r="X5">
+        <v>81</v>
+      </c>
+      <c r="Y5">
+        <v>64</v>
+      </c>
+      <c r="Z5">
+        <v>50</v>
+      </c>
+      <c r="AA5">
+        <v>60</v>
+      </c>
+      <c r="AB5">
+        <v>133</v>
+      </c>
+      <c r="AC5">
+        <v>195</v>
+      </c>
+      <c r="AD5">
+        <v>212</v>
+      </c>
+      <c r="AE5">
+        <v>316</v>
+      </c>
+      <c r="AF5">
+        <v>470</v>
+      </c>
+      <c r="AG5">
+        <v>857</v>
+      </c>
+      <c r="AH5">
+        <v>1835</v>
+      </c>
+      <c r="AI5">
+        <v>2840</v>
+      </c>
+      <c r="AJ5">
+        <v>3437</v>
+      </c>
+      <c r="AK5">
+        <v>3808</v>
+      </c>
+      <c r="AL5">
+        <v>4360</v>
+      </c>
+      <c r="AM5">
+        <v>4786</v>
+      </c>
+      <c r="AN5">
+        <v>5450</v>
+      </c>
+      <c r="AO5">
+        <v>7089</v>
+      </c>
+      <c r="AP5">
+        <v>8277</v>
+      </c>
+      <c r="AQ5">
+        <v>7438</v>
+      </c>
+      <c r="AR5">
+        <v>6875</v>
+      </c>
+      <c r="AS5">
+        <v>7675</v>
+      </c>
+      <c r="AT5">
+        <v>6690</v>
+      </c>
+      <c r="AU5">
+        <v>5328</v>
+      </c>
+      <c r="AV5">
+        <v>4195</v>
+      </c>
+      <c r="AW5">
+        <v>3145</v>
+      </c>
+      <c r="AX5">
+        <v>2299</v>
+      </c>
+      <c r="AY5">
+        <v>2002</v>
+      </c>
+      <c r="AZ5">
+        <v>1782</v>
+      </c>
+      <c r="BA5">
+        <v>1531</v>
+      </c>
+    </row>
+    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6">
+        <v>114</v>
+      </c>
+      <c r="C6">
+        <v>572</v>
+      </c>
+      <c r="D6">
+        <v>1407</v>
+      </c>
+      <c r="E6">
+        <v>1787</v>
+      </c>
+      <c r="F6">
+        <v>1314</v>
+      </c>
+      <c r="G6">
+        <v>854</v>
+      </c>
+      <c r="H6">
+        <v>587</v>
+      </c>
+      <c r="I6">
+        <v>351</v>
+      </c>
+      <c r="J6">
+        <v>275</v>
+      </c>
+      <c r="K6">
+        <v>176</v>
+      </c>
+      <c r="L6">
+        <v>106</v>
+      </c>
+      <c r="M6">
+        <v>82</v>
+      </c>
+      <c r="N6">
+        <v>58</v>
+      </c>
+      <c r="O6">
+        <v>46</v>
+      </c>
+      <c r="P6">
+        <v>65</v>
+      </c>
+      <c r="Q6">
+        <v>57</v>
+      </c>
+      <c r="R6">
+        <v>40</v>
+      </c>
+      <c r="S6">
+        <v>40</v>
+      </c>
+      <c r="T6">
+        <v>44</v>
+      </c>
+      <c r="U6">
+        <v>57</v>
+      </c>
+      <c r="V6">
+        <v>71</v>
+      </c>
+      <c r="W6">
+        <v>55</v>
+      </c>
+      <c r="X6">
+        <v>71</v>
+      </c>
+      <c r="Y6">
+        <v>67</v>
+      </c>
+      <c r="Z6">
+        <v>69</v>
+      </c>
+      <c r="AA6">
+        <v>75</v>
+      </c>
+      <c r="AB6">
+        <v>147</v>
+      </c>
+      <c r="AC6">
+        <v>181</v>
+      </c>
+      <c r="AD6">
+        <v>232</v>
+      </c>
+      <c r="AE6">
+        <v>310</v>
+      </c>
+      <c r="AF6">
+        <v>504</v>
+      </c>
+      <c r="AG6">
+        <v>903</v>
+      </c>
+      <c r="AH6">
+        <v>1626</v>
+      </c>
+      <c r="AI6">
+        <v>2651</v>
+      </c>
+      <c r="AJ6">
+        <v>3054</v>
+      </c>
+      <c r="AK6">
+        <v>3293</v>
+      </c>
+      <c r="AL6">
+        <v>3389</v>
+      </c>
+      <c r="AM6">
+        <v>3496</v>
+      </c>
+      <c r="AN6">
+        <v>3974</v>
+      </c>
+      <c r="AO6">
+        <v>4997</v>
+      </c>
+      <c r="AP6">
+        <v>5945</v>
+      </c>
+      <c r="AQ6">
+        <v>5117</v>
+      </c>
+      <c r="AR6">
+        <v>4642</v>
+      </c>
+      <c r="AS6">
+        <v>5229</v>
+      </c>
+      <c r="AT6">
+        <v>4315</v>
+      </c>
+      <c r="AU6">
+        <v>3421</v>
+      </c>
+      <c r="AV6">
+        <v>2826</v>
+      </c>
+      <c r="AW6">
+        <v>2211</v>
+      </c>
+      <c r="AX6">
+        <v>1702</v>
+      </c>
+      <c r="AY6">
+        <v>1714</v>
+      </c>
+      <c r="AZ6">
+        <v>1583</v>
+      </c>
+      <c r="BA6">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7">
+        <v>144</v>
+      </c>
+      <c r="C7">
+        <v>619</v>
+      </c>
+      <c r="D7">
+        <v>1327</v>
+      </c>
+      <c r="E7">
+        <v>1417</v>
+      </c>
+      <c r="F7">
+        <v>1050</v>
+      </c>
+      <c r="G7">
+        <v>631</v>
+      </c>
+      <c r="H7">
+        <v>424</v>
+      </c>
+      <c r="I7">
+        <v>275</v>
+      </c>
+      <c r="J7">
+        <v>207</v>
+      </c>
+      <c r="K7">
+        <v>129</v>
+      </c>
+      <c r="L7">
+        <v>93</v>
+      </c>
+      <c r="M7">
+        <v>80</v>
+      </c>
+      <c r="N7">
+        <v>47</v>
+      </c>
+      <c r="O7">
+        <v>40</v>
+      </c>
+      <c r="P7">
+        <v>58</v>
+      </c>
+      <c r="Q7">
+        <v>40</v>
+      </c>
+      <c r="R7">
+        <v>37</v>
+      </c>
+      <c r="S7">
+        <v>56</v>
+      </c>
+      <c r="T7">
+        <v>62</v>
+      </c>
+      <c r="U7">
+        <v>63</v>
+      </c>
+      <c r="V7">
+        <v>89</v>
+      </c>
+      <c r="W7">
+        <v>91</v>
+      </c>
+      <c r="X7">
+        <v>79</v>
+      </c>
+      <c r="Y7">
+        <v>96</v>
+      </c>
+      <c r="Z7">
+        <v>92</v>
+      </c>
+      <c r="AA7">
+        <v>106</v>
+      </c>
+      <c r="AB7">
+        <v>150</v>
+      </c>
+      <c r="AC7">
+        <v>259</v>
+      </c>
+      <c r="AD7">
+        <v>265</v>
+      </c>
+      <c r="AE7">
+        <v>348</v>
+      </c>
+      <c r="AF7">
+        <v>587</v>
+      </c>
+      <c r="AG7">
+        <v>933</v>
+      </c>
+      <c r="AH7">
+        <v>1799</v>
+      </c>
+      <c r="AI7">
+        <v>2883</v>
+      </c>
+      <c r="AJ7">
+        <v>3181</v>
+      </c>
+      <c r="AK7">
+        <v>3295</v>
+      </c>
+      <c r="AL7">
+        <v>3359</v>
+      </c>
+      <c r="AM7">
+        <v>3201</v>
+      </c>
+      <c r="AN7">
+        <v>3483</v>
+      </c>
+      <c r="AO7">
+        <v>4394</v>
+      </c>
+      <c r="AP7">
+        <v>5172</v>
+      </c>
+      <c r="AQ7">
+        <v>4454</v>
+      </c>
+      <c r="AR7">
+        <v>4139</v>
+      </c>
+      <c r="AS7">
+        <v>4826</v>
+      </c>
+      <c r="AT7">
+        <v>3661</v>
+      </c>
+      <c r="AU7">
+        <v>3064</v>
+      </c>
+      <c r="AV7">
+        <v>2483</v>
+      </c>
+      <c r="AW7">
+        <v>2066</v>
+      </c>
+      <c r="AX7">
+        <v>1576</v>
+      </c>
+      <c r="AY7">
+        <v>1591</v>
+      </c>
+      <c r="AZ7">
+        <v>1649</v>
+      </c>
+      <c r="BA7">
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8">
+        <v>237</v>
+      </c>
+      <c r="C8">
+        <v>887</v>
+      </c>
+      <c r="D8">
+        <v>1647</v>
+      </c>
+      <c r="E8">
+        <v>1692</v>
+      </c>
+      <c r="F8">
+        <v>1117</v>
+      </c>
+      <c r="G8">
+        <v>662</v>
+      </c>
+      <c r="H8">
+        <v>504</v>
+      </c>
+      <c r="I8">
+        <v>266</v>
+      </c>
+      <c r="J8">
+        <v>208</v>
+      </c>
+      <c r="K8">
+        <v>146</v>
+      </c>
+      <c r="L8">
+        <v>123</v>
+      </c>
+      <c r="M8">
+        <v>107</v>
+      </c>
+      <c r="N8">
+        <v>60</v>
+      </c>
+      <c r="O8">
+        <v>51</v>
+      </c>
+      <c r="P8">
+        <v>69</v>
+      </c>
+      <c r="Q8">
+        <v>66</v>
+      </c>
+      <c r="R8">
+        <v>62</v>
+      </c>
+      <c r="S8">
+        <v>62</v>
+      </c>
+      <c r="T8">
+        <v>71</v>
+      </c>
+      <c r="U8">
+        <v>85</v>
+      </c>
+      <c r="V8">
+        <v>86</v>
+      </c>
+      <c r="W8">
+        <v>121</v>
+      </c>
+      <c r="X8">
+        <v>110</v>
+      </c>
+      <c r="Y8">
+        <v>121</v>
+      </c>
+      <c r="Z8">
+        <v>131</v>
+      </c>
+      <c r="AA8">
+        <v>128</v>
+      </c>
+      <c r="AB8">
+        <v>225</v>
+      </c>
+      <c r="AC8">
+        <v>290</v>
+      </c>
+      <c r="AD8">
+        <v>305</v>
+      </c>
+      <c r="AE8">
+        <v>452</v>
+      </c>
+      <c r="AF8">
+        <v>684</v>
+      </c>
+      <c r="AG8">
+        <v>1285</v>
+      </c>
+      <c r="AH8">
+        <v>2266</v>
+      </c>
+      <c r="AI8">
+        <v>3553</v>
+      </c>
+      <c r="AJ8">
+        <v>4260</v>
+      </c>
+      <c r="AK8">
+        <v>4016</v>
+      </c>
+      <c r="AL8">
+        <v>4158</v>
+      </c>
+      <c r="AM8">
+        <v>4140</v>
+      </c>
+      <c r="AN8">
+        <v>4123</v>
+      </c>
+      <c r="AO8">
+        <v>5177</v>
+      </c>
+      <c r="AP8">
+        <v>6354</v>
+      </c>
+      <c r="AQ8">
+        <v>5590</v>
+      </c>
+      <c r="AR8">
+        <v>4981</v>
+      </c>
+      <c r="AS8">
+        <v>5719</v>
+      </c>
+      <c r="AT8">
+        <v>4413</v>
+      </c>
+      <c r="AU8">
+        <v>3625</v>
+      </c>
+      <c r="AV8">
+        <v>3130</v>
+      </c>
+      <c r="AW8">
+        <v>2532</v>
+      </c>
+      <c r="AX8">
+        <v>1919</v>
+      </c>
+      <c r="AY8">
+        <v>2045</v>
+      </c>
+      <c r="AZ8">
+        <v>2133</v>
+      </c>
+      <c r="BA8">
+        <v>1983</v>
+      </c>
+    </row>
+    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9">
+        <v>427</v>
+      </c>
+      <c r="C9">
+        <v>1597</v>
+      </c>
+      <c r="D9">
+        <v>2527</v>
+      </c>
+      <c r="E9">
+        <v>2782</v>
+      </c>
+      <c r="F9">
+        <v>1796</v>
+      </c>
+      <c r="G9">
+        <v>1087</v>
+      </c>
+      <c r="H9">
+        <v>674</v>
+      </c>
+      <c r="I9">
+        <v>405</v>
+      </c>
+      <c r="J9">
+        <v>332</v>
+      </c>
+      <c r="K9">
+        <v>240</v>
+      </c>
+      <c r="L9">
+        <v>175</v>
+      </c>
+      <c r="M9">
+        <v>168</v>
+      </c>
+      <c r="N9">
+        <v>107</v>
+      </c>
+      <c r="O9">
+        <v>91</v>
+      </c>
+      <c r="P9">
+        <v>122</v>
+      </c>
+      <c r="Q9">
+        <v>108</v>
+      </c>
+      <c r="R9">
+        <v>111</v>
+      </c>
+      <c r="S9">
+        <v>93</v>
+      </c>
+      <c r="T9">
+        <v>110</v>
+      </c>
+      <c r="U9">
+        <v>152</v>
+      </c>
+      <c r="V9">
+        <v>152</v>
+      </c>
+      <c r="W9">
+        <v>204</v>
+      </c>
+      <c r="X9">
+        <v>192</v>
+      </c>
+      <c r="Y9">
+        <v>237</v>
+      </c>
+      <c r="Z9">
+        <v>244</v>
+      </c>
+      <c r="AA9">
+        <v>248</v>
+      </c>
+      <c r="AB9">
+        <v>339</v>
+      </c>
+      <c r="AC9">
+        <v>493</v>
+      </c>
+      <c r="AD9">
+        <v>542</v>
+      </c>
+      <c r="AE9">
+        <v>680</v>
+      </c>
+      <c r="AF9">
+        <v>1271</v>
+      </c>
+      <c r="AG9">
+        <v>2118</v>
+      </c>
+      <c r="AH9">
+        <v>3956</v>
+      </c>
+      <c r="AI9">
+        <v>6000</v>
+      </c>
+      <c r="AJ9">
+        <v>6864</v>
+      </c>
+      <c r="AK9">
+        <v>6914</v>
+      </c>
+      <c r="AL9">
+        <v>7312</v>
+      </c>
+      <c r="AM9">
+        <v>7001</v>
+      </c>
+      <c r="AN9">
+        <v>7656</v>
+      </c>
+      <c r="AO9">
+        <v>9432</v>
+      </c>
+      <c r="AP9">
+        <v>11027</v>
+      </c>
+      <c r="AQ9">
+        <v>9188</v>
+      </c>
+      <c r="AR9">
+        <v>8277</v>
+      </c>
+      <c r="AS9">
+        <v>9269</v>
+      </c>
+      <c r="AT9">
+        <v>7551</v>
+      </c>
+      <c r="AU9">
+        <v>6233</v>
+      </c>
+      <c r="AV9">
+        <v>5130</v>
+      </c>
+      <c r="AW9">
+        <v>4217</v>
+      </c>
+      <c r="AX9">
+        <v>3193</v>
+      </c>
+      <c r="AY9">
+        <v>3263</v>
+      </c>
+      <c r="AZ9">
+        <v>3517</v>
+      </c>
+      <c r="BA9">
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10">
+        <v>751</v>
+      </c>
+      <c r="C10">
+        <v>2599</v>
+      </c>
+      <c r="D10">
+        <v>3593</v>
+      </c>
+      <c r="E10">
+        <v>3669</v>
+      </c>
+      <c r="F10">
+        <v>2609</v>
+      </c>
+      <c r="G10">
+        <v>1566</v>
+      </c>
+      <c r="H10">
+        <v>1059</v>
+      </c>
+      <c r="I10">
+        <v>600</v>
+      </c>
+      <c r="J10">
+        <v>511</v>
+      </c>
+      <c r="K10">
+        <v>360</v>
+      </c>
+      <c r="L10">
+        <v>266</v>
+      </c>
+      <c r="M10">
+        <v>237</v>
+      </c>
+      <c r="N10">
+        <v>142</v>
+      </c>
+      <c r="O10">
+        <v>134</v>
+      </c>
+      <c r="P10">
+        <v>186</v>
+      </c>
+      <c r="Q10">
+        <v>202</v>
+      </c>
+      <c r="R10">
+        <v>156</v>
+      </c>
+      <c r="S10">
+        <v>116</v>
+      </c>
+      <c r="T10">
+        <v>177</v>
+      </c>
+      <c r="U10">
+        <v>242</v>
+      </c>
+      <c r="V10">
+        <v>285</v>
+      </c>
+      <c r="W10">
+        <v>308</v>
+      </c>
+      <c r="X10">
+        <v>326</v>
+      </c>
+      <c r="Y10">
+        <v>430</v>
+      </c>
+      <c r="Z10">
+        <v>355</v>
+      </c>
+      <c r="AA10">
+        <v>393</v>
+      </c>
+      <c r="AB10">
+        <v>555</v>
+      </c>
+      <c r="AC10">
+        <v>762</v>
+      </c>
+      <c r="AD10">
+        <v>866</v>
+      </c>
+      <c r="AE10">
+        <v>1109</v>
+      </c>
+      <c r="AF10">
+        <v>1871</v>
+      </c>
+      <c r="AG10">
+        <v>2999</v>
+      </c>
+      <c r="AH10">
+        <v>5761</v>
+      </c>
+      <c r="AI10">
+        <v>8972</v>
+      </c>
+      <c r="AJ10">
+        <v>10169</v>
+      </c>
+      <c r="AK10">
+        <v>10308</v>
+      </c>
+      <c r="AL10">
+        <v>10246</v>
+      </c>
+      <c r="AM10">
+        <v>9879</v>
+      </c>
+      <c r="AN10">
+        <v>10369</v>
+      </c>
+      <c r="AO10">
+        <v>13067</v>
+      </c>
+      <c r="AP10">
+        <v>15015</v>
+      </c>
+      <c r="AQ10">
+        <v>12381</v>
+      </c>
+      <c r="AR10">
+        <v>11086</v>
+      </c>
+      <c r="AS10">
+        <v>12324</v>
+      </c>
+      <c r="AT10">
+        <v>10033</v>
+      </c>
+      <c r="AU10">
+        <v>8350</v>
+      </c>
+      <c r="AV10">
+        <v>7026</v>
+      </c>
+      <c r="AW10">
+        <v>5812</v>
+      </c>
+      <c r="AX10">
+        <v>4505</v>
+      </c>
+      <c r="AY10">
+        <v>4600</v>
+      </c>
+      <c r="AZ10">
+        <v>4840</v>
+      </c>
+      <c r="BA10">
+        <v>4582</v>
+      </c>
+    </row>
+    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11">
+        <v>978</v>
+      </c>
+      <c r="C11">
+        <v>3090</v>
+      </c>
+      <c r="D11">
+        <v>4000</v>
+      </c>
+      <c r="E11">
+        <v>3697</v>
+      </c>
+      <c r="F11">
+        <v>2613</v>
+      </c>
+      <c r="G11">
+        <v>1560</v>
+      </c>
+      <c r="H11">
+        <v>994</v>
+      </c>
+      <c r="I11">
+        <v>605</v>
+      </c>
+      <c r="J11">
+        <v>520</v>
+      </c>
+      <c r="K11">
+        <v>375</v>
+      </c>
+      <c r="L11">
+        <v>252</v>
+      </c>
+      <c r="M11">
+        <v>240</v>
+      </c>
+      <c r="N11">
+        <v>150</v>
+      </c>
+      <c r="O11">
+        <v>146</v>
+      </c>
+      <c r="P11">
+        <v>318</v>
+      </c>
+      <c r="Q11">
+        <v>268</v>
+      </c>
+      <c r="R11">
+        <v>186</v>
+      </c>
+      <c r="S11">
+        <v>172</v>
+      </c>
+      <c r="T11">
+        <v>208</v>
+      </c>
+      <c r="U11">
+        <v>294</v>
+      </c>
+      <c r="V11">
+        <v>350</v>
+      </c>
+      <c r="W11">
+        <v>418</v>
+      </c>
+      <c r="X11">
+        <v>473</v>
+      </c>
+      <c r="Y11">
+        <v>560</v>
+      </c>
+      <c r="Z11">
+        <v>538</v>
+      </c>
+      <c r="AA11">
+        <v>552</v>
+      </c>
+      <c r="AB11">
+        <v>669</v>
+      </c>
+      <c r="AC11">
+        <v>896</v>
+      </c>
+      <c r="AD11">
+        <v>995</v>
+      </c>
+      <c r="AE11">
+        <v>1207</v>
+      </c>
+      <c r="AF11">
+        <v>2267</v>
+      </c>
+      <c r="AG11">
+        <v>3577</v>
+      </c>
+      <c r="AH11">
+        <v>6422</v>
+      </c>
+      <c r="AI11">
+        <v>9779</v>
+      </c>
+      <c r="AJ11">
+        <v>10964</v>
+      </c>
+      <c r="AK11">
+        <v>11008</v>
+      </c>
+      <c r="AL11">
+        <v>10834</v>
+      </c>
+      <c r="AM11">
+        <v>10346</v>
+      </c>
+      <c r="AN11">
+        <v>10559</v>
+      </c>
+      <c r="AO11">
+        <v>13260</v>
+      </c>
+      <c r="AP11">
+        <v>14926</v>
+      </c>
+      <c r="AQ11">
+        <v>11997</v>
+      </c>
+      <c r="AR11">
+        <v>10529</v>
+      </c>
+      <c r="AS11">
+        <v>12087</v>
+      </c>
+      <c r="AT11">
+        <v>9799</v>
+      </c>
+      <c r="AU11">
+        <v>8186</v>
+      </c>
+      <c r="AV11">
+        <v>6686</v>
+      </c>
+      <c r="AW11">
+        <v>5300</v>
+      </c>
+      <c r="AX11">
+        <v>4306</v>
+      </c>
+      <c r="AY11">
+        <v>4511</v>
+      </c>
+      <c r="AZ11">
+        <v>4733</v>
+      </c>
+      <c r="BA11">
+        <v>4901</v>
+      </c>
+    </row>
+    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12">
+        <v>741</v>
+      </c>
+      <c r="C12">
+        <v>2101</v>
+      </c>
+      <c r="D12">
+        <v>2923</v>
+      </c>
+      <c r="E12">
+        <v>2720</v>
+      </c>
+      <c r="F12">
+        <v>1922</v>
+      </c>
+      <c r="G12">
+        <v>1174</v>
+      </c>
+      <c r="H12">
+        <v>790</v>
+      </c>
+      <c r="I12">
+        <v>469</v>
+      </c>
+      <c r="J12">
+        <v>448</v>
+      </c>
+      <c r="K12">
+        <v>329</v>
+      </c>
+      <c r="L12">
+        <v>254</v>
+      </c>
+      <c r="M12">
+        <v>214</v>
+      </c>
+      <c r="N12">
+        <v>162</v>
+      </c>
+      <c r="O12">
+        <v>145</v>
+      </c>
+      <c r="P12">
+        <v>375</v>
+      </c>
+      <c r="Q12">
+        <v>277</v>
+      </c>
+      <c r="R12">
+        <v>221</v>
+      </c>
+      <c r="S12">
+        <v>182</v>
+      </c>
+      <c r="T12">
+        <v>232</v>
+      </c>
+      <c r="U12">
+        <v>334</v>
+      </c>
+      <c r="V12">
+        <v>385</v>
+      </c>
+      <c r="W12">
+        <v>455</v>
+      </c>
+      <c r="X12">
+        <v>575</v>
+      </c>
+      <c r="Y12">
+        <v>695</v>
+      </c>
+      <c r="Z12">
+        <v>602</v>
+      </c>
+      <c r="AA12">
+        <v>614</v>
+      </c>
+      <c r="AB12">
+        <v>694</v>
+      </c>
+      <c r="AC12">
+        <v>875</v>
+      </c>
+      <c r="AD12">
+        <v>897</v>
+      </c>
+      <c r="AE12">
+        <v>1199</v>
+      </c>
+      <c r="AF12">
+        <v>2037</v>
+      </c>
+      <c r="AG12">
+        <v>3128</v>
+      </c>
+      <c r="AH12">
+        <v>5813</v>
+      </c>
+      <c r="AI12">
+        <v>8390</v>
+      </c>
+      <c r="AJ12">
+        <v>9473</v>
+      </c>
+      <c r="AK12">
+        <v>9299</v>
+      </c>
+      <c r="AL12">
+        <v>9676</v>
+      </c>
+      <c r="AM12">
+        <v>9061</v>
+      </c>
+      <c r="AN12">
+        <v>9238</v>
+      </c>
+      <c r="AO12">
+        <v>11102</v>
+      </c>
+      <c r="AP12">
+        <v>12442</v>
+      </c>
+      <c r="AQ12">
+        <v>9733</v>
+      </c>
+      <c r="AR12">
+        <v>8562</v>
+      </c>
+      <c r="AS12">
+        <v>9794</v>
+      </c>
+      <c r="AT12">
+        <v>7968</v>
+      </c>
+      <c r="AU12">
+        <v>6465</v>
+      </c>
+      <c r="AV12">
+        <v>5312</v>
+      </c>
+      <c r="AW12">
+        <v>4497</v>
+      </c>
+      <c r="AX12">
+        <v>3561</v>
+      </c>
+      <c r="AY12">
+        <v>3770</v>
+      </c>
+      <c r="AZ12">
+        <v>4054</v>
+      </c>
+      <c r="BA12">
+        <v>4261</v>
+      </c>
+    </row>
+    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13">
+        <v>566</v>
+      </c>
+      <c r="C13">
+        <v>1803</v>
+      </c>
+      <c r="D13">
+        <v>2328</v>
+      </c>
+      <c r="E13">
+        <v>2308</v>
+      </c>
+      <c r="F13">
+        <v>1675</v>
+      </c>
+      <c r="G13">
+        <v>1026</v>
+      </c>
+      <c r="H13">
+        <v>697</v>
+      </c>
+      <c r="I13">
+        <v>456</v>
+      </c>
+      <c r="J13">
+        <v>404</v>
+      </c>
+      <c r="K13">
+        <v>356</v>
+      </c>
+      <c r="L13">
+        <v>243</v>
+      </c>
+      <c r="M13">
+        <v>212</v>
+      </c>
+      <c r="N13">
+        <v>176</v>
+      </c>
+      <c r="O13">
+        <v>158</v>
+      </c>
+      <c r="P13">
+        <v>454</v>
+      </c>
+      <c r="Q13">
+        <v>274</v>
+      </c>
+      <c r="R13">
+        <v>215</v>
+      </c>
+      <c r="S13">
+        <v>190</v>
+      </c>
+      <c r="T13">
+        <v>252</v>
+      </c>
+      <c r="U13">
+        <v>321</v>
+      </c>
+      <c r="V13">
+        <v>429</v>
+      </c>
+      <c r="W13">
+        <v>489</v>
+      </c>
+      <c r="X13">
+        <v>639</v>
+      </c>
+      <c r="Y13">
+        <v>716</v>
+      </c>
+      <c r="Z13">
+        <v>660</v>
+      </c>
+      <c r="AA13">
+        <v>648</v>
+      </c>
+      <c r="AB13">
+        <v>687</v>
+      </c>
+      <c r="AC13">
+        <v>844</v>
+      </c>
+      <c r="AD13">
+        <v>861</v>
+      </c>
+      <c r="AE13">
+        <v>1051</v>
+      </c>
+      <c r="AF13">
+        <v>1868</v>
+      </c>
+      <c r="AG13">
+        <v>2906</v>
+      </c>
+      <c r="AH13">
+        <v>5304</v>
+      </c>
+      <c r="AI13">
+        <v>7875</v>
+      </c>
+      <c r="AJ13">
+        <v>8882</v>
+      </c>
+      <c r="AK13">
+        <v>8989</v>
+      </c>
+      <c r="AL13">
+        <v>9238</v>
+      </c>
+      <c r="AM13">
+        <v>8810</v>
+      </c>
+      <c r="AN13">
+        <v>8828</v>
+      </c>
+      <c r="AO13">
+        <v>10899</v>
+      </c>
+      <c r="AP13">
+        <v>12000</v>
+      </c>
+      <c r="AQ13">
+        <v>9528</v>
+      </c>
+      <c r="AR13">
+        <v>8033</v>
+      </c>
+      <c r="AS13">
+        <v>9525</v>
+      </c>
+      <c r="AT13">
+        <v>7560</v>
+      </c>
+      <c r="AU13">
+        <v>6226</v>
+      </c>
+      <c r="AV13">
+        <v>5124</v>
+      </c>
+      <c r="AW13">
+        <v>4287</v>
+      </c>
+      <c r="AX13">
+        <v>3470</v>
+      </c>
+      <c r="AY13">
+        <v>3588</v>
+      </c>
+      <c r="AZ13">
+        <v>4141</v>
+      </c>
+      <c r="BA13">
+        <v>4251</v>
+      </c>
+    </row>
+    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14">
+        <v>547</v>
+      </c>
+      <c r="C14">
+        <v>1755</v>
+      </c>
+      <c r="D14">
+        <v>2383</v>
+      </c>
+      <c r="E14">
+        <v>2205</v>
+      </c>
+      <c r="F14">
+        <v>1653</v>
+      </c>
+      <c r="G14">
+        <v>982</v>
+      </c>
+      <c r="H14">
+        <v>764</v>
+      </c>
+      <c r="I14">
+        <v>464</v>
+      </c>
+      <c r="J14">
+        <v>421</v>
+      </c>
+      <c r="K14">
+        <v>353</v>
+      </c>
+      <c r="L14">
+        <v>275</v>
+      </c>
+      <c r="M14">
+        <v>240</v>
+      </c>
+      <c r="N14">
+        <v>157</v>
+      </c>
+      <c r="O14">
+        <v>195</v>
+      </c>
+      <c r="P14">
+        <v>383</v>
+      </c>
+      <c r="Q14">
+        <v>298</v>
+      </c>
+      <c r="R14">
+        <v>226</v>
+      </c>
+      <c r="S14">
+        <v>206</v>
+      </c>
+      <c r="T14">
+        <v>251</v>
+      </c>
+      <c r="U14">
+        <v>360</v>
+      </c>
+      <c r="V14">
+        <v>383</v>
+      </c>
+      <c r="W14">
+        <v>514</v>
+      </c>
+      <c r="X14">
+        <v>644</v>
+      </c>
+      <c r="Y14">
+        <v>760</v>
+      </c>
+      <c r="Z14">
+        <v>716</v>
+      </c>
+      <c r="AA14">
+        <v>650</v>
+      </c>
+      <c r="AB14">
+        <v>701</v>
+      </c>
+      <c r="AC14">
+        <v>901</v>
+      </c>
+      <c r="AD14">
+        <v>1009</v>
+      </c>
+      <c r="AE14">
+        <v>1154</v>
+      </c>
+      <c r="AF14">
+        <v>1826</v>
+      </c>
+      <c r="AG14">
+        <v>3106</v>
+      </c>
+      <c r="AH14">
+        <v>5397</v>
+      </c>
+      <c r="AI14">
+        <v>8087</v>
+      </c>
+      <c r="AJ14">
+        <v>8963</v>
+      </c>
+      <c r="AK14">
+        <v>9192</v>
+      </c>
+      <c r="AL14">
+        <v>9207</v>
+      </c>
+      <c r="AM14">
+        <v>8719</v>
+      </c>
+      <c r="AN14">
+        <v>9136</v>
+      </c>
+      <c r="AO14">
+        <v>11001</v>
+      </c>
+      <c r="AP14">
+        <v>12232</v>
+      </c>
+      <c r="AQ14">
+        <v>9530</v>
+      </c>
+      <c r="AR14">
+        <v>8095</v>
+      </c>
+      <c r="AS14">
+        <v>10136</v>
+      </c>
+      <c r="AT14">
+        <v>8020</v>
+      </c>
+      <c r="AU14">
+        <v>6339</v>
+      </c>
+      <c r="AV14">
+        <v>5211</v>
+      </c>
+      <c r="AW14">
+        <v>4472</v>
+      </c>
+      <c r="AX14">
+        <v>3605</v>
+      </c>
+      <c r="AY14">
+        <v>3729</v>
+      </c>
+      <c r="AZ14">
+        <v>4182</v>
+      </c>
+      <c r="BA14">
+        <v>4535</v>
+      </c>
+    </row>
+    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15">
+        <v>535</v>
+      </c>
+      <c r="C15">
+        <v>2049</v>
+      </c>
+      <c r="D15">
+        <v>2638</v>
+      </c>
+      <c r="E15">
+        <v>2418</v>
+      </c>
+      <c r="F15">
+        <v>1752</v>
+      </c>
+      <c r="G15">
+        <v>1203</v>
+      </c>
+      <c r="H15">
+        <v>908</v>
+      </c>
+      <c r="I15">
+        <v>562</v>
+      </c>
+      <c r="J15">
+        <v>488</v>
+      </c>
+      <c r="K15">
+        <v>391</v>
+      </c>
+      <c r="L15">
+        <v>321</v>
+      </c>
+      <c r="M15">
+        <v>270</v>
+      </c>
+      <c r="N15">
+        <v>206</v>
+      </c>
+      <c r="O15">
+        <v>224</v>
+      </c>
+      <c r="P15">
+        <v>414</v>
+      </c>
+      <c r="Q15">
+        <v>334</v>
+      </c>
+      <c r="R15">
+        <v>260</v>
+      </c>
+      <c r="S15">
+        <v>260</v>
+      </c>
+      <c r="T15">
+        <v>297</v>
+      </c>
+      <c r="U15">
+        <v>384</v>
+      </c>
+      <c r="V15">
+        <v>423</v>
+      </c>
+      <c r="W15">
+        <v>513</v>
+      </c>
+      <c r="X15">
+        <v>700</v>
+      </c>
+      <c r="Y15">
+        <v>944</v>
+      </c>
+      <c r="Z15">
+        <v>856</v>
+      </c>
+      <c r="AA15">
+        <v>940</v>
+      </c>
+      <c r="AB15">
+        <v>940</v>
+      </c>
+      <c r="AC15">
+        <v>1206</v>
+      </c>
+      <c r="AD15">
+        <v>1303</v>
+      </c>
+      <c r="AE15">
+        <v>1524</v>
+      </c>
+      <c r="AF15">
+        <v>2360</v>
+      </c>
+      <c r="AG15">
+        <v>3860</v>
+      </c>
+      <c r="AH15">
+        <v>6718</v>
+      </c>
+      <c r="AI15">
+        <v>9575</v>
+      </c>
+      <c r="AJ15">
+        <v>10489</v>
+      </c>
+      <c r="AK15">
+        <v>10490</v>
+      </c>
+      <c r="AL15">
+        <v>10093</v>
+      </c>
+      <c r="AM15">
+        <v>9382</v>
+      </c>
+      <c r="AN15">
+        <v>9484</v>
+      </c>
+      <c r="AO15">
+        <v>11535</v>
+      </c>
+      <c r="AP15">
+        <v>13020</v>
+      </c>
+      <c r="AQ15">
+        <v>10047</v>
+      </c>
+      <c r="AR15">
+        <v>9197</v>
+      </c>
+      <c r="AS15">
+        <v>11597</v>
+      </c>
+      <c r="AT15">
+        <v>9052</v>
+      </c>
+      <c r="AU15">
+        <v>7031</v>
+      </c>
+      <c r="AV15">
+        <v>5781</v>
+      </c>
+      <c r="AW15">
+        <v>4919</v>
+      </c>
+      <c r="AX15">
+        <v>3903</v>
+      </c>
+      <c r="AY15">
+        <v>4113</v>
+      </c>
+      <c r="AZ15">
+        <v>4555</v>
+      </c>
+      <c r="BA15">
+        <v>4869</v>
+      </c>
+    </row>
+    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16">
+        <v>546</v>
+      </c>
+      <c r="C16">
+        <v>2004</v>
+      </c>
+      <c r="D16">
+        <v>2693</v>
+      </c>
+      <c r="E16">
+        <v>2487</v>
+      </c>
+      <c r="F16">
+        <v>1933</v>
+      </c>
+      <c r="G16">
+        <v>1297</v>
+      </c>
+      <c r="H16">
+        <v>998</v>
+      </c>
+      <c r="I16">
+        <v>681</v>
+      </c>
+      <c r="J16">
+        <v>521</v>
+      </c>
+      <c r="K16">
+        <v>389</v>
+      </c>
+      <c r="L16">
+        <v>350</v>
+      </c>
+      <c r="M16">
+        <v>316</v>
+      </c>
+      <c r="N16">
+        <v>223</v>
+      </c>
+      <c r="O16">
+        <v>243</v>
+      </c>
+      <c r="P16">
+        <v>394</v>
+      </c>
+      <c r="Q16">
+        <v>325</v>
+      </c>
+      <c r="R16">
+        <v>316</v>
+      </c>
+      <c r="S16">
+        <v>227</v>
+      </c>
+      <c r="T16">
+        <v>308</v>
+      </c>
+      <c r="U16">
+        <v>410</v>
+      </c>
+      <c r="V16">
+        <v>510</v>
+      </c>
+      <c r="W16">
+        <v>607</v>
+      </c>
+      <c r="X16">
+        <v>838</v>
+      </c>
+      <c r="Y16">
+        <v>1195</v>
+      </c>
+      <c r="Z16">
+        <v>1221</v>
+      </c>
+      <c r="AA16">
+        <v>1158</v>
+      </c>
+      <c r="AB16">
+        <v>1230</v>
+      </c>
+      <c r="AC16">
+        <v>1483</v>
+      </c>
+      <c r="AD16">
+        <v>1439</v>
+      </c>
+      <c r="AE16">
+        <v>1746</v>
+      </c>
+      <c r="AF16">
+        <v>2690</v>
+      </c>
+      <c r="AG16">
+        <v>4476</v>
+      </c>
+      <c r="AH16">
+        <v>7318</v>
+      </c>
+      <c r="AI16">
+        <v>10336</v>
+      </c>
+      <c r="AJ16">
+        <v>11152</v>
+      </c>
+      <c r="AK16">
+        <v>10705</v>
+      </c>
+      <c r="AL16">
+        <v>9943</v>
+      </c>
+      <c r="AM16">
+        <v>9009</v>
+      </c>
+      <c r="AN16">
+        <v>9145</v>
+      </c>
+      <c r="AO16">
+        <v>10805</v>
+      </c>
+      <c r="AP16">
+        <v>12110</v>
+      </c>
+      <c r="AQ16">
+        <v>9438</v>
+      </c>
+      <c r="AR16">
+        <v>8429</v>
+      </c>
+      <c r="AS16">
+        <v>10796</v>
+      </c>
+      <c r="AT16">
+        <v>8537</v>
+      </c>
+      <c r="AU16">
+        <v>6402</v>
+      </c>
+      <c r="AV16">
+        <v>5351</v>
+      </c>
+      <c r="AW16">
+        <v>4488</v>
+      </c>
+      <c r="AX16">
+        <v>3658</v>
+      </c>
+      <c r="AY16">
+        <v>3901</v>
+      </c>
+      <c r="AZ16">
+        <v>4158</v>
+      </c>
+      <c r="BA16">
+        <v>4244</v>
+      </c>
+    </row>
+    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17">
+        <v>324</v>
+      </c>
+      <c r="C17">
+        <v>1449</v>
+      </c>
+      <c r="D17">
+        <v>2270</v>
+      </c>
+      <c r="E17">
+        <v>2244</v>
+      </c>
+      <c r="F17">
+        <v>1735</v>
+      </c>
+      <c r="G17">
+        <v>1234</v>
+      </c>
+      <c r="H17">
+        <v>961</v>
+      </c>
+      <c r="I17">
+        <v>595</v>
+      </c>
+      <c r="J17">
+        <v>508</v>
+      </c>
+      <c r="K17">
+        <v>416</v>
+      </c>
+      <c r="L17">
+        <v>315</v>
+      </c>
+      <c r="M17">
+        <v>289</v>
+      </c>
+      <c r="N17">
+        <v>230</v>
+      </c>
+      <c r="O17">
+        <v>249</v>
+      </c>
+      <c r="P17">
+        <v>376</v>
+      </c>
+      <c r="Q17">
+        <v>260</v>
+      </c>
+      <c r="R17">
+        <v>258</v>
+      </c>
+      <c r="S17">
+        <v>237</v>
+      </c>
+      <c r="T17">
+        <v>300</v>
+      </c>
+      <c r="U17">
+        <v>378</v>
+      </c>
+      <c r="V17">
+        <v>521</v>
+      </c>
+      <c r="W17">
+        <v>745</v>
+      </c>
+      <c r="X17">
+        <v>1166</v>
+      </c>
+      <c r="Y17">
+        <v>1545</v>
+      </c>
+      <c r="Z17">
+        <v>1326</v>
+      </c>
+      <c r="AA17">
+        <v>1250</v>
+      </c>
+      <c r="AB17">
+        <v>1287</v>
+      </c>
+      <c r="AC17">
+        <v>1516</v>
+      </c>
+      <c r="AD17">
+        <v>1583</v>
+      </c>
+      <c r="AE17">
+        <v>1741</v>
+      </c>
+      <c r="AF17">
+        <v>2788</v>
+      </c>
+      <c r="AG17">
+        <v>4383</v>
+      </c>
+      <c r="AH17">
+        <v>7552</v>
+      </c>
+      <c r="AI17">
+        <v>10430</v>
+      </c>
+      <c r="AJ17">
+        <v>11742</v>
+      </c>
+      <c r="AK17">
+        <v>11042</v>
+      </c>
+      <c r="AL17">
+        <v>10223</v>
+      </c>
+      <c r="AM17">
+        <v>8944</v>
+      </c>
+      <c r="AN17">
+        <v>9196</v>
+      </c>
+      <c r="AO17">
+        <v>10793</v>
+      </c>
+      <c r="AP17">
+        <v>12105</v>
+      </c>
+      <c r="AQ17">
+        <v>9080</v>
+      </c>
+      <c r="AR17">
+        <v>8607</v>
+      </c>
+      <c r="AS17">
+        <v>10892</v>
+      </c>
+      <c r="AT17">
+        <v>8516</v>
+      </c>
+      <c r="AU17">
+        <v>6443</v>
+      </c>
+      <c r="AV17">
+        <v>5245</v>
+      </c>
+      <c r="AW17">
+        <v>4380</v>
+      </c>
+      <c r="AX17">
+        <v>3664</v>
+      </c>
+      <c r="AY17">
+        <v>3957</v>
+      </c>
+      <c r="AZ17">
+        <v>4206</v>
+      </c>
+      <c r="BA17">
+        <v>4376</v>
+      </c>
+    </row>
+    <row r="18" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18">
+        <v>183</v>
+      </c>
+      <c r="C18">
+        <v>541</v>
+      </c>
+      <c r="D18">
+        <v>938</v>
+      </c>
+      <c r="E18">
+        <v>1077</v>
+      </c>
+      <c r="F18">
+        <v>856</v>
+      </c>
+      <c r="G18">
+        <v>572</v>
+      </c>
+      <c r="H18">
+        <v>401</v>
+      </c>
+      <c r="I18">
+        <v>265</v>
+      </c>
+      <c r="J18">
+        <v>260</v>
+      </c>
+      <c r="K18">
+        <v>181</v>
+      </c>
+      <c r="L18">
+        <v>153</v>
+      </c>
+      <c r="M18">
+        <v>162</v>
+      </c>
+      <c r="N18">
+        <v>161</v>
+      </c>
+      <c r="O18">
+        <v>111</v>
+      </c>
+      <c r="P18">
+        <v>240</v>
+      </c>
+      <c r="Q18">
+        <v>169</v>
+      </c>
+      <c r="R18">
+        <v>138</v>
+      </c>
+      <c r="S18">
+        <v>149</v>
+      </c>
+      <c r="T18">
+        <v>191</v>
+      </c>
+      <c r="U18">
+        <v>247</v>
+      </c>
+      <c r="V18">
+        <v>364</v>
+      </c>
+      <c r="W18">
+        <v>542</v>
+      </c>
+      <c r="X18">
+        <v>742</v>
+      </c>
+      <c r="Y18">
+        <v>881</v>
+      </c>
+      <c r="Z18">
+        <v>833</v>
+      </c>
+      <c r="AA18">
+        <v>770</v>
+      </c>
+      <c r="AB18">
+        <v>831</v>
+      </c>
+      <c r="AC18">
+        <v>1040</v>
+      </c>
+      <c r="AD18">
+        <v>1046</v>
+      </c>
+      <c r="AE18">
+        <v>1327</v>
+      </c>
+      <c r="AF18">
+        <v>2067</v>
+      </c>
+      <c r="AG18">
+        <v>2962</v>
+      </c>
+      <c r="AH18">
+        <v>4858</v>
+      </c>
+      <c r="AI18">
+        <v>7194</v>
+      </c>
+      <c r="AJ18">
+        <v>8411</v>
+      </c>
+      <c r="AK18">
+        <v>8714</v>
+      </c>
+      <c r="AL18">
+        <v>8202</v>
+      </c>
+      <c r="AM18">
+        <v>7458</v>
+      </c>
+      <c r="AN18">
+        <v>7728</v>
+      </c>
+      <c r="AO18">
+        <v>8838</v>
+      </c>
+      <c r="AP18">
+        <v>8467</v>
+      </c>
+      <c r="AQ18">
+        <v>5875</v>
+      </c>
+      <c r="AR18">
+        <v>4954</v>
+      </c>
+      <c r="AS18">
+        <v>6379</v>
+      </c>
+      <c r="AT18">
+        <v>5409</v>
+      </c>
+      <c r="AU18">
+        <v>4206</v>
+      </c>
+      <c r="AV18">
+        <v>3481</v>
+      </c>
+      <c r="AW18">
+        <v>2920</v>
+      </c>
+      <c r="AX18">
+        <v>2380</v>
+      </c>
+      <c r="AY18">
+        <v>2624</v>
+      </c>
+      <c r="AZ18">
+        <v>3071</v>
+      </c>
+      <c r="BA18">
+        <v>3179</v>
+      </c>
+    </row>
+    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19">
+        <v>101</v>
+      </c>
+      <c r="C19">
+        <v>253</v>
+      </c>
+      <c r="D19">
+        <v>379</v>
+      </c>
+      <c r="E19">
+        <v>430</v>
+      </c>
+      <c r="F19">
+        <v>303</v>
+      </c>
+      <c r="G19">
+        <v>236</v>
+      </c>
+      <c r="H19">
+        <v>188</v>
+      </c>
+      <c r="I19">
+        <v>136</v>
+      </c>
+      <c r="J19">
+        <v>125</v>
+      </c>
+      <c r="K19">
+        <v>117</v>
+      </c>
+      <c r="L19">
+        <v>108</v>
+      </c>
+      <c r="M19">
+        <v>119</v>
+      </c>
+      <c r="N19">
+        <v>103</v>
+      </c>
+      <c r="O19">
+        <v>119</v>
+      </c>
+      <c r="P19">
+        <v>192</v>
+      </c>
+      <c r="Q19">
+        <v>146</v>
+      </c>
+      <c r="R19">
+        <v>105</v>
+      </c>
+      <c r="S19">
+        <v>102</v>
+      </c>
+      <c r="T19">
+        <v>148</v>
+      </c>
+      <c r="U19">
+        <v>191</v>
+      </c>
+      <c r="V19">
+        <v>251</v>
+      </c>
+      <c r="W19">
+        <v>364</v>
+      </c>
+      <c r="X19">
+        <v>544</v>
+      </c>
+      <c r="Y19">
+        <v>577</v>
+      </c>
+      <c r="Z19">
+        <v>483</v>
+      </c>
+      <c r="AA19">
+        <v>430</v>
+      </c>
+      <c r="AB19">
+        <v>498</v>
+      </c>
+      <c r="AC19">
+        <v>518</v>
+      </c>
+      <c r="AD19">
+        <v>586</v>
+      </c>
+      <c r="AE19">
+        <v>708</v>
+      </c>
+      <c r="AF19">
+        <v>1142</v>
+      </c>
+      <c r="AG19">
+        <v>1653</v>
+      </c>
+      <c r="AH19">
+        <v>2744</v>
+      </c>
+      <c r="AI19">
+        <v>4084</v>
+      </c>
+      <c r="AJ19">
+        <v>4772</v>
+      </c>
+      <c r="AK19">
+        <v>5341</v>
+      </c>
+      <c r="AL19">
+        <v>5300</v>
+      </c>
+      <c r="AM19">
+        <v>5185</v>
+      </c>
+      <c r="AN19">
+        <v>5159</v>
+      </c>
+      <c r="AO19">
+        <v>5690</v>
+      </c>
+      <c r="AP19">
+        <v>5287</v>
+      </c>
+      <c r="AQ19">
+        <v>3377</v>
+      </c>
+      <c r="AR19">
+        <v>2648</v>
+      </c>
+      <c r="AS19">
+        <v>3321</v>
+      </c>
+      <c r="AT19">
+        <v>2727</v>
+      </c>
+      <c r="AU19">
+        <v>2223</v>
+      </c>
+      <c r="AV19">
+        <v>1881</v>
+      </c>
+      <c r="AW19">
+        <v>1727</v>
+      </c>
+      <c r="AX19">
+        <v>1412</v>
+      </c>
+      <c r="AY19">
+        <v>1578</v>
+      </c>
+      <c r="AZ19">
+        <v>1883</v>
+      </c>
+      <c r="BA19">
+        <v>2278</v>
+      </c>
+    </row>
+    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20">
+        <v>56</v>
+      </c>
+      <c r="C20">
+        <v>169</v>
+      </c>
+      <c r="D20">
+        <v>249</v>
+      </c>
+      <c r="E20">
+        <v>293</v>
+      </c>
+      <c r="F20">
+        <v>236</v>
+      </c>
+      <c r="G20">
+        <v>163</v>
+      </c>
+      <c r="H20">
+        <v>153</v>
+      </c>
+      <c r="I20">
+        <v>120</v>
+      </c>
+      <c r="J20">
+        <v>105</v>
+      </c>
+      <c r="K20">
+        <v>110</v>
+      </c>
+      <c r="L20">
+        <v>81</v>
+      </c>
+      <c r="M20">
+        <v>113</v>
+      </c>
+      <c r="N20">
+        <v>99</v>
+      </c>
+      <c r="O20">
+        <v>123</v>
+      </c>
+      <c r="P20">
+        <v>176</v>
+      </c>
+      <c r="Q20">
+        <v>139</v>
+      </c>
+      <c r="R20">
+        <v>124</v>
+      </c>
+      <c r="S20">
+        <v>115</v>
+      </c>
+      <c r="T20">
+        <v>136</v>
+      </c>
+      <c r="U20">
+        <v>151</v>
+      </c>
+      <c r="V20">
+        <v>198</v>
+      </c>
+      <c r="W20">
+        <v>285</v>
+      </c>
+      <c r="X20">
+        <v>407</v>
+      </c>
+      <c r="Y20">
+        <v>380</v>
+      </c>
+      <c r="Z20">
+        <v>353</v>
+      </c>
+      <c r="AA20">
+        <v>318</v>
+      </c>
+      <c r="AB20">
+        <v>325</v>
+      </c>
+      <c r="AC20">
+        <v>354</v>
+      </c>
+      <c r="AD20">
+        <v>388</v>
+      </c>
+      <c r="AE20">
+        <v>433</v>
+      </c>
+      <c r="AF20">
+        <v>625</v>
+      </c>
+      <c r="AG20">
+        <v>970</v>
+      </c>
+      <c r="AH20">
+        <v>1832</v>
+      </c>
+      <c r="AI20">
+        <v>2792</v>
+      </c>
+      <c r="AJ20">
+        <v>3363</v>
+      </c>
+      <c r="AK20">
+        <v>3615</v>
+      </c>
+      <c r="AL20">
+        <v>3917</v>
+      </c>
+      <c r="AM20">
+        <v>3815</v>
+      </c>
+      <c r="AN20">
+        <v>3679</v>
+      </c>
+      <c r="AO20">
+        <v>4268</v>
+      </c>
+      <c r="AP20">
+        <v>4309</v>
+      </c>
+      <c r="AQ20">
+        <v>3029</v>
+      </c>
+      <c r="AR20">
+        <v>1940</v>
+      </c>
+      <c r="AS20">
+        <v>2399</v>
+      </c>
+      <c r="AT20">
+        <v>2204</v>
+      </c>
+      <c r="AU20">
+        <v>1901</v>
+      </c>
+      <c r="AV20">
+        <v>1643</v>
+      </c>
+      <c r="AW20">
+        <v>1605</v>
+      </c>
+      <c r="AX20">
+        <v>1391</v>
+      </c>
+      <c r="AY20">
+        <v>1549</v>
+      </c>
+      <c r="AZ20">
+        <v>2008</v>
+      </c>
+      <c r="BA20">
+        <v>2702</v>
+      </c>
+    </row>
+    <row r="21" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21">
+        <v>36</v>
+      </c>
+      <c r="C21">
+        <v>143</v>
+      </c>
+      <c r="D21">
+        <v>254</v>
+      </c>
+      <c r="E21">
+        <v>272</v>
+      </c>
+      <c r="F21">
+        <v>236</v>
+      </c>
+      <c r="G21">
+        <v>161</v>
+      </c>
+      <c r="H21">
+        <v>185</v>
+      </c>
+      <c r="I21">
+        <v>132</v>
+      </c>
+      <c r="J21">
+        <v>138</v>
+      </c>
+      <c r="K21">
+        <v>116</v>
+      </c>
+      <c r="L21">
+        <v>122</v>
+      </c>
+      <c r="M21">
+        <v>88</v>
+      </c>
+      <c r="N21">
+        <v>108</v>
+      </c>
+      <c r="O21">
+        <v>110</v>
+      </c>
+      <c r="P21">
+        <v>160</v>
+      </c>
+      <c r="Q21">
+        <v>136</v>
+      </c>
+      <c r="R21">
+        <v>141</v>
+      </c>
+      <c r="S21">
+        <v>147</v>
+      </c>
+      <c r="T21">
+        <v>140</v>
+      </c>
+      <c r="U21">
+        <v>161</v>
+      </c>
+      <c r="V21">
+        <v>150</v>
+      </c>
+      <c r="W21">
+        <v>189</v>
+      </c>
+      <c r="X21">
+        <v>276</v>
+      </c>
+      <c r="Y21">
+        <v>283</v>
+      </c>
+      <c r="Z21">
+        <v>223</v>
+      </c>
+      <c r="AA21">
+        <v>227</v>
+      </c>
+      <c r="AB21">
+        <v>226</v>
+      </c>
+      <c r="AC21">
+        <v>291</v>
+      </c>
+      <c r="AD21">
+        <v>301</v>
+      </c>
+      <c r="AE21">
+        <v>325</v>
+      </c>
+      <c r="AF21">
+        <v>524</v>
+      </c>
+      <c r="AG21">
+        <v>887</v>
+      </c>
+      <c r="AH21">
+        <v>1460</v>
+      </c>
+      <c r="AI21">
+        <v>2242</v>
+      </c>
+      <c r="AJ21">
+        <v>2418</v>
+      </c>
+      <c r="AK21">
+        <v>2422</v>
+      </c>
+      <c r="AL21">
+        <v>2380</v>
+      </c>
+      <c r="AM21">
+        <v>2327</v>
+      </c>
+      <c r="AN21">
+        <v>2308</v>
+      </c>
+      <c r="AO21">
+        <v>2675</v>
+      </c>
+      <c r="AP21">
+        <v>3112</v>
+      </c>
+      <c r="AQ21">
+        <v>2119</v>
+      </c>
+      <c r="AR21">
+        <v>1534</v>
+      </c>
+      <c r="AS21">
+        <v>1927</v>
+      </c>
+      <c r="AT21">
+        <v>1864</v>
+      </c>
+      <c r="AU21">
+        <v>1702</v>
+      </c>
+      <c r="AV21">
+        <v>1537</v>
+      </c>
+      <c r="AW21">
+        <v>1509</v>
+      </c>
+      <c r="AX21">
+        <v>1351</v>
+      </c>
+      <c r="AY21">
+        <v>1377</v>
+      </c>
+      <c r="AZ21">
+        <v>1893</v>
+      </c>
+      <c r="BA21">
+        <v>2366</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BA21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A3:A21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2">
         <v>7.72</v>
       </c>
       <c r="C2">

</xml_diff>